<commit_message>
separated the potions category into flasks and potion bases.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CK.DESKTOP-BR5NVLN\Documents\Git Repositories\Creative\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596D208C-1087-4BD9-9AE2-6DC05AA50EE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1375414E-CB07-469A-8026-1125AD42289B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="2" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="338">
   <si>
     <t>Weapon</t>
   </si>
@@ -758,9 +758,6 @@
     <t>MEDIUM RANGED Weapons</t>
   </si>
   <si>
-    <t>HEAVY RANGED Weapons</t>
-  </si>
-  <si>
     <t>SHIELDS</t>
   </si>
   <si>
@@ -1439,10 +1436,6 @@
     <t>Basket Hilt</t>
   </si>
   <si>
-    <t>1 MOD per 0.5 lbs
-superior parry</t>
-  </si>
-  <si>
     <t>Flamberge Blade</t>
   </si>
   <si>
@@ -1475,12 +1468,6 @@
     <t>slashing 2</t>
   </si>
   <si>
-    <t>1 bar of metal
-OR
-square plates of metal
-(20:1 lbs)</t>
-  </si>
-  <si>
     <t>Crescent Blade</t>
   </si>
   <si>
@@ -1790,6 +1777,44 @@
   </si>
   <si>
     <t>Pelt</t>
+  </si>
+  <si>
+    <t>Armourslayer Blade</t>
+  </si>
+  <si>
+    <t>slashing
+spiked 2
+precision 1
+keen 1</t>
+  </si>
+  <si>
+    <t>1 bar of metal</t>
+  </si>
+  <si>
+    <t>superior parry</t>
+  </si>
+  <si>
+    <t>Glyph Guard</t>
+  </si>
+  <si>
+    <t>Funnel Hilt</t>
+  </si>
+  <si>
+    <t>Disk Hilt</t>
+  </si>
+  <si>
+    <t>Glyph Hilt</t>
+  </si>
+  <si>
+    <t>glyph guard
+grip
+pommel</t>
+  </si>
+  <si>
+    <t>patterned</t>
+  </si>
+  <si>
+    <t>HEAVY RANGED WEAPONS</t>
   </si>
 </sst>
 </file>
@@ -1841,7 +1866,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1940,11 +1965,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1958,12 +2003,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1985,17 +2024,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2022,7 +2052,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2064,85 +2093,166 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2458,21 +2568,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:D52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="4" customWidth="1"/>
-    <col min="3" max="4" width="10" style="10" customWidth="1"/>
+    <col min="3" max="4" width="10" style="8" customWidth="1"/>
     <col min="5" max="5" width="5.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="9" customWidth="1"/>
-    <col min="8" max="9" width="10" style="9" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="7" customWidth="1"/>
+    <col min="8" max="9" width="10" style="7" customWidth="1"/>
     <col min="10" max="10" width="5.140625" style="4" customWidth="1"/>
     <col min="11" max="11" width="20.5703125" style="4" customWidth="1"/>
     <col min="12" max="12" width="18.85546875" style="4" customWidth="1"/>
@@ -2520,887 +2630,931 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="F2" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="K2" s="7" t="s">
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="K2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="K6" s="7" t="s">
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="K6" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="F7" s="11" t="s">
+      <c r="A7" s="70"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="F7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="195" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="20"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="15"/>
     </row>
     <row r="10" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="210" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="F14" s="11" t="s">
+      <c r="A14" s="70"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="F14" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="285" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="K15" s="9"/>
+      <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="165" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="19" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
     </row>
     <row r="19" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="58" t="s">
-        <v>328</v>
-      </c>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
+      <c r="F19" s="68" t="s">
+        <v>325</v>
+      </c>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68"/>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68"/>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="8" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="8" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="69" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="8" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="8" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="8" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="8" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="69" t="s">
         <v>168</v>
       </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
+      <c r="B44" s="69"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="8" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="8" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="69" t="s">
         <v>177</v>
       </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="9"/>
+      <c r="A49" s="63"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="5"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="17"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="69" t="s">
         <v>178</v>
       </c>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="B52" s="69"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="63"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="17"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="58"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="69" t="s">
+        <v>337</v>
+      </c>
+      <c r="B56" s="69"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="69"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="63"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="56"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="58"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="17"/>
+      <c r="B59" s="65"/>
+      <c r="C59" s="66"/>
+      <c r="D59" s="66"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="67" t="s">
         <v>179</v>
       </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
+      <c r="B60" s="67"/>
+      <c r="C60" s="67"/>
+      <c r="D60" s="67"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="63"/>
+      <c r="B61" s="62"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="62"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="56"/>
+      <c r="C62" s="58"/>
+      <c r="D62" s="58"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="13"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="64"/>
+      <c r="D63" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F19:I21"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="F13:I13"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="F2:I2"/>
@@ -3409,6 +3563,18 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="F19:I21"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A56:D56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3417,10 +3583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E7B11-1527-417B-9532-F0F2C5A89902}">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3428,760 +3594,819 @@
     <col min="1" max="1" width="28" style="4" customWidth="1"/>
     <col min="2" max="2" width="20" style="4" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="4" style="30" customWidth="1"/>
-    <col min="6" max="6" width="10" style="10" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="4" style="24" customWidth="1"/>
+    <col min="6" max="6" width="10" style="8" customWidth="1"/>
     <col min="7" max="7" width="28" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20" style="9" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="29" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="4" style="10" customWidth="1"/>
-    <col min="12" max="12" width="10" style="9" customWidth="1"/>
+    <col min="8" max="8" width="20" style="7" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="23" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="4" style="8" customWidth="1"/>
+    <col min="12" max="12" width="10" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E1" s="62" t="s">
-        <v>298</v>
+        <v>296</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>295</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="K1" s="62" t="s">
-        <v>298</v>
-      </c>
-      <c r="L1" s="61"/>
+        <v>296</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>295</v>
+      </c>
+      <c r="L1" s="44"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="60"/>
-    </row>
-    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="B3" s="59" t="s">
+      <c r="A2" s="67" t="s">
         <v>294</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>228</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="74" t="s">
         <v>293</v>
       </c>
-      <c r="E3" s="30">
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="43"/>
+    </row>
+    <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="87" t="s">
+        <v>329</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="24">
         <v>3</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="J3" s="9" t="s">
         <v>290</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>288</v>
       </c>
       <c r="K3" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="E4" s="56">
+      <c r="A4" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="88"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" s="41">
         <v>2</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="K4" s="9">
+      <c r="G4" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="K4" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="E5" s="30">
+      <c r="A5" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" s="88"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E5" s="24">
         <v>3</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="G5" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="H5" s="7" t="s">
         <v>281</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="K5" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="9" t="s">
+      <c r="A6" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="E6" s="56">
+      <c r="B6" s="88"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E6" s="41">
         <v>1</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="H6" s="9" t="s">
+      <c r="G6" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="H6" s="7" t="s">
         <v>276</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>275</v>
       </c>
       <c r="K6" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="9" t="s">
+      <c r="A7" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="E7" s="9">
+      <c r="B7" s="88"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E7" s="7">
         <v>2</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="J7" s="55" t="s">
-        <v>262</v>
+      <c r="G7" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>261</v>
       </c>
       <c r="K7" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="B8" s="29" t="s">
+    <row r="8" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8" s="88"/>
+      <c r="C8" s="75" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="E8" s="7">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I8" s="42"/>
+      <c r="J8" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="K8" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="B9" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="C9" s="75"/>
+      <c r="D9" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="E9" s="41">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="I9" s="33"/>
+      <c r="J9" s="40" t="s">
+        <v>336</v>
+      </c>
+      <c r="K9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="27">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="E10" s="41">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="I10" s="33"/>
+      <c r="J10" s="40" t="s">
+        <v>261</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="70" t="s">
+        <v>260</v>
+      </c>
+      <c r="B11" s="77" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="84" t="s">
+        <v>227</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>258</v>
+      </c>
+      <c r="E11" s="82">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="73" t="s">
+        <v>257</v>
+      </c>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+    </row>
+    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="86"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="69" t="s">
+        <v>253</v>
+      </c>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="K13" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="E8" s="56">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="I8" s="57"/>
-      <c r="J8" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="K8" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>266</v>
-      </c>
-      <c r="C9" s="33">
+      <c r="C14" s="79" t="s">
+        <v>248</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E14" s="24">
         <v>1</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="E9" s="56">
-        <v>2</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="J9" s="55" t="s">
-        <v>262</v>
-      </c>
-      <c r="K9" s="4">
+      <c r="F14" s="4"/>
+      <c r="G14" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="K14" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="54" t="s">
-        <v>228</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="E10" s="53">
-        <v>3</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-    </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="46" t="s">
-        <v>256</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="K11" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>254</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="29" t="s">
-        <v>252</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="K12" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="C13" s="48" t="s">
-        <v>249</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="E13" s="30">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="J13" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="K13" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="B14" s="29" t="s">
+    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="13" t="s">
+      <c r="B15" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="E14" s="30">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
+      <c r="C15" s="75"/>
+      <c r="D15" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="H14" s="47"/>
-      <c r="I14" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="K14" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>238</v>
-      </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="E15" s="38">
+      <c r="E15" s="24">
         <v>1</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="H15" s="38"/>
+      <c r="I15" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="K15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="70" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" s="77" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="75"/>
+      <c r="D16" s="71" t="s">
         <v>236</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-    </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="38"/>
+      <c r="E16" s="78">
+        <v>1</v>
+      </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="73" t="s">
         <v>235</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="K16" s="4"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="70"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="H17" s="12"/>
+      <c r="I17" s="33"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="9" t="s">
+      <c r="B18" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="E17" s="30">
+      <c r="C18" s="75"/>
+      <c r="D18" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E18" s="24">
         <v>1</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="K17"/>
-    </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="F18" s="4"/>
+      <c r="G18" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="H18" s="12"/>
+      <c r="I18" s="33"/>
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="B19" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="C19" s="75" t="s">
         <v>227</v>
       </c>
-      <c r="E18" s="30">
+      <c r="D19" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E19" s="24">
         <v>2</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="H18" s="13"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="F19" s="4"/>
+      <c r="G19" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="H19" s="12"/>
+      <c r="I19" s="33"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="9" t="s">
+      <c r="B20" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="E19" s="30">
+      <c r="C20" s="75"/>
+      <c r="D20" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E20" s="24">
         <v>3</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="H19" s="13"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="F20" s="4"/>
+      <c r="G20" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="H20" s="12"/>
+      <c r="I20" s="33"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="9" t="s">
+      <c r="B21" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="E20" s="30">
+      <c r="C21" s="75"/>
+      <c r="D21" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E21" s="24">
         <v>4</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="H20" s="13"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="F21" s="4"/>
+      <c r="G21" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="H21" s="12"/>
+      <c r="I21" s="33"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="9" t="s">
+      <c r="B22" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="E21" s="30">
+      <c r="C22" s="75"/>
+      <c r="D22" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E22" s="24">
         <v>3</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H21" s="13"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="F22" s="4"/>
+      <c r="G22" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="H22" s="12"/>
+      <c r="I22" s="33"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="9" t="s">
+      <c r="B23" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="E22" s="30">
+      <c r="C23" s="76"/>
+      <c r="D23" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E23" s="24">
         <v>2</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="H22" s="13"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="F23" s="4"/>
+      <c r="G23" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="H23" s="12"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="H23" s="15"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="15" t="s">
+      <c r="H24" s="12"/>
+      <c r="I24" s="33"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="E25" s="34">
+        <v>2</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="K23" s="38"/>
-    </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="38"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+      <c r="H25" s="12"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B25" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="C25" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="D25" s="41" t="s">
-        <v>203</v>
-      </c>
-      <c r="E25" s="40">
-        <v>2</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
+      <c r="K25" s="32"/>
+    </row>
+    <row r="26" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="H25" s="13"/>
-      <c r="K25" s="35"/>
-    </row>
-    <row r="26" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="E26" s="36">
+      <c r="E26" s="30">
         <v>3</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="16"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="32"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="54"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="H26" s="13"/>
-      <c r="K26" s="9"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="9"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4" t="s">
+      <c r="H27" s="12"/>
+      <c r="I27" s="33"/>
+      <c r="K27" s="29"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="K27" s="9"/>
-    </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H28" s="12"/>
+      <c r="I28" s="33"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="K29" s="4"/>
+      <c r="I29" s="33"/>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="32" t="s">
+      <c r="G30" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-    </row>
-    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I30" s="33"/>
+      <c r="J30" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="H31" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="K31" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="I32" s="33"/>
+      <c r="J32" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="H32" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="K32" s="9">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="I33" s="33"/>
+      <c r="J33" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="J33" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="K33" s="4"/>
-    </row>
-    <row r="34" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K33" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="I34" s="33"/>
+      <c r="J34" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="H34" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>184</v>
-      </c>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I35" s="33"/>
+      <c r="J35" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="H35" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="I35" s="31"/>
-      <c r="J35" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="K35" s="19"/>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="K36" s="4"/>
+      <c r="G36" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="I36" s="25"/>
+      <c r="J36" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="K36" s="14"/>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="K37" s="4"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="54"/>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="54"/>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="K39" s="4"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="56"/>
+      <c r="K39" s="54"/>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
@@ -4273,33 +4498,32 @@
       <c r="F57" s="4"/>
       <c r="K57" s="4"/>
     </row>
+    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="K58" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="C18:C22"/>
+  <mergeCells count="19">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G2:K2"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="G11:K11"/>
     <mergeCell ref="C3:C7"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C14:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4310,8 +4534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6E6499-880E-4FF5-B745-8B197E0A76DF}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4319,365 +4543,365 @@
     <col min="1" max="1" width="28" style="4" customWidth="1"/>
     <col min="2" max="2" width="20" style="4" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="4" style="30" customWidth="1"/>
-    <col min="6" max="6" width="10" style="10" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="4" style="24" customWidth="1"/>
+    <col min="6" max="6" width="10" style="8" customWidth="1"/>
     <col min="7" max="7" width="28" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20" style="9" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="4" style="10" customWidth="1"/>
-    <col min="12" max="12" width="10" style="9" customWidth="1"/>
+    <col min="8" max="8" width="20" style="7" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="4" style="8" customWidth="1"/>
+    <col min="12" max="12" width="10" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E1" s="62" t="s">
-        <v>298</v>
+        <v>296</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>295</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>295</v>
+      </c>
+      <c r="L1" s="44"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="89" t="s">
+        <v>320</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="60" t="s">
+        <v>322</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="K2" s="51" t="s">
+        <v>303</v>
+      </c>
+      <c r="L2" s="43"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="I3" s="27">
+        <v>0</v>
+      </c>
+      <c r="K3" s="50" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="75" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="50" t="s">
+        <v>303</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="49" t="s">
+        <v>315</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="K1" s="62" t="s">
-        <v>298</v>
-      </c>
-      <c r="L1" s="61"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="34" t="s">
-        <v>323</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="68" t="s">
-        <v>322</v>
-      </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>252</v>
-      </c>
-      <c r="K2" s="68" t="s">
-        <v>306</v>
-      </c>
-      <c r="L2" s="60"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="34" t="s">
-        <v>323</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="68" t="s">
-        <v>322</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="I3" s="33">
-        <v>0</v>
-      </c>
-      <c r="K3" s="67" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="45" t="s">
-        <v>319</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="67" t="s">
-        <v>306</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="I4" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="K4" s="68" t="s">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="51" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="68" t="s">
-        <v>306</v>
       </c>
       <c r="F5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="34">
+      <c r="A6" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="28">
         <v>0</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="56">
+      <c r="D6" s="7"/>
+      <c r="E6" s="41">
         <v>0</v>
       </c>
       <c r="F6" s="4"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>314</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="67" t="s">
+      <c r="A7" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="50" t="s">
+        <v>303</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C8" s="75"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="50" t="s">
+        <v>303</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="50" t="s">
+        <v>300</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C10" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="67" t="s">
-        <v>306</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-    </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>311</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="67" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="50" t="s">
+        <v>300</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="27" t="s">
+        <v>304</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="50" t="s">
         <v>303</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>309</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="67" t="s">
-        <v>303</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="33" t="s">
-        <v>307</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="67" t="s">
-        <v>306</v>
-      </c>
       <c r="F11" s="4"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="K11" s="9"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
-        <v>305</v>
-      </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="66" t="s">
-        <v>304</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="65" t="s">
-        <v>303</v>
+      <c r="A12" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="49" t="s">
+        <v>301</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="48" t="s">
+        <v>300</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="56"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="4"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="9"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="7"/>
       <c r="F15" s="4"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
       <c r="K15"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="13"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="11"/>
       <c r="F16" s="4"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="9"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="7"/>
       <c r="F17" s="4"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="9"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="7"/>
       <c r="F18" s="4"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
       <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="9"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="7"/>
       <c r="F19" s="4"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="9"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="7"/>
       <c r="F20" s="4"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="K20" s="35"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="K20" s="29"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="9"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="7"/>
       <c r="F21" s="4"/>
-      <c r="K21" s="9"/>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="7"/>
       <c r="F22" s="4"/>
-      <c r="K22" s="9"/>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="4"/>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="64"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="47"/>
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="K24" s="9"/>
+      <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="9"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="7"/>
       <c r="F25" s="4"/>
-      <c r="K25" s="9"/>
+      <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
       <c r="K26" s="4"/>
@@ -4685,27 +4909,27 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="63"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
     </row>
     <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="9"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="7"/>
       <c r="F28" s="4"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="K28" s="9"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="K29" s="9"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
@@ -4851,9 +5075,10 @@
       <c r="D58" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fleshed out the enchanting system and gemstone grades, and added gold cost to materials.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CK.DESKTOP-BR5NVLN\Documents\Git Repositories\Creative\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1375414E-CB07-469A-8026-1125AD42289B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF9876D-D782-4D7B-A136-345C56013473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -1989,7 +1989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2077,9 +2077,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -2101,113 +2098,143 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2216,42 +2243,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2570,8 +2567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2630,18 +2627,18 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="F2" s="74" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="F2" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
       <c r="K2" s="5" t="s">
         <v>8</v>
       </c>
@@ -2734,33 +2731,33 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="72" t="s">
+      <c r="D6" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
       <c r="K6" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
       <c r="F7" s="9" t="s">
         <v>39</v>
       </c>
@@ -2917,30 +2914,30 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="72" t="s">
+      <c r="D13" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
     </row>
     <row r="14" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="70"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
       <c r="F14" s="9" t="s">
         <v>79</v>
       </c>
@@ -3034,12 +3031,12 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="69" t="s">
+      <c r="A18" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
     </row>
     <row r="19" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -3054,12 +3051,12 @@
       <c r="D19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="68" t="s">
+      <c r="F19" s="72" t="s">
         <v>325</v>
       </c>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -3074,10 +3071,10 @@
       <c r="D20" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="72"/>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -3092,10 +3089,10 @@
       <c r="D21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -3280,12 +3277,12 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="69" t="s">
+      <c r="A35" s="65" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -3400,12 +3397,12 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="69" t="s">
+      <c r="A44" s="65" t="s">
         <v>168</v>
       </c>
-      <c r="B44" s="69"/>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
+      <c r="B44" s="65"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
@@ -3450,111 +3447,118 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="69" t="s">
+      <c r="A48" s="65" t="s">
         <v>177</v>
       </c>
-      <c r="B48" s="69"/>
-      <c r="C48" s="69"/>
-      <c r="D48" s="69"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="63"/>
-      <c r="B49" s="62"/>
-      <c r="C49" s="62"/>
-      <c r="D49" s="62"/>
+      <c r="A49" s="61"/>
+      <c r="B49" s="60"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="60"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
-      <c r="B50" s="56"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="17"/>
-      <c r="B51" s="56"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="69" t="s">
+      <c r="A52" s="65" t="s">
         <v>178</v>
       </c>
-      <c r="B52" s="69"/>
-      <c r="C52" s="69"/>
-      <c r="D52" s="69"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="65"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="63"/>
-      <c r="B53" s="62"/>
-      <c r="C53" s="62"/>
-      <c r="D53" s="62"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="60"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
-      <c r="B54" s="56"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
+      <c r="B54" s="54"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="56"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="17"/>
-      <c r="B55" s="56"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
+      <c r="B55" s="54"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="69" t="s">
+      <c r="A56" s="65" t="s">
         <v>337</v>
       </c>
-      <c r="B56" s="69"/>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
+      <c r="B56" s="65"/>
+      <c r="C56" s="65"/>
+      <c r="D56" s="65"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="63"/>
-      <c r="B57" s="62"/>
-      <c r="C57" s="62"/>
-      <c r="D57" s="62"/>
+      <c r="A57" s="61"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
-      <c r="B58" s="56"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
+      <c r="B58" s="54"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="17"/>
-      <c r="B59" s="65"/>
-      <c r="C59" s="66"/>
-      <c r="D59" s="66"/>
+      <c r="B59" s="63"/>
+      <c r="C59" s="64"/>
+      <c r="D59" s="64"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="67" t="s">
+      <c r="A60" s="66" t="s">
         <v>179</v>
       </c>
-      <c r="B60" s="67"/>
-      <c r="C60" s="67"/>
-      <c r="D60" s="67"/>
+      <c r="B60" s="66"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="66"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="63"/>
-      <c r="B61" s="62"/>
-      <c r="C61" s="62"/>
-      <c r="D61" s="62"/>
+      <c r="A61" s="61"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
-      <c r="B62" s="56"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="58"/>
+      <c r="B62" s="54"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="56"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13"/>
       <c r="B63" s="19"/>
-      <c r="C63" s="64"/>
-      <c r="D63" s="64"/>
+      <c r="C63" s="62"/>
+      <c r="D63" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="F19:I21"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A56:D56"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="F2:I2"/>
@@ -3568,13 +3572,6 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="F13:I13"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="F19:I21"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A56:D56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3585,8 +3582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E7B11-1527-417B-9532-F0F2C5A89902}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3618,7 +3615,7 @@
       <c r="D1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="43" t="s">
         <v>295</v>
       </c>
       <c r="F1" s="2"/>
@@ -3634,37 +3631,37 @@
       <c r="J1" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="43" t="s">
         <v>295</v>
       </c>
-      <c r="L1" s="44"/>
+      <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="66" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
       <c r="F2" s="22"/>
-      <c r="G2" s="74" t="s">
+      <c r="G2" s="67" t="s">
         <v>293</v>
       </c>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="43"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="41"/>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="82" t="s">
         <v>329</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="73" t="s">
         <v>227</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -3691,12 +3688,12 @@
       <c r="A4" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="80"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="39">
         <v>2</v>
       </c>
       <c r="F4" s="4"/>
@@ -3717,8 +3714,8 @@
       <c r="A5" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="80"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="7" t="s">
         <v>330</v>
       </c>
@@ -3743,12 +3740,12 @@
       <c r="A6" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="80"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="74"/>
       <c r="D6" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>1</v>
       </c>
       <c r="F6" s="4"/>
@@ -3769,8 +3766,8 @@
       <c r="A7" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="80"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="7" t="s">
         <v>273</v>
       </c>
@@ -3784,7 +3781,7 @@
       <c r="H7" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="38" t="s">
         <v>261</v>
       </c>
       <c r="K7" s="4">
@@ -3795,8 +3792,8 @@
       <c r="A8" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="75" t="s">
+      <c r="B8" s="83"/>
+      <c r="C8" s="84" t="s">
         <v>248</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -3812,7 +3809,7 @@
       <c r="H8" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="I8" s="42"/>
+      <c r="I8" s="40"/>
       <c r="J8" s="7" t="s">
         <v>267</v>
       </c>
@@ -3827,11 +3824,11 @@
       <c r="B9" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="C9" s="75"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
       <c r="F9" s="4"/>
@@ -3841,8 +3838,8 @@
       <c r="H9" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="I9" s="33"/>
-      <c r="J9" s="40" t="s">
+      <c r="I9" s="32"/>
+      <c r="J9" s="38" t="s">
         <v>336</v>
       </c>
       <c r="K9" s="4">
@@ -3862,7 +3859,7 @@
       <c r="D10" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>2</v>
       </c>
       <c r="F10" s="4"/>
@@ -3872,8 +3869,8 @@
       <c r="H10" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="40" t="s">
+      <c r="I10" s="32"/>
+      <c r="J10" s="38" t="s">
         <v>261</v>
       </c>
       <c r="K10" s="4">
@@ -3881,42 +3878,42 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="68" t="s">
         <v>260</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="80" t="s">
         <v>259</v>
       </c>
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="78" t="s">
         <v>227</v>
       </c>
-      <c r="D11" s="71" t="s">
+      <c r="D11" s="69" t="s">
         <v>258</v>
       </c>
-      <c r="E11" s="82">
+      <c r="E11" s="76">
         <v>3</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="73" t="s">
+      <c r="G11" s="71" t="s">
         <v>257</v>
       </c>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="86"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="83"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="77"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
         <v>256</v>
       </c>
       <c r="H12" s="12"/>
-      <c r="I12" s="37" t="s">
+      <c r="I12" s="36" t="s">
         <v>255</v>
       </c>
       <c r="J12" s="7" t="s">
@@ -3927,19 +3924,19 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="65" t="s">
         <v>253</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
         <v>252</v>
       </c>
       <c r="H13" s="12"/>
-      <c r="I13" s="33" t="s">
+      <c r="I13" s="32" t="s">
         <v>251</v>
       </c>
       <c r="J13" s="7" t="s">
@@ -3956,7 +3953,7 @@
       <c r="B14" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="73" t="s">
         <v>248</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -3970,7 +3967,7 @@
         <v>246</v>
       </c>
       <c r="H14" s="12"/>
-      <c r="I14" s="33"/>
+      <c r="I14" s="32"/>
       <c r="J14" s="7" t="s">
         <v>245</v>
       </c>
@@ -3985,7 +3982,7 @@
       <c r="B15" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="C15" s="75"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="11" t="s">
         <v>242</v>
       </c>
@@ -3996,8 +3993,8 @@
       <c r="G15" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="H15" s="38"/>
-      <c r="I15" s="37" t="s">
+      <c r="H15" s="37"/>
+      <c r="I15" s="36" t="s">
         <v>240</v>
       </c>
       <c r="J15" s="7" t="s">
@@ -4008,40 +4005,40 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="68" t="s">
         <v>238</v>
       </c>
-      <c r="B16" s="77" t="s">
+      <c r="B16" s="80" t="s">
         <v>237</v>
       </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="71" t="s">
+      <c r="C16" s="84"/>
+      <c r="D16" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="E16" s="78">
+      <c r="E16" s="86">
         <v>1</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="73" t="s">
+      <c r="G16" s="71" t="s">
         <v>235</v>
       </c>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="70"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="78"/>
+      <c r="A17" s="68"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="86"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
         <v>234</v>
       </c>
       <c r="H17" s="12"/>
-      <c r="I17" s="33"/>
+      <c r="I17" s="32"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4051,7 +4048,7 @@
       <c r="B18" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="C18" s="75"/>
+      <c r="C18" s="84"/>
       <c r="D18" s="7" t="s">
         <v>231</v>
       </c>
@@ -4063,7 +4060,7 @@
         <v>230</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="33"/>
+      <c r="I18" s="32"/>
       <c r="K18"/>
     </row>
     <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4073,7 +4070,7 @@
       <c r="B19" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="84" t="s">
         <v>227</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -4087,7 +4084,7 @@
         <v>225</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="I19" s="33"/>
+      <c r="I19" s="32"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4097,7 +4094,7 @@
       <c r="B20" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="C20" s="75"/>
+      <c r="C20" s="84"/>
       <c r="D20" s="7" t="s">
         <v>222</v>
       </c>
@@ -4109,7 +4106,7 @@
         <v>221</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="33"/>
+      <c r="I20" s="32"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4119,7 +4116,7 @@
       <c r="B21" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="C21" s="75"/>
+      <c r="C21" s="84"/>
       <c r="D21" s="7" t="s">
         <v>218</v>
       </c>
@@ -4131,7 +4128,7 @@
         <v>217</v>
       </c>
       <c r="H21" s="12"/>
-      <c r="I21" s="33"/>
+      <c r="I21" s="32"/>
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4141,7 +4138,7 @@
       <c r="B22" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="C22" s="75"/>
+      <c r="C22" s="84"/>
       <c r="D22" s="7" t="s">
         <v>214</v>
       </c>
@@ -4153,7 +4150,7 @@
         <v>213</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="I22" s="33"/>
+      <c r="I22" s="32"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4163,7 +4160,7 @@
       <c r="B23" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="C23" s="76"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="7" t="s">
         <v>210</v>
       </c>
@@ -4175,7 +4172,7 @@
         <v>331</v>
       </c>
       <c r="H23" s="12"/>
-      <c r="I23" s="33"/>
+      <c r="I23" s="32"/>
       <c r="J23" s="7" t="s">
         <v>336</v>
       </c>
@@ -4194,23 +4191,23 @@
         <v>209</v>
       </c>
       <c r="H24" s="12"/>
-      <c r="I24" s="33"/>
+      <c r="I24" s="32"/>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="E25" s="34">
+      <c r="E25" s="33">
         <v>2</v>
       </c>
       <c r="F25" s="4"/>
@@ -4218,11 +4215,11 @@
         <v>207</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="33"/>
+      <c r="I25" s="32"/>
       <c r="J25" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="K25" s="32"/>
+      <c r="K25" s="31"/>
     </row>
     <row r="26" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
@@ -4231,7 +4228,7 @@
       <c r="B26" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="C26" s="31"/>
+      <c r="C26" s="88"/>
       <c r="D26" s="19" t="s">
         <v>199</v>
       </c>
@@ -4241,36 +4238,36 @@
       <c r="F26" s="4"/>
       <c r="G26" s="16"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="33"/>
+      <c r="I26" s="32"/>
       <c r="J26" s="12"/>
-      <c r="K26" s="32"/>
+      <c r="K26" s="31"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="57"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="55"/>
       <c r="F27" s="4"/>
       <c r="G27" s="5" t="s">
         <v>198</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="33"/>
+      <c r="I27" s="32"/>
       <c r="K27" s="29"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="57"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="55"/>
       <c r="F28" s="4"/>
       <c r="G28" s="5" t="s">
         <v>197</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="33"/>
+      <c r="I28" s="32"/>
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4279,7 +4276,7 @@
       <c r="G29" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="I29" s="33"/>
+      <c r="I29" s="32"/>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -4288,7 +4285,7 @@
       <c r="G30" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="I30" s="33"/>
+      <c r="I30" s="32"/>
       <c r="J30" s="7" t="s">
         <v>336</v>
       </c>
@@ -4314,7 +4311,7 @@
       <c r="H32" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="I32" s="33"/>
+      <c r="I32" s="32"/>
       <c r="J32" s="7" t="s">
         <v>191</v>
       </c>
@@ -4331,7 +4328,7 @@
       <c r="H33" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="I33" s="33"/>
+      <c r="I33" s="32"/>
       <c r="J33" s="7" t="s">
         <v>188</v>
       </c>
@@ -4345,7 +4342,7 @@
       <c r="G34" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="I34" s="33"/>
+      <c r="I34" s="32"/>
       <c r="J34" s="7" t="s">
         <v>186</v>
       </c>
@@ -4360,7 +4357,7 @@
       <c r="H35" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="I35" s="33"/>
+      <c r="I35" s="32"/>
       <c r="J35" s="7" t="s">
         <v>183</v>
       </c>
@@ -4384,29 +4381,29 @@
     <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="54"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="52"/>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="54"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="52"/>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="56"/>
-      <c r="K39" s="54"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="52"/>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
@@ -4504,7 +4501,15 @@
       <c r="K58" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C14:C18"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="A13:E13"/>
@@ -4517,13 +4522,6 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C14:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4567,7 +4565,7 @@
       <c r="D1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="43" t="s">
         <v>295</v>
       </c>
       <c r="F1" s="2"/>
@@ -4583,43 +4581,43 @@
       <c r="J1" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="43" t="s">
         <v>295</v>
       </c>
-      <c r="L1" s="44"/>
+      <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="59" t="s">
         <v>323</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="87" t="s">
         <v>320</v>
       </c>
       <c r="D2" s="7"/>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="49" t="s">
         <v>319</v>
       </c>
       <c r="F2" s="22"/>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="58" t="s">
         <v>322</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="49" t="s">
         <v>303</v>
       </c>
-      <c r="L2" s="43"/>
+      <c r="L2" s="41"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>321</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="75"/>
+      <c r="C3" s="84"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="49" t="s">
         <v>319</v>
       </c>
       <c r="F3" s="4"/>
@@ -4629,7 +4627,7 @@
       <c r="I3" s="27">
         <v>0</v>
       </c>
-      <c r="K3" s="50" t="s">
+      <c r="K3" s="48" t="s">
         <v>303</v>
       </c>
     </row>
@@ -4638,11 +4636,11 @@
         <v>317</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="84" t="s">
         <v>316</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="48" t="s">
         <v>303</v>
       </c>
       <c r="F4" s="4"/>
@@ -4650,11 +4648,11 @@
         <v>326</v>
       </c>
       <c r="H4" s="19"/>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="47" t="s">
         <v>315</v>
       </c>
       <c r="J4" s="19"/>
-      <c r="K4" s="53" t="s">
+      <c r="K4" s="51" t="s">
         <v>300</v>
       </c>
     </row>
@@ -4663,9 +4661,9 @@
         <v>314</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="75"/>
+      <c r="C5" s="84"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="49" t="s">
         <v>303</v>
       </c>
       <c r="F5" s="4"/>
@@ -4680,7 +4678,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>0</v>
       </c>
       <c r="F6" s="4"/>
@@ -4690,32 +4688,32 @@
       <c r="A7" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="84" t="s">
         <v>311</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="48" t="s">
         <v>303</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="J7" s="40"/>
+      <c r="J7" s="38"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="C8" s="75"/>
+      <c r="C8" s="84"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="50" t="s">
+      <c r="E8" s="48" t="s">
         <v>303</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -4725,7 +4723,7 @@
         <v>308</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="48" t="s">
         <v>300</v>
       </c>
       <c r="F9" s="4"/>
@@ -4741,7 +4739,7 @@
         <v>306</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="48" t="s">
         <v>300</v>
       </c>
       <c r="F10" s="4"/>
@@ -4758,7 +4756,7 @@
         <v>304</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="48" t="s">
         <v>303</v>
       </c>
       <c r="F11" s="4"/>
@@ -4771,30 +4769,30 @@
         <v>302</v>
       </c>
       <c r="B12" s="19"/>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="47" t="s">
         <v>301</v>
       </c>
       <c r="D12" s="19"/>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="46" t="s">
         <v>300</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" s="27"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="41"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
@@ -4809,7 +4807,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
-      <c r="C15" s="47"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="7"/>
       <c r="F15" s="4"/>
       <c r="H15" s="11"/>
@@ -4819,7 +4817,7 @@
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="47"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="11"/>
       <c r="F16" s="4"/>
       <c r="H16" s="11"/>
@@ -4828,7 +4826,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
-      <c r="C17" s="47"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="7"/>
       <c r="F17" s="4"/>
       <c r="H17" s="11"/>
@@ -4837,7 +4835,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
-      <c r="C18" s="47"/>
+      <c r="C18" s="45"/>
       <c r="D18" s="7"/>
       <c r="F18" s="4"/>
       <c r="H18" s="11"/>
@@ -4846,7 +4844,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
-      <c r="C19" s="47"/>
+      <c r="C19" s="45"/>
       <c r="D19" s="7"/>
       <c r="F19" s="4"/>
       <c r="H19" s="11"/>
@@ -4855,7 +4853,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
-      <c r="C20" s="47"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="7"/>
       <c r="F20" s="4"/>
       <c r="H20" s="11"/>
@@ -4864,14 +4862,14 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
-      <c r="C21" s="47"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="7"/>
       <c r="F21" s="4"/>
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
-      <c r="C22" s="47"/>
+      <c r="C22" s="45"/>
       <c r="D22" s="7"/>
       <c r="F22" s="4"/>
       <c r="K22" s="7"/>
@@ -4887,14 +4885,14 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
-      <c r="C24" s="47"/>
+      <c r="C24" s="45"/>
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
-      <c r="C25" s="47"/>
+      <c r="C25" s="45"/>
       <c r="D25" s="7"/>
       <c r="F25" s="4"/>
       <c r="K25" s="7"/>
@@ -4909,11 +4907,11 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
     </row>
     <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
@@ -5089,7 +5087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BDD3E4-CD4B-4172-8C8B-0D7A30DAAB4E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
continued working on crafting challenges, and made slight progress on staff and potion components.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CK.DESKTOP-BR5NVLN\Documents\Git Repositories\Creative\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF9876D-D782-4D7B-A136-345C56013473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A8DE61-2484-49CC-9D90-1DC4C072B860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="4" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
     <sheet name="WEAPON COMPONENTS" sheetId="2" r:id="rId2"/>
     <sheet name="ARMOUR COMPONENTS" sheetId="3" r:id="rId3"/>
     <sheet name="STAFF COMPONENTS" sheetId="5" r:id="rId4"/>
-    <sheet name="POTION COMPONENTS" sheetId="4" r:id="rId5"/>
+    <sheet name="POTION COMPONENTS" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="345">
   <si>
     <t>Weapon</t>
   </si>
@@ -1815,6 +1815,27 @@
   </si>
   <si>
     <t>HEAVY RANGED WEAPONS</t>
+  </si>
+  <si>
+    <t>CORES</t>
+  </si>
+  <si>
+    <t>CONDUITS</t>
+  </si>
+  <si>
+    <t>wires</t>
+  </si>
+  <si>
+    <t>GRIPS</t>
+  </si>
+  <si>
+    <t>Flasks</t>
+  </si>
+  <si>
+    <t>Corks</t>
+  </si>
+  <si>
+    <t>WRAPS</t>
   </si>
 </sst>
 </file>
@@ -1989,7 +2010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2179,13 +2200,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2200,12 +2224,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2224,9 +2260,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2236,20 +2269,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2567,8 +2595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:I6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2627,18 +2655,18 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="F2" s="67" t="s">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="F2" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
       <c r="K2" s="5" t="s">
         <v>8</v>
       </c>
@@ -2731,33 +2759,33 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="71" t="s">
+      <c r="F6" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
       <c r="K6" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
       <c r="F7" s="9" t="s">
         <v>39</v>
       </c>
@@ -2914,30 +2942,30 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="71" t="s">
+      <c r="F13" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
     </row>
     <row r="14" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="68"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
       <c r="F14" s="9" t="s">
         <v>79</v>
       </c>
@@ -3031,12 +3059,12 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
     </row>
     <row r="19" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -3051,12 +3079,12 @@
       <c r="D19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="72" t="s">
+      <c r="F19" s="66" t="s">
         <v>325</v>
       </c>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -3071,10 +3099,10 @@
       <c r="D20" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="66"/>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -3089,10 +3117,10 @@
       <c r="D21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -3277,12 +3305,12 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="65" t="s">
+      <c r="A35" s="67" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="65"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="67"/>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -3397,12 +3425,12 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="65" t="s">
+      <c r="A44" s="67" t="s">
         <v>168</v>
       </c>
-      <c r="B44" s="65"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
@@ -3447,12 +3475,12 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="65" t="s">
+      <c r="A48" s="67" t="s">
         <v>177</v>
       </c>
-      <c r="B48" s="65"/>
-      <c r="C48" s="65"/>
-      <c r="D48" s="65"/>
+      <c r="B48" s="67"/>
+      <c r="C48" s="67"/>
+      <c r="D48" s="67"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="61"/>
@@ -3473,12 +3501,12 @@
       <c r="D51" s="56"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="65" t="s">
+      <c r="A52" s="67" t="s">
         <v>178</v>
       </c>
-      <c r="B52" s="65"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="65"/>
+      <c r="B52" s="67"/>
+      <c r="C52" s="67"/>
+      <c r="D52" s="67"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="61"/>
@@ -3499,12 +3527,12 @@
       <c r="D55" s="56"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="65" t="s">
+      <c r="A56" s="67" t="s">
         <v>337</v>
       </c>
-      <c r="B56" s="65"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="65"/>
+      <c r="B56" s="67"/>
+      <c r="C56" s="67"/>
+      <c r="D56" s="67"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="61"/>
@@ -3525,12 +3553,12 @@
       <c r="D59" s="64"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="65" t="s">
         <v>179</v>
       </c>
-      <c r="B60" s="66"/>
-      <c r="C60" s="66"/>
-      <c r="D60" s="66"/>
+      <c r="B60" s="65"/>
+      <c r="C60" s="65"/>
+      <c r="D60" s="65"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="61"/>
@@ -3552,13 +3580,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="F19:I21"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A56:D56"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="F2:I2"/>
@@ -3572,6 +3593,13 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="F13:I13"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="F19:I21"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A56:D56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3582,8 +3610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E7B11-1527-417B-9532-F0F2C5A89902}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3637,28 +3665,28 @@
       <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="65" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
       <c r="F2" s="22"/>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="68" t="s">
         <v>293</v>
       </c>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
       <c r="L2" s="41"/>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="86" t="s">
         <v>329</v>
       </c>
       <c r="C3" s="73" t="s">
@@ -3688,8 +3716,8 @@
       <c r="A4" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="74"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="7" t="s">
         <v>286</v>
       </c>
@@ -3714,8 +3742,8 @@
       <c r="A5" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="74"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="7" t="s">
         <v>330</v>
       </c>
@@ -3740,8 +3768,8 @@
       <c r="A6" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="74"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="7" t="s">
         <v>278</v>
       </c>
@@ -3766,8 +3794,8 @@
       <c r="A7" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="74"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="7" t="s">
         <v>273</v>
       </c>
@@ -3792,8 +3820,8 @@
       <c r="A8" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="84" t="s">
+      <c r="B8" s="87"/>
+      <c r="C8" s="75" t="s">
         <v>248</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -3824,7 +3852,7 @@
       <c r="B9" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="C9" s="84"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="7" t="s">
         <v>269</v>
       </c>
@@ -3878,36 +3906,36 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="69" t="s">
         <v>260</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="77" t="s">
         <v>259</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="83" t="s">
         <v>227</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="70" t="s">
         <v>258</v>
       </c>
-      <c r="E11" s="76">
+      <c r="E11" s="81">
         <v>3</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="71" t="s">
+      <c r="G11" s="72" t="s">
         <v>257</v>
       </c>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="81"/>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="77"/>
+      <c r="A12" s="85"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="82"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
         <v>256</v>
@@ -3924,13 +3952,13 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
         <v>252</v>
@@ -3982,7 +4010,7 @@
       <c r="B15" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="C15" s="84"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="11" t="s">
         <v>242</v>
       </c>
@@ -4005,34 +4033,34 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="69" t="s">
         <v>238</v>
       </c>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="77" t="s">
         <v>237</v>
       </c>
-      <c r="C16" s="84"/>
-      <c r="D16" s="69" t="s">
+      <c r="C16" s="75"/>
+      <c r="D16" s="70" t="s">
         <v>236</v>
       </c>
-      <c r="E16" s="86">
+      <c r="E16" s="78">
         <v>1</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="71" t="s">
+      <c r="G16" s="72" t="s">
         <v>235</v>
       </c>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="71"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="72"/>
+      <c r="K16" s="72"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="68"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="86"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="78"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
         <v>234</v>
@@ -4048,7 +4076,7 @@
       <c r="B18" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="C18" s="84"/>
+      <c r="C18" s="75"/>
       <c r="D18" s="7" t="s">
         <v>231</v>
       </c>
@@ -4070,7 +4098,7 @@
       <c r="B19" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="75" t="s">
         <v>227</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -4094,7 +4122,7 @@
       <c r="B20" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="C20" s="84"/>
+      <c r="C20" s="75"/>
       <c r="D20" s="7" t="s">
         <v>222</v>
       </c>
@@ -4116,7 +4144,7 @@
       <c r="B21" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="C21" s="84"/>
+      <c r="C21" s="75"/>
       <c r="D21" s="7" t="s">
         <v>218</v>
       </c>
@@ -4138,7 +4166,7 @@
       <c r="B22" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="C22" s="84"/>
+      <c r="C22" s="75"/>
       <c r="D22" s="7" t="s">
         <v>214</v>
       </c>
@@ -4160,7 +4188,7 @@
       <c r="B23" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="C23" s="85"/>
+      <c r="C23" s="76"/>
       <c r="D23" s="7" t="s">
         <v>210</v>
       </c>
@@ -4228,7 +4256,7 @@
       <c r="B26" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="C26" s="88"/>
+      <c r="C26" s="74"/>
       <c r="D26" s="19" t="s">
         <v>199</v>
       </c>
@@ -4502,14 +4530,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C14:C18"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="A13:E13"/>
@@ -4522,6 +4542,14 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C14:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4533,7 +4561,7 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4591,7 +4619,7 @@
         <v>323</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="88" t="s">
         <v>320</v>
       </c>
       <c r="D2" s="7"/>
@@ -4615,7 +4643,7 @@
         <v>321</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="84"/>
+      <c r="C3" s="75"/>
       <c r="D3" s="7"/>
       <c r="E3" s="49" t="s">
         <v>319</v>
@@ -4636,7 +4664,7 @@
         <v>317</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="75" t="s">
         <v>316</v>
       </c>
       <c r="D4" s="7"/>
@@ -4661,7 +4689,7 @@
         <v>314</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="84"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="7"/>
       <c r="E5" s="49" t="s">
         <v>303</v>
@@ -4688,7 +4716,7 @@
       <c r="A7" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="75" t="s">
         <v>311</v>
       </c>
       <c r="D7" s="7"/>
@@ -4703,7 +4731,7 @@
       <c r="A8" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="C8" s="84"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="7"/>
       <c r="E8" s="48" t="s">
         <v>303</v>
@@ -5085,24 +5113,188 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BDD3E4-CD4B-4172-8C8B-0D7A30DAAB4E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>295</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="K1" s="43" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>295</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="K4" s="43" t="s">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636A51BB-5671-4BF5-96B7-8B558455B099}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614F32F9-8D4F-4B7C-ACE2-D0F7B904B029}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>295</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="K1" s="43" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>295</v>
+      </c>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="91"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started working on staff components, and continued adding descriptions to materials.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CK.DESKTOP-BR5NVLN\Documents\Git Repositories\Creative\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A8DE61-2484-49CC-9D90-1DC4C072B860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0222B01E-7FBF-41C6-BE53-D40616A2D86F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="4" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="383">
   <si>
     <t>Weapon</t>
   </si>
@@ -54,16 +54,10 @@
     <t>WORN ITEMS</t>
   </si>
   <si>
-    <t>JEWELLERY</t>
-  </si>
-  <si>
     <t>Light MELEE Weapons</t>
   </si>
   <si>
     <t>Light ARMOUR</t>
-  </si>
-  <si>
-    <t>Ring</t>
   </si>
   <si>
     <t>Athame</t>
@@ -88,9 +82,6 @@
     <t>10 lbs.</t>
   </si>
   <si>
-    <t>Amulet</t>
-  </si>
-  <si>
     <t>Chain Knife</t>
   </si>
   <si>
@@ -116,9 +107,6 @@
     <t>5 gp</t>
   </si>
   <si>
-    <t>Talisman</t>
-  </si>
-  <si>
     <t>Chain Sickle</t>
   </si>
   <si>
@@ -139,9 +127,6 @@
     <t>45 gp</t>
   </si>
   <si>
-    <t>Choker</t>
-  </si>
-  <si>
     <t>Club</t>
   </si>
   <si>
@@ -156,9 +141,6 @@
   </si>
   <si>
     <t>MedIum ARMOUR</t>
-  </si>
-  <si>
-    <t>Necklace</t>
   </si>
   <si>
     <t>Breastplate</t>
@@ -173,9 +155,6 @@
   </si>
   <si>
     <t>400 gp</t>
-  </si>
-  <si>
-    <t>Wristband</t>
   </si>
   <si>
     <t>Dagger</t>
@@ -220,9 +199,6 @@
   </si>
   <si>
     <t>50 gp</t>
-  </si>
-  <si>
-    <t>Wristwatch</t>
   </si>
   <si>
     <t>Handaxe</t>
@@ -262,9 +238,6 @@
     <t>750 gp</t>
   </si>
   <si>
-    <t>Pocket Watch</t>
-  </si>
-  <si>
     <t>Handstaff</t>
   </si>
   <si>
@@ -1829,13 +1802,172 @@
     <t>GRIPS</t>
   </si>
   <si>
-    <t>Flasks</t>
-  </si>
-  <si>
-    <t>Corks</t>
-  </si>
-  <si>
     <t>WRAPS</t>
+  </si>
+  <si>
+    <t>Tube Flask</t>
+  </si>
+  <si>
+    <t>Wooden Cork</t>
+  </si>
+  <si>
+    <t>Gemstone Cork</t>
+  </si>
+  <si>
+    <t>brittle</t>
+  </si>
+  <si>
+    <t>Metal Cap</t>
+  </si>
+  <si>
+    <t>VIALS</t>
+  </si>
+  <si>
+    <t>Tube Vial</t>
+  </si>
+  <si>
+    <t>FLASKS</t>
+  </si>
+  <si>
+    <t>Orb Flask</t>
+  </si>
+  <si>
+    <t>Conical Flask</t>
+  </si>
+  <si>
+    <t>Teardrop Flask</t>
+  </si>
+  <si>
+    <t>Hip Flask</t>
+  </si>
+  <si>
+    <t>STOPPER</t>
+  </si>
+  <si>
+    <t>tube vial
+stopper</t>
+  </si>
+  <si>
+    <t>orb vial
+stopper</t>
+  </si>
+  <si>
+    <t>conical vial
+stopper</t>
+  </si>
+  <si>
+    <t>teardrop flask
+stopper</t>
+  </si>
+  <si>
+    <t>curved vial
+stopper</t>
+  </si>
+  <si>
+    <t>0.05 lbs.</t>
+  </si>
+  <si>
+    <t>0.1 lbs.</t>
+  </si>
+  <si>
+    <t>0.2 lbs.</t>
+  </si>
+  <si>
+    <t>40 gp</t>
+  </si>
+  <si>
+    <t>STAVES</t>
+  </si>
+  <si>
+    <t>Crystal Staff</t>
+  </si>
+  <si>
+    <t>Orb Staff</t>
+  </si>
+  <si>
+    <t>Cane Staff</t>
+  </si>
+  <si>
+    <t>Wand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/4" staff core
+rod
+</t>
+  </si>
+  <si>
+    <t>2" gemstone core
+quarterstaff
+conduit
+grip</t>
+  </si>
+  <si>
+    <t>2" glass core
+quarterstaff
+conduit
+grip</t>
+  </si>
+  <si>
+    <t>1/2" staff core
+hand staff
+conduit
+grip</t>
+  </si>
+  <si>
+    <t>Arcane Focus</t>
+  </si>
+  <si>
+    <t>staff core
+conduit</t>
+  </si>
+  <si>
+    <t>Glass Core</t>
+  </si>
+  <si>
+    <t>Gemstone Core</t>
+  </si>
+  <si>
+    <t>1 cut gemstone</t>
+  </si>
+  <si>
+    <t>1 symmetric glass piece</t>
+  </si>
+  <si>
+    <t>Metal Wire</t>
+  </si>
+  <si>
+    <t>1 length of metal silk</t>
+  </si>
+  <si>
+    <t>Sheathed Wire</t>
+  </si>
+  <si>
+    <t>1 length of metal wire</t>
+  </si>
+  <si>
+    <t>Threaded Wire</t>
+  </si>
+  <si>
+    <t>1 length of metal wire
+1 lbs. of gemstone grains</t>
+  </si>
+  <si>
+    <t>Orb Vial</t>
+  </si>
+  <si>
+    <t>Conical Vial</t>
+  </si>
+  <si>
+    <t>Teardrop Vial</t>
+  </si>
+  <si>
+    <t>Silk Wrapping</t>
+  </si>
+  <si>
+    <t>Leather Sheathe</t>
+  </si>
+  <si>
+    <t>Metal Plating</t>
   </si>
 </sst>
 </file>
@@ -2010,7 +2142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2054,7 +2186,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2200,77 +2331,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2278,6 +2343,90 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2593,10 +2742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:S63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2609,13 +2758,16 @@
     <col min="7" max="7" width="18.85546875" style="7" customWidth="1"/>
     <col min="8" max="9" width="10" style="7" customWidth="1"/>
     <col min="10" max="10" width="5.140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="10" style="4" customWidth="1"/>
-    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="14" width="10" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" customWidth="1"/>
+    <col min="18" max="19" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2642,7 +2794,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>5</v>
+        <v>341</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>1</v>
@@ -2653,933 +2805,1072 @@
       <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="P1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="F2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="F2" s="68" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="K2" s="94" t="s">
+        <v>334</v>
+      </c>
+      <c r="L2" s="95" t="s">
+        <v>347</v>
+      </c>
+      <c r="M2" s="93" t="s">
+        <v>352</v>
+      </c>
+      <c r="N2" s="93" t="s">
+        <v>140</v>
+      </c>
+      <c r="P2" s="94" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q2" s="95" t="s">
+        <v>362</v>
+      </c>
+      <c r="R2" s="93" t="s">
+        <v>352</v>
+      </c>
+      <c r="S2" s="93" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="K2" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="I3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="72"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+    </row>
+    <row r="4" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="5" t="s">
+      <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="F4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="G4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="K4" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="L4" s="64" t="s">
+        <v>348</v>
+      </c>
+      <c r="M4" s="65" t="s">
+        <v>354</v>
+      </c>
+      <c r="N4" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q4" s="64" t="s">
+        <v>363</v>
+      </c>
+      <c r="R4" s="65" t="s">
+        <v>354</v>
+      </c>
+      <c r="S4" s="65" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="C5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="G5" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="H5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="K5" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="L5" s="64" t="s">
+        <v>349</v>
+      </c>
+      <c r="M5" s="65" t="s">
+        <v>353</v>
+      </c>
+      <c r="N5" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q5" s="64" t="s">
+        <v>364</v>
+      </c>
+      <c r="R5" s="65" t="s">
+        <v>353</v>
+      </c>
+      <c r="S5" s="65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="B6" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="C6" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="D6" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="F6" s="75" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="69" t="s">
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="K6" s="72" t="s">
+        <v>344</v>
+      </c>
+      <c r="L6" s="73" t="s">
+        <v>350</v>
+      </c>
+      <c r="M6" s="74" t="s">
+        <v>353</v>
+      </c>
+      <c r="N6" s="74" t="s">
+        <v>85</v>
+      </c>
+      <c r="P6" s="72" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q6" s="73" t="s">
+        <v>361</v>
+      </c>
+      <c r="R6" s="74" t="s">
+        <v>353</v>
+      </c>
+      <c r="S6" s="74" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="72"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="F7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="G7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="H7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="I7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="72" t="s">
+      <c r="K7" s="72"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+    </row>
+    <row r="8" spans="1:19" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="K6" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="69"/>
-      <c r="B7" s="70"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="F7" s="9" t="s">
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="F8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="G8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="H8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K8" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q8" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+    </row>
+    <row r="9" spans="1:19" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="H9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="I9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="7" t="s">
+    </row>
+    <row r="10" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="195" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="C10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="H10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="I10" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="D11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
-    </row>
-    <row r="10" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="G11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="H11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="I11" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="D12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="H12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="10" t="s">
+    </row>
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="B13" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="C13" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="210" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="F13" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+    </row>
+    <row r="14" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="72"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="F14" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="10" t="s">
+      <c r="H14" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="I14" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="285" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="7" t="s">
+      <c r="B15" s="11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69" t="s">
+      <c r="C15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="G15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="71" t="s">
+      <c r="H15" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="72" t="s">
+      <c r="I15" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-    </row>
-    <row r="14" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
-      <c r="B14" s="70"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="F14" s="9" t="s">
+    </row>
+    <row r="16" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="C16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="285" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="F16" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="G16" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="10" t="s">
+      <c r="H16" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="I16" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="7" t="s">
+    </row>
+    <row r="17" spans="1:9" ht="165" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="C17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="F17" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="G17" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="H17" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="I17" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="7" t="s">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="165" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
     </row>
     <row r="19" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="66" t="s">
-        <v>325</v>
-      </c>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="66"/>
+        <v>10</v>
+      </c>
+      <c r="F19" s="76" t="s">
+        <v>316</v>
+      </c>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="66"/>
+        <v>85</v>
+      </c>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="66"/>
+        <v>10</v>
+      </c>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>143</v>
+      <c r="A34" s="16" t="s">
+        <v>134</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="67" t="s">
-        <v>145</v>
-      </c>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
+      <c r="A35" s="69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C39" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="69"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="67" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44" s="67"/>
-      <c r="C44" s="67"/>
-      <c r="D44" s="67"/>
-    </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>174</v>
+      <c r="A47" s="16" t="s">
+        <v>165</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="67" t="s">
-        <v>177</v>
-      </c>
-      <c r="B48" s="67"/>
-      <c r="C48" s="67"/>
-      <c r="D48" s="67"/>
+      <c r="A48" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="61"/>
-      <c r="B49" s="60"/>
-      <c r="C49" s="60"/>
-      <c r="D49" s="60"/>
+      <c r="A49" s="60"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
-      <c r="B50" s="54"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="54"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
+      <c r="A51" s="16"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="55"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="67" t="s">
-        <v>178</v>
-      </c>
-      <c r="B52" s="67"/>
-      <c r="C52" s="67"/>
-      <c r="D52" s="67"/>
+      <c r="A52" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="B52" s="69"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="61"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="60"/>
+      <c r="A53" s="60"/>
+      <c r="B53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
-      <c r="B54" s="54"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="56"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="54"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
+      <c r="A55" s="16"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="55"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="67" t="s">
-        <v>337</v>
-      </c>
-      <c r="B56" s="67"/>
-      <c r="C56" s="67"/>
-      <c r="D56" s="67"/>
+      <c r="A56" s="69" t="s">
+        <v>328</v>
+      </c>
+      <c r="B56" s="69"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="69"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="61"/>
-      <c r="B57" s="60"/>
-      <c r="C57" s="60"/>
-      <c r="D57" s="60"/>
+      <c r="A57" s="60"/>
+      <c r="B57" s="59"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
-      <c r="B58" s="54"/>
-      <c r="C58" s="56"/>
-      <c r="D58" s="56"/>
+      <c r="B58" s="53"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="63"/>
-      <c r="C59" s="64"/>
-      <c r="D59" s="64"/>
+      <c r="A59" s="16"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="63"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="65" t="s">
-        <v>179</v>
-      </c>
-      <c r="B60" s="65"/>
-      <c r="C60" s="65"/>
-      <c r="D60" s="65"/>
+      <c r="A60" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60" s="70"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="70"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="61"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="60"/>
-      <c r="D61" s="60"/>
+      <c r="A61" s="60"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
-      <c r="B62" s="54"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="56"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="62"/>
-      <c r="D63" s="62"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="61"/>
+      <c r="D63" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="36">
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="F19:I21"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A56:D56"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="F2:I2"/>
@@ -3593,13 +3884,6 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="F13:I13"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="F19:I21"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A56:D56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3610,7 +3894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E7B11-1527-417B-9532-F0F2C5A89902}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
@@ -3620,11 +3904,11 @@
     <col min="2" max="2" width="20" style="4" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="4" style="24" customWidth="1"/>
+    <col min="5" max="5" width="4" style="23" customWidth="1"/>
     <col min="6" max="6" width="10" style="8" customWidth="1"/>
     <col min="7" max="7" width="28" style="4" customWidth="1"/>
     <col min="8" max="8" width="20" style="7" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="23" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="22" customWidth="1"/>
     <col min="10" max="10" width="22.85546875" style="7" customWidth="1"/>
     <col min="11" max="11" width="4" style="8" customWidth="1"/>
     <col min="12" max="12" width="10" style="7" customWidth="1"/>
@@ -3632,81 +3916,81 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>286</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>295</v>
-      </c>
-      <c r="L1" s="42"/>
+        <v>287</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="L1" s="41"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
-        <v>294</v>
-      </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="68" t="s">
-        <v>293</v>
-      </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="41"/>
+      <c r="A2" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="71" t="s">
+        <v>284</v>
+      </c>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="40"/>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B3" s="86" t="s">
-        <v>329</v>
-      </c>
-      <c r="C3" s="73" t="s">
-        <v>227</v>
+        <v>320</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>218</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="E3" s="24">
+        <v>282</v>
+      </c>
+      <c r="E3" s="23">
         <v>3</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="9" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="K3" s="4">
         <v>2</v>
@@ -3714,25 +3998,25 @@
     </row>
     <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="79"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="E4" s="39">
+        <v>277</v>
+      </c>
+      <c r="E4" s="38">
         <v>2</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="10" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="K4" s="7">
         <v>2</v>
@@ -3740,25 +4024,25 @@
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B5" s="87"/>
-      <c r="C5" s="79"/>
+      <c r="C5" s="78"/>
       <c r="D5" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="E5" s="24">
+        <v>321</v>
+      </c>
+      <c r="E5" s="23">
         <v>3</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="10" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="K5" s="4">
         <v>3</v>
@@ -3766,25 +4050,25 @@
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="B6" s="87"/>
-      <c r="C6" s="79"/>
+      <c r="C6" s="78"/>
       <c r="D6" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="E6" s="39">
+        <v>269</v>
+      </c>
+      <c r="E6" s="38">
         <v>1</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="K6" s="4">
         <v>2</v>
@@ -3792,25 +4076,25 @@
     </row>
     <row r="7" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B7" s="87"/>
-      <c r="C7" s="79"/>
+      <c r="C7" s="78"/>
       <c r="D7" s="7" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="E7" s="7">
         <v>2</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="J7" s="38" t="s">
-        <v>261</v>
+        <v>263</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>252</v>
       </c>
       <c r="K7" s="4">
         <v>2</v>
@@ -3818,28 +4102,28 @@
     </row>
     <row r="8" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B8" s="87"/>
-      <c r="C8" s="75" t="s">
-        <v>248</v>
+      <c r="C8" s="88" t="s">
+        <v>239</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="E8" s="7">
         <v>5</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="10" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="I8" s="40"/>
+        <v>259</v>
+      </c>
+      <c r="I8" s="39"/>
       <c r="J8" s="7" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="K8" s="7">
         <v>2</v>
@@ -3847,28 +4131,28 @@
     </row>
     <row r="9" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>270</v>
-      </c>
-      <c r="C9" s="75"/>
+        <v>262</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9" s="88"/>
       <c r="D9" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="E9" s="39">
+        <v>260</v>
+      </c>
+      <c r="E9" s="38">
         <v>2</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="5" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="I9" s="32"/>
-      <c r="J9" s="38" t="s">
-        <v>336</v>
+        <v>326</v>
+      </c>
+      <c r="I9" s="31"/>
+      <c r="J9" s="37" t="s">
+        <v>327</v>
       </c>
       <c r="K9" s="4">
         <v>3</v>
@@ -3876,99 +4160,99 @@
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>265</v>
-      </c>
-      <c r="C10" s="27">
+        <v>257</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="26">
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E10" s="39">
+        <v>255</v>
+      </c>
+      <c r="E10" s="38">
         <v>2</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="5" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="38" t="s">
-        <v>261</v>
+        <v>253</v>
+      </c>
+      <c r="I10" s="31"/>
+      <c r="J10" s="37" t="s">
+        <v>252</v>
       </c>
       <c r="K10" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="69" t="s">
-        <v>260</v>
-      </c>
-      <c r="B11" s="77" t="s">
-        <v>259</v>
-      </c>
-      <c r="C11" s="83" t="s">
-        <v>227</v>
-      </c>
-      <c r="D11" s="70" t="s">
-        <v>258</v>
-      </c>
-      <c r="E11" s="81">
+      <c r="A11" s="72" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="84" t="s">
+        <v>250</v>
+      </c>
+      <c r="C11" s="82" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" s="73" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" s="80">
         <v>3</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="72" t="s">
-        <v>257</v>
-      </c>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="72"/>
+      <c r="G11" s="75" t="s">
+        <v>248</v>
+      </c>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="85"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="82"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="81"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="H12" s="12"/>
-      <c r="I12" s="36" t="s">
-        <v>255</v>
+      <c r="I12" s="35" t="s">
+        <v>246</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="K12" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="67" t="s">
-        <v>253</v>
-      </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
+      <c r="A13" s="69" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="H13" s="12"/>
-      <c r="I13" s="32" t="s">
-        <v>251</v>
+      <c r="I13" s="31" t="s">
+        <v>242</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="K13" s="7">
         <v>1</v>
@@ -3976,372 +4260,372 @@
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>249</v>
-      </c>
-      <c r="C14" s="73" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="C14" s="77" t="s">
+        <v>239</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="E14" s="24">
+        <v>238</v>
+      </c>
+      <c r="E14" s="23">
         <v>1</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="5" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="H14" s="12"/>
-      <c r="I14" s="32"/>
+      <c r="I14" s="31"/>
       <c r="J14" s="7" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="K14" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="C15" s="75"/>
+      <c r="A15" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="88"/>
       <c r="D15" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="E15" s="24">
+        <v>233</v>
+      </c>
+      <c r="E15" s="23">
         <v>1</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="17" t="s">
-        <v>241</v>
-      </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="36" t="s">
-        <v>240</v>
+      <c r="G15" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="H15" s="36"/>
+      <c r="I15" s="35" t="s">
+        <v>231</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="K15" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
-        <v>238</v>
-      </c>
-      <c r="B16" s="77" t="s">
-        <v>237</v>
-      </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="70" t="s">
-        <v>236</v>
-      </c>
-      <c r="E16" s="78">
+      <c r="A16" s="72" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" s="84" t="s">
+        <v>228</v>
+      </c>
+      <c r="C16" s="88"/>
+      <c r="D16" s="73" t="s">
+        <v>227</v>
+      </c>
+      <c r="E16" s="91">
         <v>1</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="72" t="s">
-        <v>235</v>
-      </c>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
+      <c r="G16" s="75" t="s">
+        <v>226</v>
+      </c>
+      <c r="H16" s="75"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="75"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="78"/>
+      <c r="A17" s="72"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="91"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="H17" s="12"/>
-      <c r="I17" s="32"/>
+      <c r="I17" s="31"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="C18" s="75"/>
+        <v>224</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" s="88"/>
       <c r="D18" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="E18" s="24">
+        <v>222</v>
+      </c>
+      <c r="E18" s="23">
         <v>1</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="5" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="32"/>
+      <c r="I18" s="31"/>
       <c r="K18"/>
     </row>
     <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="C19" s="75" t="s">
-        <v>227</v>
+        <v>220</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" s="88" t="s">
+        <v>218</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="E19" s="24">
+        <v>217</v>
+      </c>
+      <c r="E19" s="23">
         <v>2</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="I19" s="32"/>
+      <c r="I19" s="31"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="C20" s="75"/>
+        <v>215</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" s="88"/>
       <c r="D20" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E20" s="24">
+        <v>213</v>
+      </c>
+      <c r="E20" s="23">
         <v>3</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="32"/>
+      <c r="I20" s="31"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>219</v>
-      </c>
-      <c r="C21" s="75"/>
+        <v>211</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="C21" s="88"/>
       <c r="D21" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E21" s="24">
+        <v>209</v>
+      </c>
+      <c r="E21" s="23">
         <v>4</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="5" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="H21" s="12"/>
-      <c r="I21" s="32"/>
+      <c r="I21" s="31"/>
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="C22" s="75"/>
+        <v>207</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" s="88"/>
       <c r="D22" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="E22" s="24">
+        <v>205</v>
+      </c>
+      <c r="E22" s="23">
         <v>3</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="5" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="I22" s="32"/>
+      <c r="I22" s="31"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="C23" s="76"/>
+      <c r="A23" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="C23" s="90"/>
       <c r="D23" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E23" s="24">
+        <v>201</v>
+      </c>
+      <c r="E23" s="23">
         <v>2</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="5" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="H23" s="12"/>
-      <c r="I23" s="32"/>
+      <c r="I23" s="31"/>
       <c r="J23" s="7" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="A24" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="4"/>
       <c r="G24" s="5" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="H24" s="12"/>
-      <c r="I24" s="32"/>
+      <c r="I24" s="31"/>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B25" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="C25" s="73" t="s">
-        <v>203</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="E25" s="33">
+        <v>196</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" s="32">
         <v>2</v>
       </c>
       <c r="F25" s="4"/>
-      <c r="G25" s="16" t="s">
-        <v>207</v>
+      <c r="G25" s="15" t="s">
+        <v>198</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="32"/>
+      <c r="I25" s="31"/>
       <c r="J25" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="K25" s="31"/>
+        <v>197</v>
+      </c>
+      <c r="K25" s="30"/>
     </row>
     <row r="26" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="C26" s="74"/>
-      <c r="D26" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="E26" s="30">
+        <v>192</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" s="89"/>
+      <c r="D26" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="E26" s="29">
         <v>3</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="16"/>
+      <c r="G26" s="15"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="32"/>
+      <c r="I26" s="31"/>
       <c r="J26" s="12"/>
-      <c r="K26" s="31"/>
+      <c r="K26" s="30"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="55"/>
+      <c r="A27" s="51"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="54"/>
       <c r="F27" s="4"/>
       <c r="G27" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="32"/>
-      <c r="K27" s="29"/>
+      <c r="I27" s="31"/>
+      <c r="K27" s="28"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="55"/>
+      <c r="A28" s="51"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="54"/>
       <c r="F28" s="4"/>
       <c r="G28" s="5" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="32"/>
+      <c r="I28" s="31"/>
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="I29" s="32"/>
+        <v>187</v>
+      </c>
+      <c r="I29" s="31"/>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="I30" s="32"/>
+        <v>186</v>
+      </c>
+      <c r="I30" s="31"/>
       <c r="J30" s="7" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="K30" s="4"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
+      <c r="G31" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
     </row>
     <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="6" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="I32" s="32"/>
+        <v>183</v>
+      </c>
+      <c r="I32" s="31"/>
       <c r="J32" s="7" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="K32" s="7">
         <v>1</v>
@@ -4351,14 +4635,14 @@
       <c r="D33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="5" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="I33" s="32"/>
+        <v>180</v>
+      </c>
+      <c r="I33" s="31"/>
       <c r="J33" s="7" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="K33" s="7">
         <v>-1</v>
@@ -4368,11 +4652,11 @@
       <c r="D34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="I34" s="32"/>
+        <v>178</v>
+      </c>
+      <c r="I34" s="31"/>
       <c r="J34" s="7" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="K34" s="4"/>
     </row>
@@ -4380,14 +4664,14 @@
       <c r="D35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="5" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="I35" s="32"/>
+        <v>175</v>
+      </c>
+      <c r="I35" s="31"/>
       <c r="J35" s="7" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="K35" s="4"/>
     </row>
@@ -4395,43 +4679,43 @@
       <c r="D36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="H36" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="19" t="s">
-        <v>180</v>
+        <v>173</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="I36" s="24"/>
+      <c r="J36" s="18" t="s">
+        <v>171</v>
       </c>
       <c r="K36" s="14"/>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="52"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="51"/>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="52"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="51"/>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="52"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="51"/>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
@@ -4530,6 +4814,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C14:C18"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="A13:E13"/>
@@ -4542,14 +4834,6 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C14:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4570,7 +4854,7 @@
     <col min="2" max="2" width="20" style="4" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="4" style="24" customWidth="1"/>
+    <col min="5" max="5" width="4" style="23" customWidth="1"/>
     <col min="6" max="6" width="10" style="8" customWidth="1"/>
     <col min="7" max="7" width="28" style="4" customWidth="1"/>
     <col min="8" max="8" width="20" style="7" customWidth="1"/>
@@ -4582,131 +4866,131 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>286</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>295</v>
-      </c>
-      <c r="L1" s="42"/>
+        <v>287</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="L1" s="41"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
-        <v>323</v>
+      <c r="A2" s="58" t="s">
+        <v>314</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="88" t="s">
-        <v>320</v>
+      <c r="C2" s="92" t="s">
+        <v>311</v>
       </c>
       <c r="D2" s="7"/>
-      <c r="E2" s="49" t="s">
-        <v>319</v>
-      </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="58" t="s">
-        <v>322</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="K2" s="49" t="s">
-        <v>303</v>
-      </c>
-      <c r="L2" s="41"/>
+      <c r="E2" s="48" t="s">
+        <v>310</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="57" t="s">
+        <v>313</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="L2" s="40"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="75"/>
+      <c r="C3" s="88"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="49" t="s">
-        <v>319</v>
+      <c r="E3" s="48" t="s">
+        <v>310</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="I3" s="27">
+        <v>309</v>
+      </c>
+      <c r="I3" s="26">
         <v>0</v>
       </c>
-      <c r="K3" s="48" t="s">
-        <v>303</v>
+      <c r="K3" s="47" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="75" t="s">
-        <v>316</v>
+      <c r="C4" s="88" t="s">
+        <v>307</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="48" t="s">
-        <v>303</v>
+      <c r="E4" s="47" t="s">
+        <v>294</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="47" t="s">
-        <v>315</v>
-      </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="51" t="s">
-        <v>300</v>
+        <v>317</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="46" t="s">
+        <v>306</v>
+      </c>
+      <c r="J4" s="18"/>
+      <c r="K4" s="50" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="75"/>
+      <c r="C5" s="88"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="49" t="s">
-        <v>303</v>
+      <c r="E5" s="48" t="s">
+        <v>294</v>
       </c>
       <c r="F5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="28">
+      <c r="C6" s="27">
         <v>0</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="39">
+      <c r="E6" s="38">
         <v>0</v>
       </c>
       <c r="F6" s="4"/>
@@ -4714,45 +4998,45 @@
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="C7" s="75" t="s">
-        <v>311</v>
+        <v>303</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>302</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="48" t="s">
-        <v>303</v>
+      <c r="E7" s="47" t="s">
+        <v>294</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="J7" s="38"/>
+      <c r="J7" s="37"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="C8" s="75"/>
+        <v>301</v>
+      </c>
+      <c r="C8" s="88"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="48" t="s">
-        <v>303</v>
+      <c r="E8" s="47" t="s">
+        <v>294</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>308</v>
+        <v>300</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>299</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="48" t="s">
-        <v>300</v>
+      <c r="E9" s="47" t="s">
+        <v>291</v>
       </c>
       <c r="F9" s="4"/>
       <c r="H9" s="11"/>
@@ -4761,14 +5045,14 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>306</v>
+        <v>298</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>297</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="48" t="s">
-        <v>300</v>
+      <c r="E10" s="47" t="s">
+        <v>291</v>
       </c>
       <c r="F10" s="4"/>
       <c r="H10" s="11"/>
@@ -4777,15 +5061,15 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="27" t="s">
-        <v>304</v>
+      <c r="C11" s="26" t="s">
+        <v>295</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="48" t="s">
-        <v>303</v>
+      <c r="E11" s="47" t="s">
+        <v>294</v>
       </c>
       <c r="F11" s="4"/>
       <c r="H11" s="11"/>
@@ -4794,40 +5078,40 @@
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="46" t="s">
-        <v>300</v>
+        <v>293</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="46" t="s">
+        <v>292</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="45" t="s">
+        <v>291</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="27"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="39"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="4"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
@@ -4835,7 +5119,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
-      <c r="C15" s="45"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="7"/>
       <c r="F15" s="4"/>
       <c r="H15" s="11"/>
@@ -4845,7 +5129,7 @@
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="45"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="11"/>
       <c r="F16" s="4"/>
       <c r="H16" s="11"/>
@@ -4854,7 +5138,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
-      <c r="C17" s="45"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="7"/>
       <c r="F17" s="4"/>
       <c r="H17" s="11"/>
@@ -4863,7 +5147,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
-      <c r="C18" s="45"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="7"/>
       <c r="F18" s="4"/>
       <c r="H18" s="11"/>
@@ -4872,7 +5156,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
-      <c r="C19" s="45"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="7"/>
       <c r="F19" s="4"/>
       <c r="H19" s="11"/>
@@ -4881,46 +5165,46 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
-      <c r="C20" s="45"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="7"/>
       <c r="F20" s="4"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
-      <c r="K20" s="29"/>
+      <c r="K20" s="28"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
-      <c r="C21" s="45"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="7"/>
       <c r="F21" s="4"/>
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
-      <c r="C22" s="45"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="7"/>
       <c r="F22" s="4"/>
       <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
       <c r="F23" s="4"/>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
-      <c r="C24" s="45"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
-      <c r="C25" s="45"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="7"/>
       <c r="F25" s="4"/>
       <c r="K25" s="7"/>
@@ -4935,15 +5219,15 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
     </row>
     <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
-      <c r="C28" s="27"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="7"/>
       <c r="F28" s="4"/>
       <c r="H28" s="11"/>
@@ -5113,89 +5397,118 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BDD3E4-CD4B-4172-8C8B-0D7A30DAAB4E}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="11" width="4" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>339</v>
+        <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B2" s="96" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B3" s="96" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>295</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="K4" s="43" t="s">
-        <v>295</v>
+      <c r="H6" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I6" s="42" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>371</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>373</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -5205,94 +5518,140 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614F32F9-8D4F-4B7C-ACE2-D0F7B904B029}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="11" width="4" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>346</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>343</v>
+        <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>377</v>
+      </c>
+      <c r="F3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>378</v>
+      </c>
+      <c r="F4" s="66" t="s">
+        <v>336</v>
+      </c>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66" t="s">
+        <v>337</v>
+      </c>
+      <c r="I4" s="66"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>379</v>
+      </c>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>345</v>
+      </c>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>295</v>
-      </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="91"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
+      <c r="C8" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="68"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>380</v>
+      </c>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>382</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
continued working on tweaking weights and tags, and implemented terran and aquan affinity. codified the rules for weapon and armour weights in the booklet, and codified the rules for weapon components as well.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CK.DESKTOP-BR5NVLN\Documents\Git Repositories\Creative\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58529FD0-63DD-473E-BC39-361E02F334C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1725A9A5-D857-470F-A055-06469C05DA13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="435">
   <si>
     <t>Weapon</t>
   </si>
@@ -642,9 +642,6 @@
   </si>
   <si>
     <t>Pike</t>
-  </si>
-  <si>
-    <t>12 lbs.</t>
   </si>
   <si>
     <t>GIANT Melee Weapons</t>
@@ -2060,11 +2057,6 @@
 1 long shaft (8 lbs)</t>
   </si>
   <si>
-    <t xml:space="preserve">1 double-edged straight blade (3.75 lbs)
-1 two-handed hilt (2.25 lbs)
-</t>
-  </si>
-  <si>
     <t>slashing
 spiked 2
 precision 1
@@ -2077,6 +2069,462 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">windup
+reach
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CANNOT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> be applied to a heavy weapon</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1 double-edged straight blade (4 lbs)
+1 two-handed hilt (2.5 lbs)
+</t>
+  </si>
+  <si>
+    <t>6.5 lbs.
+(10.5 lbs.)</t>
+  </si>
+  <si>
+    <t>12 lbs.
+(16 lbs.)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">windup 2
+reach
+heavy
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CANNOT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> be applied to a light weapon</t>
+    </r>
+  </si>
+  <si>
+    <t>13 lbs.
+(17 lbs.)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">windup 1
+reach
+weighted
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CANNOT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> be applied to a heavy weapon</t>
+    </r>
+  </si>
+  <si>
+    <t>FLUIDS</t>
+  </si>
+  <si>
+    <t>POTIONS</t>
+  </si>
+  <si>
+    <t>Potion of Healing</t>
+  </si>
+  <si>
+    <t>Potion of Health</t>
+  </si>
+  <si>
+    <t>Elixir of Freedom</t>
+  </si>
+  <si>
+    <t>OILS</t>
+  </si>
+  <si>
+    <t>Oil of Sharpening</t>
+  </si>
+  <si>
+    <t>animal fat
+spearleaf</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spring water
+mandrake root</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+daybrush
+daybrush</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spring water
+angel's hair</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+angel's hair
+daybrush</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spring water
+wild sageberry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+wild sageberry</t>
+    </r>
+  </si>
+  <si>
+    <t>POISONS</t>
+  </si>
+  <si>
+    <t>Basic Poison</t>
+  </si>
+  <si>
+    <t>Assassin's Blood</t>
+  </si>
+  <si>
+    <t>ethanol
+wyrmtongue petals</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">methanol
+belladonna
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wyrmtongue petals
+wyrmtongue petals</t>
+    </r>
+  </si>
+  <si>
+    <t>Malice</t>
+  </si>
+  <si>
+    <t>Mercury's Tears</t>
+  </si>
+  <si>
+    <t>methanol
+daybrush</t>
+  </si>
+  <si>
+    <t>mercury
+daybrush</t>
+  </si>
+  <si>
+    <t>4 lbs.
+(6.25 lbs.)</t>
+  </si>
+  <si>
+    <t>7 lbs.
+(9.5 lbs.)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">slashing 1
+thrusting
+heavy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lbs. &gt; 2.25
+reach </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lbs. &gt; 3.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">slashing 2
+heavy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lbs. &gt; 2.25
+reach </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lbs. &gt; 3.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">superior parry
+heavy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lbs. &gt; 2.25
+reach </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lbs. &gt; 3.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">slashing
+thrusting
+heavy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lbs. &gt; 2.25
+reach </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lbs. &gt; 3.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">slashing
 thrusting
 forceful 1 </t>
@@ -2101,6 +2549,28 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> slashing
+heavy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lbs. &gt; 2.25
 reach </t>
     </r>
     <r>
@@ -2123,200 +2593,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> lbs. &gt; 3.5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">slashing
-thrusting
-reach </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> lbs. &gt; 3.5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">superior parry
-reach </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> lbs. &gt; 3.5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">slashing 1
-thrusting
-reach </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> lbs. &gt; 3.5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">slashing 2
-reach </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> lbs. &gt; 3.5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">windup
-reach
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CANNOT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> be applied to a heavy weapon</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">windup 1
-reach
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CANNOT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> be applied to a heavy weapon</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">windup 2
-reach
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CANNOT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> be applied to a heavy weapon</t>
     </r>
   </si>
 </sst>
@@ -2369,7 +2645,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2488,11 +2764,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2712,45 +2997,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2760,15 +3093,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2781,23 +3105,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3113,10 +3422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
-  <dimension ref="A1:S75"/>
+  <dimension ref="A1:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3136,9 +3445,13 @@
     <col min="16" max="16" width="20.5703125" customWidth="1"/>
     <col min="17" max="17" width="18.85546875" customWidth="1"/>
     <col min="18" max="19" width="10" customWidth="1"/>
+    <col min="20" max="20" width="5.140625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" style="7" customWidth="1"/>
+    <col min="22" max="22" width="18.85546875" style="75" customWidth="1"/>
+    <col min="23" max="24" width="10" style="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3165,7 +3478,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>1</v>
@@ -3177,7 +3490,7 @@
         <v>3</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>1</v>
@@ -3188,46 +3501,64 @@
       <c r="S1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="U1" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="F2" s="77" t="s">
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="F2" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="K2" s="83" t="s">
-        <v>311</v>
-      </c>
-      <c r="L2" s="84" t="s">
-        <v>371</v>
-      </c>
-      <c r="M2" s="85" t="s">
-        <v>324</v>
-      </c>
-      <c r="N2" s="85" t="s">
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="K2" s="87" t="s">
+        <v>310</v>
+      </c>
+      <c r="L2" s="88" t="s">
+        <v>370</v>
+      </c>
+      <c r="M2" s="94" t="s">
+        <v>323</v>
+      </c>
+      <c r="N2" s="94" t="s">
         <v>135</v>
       </c>
-      <c r="P2" s="83" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q2" s="84" t="s">
-        <v>383</v>
-      </c>
-      <c r="R2" s="85" t="s">
-        <v>324</v>
-      </c>
-      <c r="S2" s="85" t="s">
+      <c r="P2" s="87" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q2" s="88" t="s">
+        <v>382</v>
+      </c>
+      <c r="R2" s="94" t="s">
+        <v>323</v>
+      </c>
+      <c r="S2" s="94" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="U2" s="91" t="s">
+        <v>409</v>
+      </c>
+      <c r="V2" s="91"/>
+      <c r="W2" s="91"/>
+      <c r="X2" s="91"/>
+    </row>
+    <row r="3" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -3252,21 +3583,27 @@
       <c r="I3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="78"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="80"/>
-    </row>
-    <row r="4" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="K3" s="86"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+      <c r="U3" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="V3" s="75" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>27</v>
@@ -3287,36 +3624,42 @@
         <v>19</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L4" s="55" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M4" s="56" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N4" s="56" t="s">
         <v>39</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q4" s="55" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R4" s="56" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="S4" s="56" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U4" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="V4" s="75" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>27</v>
@@ -3337,79 +3680,93 @@
         <v>24</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L5" s="55" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M5" s="56" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N5" s="56" t="s">
         <v>80</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q5" s="55" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="R5" s="56" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="S5" s="56" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="s">
+      <c r="U5" s="79" t="s">
+        <v>412</v>
+      </c>
+      <c r="V5" s="76" t="s">
+        <v>416</v>
+      </c>
+      <c r="W5" s="76"/>
+      <c r="X5" s="76"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="C6" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="80" t="s">
+      <c r="D6" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="81" t="s">
+      <c r="F6" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="81"/>
-      <c r="K6" s="78" t="s">
-        <v>321</v>
-      </c>
-      <c r="L6" s="79" t="s">
-        <v>374</v>
-      </c>
-      <c r="M6" s="80" t="s">
-        <v>325</v>
-      </c>
-      <c r="N6" s="80" t="s">
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="K6" s="86" t="s">
+        <v>320</v>
+      </c>
+      <c r="L6" s="92" t="s">
+        <v>373</v>
+      </c>
+      <c r="M6" s="84" t="s">
+        <v>324</v>
+      </c>
+      <c r="N6" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="P6" s="78" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q6" s="79" t="s">
-        <v>378</v>
-      </c>
-      <c r="R6" s="80" t="s">
-        <v>325</v>
-      </c>
-      <c r="S6" s="80" t="s">
+      <c r="P6" s="86" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q6" s="92" t="s">
+        <v>377</v>
+      </c>
+      <c r="R6" s="84" t="s">
+        <v>324</v>
+      </c>
+      <c r="S6" s="84" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="78"/>
-      <c r="B7" s="79"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
+      <c r="U6" s="91" t="s">
+        <v>419</v>
+      </c>
+      <c r="V6" s="91"/>
+      <c r="W6" s="91"/>
+      <c r="X6" s="91"/>
+    </row>
+    <row r="7" spans="1:24" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="86"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
       <c r="F7" s="9" t="s">
         <v>30</v>
       </c>
@@ -3422,16 +3779,24 @@
       <c r="I7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="78"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="P7" s="78"/>
-      <c r="Q7" s="80"/>
-      <c r="R7" s="80"/>
-      <c r="S7" s="80"/>
-    </row>
-    <row r="8" spans="1:19" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="86"/>
+      <c r="L7" s="84"/>
+      <c r="M7" s="84"/>
+      <c r="N7" s="84"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="84"/>
+      <c r="R7" s="84"/>
+      <c r="S7" s="84"/>
+      <c r="U7" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="V7" s="80" t="s">
+        <v>422</v>
+      </c>
+      <c r="W7" s="49"/>
+      <c r="X7" s="49"/>
+    </row>
+    <row r="8" spans="1:24" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -3457,29 +3822,37 @@
         <v>39</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="P8" s="13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="R8" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S8" s="14"/>
-    </row>
-    <row r="9" spans="1:19" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U8" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="V8" s="81" t="s">
+        <v>423</v>
+      </c>
+      <c r="W8" s="78"/>
+      <c r="X8" s="78"/>
+    </row>
+    <row r="9" spans="1:24" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
@@ -3504,8 +3877,16 @@
       <c r="I9" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="U9" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="V9" s="81" t="s">
+        <v>426</v>
+      </c>
+      <c r="W9" s="78"/>
+      <c r="X9" s="78"/>
+    </row>
+    <row r="10" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -3522,7 +3903,7 @@
         <v>48</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>49</v>
@@ -3530,8 +3911,14 @@
       <c r="I10" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U10" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="V10" s="82" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>50</v>
       </c>
@@ -3556,8 +3943,9 @@
       <c r="I11" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="10"/>
+    </row>
+    <row r="12" spans="1:24" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>56</v>
       </c>
@@ -3582,32 +3970,39 @@
       <c r="I12" s="7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="78" t="s">
+      <c r="U12" s="10"/>
+    </row>
+    <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="80" t="s">
+      <c r="C13" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="80" t="s">
+      <c r="D13" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="81" t="s">
+      <c r="F13" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-    </row>
-    <row r="14" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="78"/>
-      <c r="B14" s="79"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="93"/>
+      <c r="U13" s="93" t="s">
+        <v>413</v>
+      </c>
+      <c r="V13" s="93"/>
+      <c r="W13" s="93"/>
+      <c r="X13" s="93"/>
+    </row>
+    <row r="14" spans="1:24" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="86"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="84"/>
       <c r="F14" s="9" t="s">
         <v>66</v>
       </c>
@@ -3620,8 +4015,16 @@
       <c r="I14" s="7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" ht="285" x14ac:dyDescent="0.25">
+      <c r="U14" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="V14" s="80" t="s">
+        <v>415</v>
+      </c>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49"/>
+    </row>
+    <row r="15" spans="1:24" ht="285" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>69</v>
       </c>
@@ -3638,7 +4041,7 @@
         <v>71</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>72</v>
@@ -3647,7 +4050,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>74</v>
       </c>
@@ -3700,12 +4103,12 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="85"/>
     </row>
     <row r="19" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -3720,12 +4123,12 @@
       <c r="D19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="82" t="s">
-        <v>297</v>
-      </c>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
+      <c r="F19" s="89" t="s">
+        <v>296</v>
+      </c>
+      <c r="G19" s="89"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="89"/>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -3740,10 +4143,10 @@
       <c r="D20" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -3758,10 +4161,10 @@
       <c r="D21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="82"/>
-      <c r="I21" s="82"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="89"/>
+      <c r="I21" s="89"/>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -3946,202 +4349,196 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="75" t="s">
+      <c r="A35" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="75"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="75"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="85"/>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>158</v>
+      <c r="A36" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="65" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C37" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="D37" s="65" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>138</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>138</v>
+        <v>400</v>
+      </c>
+      <c r="C39" s="83" t="s">
+        <v>429</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40" s="83" t="s">
+        <v>428</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="85" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="85"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="85"/>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="75" t="s">
+        <v>404</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="75" t="s">
+        <v>406</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="75" t="s">
-        <v>152</v>
-      </c>
-      <c r="B45" s="75"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-    </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>49</v>
+      <c r="C47" s="75" t="s">
+        <v>403</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>159</v>
-      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="85" t="s">
+        <v>349</v>
+      </c>
+      <c r="B48" s="85"/>
+      <c r="C48" s="85"/>
+      <c r="D48" s="85"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="75" t="s">
-        <v>350</v>
-      </c>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
-      <c r="D49" s="75"/>
+      <c r="A49" s="73" t="s">
+        <v>357</v>
+      </c>
+      <c r="B49" s="66"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="66"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="73" t="s">
-        <v>358</v>
-      </c>
-      <c r="B50" s="66"/>
+      <c r="A50" s="68" t="s">
+        <v>352</v>
+      </c>
+      <c r="B50" s="69"/>
       <c r="C50" s="66"/>
       <c r="D50" s="66"/>
     </row>
@@ -4154,7 +4551,7 @@
       <c r="D51" s="66"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="68" t="s">
+      <c r="A52" s="70" t="s">
         <v>354</v>
       </c>
       <c r="B52" s="69"/>
@@ -4162,23 +4559,23 @@
       <c r="D52" s="66"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="70" t="s">
+      <c r="A53" s="85" t="s">
+        <v>350</v>
+      </c>
+      <c r="B53" s="85"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="85"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="73" t="s">
         <v>355</v>
       </c>
-      <c r="B53" s="69"/>
-      <c r="C53" s="66"/>
-      <c r="D53" s="66"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="75" t="s">
-        <v>351</v>
-      </c>
-      <c r="B54" s="75"/>
-      <c r="C54" s="75"/>
-      <c r="D54" s="75"/>
+      <c r="B54" s="66"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="66"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="73" t="s">
+      <c r="A55" s="68" t="s">
         <v>356</v>
       </c>
       <c r="B55" s="66"/>
@@ -4187,7 +4584,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="68" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B56" s="66"/>
       <c r="C56" s="66"/>
@@ -4197,53 +4594,53 @@
       <c r="A57" s="68" t="s">
         <v>359</v>
       </c>
-      <c r="B57" s="66"/>
+      <c r="B57" s="69"/>
       <c r="C57" s="66"/>
       <c r="D57" s="66"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="68" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B58" s="69"/>
       <c r="C58" s="66"/>
       <c r="D58" s="66"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="68" t="s">
-        <v>362</v>
+      <c r="A59" s="70" t="s">
+        <v>360</v>
       </c>
       <c r="B59" s="69"/>
       <c r="C59" s="66"/>
       <c r="D59" s="66"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="70" t="s">
-        <v>361</v>
-      </c>
-      <c r="B60" s="69"/>
-      <c r="C60" s="66"/>
-      <c r="D60" s="66"/>
+      <c r="A60" s="85" t="s">
+        <v>351</v>
+      </c>
+      <c r="B60" s="85"/>
+      <c r="C60" s="85"/>
+      <c r="D60" s="85"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="75" t="s">
-        <v>352</v>
-      </c>
-      <c r="B61" s="75"/>
-      <c r="C61" s="75"/>
-      <c r="D61" s="75"/>
+      <c r="A61" s="73" t="s">
+        <v>362</v>
+      </c>
+      <c r="B61" s="66"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="73" t="s">
+      <c r="A62" s="68" t="s">
         <v>363</v>
       </c>
-      <c r="B62" s="66"/>
+      <c r="B62" s="69"/>
       <c r="C62" s="66"/>
       <c r="D62" s="66"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="68" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B63" s="69"/>
       <c r="C63" s="66"/>
@@ -4251,7 +4648,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="68" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B64" s="69"/>
       <c r="C64" s="66"/>
@@ -4259,31 +4656,31 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="68" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B65" s="69"/>
       <c r="C65" s="66"/>
       <c r="D65" s="66"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="68" t="s">
+      <c r="A66" s="85" t="s">
         <v>367</v>
       </c>
-      <c r="B66" s="69"/>
-      <c r="C66" s="66"/>
-      <c r="D66" s="66"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="75" t="s">
+      <c r="B66" s="85"/>
+      <c r="C66" s="85"/>
+      <c r="D66" s="85"/>
+    </row>
+    <row r="67" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="68" t="s">
+        <v>378</v>
+      </c>
+      <c r="B67" s="69"/>
+      <c r="C67" s="66"/>
+      <c r="D67" s="66"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="68" t="s">
         <v>368</v>
-      </c>
-      <c r="B67" s="75"/>
-      <c r="C67" s="75"/>
-      <c r="D67" s="75"/>
-    </row>
-    <row r="68" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="68" t="s">
-        <v>379</v>
       </c>
       <c r="B68" s="69"/>
       <c r="C68" s="66"/>
@@ -4291,100 +4688,95 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="68" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="B69" s="69"/>
       <c r="C69" s="66"/>
       <c r="D69" s="66"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="240" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="68" t="s">
-        <v>380</v>
-      </c>
-      <c r="B70" s="69"/>
-      <c r="C70" s="66"/>
+        <v>369</v>
+      </c>
+      <c r="B70" s="69" t="s">
+        <v>386</v>
+      </c>
+      <c r="C70" s="66" t="s">
+        <v>149</v>
+      </c>
       <c r="D70" s="66"/>
     </row>
-    <row r="71" spans="1:4" ht="240" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="68" t="s">
-        <v>370</v>
-      </c>
-      <c r="B71" s="69" t="s">
-        <v>387</v>
-      </c>
-      <c r="C71" s="66" t="s">
-        <v>149</v>
-      </c>
-      <c r="D71" s="66"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="B71" s="60"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="60"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="60" t="s">
-        <v>160</v>
-      </c>
-      <c r="B72" s="60"/>
-      <c r="C72" s="60"/>
-      <c r="D72" s="60"/>
+      <c r="A72" s="73" t="s">
+        <v>383</v>
+      </c>
+      <c r="B72" s="66"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="66"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="73" t="s">
-        <v>384</v>
-      </c>
-      <c r="B73" s="66"/>
+      <c r="A73" s="68"/>
+      <c r="B73" s="69"/>
       <c r="C73" s="66"/>
       <c r="D73" s="66"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="68"/>
-      <c r="B74" s="69"/>
-      <c r="C74" s="66"/>
-      <c r="D74" s="66"/>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="71" t="s">
-        <v>385</v>
-      </c>
-      <c r="B75" s="72"/>
-      <c r="C75" s="67"/>
-      <c r="D75" s="67"/>
+    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="71" t="s">
+        <v>384</v>
+      </c>
+      <c r="B74" s="72"/>
+      <c r="C74" s="67"/>
+      <c r="D74" s="67"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="39">
+    <mergeCell ref="U13:X13"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="P6:P7"/>
     <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="K6:K7"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="F19:I21"/>
     <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A44:D44"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:I6"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="F13:I13"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A53:D53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4395,8 +4787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E7B11-1527-417B-9532-F0F2C5A89902}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4417,109 +4809,109 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E1" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K1" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
-        <v>266</v>
-      </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
+      <c r="A2" s="90" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
       <c r="F2" s="21"/>
-      <c r="G2" s="77" t="s">
-        <v>265</v>
-      </c>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
+      <c r="G2" s="91" t="s">
+        <v>264</v>
+      </c>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
       <c r="L2" s="37"/>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="B3" s="96" t="s">
-        <v>299</v>
-      </c>
-      <c r="C3" s="86" t="s">
-        <v>203</v>
+        <v>263</v>
+      </c>
+      <c r="B3" s="109" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="98" t="s">
+        <v>202</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>407</v>
+        <v>431</v>
       </c>
       <c r="E3" s="23">
         <v>3</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="I3" s="101"/>
+        <v>261</v>
+      </c>
+      <c r="I3" s="95"/>
       <c r="J3" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K3" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="B4" s="97"/>
-      <c r="C4" s="87"/>
+        <v>259</v>
+      </c>
+      <c r="B4" s="110"/>
+      <c r="C4" s="99"/>
       <c r="D4" s="7" t="s">
-        <v>406</v>
+        <v>430</v>
       </c>
       <c r="E4" s="35">
         <v>2</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="I4" s="93"/>
+        <v>257</v>
+      </c>
+      <c r="I4" s="96"/>
       <c r="J4" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K4" s="7">
         <v>2</v>
@@ -4527,80 +4919,80 @@
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="87"/>
+        <v>256</v>
+      </c>
+      <c r="B5" s="110"/>
+      <c r="C5" s="99"/>
       <c r="D5" s="7" t="s">
-        <v>405</v>
+        <v>432</v>
       </c>
       <c r="E5" s="23">
         <v>3</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="I5" s="93"/>
+        <v>254</v>
+      </c>
+      <c r="I5" s="96"/>
       <c r="J5" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K5" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="87"/>
+        <v>252</v>
+      </c>
+      <c r="B6" s="110"/>
+      <c r="C6" s="99"/>
       <c r="D6" s="7" t="s">
-        <v>404</v>
+        <v>433</v>
       </c>
       <c r="E6" s="35">
         <v>1</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="I6" s="93"/>
+        <v>250</v>
+      </c>
+      <c r="I6" s="96"/>
       <c r="J6" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K6" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="87"/>
+        <v>248</v>
+      </c>
+      <c r="B7" s="110"/>
+      <c r="C7" s="99"/>
       <c r="D7" s="7" t="s">
-        <v>403</v>
+        <v>434</v>
       </c>
       <c r="E7" s="7">
         <v>2</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="I7" s="93"/>
+        <v>247</v>
+      </c>
+      <c r="I7" s="96"/>
       <c r="J7" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K7" s="4">
         <v>2</v>
@@ -4608,28 +5000,28 @@
     </row>
     <row r="8" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B8" s="97"/>
-      <c r="C8" s="91" t="s">
-        <v>224</v>
+        <v>297</v>
+      </c>
+      <c r="B8" s="110"/>
+      <c r="C8" s="100" t="s">
+        <v>223</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E8" s="7">
         <v>5</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="I8" s="93"/>
+        <v>243</v>
+      </c>
+      <c r="I8" s="96"/>
       <c r="J8" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K8" s="7">
         <v>2</v>
@@ -4637,28 +5029,28 @@
     </row>
     <row r="9" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="C9" s="91"/>
+        <v>245</v>
+      </c>
+      <c r="C9" s="100"/>
       <c r="D9" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E9" s="35">
         <v>2</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="I9" s="96"/>
+      <c r="J9" s="34" t="s">
         <v>304</v>
-      </c>
-      <c r="I9" s="93"/>
-      <c r="J9" s="34" t="s">
-        <v>305</v>
       </c>
       <c r="K9" s="4">
         <v>3</v>
@@ -4666,99 +5058,99 @@
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C10" s="62">
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E10" s="35">
         <v>2</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="I10" s="102"/>
+        <v>237</v>
+      </c>
+      <c r="I10" s="103"/>
       <c r="J10" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K10" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="78" t="s">
-        <v>236</v>
-      </c>
-      <c r="B11" s="93" t="s">
+      <c r="A11" s="86" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="91" t="s">
-        <v>203</v>
-      </c>
-      <c r="D11" s="79" t="s">
+      <c r="B11" s="96" t="s">
         <v>234</v>
       </c>
-      <c r="E11" s="89">
+      <c r="C11" s="100" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="92" t="s">
+        <v>233</v>
+      </c>
+      <c r="E11" s="105">
         <v>3</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="81" t="s">
-        <v>233</v>
-      </c>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
+      <c r="G11" s="93" t="s">
+        <v>232</v>
+      </c>
+      <c r="H11" s="93"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="93"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="95"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="90"/>
+      <c r="A12" s="108"/>
+      <c r="B12" s="107"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="104"/>
+      <c r="E12" s="106"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="74" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K12" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="75" t="s">
-        <v>229</v>
-      </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
+      <c r="A13" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="61" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K13" s="7">
         <v>1</v>
@@ -4766,30 +5158,30 @@
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="C14" s="86" t="s">
         <v>224</v>
       </c>
+      <c r="C14" s="98" t="s">
+        <v>223</v>
+      </c>
       <c r="D14" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E14" s="23">
         <v>1</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="61">
         <v>0</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K14" s="7">
         <v>1</v>
@@ -4797,210 +5189,210 @@
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="C15" s="91"/>
+        <v>218</v>
+      </c>
+      <c r="C15" s="100"/>
       <c r="D15" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E15" s="23">
         <v>1</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H15" s="33"/>
       <c r="I15" s="74" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K15" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="78" t="s">
-        <v>214</v>
-      </c>
-      <c r="B16" s="93" t="s">
+      <c r="A16" s="86" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="91"/>
-      <c r="D16" s="79" t="s">
+      <c r="B16" s="96" t="s">
         <v>212</v>
       </c>
-      <c r="E16" s="98">
+      <c r="C16" s="100"/>
+      <c r="D16" s="92" t="s">
+        <v>211</v>
+      </c>
+      <c r="E16" s="102">
         <v>1</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="81" t="s">
-        <v>211</v>
-      </c>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
+      <c r="G16" s="93" t="s">
+        <v>210</v>
+      </c>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="98"/>
+      <c r="A17" s="86"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="102"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H17" s="12"/>
-      <c r="I17" s="101"/>
+      <c r="I17" s="95"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C18" s="91"/>
+        <v>207</v>
+      </c>
+      <c r="C18" s="100"/>
       <c r="D18" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E18" s="23">
         <v>1</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="93"/>
+      <c r="I18" s="96"/>
       <c r="K18"/>
     </row>
     <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="C19" s="91" t="s">
         <v>203</v>
       </c>
+      <c r="C19" s="100" t="s">
+        <v>202</v>
+      </c>
       <c r="D19" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E19" s="23">
         <v>2</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="I19" s="93"/>
+      <c r="I19" s="96"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="C20" s="91"/>
+        <v>198</v>
+      </c>
+      <c r="C20" s="100"/>
       <c r="D20" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E20" s="23">
         <v>3</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="93"/>
+      <c r="I20" s="96"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="C21" s="91"/>
+        <v>194</v>
+      </c>
+      <c r="C21" s="100"/>
       <c r="D21" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E21" s="23">
         <v>4</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H21" s="12"/>
-      <c r="I21" s="93"/>
+      <c r="I21" s="96"/>
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="C22" s="91"/>
+        <v>190</v>
+      </c>
+      <c r="C22" s="100"/>
       <c r="D22" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E22" s="23">
         <v>3</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="I22" s="93"/>
+      <c r="I22" s="96"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="C23" s="92"/>
+        <v>186</v>
+      </c>
+      <c r="C23" s="101"/>
       <c r="D23" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E23" s="23">
         <v>2</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H23" s="12"/>
-      <c r="I23" s="93"/>
+      <c r="I23" s="96"/>
       <c r="J23" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -5008,49 +5400,49 @@
       <c r="E24" s="19"/>
       <c r="F24" s="4"/>
       <c r="G24" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H24" s="12"/>
-      <c r="I24" s="93"/>
+      <c r="I24" s="96"/>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="C25" s="86" t="s">
         <v>179</v>
       </c>
-      <c r="D25" s="100" t="s">
-        <v>395</v>
+      <c r="C25" s="98" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="77" t="s">
+        <v>394</v>
       </c>
       <c r="E25" s="31">
         <v>2</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="93"/>
+      <c r="I25" s="96"/>
       <c r="J25" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K25" s="30"/>
     </row>
     <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B26" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="C26" s="87"/>
+        <v>176</v>
+      </c>
+      <c r="C26" s="99"/>
       <c r="D26" s="49" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E26" s="50">
         <v>3</v>
@@ -5058,32 +5450,32 @@
       <c r="F26" s="4"/>
       <c r="G26" s="15"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="93"/>
+      <c r="I26" s="96"/>
       <c r="J26" s="12"/>
       <c r="K26" s="30"/>
     </row>
     <row r="27" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="B27" s="24" t="s">
         <v>381</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>382</v>
       </c>
       <c r="C27" s="63">
         <v>0</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E27" s="29">
         <v>5</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="93"/>
+      <c r="I27" s="96"/>
       <c r="K27" s="28"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -5094,30 +5486,33 @@
       <c r="E28" s="50"/>
       <c r="F28" s="4"/>
       <c r="G28" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="93"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="7" t="s">
+        <v>392</v>
+      </c>
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="I29" s="93"/>
+        <v>173</v>
+      </c>
+      <c r="I29" s="96"/>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="I30" s="102"/>
+        <v>172</v>
+      </c>
+      <c r="I30" s="103"/>
       <c r="J30" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K30" s="4"/>
     </row>
@@ -5125,7 +5520,7 @@
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H31" s="25"/>
       <c r="I31" s="25"/>
@@ -5136,14 +5531,14 @@
       <c r="D32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="I32" s="101"/>
+        <v>169</v>
+      </c>
+      <c r="I32" s="95"/>
       <c r="J32" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K32" s="7">
         <v>1</v>
@@ -5153,14 +5548,14 @@
       <c r="D33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="I33" s="93"/>
+        <v>166</v>
+      </c>
+      <c r="I33" s="96"/>
       <c r="J33" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K33" s="7">
         <v>-1</v>
@@ -5170,41 +5565,41 @@
       <c r="D34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I34" s="93"/>
+        <v>164</v>
+      </c>
+      <c r="I34" s="96"/>
       <c r="J34" s="7" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="4:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:11" ht="75" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="I35" s="93"/>
+        <v>162</v>
+      </c>
+      <c r="I35" s="96"/>
       <c r="J35" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="I36" s="103"/>
+        <v>160</v>
+      </c>
+      <c r="I36" s="97"/>
       <c r="J36" s="18" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="K36" s="14"/>
     </row>
@@ -5332,16 +5727,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="I17:I30"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="A13:E13"/>
@@ -5355,6 +5740,16 @@
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="I3:I10"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="I17:I30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5387,128 +5782,128 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E1" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K1" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="99" t="s">
-        <v>292</v>
+      <c r="C2" s="111" t="s">
+        <v>291</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="53" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K2" s="45" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L2" s="37"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="91"/>
+      <c r="C3" s="100"/>
       <c r="D3" s="7"/>
       <c r="E3" s="45" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I3" s="26">
         <v>0</v>
       </c>
       <c r="K3" s="44" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="91" t="s">
-        <v>288</v>
+      <c r="C4" s="100" t="s">
+        <v>287</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="44" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="43" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K4" s="46" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="91"/>
+      <c r="C5" s="100"/>
       <c r="D5" s="7"/>
       <c r="E5" s="45" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="27">
@@ -5523,14 +5918,14 @@
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="C7" s="91" t="s">
         <v>283</v>
+      </c>
+      <c r="C7" s="100" t="s">
+        <v>282</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="44" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F7" s="4"/>
       <c r="J7" s="34"/>
@@ -5538,12 +5933,12 @@
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="C8" s="91"/>
+        <v>281</v>
+      </c>
+      <c r="C8" s="100"/>
       <c r="D8" s="7"/>
       <c r="E8" s="44" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="37"/>
@@ -5554,14 +5949,14 @@
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="44" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F9" s="4"/>
       <c r="H9" s="11"/>
@@ -5570,14 +5965,14 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="44" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F10" s="4"/>
       <c r="H10" s="11"/>
@@ -5586,17 +5981,17 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F11" s="4"/>
       <c r="H11" s="11"/>
@@ -5605,15 +6000,15 @@
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="42" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F12" s="4"/>
       <c r="H12" s="33"/>
@@ -5945,44 +6340,44 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I1" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B2" s="64" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B3" s="64" t="s">
         <v>335</v>
-      </c>
-      <c r="B3" s="64" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -5990,52 +6385,52 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I6" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
+        <v>337</v>
+      </c>
+      <c r="G7" s="36" t="s">
         <v>338</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
+        <v>339</v>
+      </c>
+      <c r="G8" s="36" t="s">
         <v>340</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
+        <v>341</v>
+      </c>
+      <c r="G9" s="36" t="s">
         <v>342</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -6066,62 +6461,62 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I1" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F4" s="57" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G4" s="57"/>
       <c r="H4" s="57" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I4" s="57"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F5" s="57"/>
       <c r="G5" s="57"/>
@@ -6130,7 +6525,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F6" s="57"/>
       <c r="G6" s="57"/>
@@ -6145,16 +6540,16 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F8" s="58"/>
       <c r="G8" s="58"/>
@@ -6163,7 +6558,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F9" s="57"/>
       <c r="G9" s="57"/>
@@ -6172,12 +6567,12 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked on ranged weapons and elemental affinities.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CK.DESKTOP-BR5NVLN\Documents\Git Repositories\Creative\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3A9796-A550-44D2-A69D-734217F0603D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0492A019-F26D-46B7-AA08-B252930648AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="1" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="506">
   <si>
     <t>Weapon</t>
   </si>
@@ -1349,9 +1349,6 @@
     <t>Sheathed Wire</t>
   </si>
   <si>
-    <t>1 length of metal wire</t>
-  </si>
-  <si>
     <t>Threaded Wire</t>
   </si>
   <si>
@@ -1384,21 +1381,6 @@
   </si>
   <si>
     <t>FIREARMS</t>
-  </si>
-  <si>
-    <t>Pistol</t>
-  </si>
-  <si>
-    <t>Musket</t>
-  </si>
-  <si>
-    <t>Rifle</t>
-  </si>
-  <si>
-    <t>Shotgun</t>
-  </si>
-  <si>
-    <t>Thunder Cannon</t>
   </si>
   <si>
     <t>Arcane Firearms</t>
@@ -3240,34 +3222,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1 barrel
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 hammer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 firearm grip</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -3599,17 +3553,7 @@
     <t>Blunthead Arrow (+0 MOD; pummelling)</t>
   </si>
   <si>
-    <t>Metal Jacket Bullet (+1 MOD; thrusting; piercing)</t>
-  </si>
-  <si>
     <t>Open Tip Bullet (+0 MOD; thrusting; weightless)</t>
-  </si>
-  <si>
-    <t>Hollow Point Bullet (+2 MOD; pummelling; forceful 1)</t>
-  </si>
-  <si>
-    <t>Ballistic Tip (+2 MOD; weightless; pummelling;
-forceful 1)</t>
   </si>
   <si>
     <t>Serrated Arrow (+1 MOD; thrusting; wounding)</t>
@@ -4031,10 +3975,6 @@
     </r>
   </si>
   <si>
-    <t>piercing
-grappling</t>
-  </si>
-  <si>
     <t>1 piece of metal OR glass OR chitin
 1 weave of silk</t>
   </si>
@@ -4055,6 +3995,105 @@
   </si>
   <si>
     <t>1 piece of soft metal</t>
+  </si>
+  <si>
+    <t>piercing 1</t>
+  </si>
+  <si>
+    <t>Metal Jacket Bullet (+1 MOD; thrusting; piercing 1)</t>
+  </si>
+  <si>
+    <t>thrusting
+grappling</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 y-haft (1 lb)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 bowstring (0.5 lbs)</t>
+    </r>
+  </si>
+  <si>
+    <t>Bowstring</t>
+  </si>
+  <si>
+    <t>Gun Hammer</t>
+  </si>
+  <si>
+    <t>projectile</t>
+  </si>
+  <si>
+    <t>1 weave of silk</t>
+  </si>
+  <si>
+    <t>500 gp</t>
+  </si>
+  <si>
+    <t>15 lbs.</t>
+  </si>
+  <si>
+    <t>Thunder Cannon (2d10; giant; two-handed; loading; fires slugs)</t>
+  </si>
+  <si>
+    <t>Ballistic Tip (+1 MOD; weightless; pummelling;
+forceful 1)</t>
+  </si>
+  <si>
+    <t>Hollow Point Bullet (+1 MOD; pummelling; forceful 1)</t>
+  </si>
+  <si>
+    <t>Rifle (2d6; heavy; two-handed; loading; fires bullets)</t>
+  </si>
+  <si>
+    <t>Shotgun (1d10; heavy; two-handed; loading; fires slugs)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 barrel (1.25 lbs)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 hammer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1 firearm grip</t>
+    </r>
+  </si>
+  <si>
+    <t>Musket (1d12; heavy; two-handed; loading; fires bullets)</t>
+  </si>
+  <si>
+    <t>Pistol (1d10; fires bullets)</t>
+  </si>
+  <si>
+    <t>1 length of metal wire
+1 sheathe of soft insulative metal</t>
   </si>
 </sst>
 </file>
@@ -4288,7 +4327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4503,194 +4542,107 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4699,20 +4651,170 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5030,8 +5132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
   <dimension ref="A1:AC70"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:N11"/>
+    <sheetView topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5046,7 +5148,7 @@
     <col min="10" max="10" width="5.140625" style="4" customWidth="1"/>
     <col min="11" max="11" width="20.5703125" customWidth="1"/>
     <col min="12" max="12" width="18.85546875" customWidth="1"/>
-    <col min="13" max="13" width="10" style="80" customWidth="1"/>
+    <col min="13" max="13" width="10" style="79" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
     <col min="15" max="15" width="5.140625" style="4" customWidth="1"/>
     <col min="16" max="16" width="20.5703125" customWidth="1"/>
@@ -5058,8 +5160,8 @@
     <col min="23" max="24" width="10" customWidth="1"/>
     <col min="25" max="25" width="5.140625" style="4" customWidth="1"/>
     <col min="26" max="26" width="20.5703125" style="7" customWidth="1"/>
-    <col min="27" max="27" width="18.85546875" style="76" customWidth="1"/>
-    <col min="28" max="29" width="10" style="76" customWidth="1"/>
+    <col min="27" max="27" width="18.85546875" style="75" customWidth="1"/>
+    <col min="28" max="29" width="10" style="75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5089,7 +5191,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>1</v>
@@ -5125,7 +5227,7 @@
         <v>3</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>1</v>
@@ -5138,61 +5240,61 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="F2" s="105" t="s">
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="F2" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="K2" s="105" t="s">
-        <v>455</v>
-      </c>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="P2" s="102" t="s">
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="K2" s="125" t="s">
+        <v>448</v>
+      </c>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+      <c r="P2" s="116" t="s">
         <v>215</v>
       </c>
-      <c r="Q2" s="103" t="s">
-        <v>264</v>
-      </c>
-      <c r="R2" s="106" t="s">
+      <c r="Q2" s="123" t="s">
+        <v>258</v>
+      </c>
+      <c r="R2" s="120" t="s">
         <v>228</v>
       </c>
-      <c r="S2" s="106" t="s">
+      <c r="S2" s="120" t="s">
         <v>62</v>
       </c>
-      <c r="U2" s="102" t="s">
+      <c r="U2" s="116" t="s">
         <v>233</v>
       </c>
-      <c r="V2" s="126" t="s">
-        <v>276</v>
-      </c>
-      <c r="W2" s="106" t="s">
+      <c r="V2" s="118" t="s">
+        <v>270</v>
+      </c>
+      <c r="W2" s="120" t="s">
         <v>228</v>
       </c>
-      <c r="X2" s="106" t="s">
+      <c r="X2" s="120" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" s="127" t="s">
-        <v>290</v>
-      </c>
-      <c r="AA2" s="127"/>
-      <c r="AB2" s="127"/>
-      <c r="AC2" s="127"/>
+      <c r="Z2" s="115" t="s">
+        <v>284</v>
+      </c>
+      <c r="AA2" s="115"/>
+      <c r="AB2" s="115"/>
+      <c r="AC2" s="115"/>
     </row>
     <row r="3" spans="1:29" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>7</v>
@@ -5201,7 +5303,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>9</v>
@@ -5213,36 +5315,36 @@
         <v>8</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="L3" s="64" t="s">
-        <v>480</v>
-      </c>
-      <c r="M3" s="80">
+        <v>470</v>
+      </c>
+      <c r="M3" s="79">
         <v>0.06</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="P3" s="101"/>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="98"/>
-      <c r="U3" s="101"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="125"/>
-      <c r="X3" s="125"/>
+      <c r="P3" s="117"/>
+      <c r="Q3" s="122"/>
+      <c r="R3" s="122"/>
+      <c r="S3" s="122"/>
+      <c r="U3" s="117"/>
+      <c r="V3" s="119"/>
+      <c r="W3" s="121"/>
+      <c r="X3" s="121"/>
       <c r="Z3" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="AA3" s="76" t="s">
-        <v>299</v>
+        <v>285</v>
+      </c>
+      <c r="AA3" s="75" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>31</v>
@@ -5251,7 +5353,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>12</v>
@@ -5263,52 +5365,52 @@
         <v>14</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="L4" s="64" t="s">
-        <v>469</v>
-      </c>
-      <c r="M4" s="80">
+        <v>459</v>
+      </c>
+      <c r="M4" s="79">
         <v>0.05</v>
       </c>
       <c r="N4" s="50"/>
       <c r="P4" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="Q4" s="76" t="s">
-        <v>265</v>
-      </c>
-      <c r="R4" s="75" t="s">
+      <c r="Q4" s="75" t="s">
+        <v>259</v>
+      </c>
+      <c r="R4" s="74" t="s">
         <v>230</v>
       </c>
-      <c r="S4" s="75" t="s">
+      <c r="S4" s="74" t="s">
         <v>23</v>
       </c>
       <c r="U4" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="V4" s="76" t="s">
-        <v>269</v>
-      </c>
-      <c r="W4" s="75" t="s">
+      <c r="V4" s="75" t="s">
+        <v>263</v>
+      </c>
+      <c r="W4" s="74" t="s">
         <v>230</v>
       </c>
-      <c r="X4" s="75" t="s">
+      <c r="X4" s="74" t="s">
         <v>23</v>
       </c>
       <c r="Z4" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA4" s="75" t="s">
         <v>292</v>
-      </c>
-      <c r="AA4" s="76" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>17</v>
@@ -5317,22 +5419,22 @@
         <v>8</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="L5" s="64" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="M5" s="45">
         <v>0.06</v>
@@ -5341,102 +5443,102 @@
       <c r="P5" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="Q5" s="76" t="s">
-        <v>266</v>
-      </c>
-      <c r="R5" s="75" t="s">
+      <c r="Q5" s="75" t="s">
+        <v>260</v>
+      </c>
+      <c r="R5" s="74" t="s">
         <v>229</v>
       </c>
-      <c r="S5" s="75" t="s">
+      <c r="S5" s="74" t="s">
         <v>43</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="V5" s="76" t="s">
-        <v>270</v>
-      </c>
-      <c r="W5" s="75" t="s">
+      <c r="V5" s="75" t="s">
+        <v>264</v>
+      </c>
+      <c r="W5" s="74" t="s">
         <v>229</v>
       </c>
-      <c r="X5" s="75" t="s">
+      <c r="X5" s="74" t="s">
         <v>43</v>
       </c>
       <c r="Z5" s="65" t="s">
-        <v>293</v>
-      </c>
-      <c r="AA5" s="78" t="s">
-        <v>297</v>
-      </c>
-      <c r="AB5" s="78"/>
-      <c r="AC5" s="78"/>
+        <v>287</v>
+      </c>
+      <c r="AA5" s="77" t="s">
+        <v>291</v>
+      </c>
+      <c r="AB5" s="77"/>
+      <c r="AC5" s="77"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
-        <v>339</v>
-      </c>
-      <c r="B6" s="99" t="s">
-        <v>413</v>
-      </c>
-      <c r="C6" s="98" t="s">
+      <c r="A6" s="128" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" s="124" t="s">
+        <v>407</v>
+      </c>
+      <c r="C6" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="98" t="s">
+      <c r="D6" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="K6" s="95" t="s">
-        <v>457</v>
-      </c>
-      <c r="L6" s="95"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
-      <c r="P6" s="101" t="s">
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="K6" s="114" t="s">
+        <v>450</v>
+      </c>
+      <c r="L6" s="114"/>
+      <c r="M6" s="114"/>
+      <c r="N6" s="114"/>
+      <c r="P6" s="117" t="s">
         <v>225</v>
       </c>
-      <c r="Q6" s="99" t="s">
-        <v>267</v>
-      </c>
-      <c r="R6" s="98" t="s">
+      <c r="Q6" s="124" t="s">
+        <v>261</v>
+      </c>
+      <c r="R6" s="122" t="s">
         <v>229</v>
       </c>
-      <c r="S6" s="98" t="s">
+      <c r="S6" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="U6" s="101" t="s">
+      <c r="U6" s="117" t="s">
         <v>236</v>
       </c>
-      <c r="V6" s="97" t="s">
-        <v>271</v>
-      </c>
-      <c r="W6" s="98" t="s">
+      <c r="V6" s="119" t="s">
+        <v>265</v>
+      </c>
+      <c r="W6" s="122" t="s">
         <v>229</v>
       </c>
-      <c r="X6" s="98" t="s">
+      <c r="X6" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="Z6" s="95" t="s">
-        <v>300</v>
-      </c>
-      <c r="AA6" s="95"/>
-      <c r="AB6" s="95"/>
-      <c r="AC6" s="95"/>
+      <c r="Z6" s="114" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA6" s="114"/>
+      <c r="AB6" s="114"/>
+      <c r="AC6" s="114"/>
     </row>
     <row r="7" spans="1:29" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="96"/>
-      <c r="B7" s="99"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
+      <c r="A7" s="128"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
       <c r="F7" s="9" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>20</v>
@@ -5445,38 +5547,38 @@
         <v>21</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="L7" s="64" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="M7" s="45">
         <v>0.08</v>
       </c>
-      <c r="N7" s="128"/>
-      <c r="P7" s="101"/>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="98"/>
-      <c r="S7" s="98"/>
-      <c r="U7" s="101"/>
-      <c r="V7" s="97"/>
-      <c r="W7" s="98"/>
-      <c r="X7" s="98"/>
+      <c r="N7" s="103"/>
+      <c r="P7" s="117"/>
+      <c r="Q7" s="122"/>
+      <c r="R7" s="122"/>
+      <c r="S7" s="122"/>
+      <c r="U7" s="117"/>
+      <c r="V7" s="119"/>
+      <c r="W7" s="122"/>
+      <c r="X7" s="122"/>
       <c r="Z7" s="10" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="AA7" s="66" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="AB7" s="44"/>
       <c r="AC7" s="44"/>
     </row>
     <row r="8" spans="1:29" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>7</v>
@@ -5485,22 +5587,22 @@
         <v>22</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="L8" s="64" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="M8" s="45">
         <v>0.08</v>
@@ -5510,7 +5612,7 @@
         <v>226</v>
       </c>
       <c r="Q8" s="17" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="R8" s="14" t="s">
         <v>229</v>
@@ -5522,27 +5624,27 @@
         <v>237</v>
       </c>
       <c r="V8" s="17" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="W8" s="14" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="X8" s="14"/>
       <c r="Z8" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="AA8" s="67" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="AB8" s="64"/>
       <c r="AC8" s="64"/>
     </row>
     <row r="9" spans="1:29" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>17</v>
@@ -5551,7 +5653,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>24</v>
@@ -5562,31 +5664,31 @@
       <c r="I9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="129" t="s">
-        <v>474</v>
+      <c r="K9" s="104" t="s">
+        <v>464</v>
       </c>
       <c r="L9" s="64" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="M9" s="45">
         <v>0.08</v>
       </c>
       <c r="N9" s="51"/>
       <c r="Z9" s="10" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="AA9" s="67" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="AB9" s="64"/>
       <c r="AC9" s="64"/>
     </row>
     <row r="10" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>343</v>
-      </c>
-      <c r="B10" s="89" t="s">
-        <v>342</v>
+        <v>337</v>
+      </c>
+      <c r="B10" s="88" t="s">
+        <v>336</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>31</v>
@@ -5595,102 +5697,102 @@
         <v>18</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="129" t="s">
-        <v>486</v>
+      <c r="K10" s="104" t="s">
+        <v>476</v>
       </c>
       <c r="L10" s="64" t="s">
-        <v>485</v>
-      </c>
-      <c r="M10" s="80">
+        <v>475</v>
+      </c>
+      <c r="M10" s="79">
         <v>0.08</v>
       </c>
       <c r="Z10" s="10" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="AA10" s="68" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="96" t="s">
-        <v>344</v>
-      </c>
-      <c r="B11" s="97" t="s">
-        <v>410</v>
-      </c>
-      <c r="C11" s="98" t="s">
+      <c r="A11" s="128" t="s">
+        <v>338</v>
+      </c>
+      <c r="B11" s="119" t="s">
+        <v>404</v>
+      </c>
+      <c r="C11" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="98" t="s">
+      <c r="D11" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="96" t="s">
-        <v>322</v>
-      </c>
-      <c r="G11" s="97" t="s">
+      <c r="F11" s="128" t="s">
+        <v>316</v>
+      </c>
+      <c r="G11" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="99" t="s">
+      <c r="H11" s="124" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="99" t="s">
+      <c r="I11" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="95" t="s">
-        <v>454</v>
-      </c>
-      <c r="L11" s="95"/>
-      <c r="M11" s="95"/>
-      <c r="N11" s="95"/>
-      <c r="Z11" s="95" t="s">
-        <v>294</v>
-      </c>
-      <c r="AA11" s="95"/>
-      <c r="AB11" s="95"/>
-      <c r="AC11" s="95"/>
+      <c r="K11" s="114" t="s">
+        <v>447</v>
+      </c>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="114"/>
+      <c r="Z11" s="114" t="s">
+        <v>288</v>
+      </c>
+      <c r="AA11" s="114"/>
+      <c r="AB11" s="114"/>
+      <c r="AC11" s="114"/>
     </row>
     <row r="12" spans="1:29" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="96"/>
-      <c r="B12" s="97"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="99"/>
-      <c r="I12" s="99"/>
+      <c r="A12" s="128"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122"/>
+      <c r="F12" s="128"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="124"/>
+      <c r="I12" s="124"/>
       <c r="K12" s="9" t="s">
-        <v>459</v>
+        <v>488</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="N12" s="4"/>
       <c r="Z12" s="10" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="AA12" s="66" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="AB12" s="44"/>
       <c r="AC12" s="44"/>
     </row>
     <row r="13" spans="1:29" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="C13" s="69" t="s">
         <v>31</v>
@@ -5699,7 +5801,7 @@
         <v>22</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>32</v>
@@ -5710,55 +5812,55 @@
       <c r="I13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="131" t="s">
-        <v>460</v>
+      <c r="K13" s="106" t="s">
+        <v>452</v>
       </c>
       <c r="Z13" s="10" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="AA13" s="66" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="AB13" s="44"/>
       <c r="AC13" s="44"/>
     </row>
     <row r="14" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="96" t="s">
-        <v>346</v>
-      </c>
-      <c r="B14" s="97" t="s">
-        <v>408</v>
-      </c>
-      <c r="C14" s="98" t="s">
+      <c r="A14" s="128" t="s">
+        <v>340</v>
+      </c>
+      <c r="B14" s="119" t="s">
+        <v>402</v>
+      </c>
+      <c r="C14" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="98" t="s">
+      <c r="D14" s="122" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="95" t="s">
+      <c r="F14" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="95"/>
-      <c r="H14" s="95"/>
-      <c r="I14" s="95"/>
-      <c r="K14" s="132" t="s">
-        <v>461</v>
+      <c r="G14" s="114"/>
+      <c r="H14" s="114"/>
+      <c r="I14" s="114"/>
+      <c r="K14" s="129" t="s">
+        <v>499</v>
       </c>
       <c r="L14" s="130"/>
-      <c r="M14" s="133"/>
+      <c r="M14" s="131"/>
       <c r="N14" s="130"/>
       <c r="Z14" s="44"/>
-      <c r="AA14" s="93"/>
+      <c r="AA14" s="92"/>
       <c r="AB14" s="44"/>
       <c r="AC14" s="44"/>
     </row>
     <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="96"/>
-      <c r="B15" s="97"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
+      <c r="A15" s="128"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="122"/>
       <c r="F15" s="9" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>36</v>
@@ -5769,9 +5871,9 @@
       <c r="I15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="132"/>
+      <c r="K15" s="129"/>
       <c r="L15" s="130"/>
-      <c r="M15" s="133"/>
+      <c r="M15" s="131"/>
       <c r="N15" s="130"/>
       <c r="Z15" s="44"/>
       <c r="AA15" s="64"/>
@@ -5779,11 +5881,11 @@
       <c r="AC15" s="64"/>
     </row>
     <row r="16" spans="1:29" ht="285" x14ac:dyDescent="0.25">
-      <c r="A16" s="86" t="s">
-        <v>347</v>
+      <c r="A16" s="85" t="s">
+        <v>341</v>
       </c>
       <c r="B16" s="71" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="C16" s="69" t="s">
         <v>17</v>
@@ -5792,10 +5894,10 @@
         <v>8</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>38</v>
@@ -5803,16 +5905,16 @@
       <c r="I16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K16" s="131" t="s">
-        <v>462</v>
+      <c r="K16" s="106" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="C17" s="69" t="s">
         <v>28</v>
@@ -5821,7 +5923,7 @@
         <v>40</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>41</v>
@@ -5832,13 +5934,14 @@
       <c r="I17" s="7" t="s">
         <v>43</v>
       </c>
+      <c r="K17" s="106"/>
     </row>
     <row r="18" spans="1:16" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="65" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="C18" s="69" t="s">
         <v>17</v>
@@ -5847,7 +5950,7 @@
         <v>44</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="G18" s="44" t="s">
         <v>45</v>
@@ -5858,27 +5961,28 @@
       <c r="I18" s="44" t="s">
         <v>47</v>
       </c>
+      <c r="K18" s="159"/>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="100" t="s">
+      <c r="A19" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="100"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
-      <c r="F19" s="95" t="s">
-        <v>316</v>
-      </c>
-      <c r="G19" s="95"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="95"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="F19" s="114" t="s">
+        <v>310</v>
+      </c>
+      <c r="G19" s="114"/>
+      <c r="H19" s="114"/>
+      <c r="I19" s="114"/>
     </row>
     <row r="20" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="C20" s="69" t="s">
         <v>49</v>
@@ -5887,24 +5991,24 @@
         <v>8</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="G20" s="90" t="s">
-        <v>423</v>
+        <v>412</v>
+      </c>
+      <c r="G20" s="89" t="s">
+        <v>416</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C21" s="69" t="s">
         <v>49</v>
@@ -5913,10 +6017,10 @@
         <v>43</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="G21" s="91" t="s">
-        <v>433</v>
+        <v>425</v>
+      </c>
+      <c r="G21" s="90" t="s">
+        <v>426</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>61</v>
@@ -5924,15 +6028,15 @@
       <c r="I21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K21" s="94"/>
-      <c r="P21" s="94"/>
+      <c r="K21" s="93"/>
+      <c r="P21" s="93"/>
     </row>
     <row r="22" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C22" s="69" t="s">
         <v>50</v>
@@ -5941,10 +6045,10 @@
         <v>8</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="G22" s="91" t="s">
-        <v>424</v>
+        <v>413</v>
+      </c>
+      <c r="G22" s="90" t="s">
+        <v>417</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>65</v>
@@ -5955,10 +6059,10 @@
     </row>
     <row r="23" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C23" s="69" t="s">
         <v>51</v>
@@ -5967,10 +6071,10 @@
         <v>52</v>
       </c>
       <c r="F23" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="G23" s="91" t="s">
         <v>418</v>
-      </c>
-      <c r="G23" s="92" t="s">
-        <v>425</v>
       </c>
       <c r="H23" s="17" t="s">
         <v>27</v>
@@ -5981,10 +6085,10 @@
     </row>
     <row r="24" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="C24" s="69" t="s">
         <v>53</v>
@@ -5995,10 +6099,10 @@
     </row>
     <row r="25" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C25" s="69" t="s">
         <v>50</v>
@@ -6009,10 +6113,10 @@
     </row>
     <row r="26" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C26" s="69" t="s">
         <v>54</v>
@@ -6023,10 +6127,10 @@
     </row>
     <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="C27" s="69" t="s">
         <v>50</v>
@@ -6037,10 +6141,10 @@
     </row>
     <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C28" s="69" t="s">
         <v>51</v>
@@ -6051,9 +6155,9 @@
     </row>
     <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="B29" s="89" t="s">
+        <v>349</v>
+      </c>
+      <c r="B29" s="88" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="69" t="s">
@@ -6065,10 +6169,10 @@
     </row>
     <row r="30" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="C30" s="69" t="s">
         <v>50</v>
@@ -6079,10 +6183,10 @@
     </row>
     <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C31" s="69" t="s">
         <v>58</v>
@@ -6093,10 +6197,10 @@
     </row>
     <row r="32" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C32" s="69" t="s">
         <v>59</v>
@@ -6107,10 +6211,10 @@
     </row>
     <row r="33" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="B33" s="88" t="s">
-        <v>403</v>
+        <v>351</v>
+      </c>
+      <c r="B33" s="87" t="s">
+        <v>397</v>
       </c>
       <c r="C33" s="69" t="s">
         <v>51</v>
@@ -6121,13 +6225,13 @@
     </row>
     <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="B34" s="88" t="s">
-        <v>404</v>
+        <v>354</v>
+      </c>
+      <c r="B34" s="87" t="s">
+        <v>398</v>
       </c>
       <c r="C34" s="69" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D34" s="69" t="s">
         <v>55</v>
@@ -6135,10 +6239,10 @@
     </row>
     <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="65" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C35" s="69" t="s">
         <v>51</v>
@@ -6148,19 +6252,19 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="100" t="s">
+      <c r="A36" s="126" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="100"/>
-      <c r="C36" s="100"/>
-      <c r="D36" s="100"/>
+      <c r="B36" s="126"/>
+      <c r="C36" s="126"/>
+      <c r="D36" s="126"/>
     </row>
     <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="C37" s="69" t="s">
         <v>61</v>
@@ -6171,10 +6275,10 @@
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C38" s="69" t="s">
         <v>63</v>
@@ -6185,10 +6289,10 @@
     </row>
     <row r="39" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C39" s="69" t="s">
         <v>63</v>
@@ -6199,13 +6303,13 @@
     </row>
     <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="C40" s="71" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D40" s="69" t="s">
         <v>64</v>
@@ -6213,13 +6317,13 @@
     </row>
     <row r="41" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="C41" s="71" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D41" s="69" t="s">
         <v>23</v>
@@ -6227,10 +6331,10 @@
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C42" s="69" t="s">
         <v>61</v>
@@ -6241,10 +6345,10 @@
     </row>
     <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C43" s="69" t="s">
         <v>65</v>
@@ -6255,10 +6359,10 @@
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="65" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C44" s="69" t="s">
         <v>10</v>
@@ -6268,22 +6372,22 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="100" t="s">
+      <c r="A45" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="100"/>
-      <c r="C45" s="100"/>
-      <c r="D45" s="100"/>
+      <c r="B45" s="126"/>
+      <c r="C45" s="126"/>
+      <c r="D45" s="126"/>
     </row>
     <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="85" t="s">
-        <v>375</v>
+      <c r="A46" s="84" t="s">
+        <v>369</v>
       </c>
       <c r="B46" s="71" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C46" s="71" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D46" s="69" t="s">
         <v>67</v>
@@ -6291,13 +6395,13 @@
     </row>
     <row r="47" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C47" s="71" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D47" s="69" t="s">
         <v>44</v>
@@ -6305,29 +6409,29 @@
     </row>
     <row r="48" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="65" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C48" s="71" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D48" s="69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="100" t="s">
-        <v>254</v>
-      </c>
-      <c r="B49" s="100"/>
-      <c r="C49" s="100"/>
-      <c r="D49" s="100"/>
-    </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="81" t="s">
-        <v>446</v>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A49" s="126" t="s">
+        <v>253</v>
+      </c>
+      <c r="B49" s="126"/>
+      <c r="C49" s="126"/>
+      <c r="D49" s="126"/>
+    </row>
+    <row r="50" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="80" t="s">
+        <v>439</v>
       </c>
       <c r="B50" s="58"/>
       <c r="C50" s="58" t="s">
@@ -6337,26 +6441,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="82" t="s">
-        <v>441</v>
+    <row r="51" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="81" t="s">
+        <v>434</v>
       </c>
       <c r="B51" s="67" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="D51" s="58" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="82" t="s">
-        <v>447</v>
+    <row r="52" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="81" t="s">
+        <v>440</v>
       </c>
       <c r="B52" s="60" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="C52" s="58" t="s">
         <v>51</v>
@@ -6365,32 +6469,34 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="84" t="s">
-        <v>445</v>
-      </c>
-      <c r="B53" s="60"/>
+    <row r="53" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="83" t="s">
+        <v>438</v>
+      </c>
+      <c r="B53" s="60" t="s">
+        <v>490</v>
+      </c>
       <c r="C53" s="58" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D53" s="58" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="100" t="s">
-        <v>255</v>
-      </c>
-      <c r="B54" s="100"/>
-      <c r="C54" s="100"/>
-      <c r="D54" s="100"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="81" t="s">
-        <v>442</v>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A54" s="126" t="s">
+        <v>254</v>
+      </c>
+      <c r="B54" s="126"/>
+      <c r="C54" s="126"/>
+      <c r="D54" s="126"/>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A55" s="80" t="s">
+        <v>435</v>
       </c>
       <c r="B55" s="58" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="C55" s="58" t="s">
         <v>7</v>
@@ -6399,9 +6505,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="82" t="s">
-        <v>440</v>
+    <row r="56" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="81" t="s">
+        <v>433</v>
       </c>
       <c r="B56" s="58"/>
       <c r="C56" s="58" t="s">
@@ -6411,9 +6517,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="82" t="s">
-        <v>439</v>
+    <row r="57" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="81" t="s">
+        <v>432</v>
       </c>
       <c r="B57" s="58"/>
       <c r="C57" s="58" t="s">
@@ -6423,12 +6529,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="82" t="s">
+    <row r="58" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="81" t="s">
+        <v>437</v>
+      </c>
+      <c r="B58" s="60" t="s">
         <v>444</v>
-      </c>
-      <c r="B58" s="60" t="s">
-        <v>451</v>
       </c>
       <c r="C58" s="58" t="s">
         <v>61</v>
@@ -6437,124 +6543,214 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="82" t="s">
-        <v>443</v>
+    <row r="59" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="81" t="s">
+        <v>436</v>
       </c>
       <c r="B59" s="60" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="C59" s="58" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="D59" s="58" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="100" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A60" s="126" t="s">
+        <v>255</v>
+      </c>
+      <c r="B60" s="126"/>
+      <c r="C60" s="126"/>
+      <c r="D60" s="126"/>
+    </row>
+    <row r="61" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="B61" s="60" t="s">
+        <v>502</v>
+      </c>
+      <c r="C61" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="D61" s="58"/>
+    </row>
+    <row r="62" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="107" t="s">
+        <v>503</v>
+      </c>
+      <c r="B62" s="105"/>
+      <c r="C62" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="58" t="s">
+        <v>495</v>
+      </c>
+      <c r="M62" s="99"/>
+      <c r="AA62" s="95"/>
+      <c r="AB62" s="95"/>
+      <c r="AC62" s="95"/>
+    </row>
+    <row r="63" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="107" t="s">
+        <v>501</v>
+      </c>
+      <c r="B63" s="105"/>
+      <c r="C63" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="58"/>
+      <c r="M63" s="99"/>
+      <c r="AA63" s="95"/>
+      <c r="AB63" s="95"/>
+      <c r="AC63" s="95"/>
+    </row>
+    <row r="64" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="107" t="s">
+        <v>500</v>
+      </c>
+      <c r="B64" s="105"/>
+      <c r="C64" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64" s="58"/>
+      <c r="M64" s="99"/>
+      <c r="AA64" s="95"/>
+      <c r="AB64" s="95"/>
+      <c r="AC64" s="95"/>
+    </row>
+    <row r="65" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="107" t="s">
+        <v>497</v>
+      </c>
+      <c r="B65" s="105"/>
+      <c r="C65" s="58" t="s">
+        <v>496</v>
+      </c>
+      <c r="D65" s="58"/>
+      <c r="M65" s="99"/>
+      <c r="AA65" s="95"/>
+      <c r="AB65" s="95"/>
+      <c r="AC65" s="95"/>
+    </row>
+    <row r="66" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="96" t="s">
         <v>256</v>
       </c>
-      <c r="B60" s="100"/>
-      <c r="C60" s="100"/>
-      <c r="D60" s="100"/>
-    </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="81" t="s">
-        <v>257</v>
-      </c>
-      <c r="B61" s="60" t="s">
-        <v>416</v>
-      </c>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="82" t="s">
-        <v>258</v>
-      </c>
-      <c r="B62" s="60"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="58"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="82" t="s">
-        <v>260</v>
-      </c>
-      <c r="B63" s="60"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="82" t="s">
-        <v>259</v>
-      </c>
-      <c r="B64" s="60"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="58"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="82" t="s">
-        <v>261</v>
-      </c>
-      <c r="B65" s="60"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
-    </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="100" t="s">
-        <v>262</v>
-      </c>
-      <c r="B66" s="100"/>
-      <c r="C66" s="100"/>
-      <c r="D66" s="100"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="82" t="s">
-        <v>272</v>
-      </c>
-      <c r="B67" s="60"/>
+      <c r="B66" s="96"/>
+      <c r="C66" s="96"/>
+      <c r="D66" s="96"/>
+      <c r="M66" s="99"/>
+      <c r="AA66" s="95"/>
+      <c r="AB66" s="95"/>
+      <c r="AC66" s="95"/>
+    </row>
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A67" s="107" t="s">
+        <v>266</v>
+      </c>
+      <c r="B67" s="105"/>
       <c r="C67" s="58"/>
       <c r="D67" s="58" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="82" t="s">
-        <v>263</v>
-      </c>
-      <c r="B68" s="60"/>
+      <c r="M67" s="99"/>
+      <c r="AA67" s="95"/>
+      <c r="AB67" s="95"/>
+      <c r="AC67" s="95"/>
+    </row>
+    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A68" s="107" t="s">
+        <v>257</v>
+      </c>
+      <c r="B68" s="105"/>
       <c r="C68" s="58"/>
       <c r="D68" s="58" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="82" t="s">
-        <v>273</v>
-      </c>
-      <c r="B69" s="60"/>
+      <c r="M68" s="99"/>
+      <c r="AA68" s="95"/>
+      <c r="AB68" s="95"/>
+      <c r="AC68" s="95"/>
+    </row>
+    <row r="69" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="107" t="s">
+        <v>267</v>
+      </c>
+      <c r="B69" s="105"/>
       <c r="C69" s="58"/>
       <c r="D69" s="58" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="225" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="83" t="s">
-        <v>427</v>
+        <v>421</v>
+      </c>
+      <c r="M69" s="99"/>
+      <c r="AA69" s="95"/>
+      <c r="AB69" s="95"/>
+      <c r="AC69" s="95"/>
+    </row>
+    <row r="70" spans="1:29" ht="225" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="82" t="s">
+        <v>420</v>
       </c>
       <c r="B70" s="61" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="C70" s="59" t="s">
         <v>10</v>
       </c>
       <c r="D70" s="59" t="s">
-        <v>429</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="M70" s="99"/>
+      <c r="AA70" s="95"/>
+      <c r="AB70" s="95"/>
+      <c r="AC70" s="95"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
+  <mergeCells count="53">
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="Z11:AC11"/>
     <mergeCell ref="Z6:AC6"/>
     <mergeCell ref="Z2:AC2"/>
@@ -6566,49 +6762,6 @@
     <mergeCell ref="U6:U7"/>
     <mergeCell ref="W6:W7"/>
     <mergeCell ref="X6:X7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6619,8 +6772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E7B11-1527-417B-9532-F0F2C5A89902}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6674,35 +6827,35 @@
       <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="127" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
       <c r="F2" s="18"/>
-      <c r="G2" s="105" t="s">
+      <c r="G2" s="125" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
       <c r="L2" s="32"/>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="144" t="s">
         <v>203</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="134" t="s">
         <v>131</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E3" s="20">
         <v>3</v>
@@ -6714,7 +6867,7 @@
       <c r="H3" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I3" s="113"/>
+      <c r="I3" s="132"/>
       <c r="J3" s="7" t="s">
         <v>168</v>
       </c>
@@ -6726,10 +6879,10 @@
       <c r="A4" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="123"/>
-      <c r="C4" s="116"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="135"/>
       <c r="D4" s="7" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E4" s="30">
         <v>2</v>
@@ -6741,7 +6894,7 @@
       <c r="H4" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="I4" s="111"/>
+      <c r="I4" s="141"/>
       <c r="J4" s="7" t="s">
         <v>150</v>
       </c>
@@ -6753,10 +6906,10 @@
       <c r="A5" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="123"/>
-      <c r="C5" s="116"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="135"/>
       <c r="D5" s="7" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E5" s="20">
         <v>3</v>
@@ -6768,7 +6921,7 @@
       <c r="H5" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="I5" s="111"/>
+      <c r="I5" s="141"/>
       <c r="J5" s="7" t="s">
         <v>161</v>
       </c>
@@ -6780,10 +6933,10 @@
       <c r="A6" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B6" s="123"/>
-      <c r="C6" s="116"/>
+      <c r="B6" s="145"/>
+      <c r="C6" s="135"/>
       <c r="D6" s="7" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E6" s="30">
         <v>1</v>
@@ -6795,7 +6948,7 @@
       <c r="H6" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="I6" s="111"/>
+      <c r="I6" s="141"/>
       <c r="J6" s="7" t="s">
         <v>157</v>
       </c>
@@ -6807,10 +6960,10 @@
       <c r="A7" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="123"/>
-      <c r="C7" s="116"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="135"/>
       <c r="D7" s="7" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E7" s="7">
         <v>2</v>
@@ -6822,7 +6975,7 @@
       <c r="H7" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="I7" s="111"/>
+      <c r="I7" s="141"/>
       <c r="J7" s="29" t="s">
         <v>144</v>
       </c>
@@ -6834,12 +6987,12 @@
       <c r="A8" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B8" s="123"/>
-      <c r="C8" s="109" t="s">
+      <c r="B8" s="145"/>
+      <c r="C8" s="139" t="s">
         <v>87</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="7">
         <v>5</v>
@@ -6851,7 +7004,7 @@
       <c r="H8" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I8" s="111"/>
+      <c r="I8" s="141"/>
       <c r="J8" s="7" t="s">
         <v>150</v>
       </c>
@@ -6866,7 +7019,7 @@
       <c r="B9" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="109"/>
+      <c r="C9" s="139"/>
       <c r="D9" s="7" t="s">
         <v>152</v>
       </c>
@@ -6880,7 +7033,7 @@
       <c r="H9" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="I9" s="111"/>
+      <c r="I9" s="141"/>
       <c r="J9" s="29" t="s">
         <v>209</v>
       </c>
@@ -6911,7 +7064,7 @@
       <c r="H10" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I10" s="114"/>
+      <c r="I10" s="146"/>
       <c r="J10" s="29" t="s">
         <v>144</v>
       </c>
@@ -6920,36 +7073,36 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="117" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="111" t="s">
+      <c r="B11" s="141" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="139" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="99" t="s">
+      <c r="D11" s="124" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="118">
+      <c r="E11" s="137">
         <v>3</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="95" t="s">
+      <c r="G11" s="114" t="s">
         <v>140</v>
       </c>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="95"/>
+      <c r="H11" s="114"/>
+      <c r="I11" s="114"/>
+      <c r="J11" s="114"/>
+      <c r="K11" s="114"/>
     </row>
     <row r="12" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="121"/>
-      <c r="B12" s="120"/>
-      <c r="C12" s="110"/>
-      <c r="D12" s="117"/>
-      <c r="E12" s="119"/>
+      <c r="A12" s="143"/>
+      <c r="B12" s="142"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="138"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
         <v>139</v>
@@ -6966,13 +7119,13 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="126" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="100"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
+      <c r="B13" s="126"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="126"/>
+      <c r="E13" s="126"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
         <v>135</v>
@@ -6995,7 +7148,7 @@
       <c r="B14" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="107" t="s">
+      <c r="C14" s="134" t="s">
         <v>87</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -7026,7 +7179,7 @@
       <c r="B15" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="109"/>
+      <c r="C15" s="139"/>
       <c r="D15" s="11" t="s">
         <v>125</v>
       </c>
@@ -7049,40 +7202,40 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="101" t="s">
+      <c r="A16" s="117" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="111" t="s">
+      <c r="B16" s="141" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="99" t="s">
+      <c r="C16" s="139"/>
+      <c r="D16" s="124" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="112">
+      <c r="E16" s="147">
         <v>1</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="95" t="s">
+      <c r="G16" s="114" t="s">
         <v>118</v>
       </c>
-      <c r="H16" s="95"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="95"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="114"/>
+      <c r="K16" s="114"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="101"/>
-      <c r="B17" s="111"/>
-      <c r="C17" s="109"/>
-      <c r="D17" s="99"/>
-      <c r="E17" s="112"/>
+      <c r="A17" s="117"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="124"/>
+      <c r="E17" s="147"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
         <v>117</v>
       </c>
       <c r="H17" s="12"/>
-      <c r="I17" s="113"/>
+      <c r="I17" s="132"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7092,7 +7245,7 @@
       <c r="B18" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="109"/>
+      <c r="C18" s="139"/>
       <c r="D18" s="7" t="s">
         <v>114</v>
       </c>
@@ -7104,7 +7257,7 @@
         <v>113</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="111"/>
+      <c r="I18" s="141"/>
       <c r="K18"/>
     </row>
     <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7114,7 +7267,7 @@
       <c r="B19" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="109" t="s">
+      <c r="C19" s="139" t="s">
         <v>131</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -7128,7 +7281,7 @@
         <v>109</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="I19" s="111"/>
+      <c r="I19" s="141"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7138,7 +7291,7 @@
       <c r="B20" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="109"/>
+      <c r="C20" s="139"/>
       <c r="D20" s="7" t="s">
         <v>106</v>
       </c>
@@ -7150,7 +7303,7 @@
         <v>105</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="111"/>
+      <c r="I20" s="141"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -7160,7 +7313,7 @@
       <c r="B21" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="109"/>
+      <c r="C21" s="139"/>
       <c r="D21" s="7" t="s">
         <v>102</v>
       </c>
@@ -7172,7 +7325,7 @@
         <v>101</v>
       </c>
       <c r="H21" s="12"/>
-      <c r="I21" s="111"/>
+      <c r="I21" s="141"/>
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7182,7 +7335,7 @@
       <c r="B22" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="109"/>
+      <c r="C22" s="139"/>
       <c r="D22" s="7" t="s">
         <v>98</v>
       </c>
@@ -7194,7 +7347,7 @@
         <v>97</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="I22" s="111"/>
+      <c r="I22" s="141"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7204,7 +7357,7 @@
       <c r="B23" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="110"/>
+      <c r="C23" s="140"/>
       <c r="D23" s="7" t="s">
         <v>94</v>
       </c>
@@ -7216,26 +7369,26 @@
         <v>204</v>
       </c>
       <c r="H23" s="12"/>
-      <c r="I23" s="111"/>
+      <c r="I23" s="141"/>
       <c r="J23" s="7" t="s">
         <v>209</v>
       </c>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="100" t="s">
+      <c r="A24" s="126" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="100"/>
-      <c r="C24" s="100"/>
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
+      <c r="B24" s="126"/>
+      <c r="C24" s="126"/>
+      <c r="D24" s="126"/>
+      <c r="E24" s="126"/>
       <c r="F24" s="4"/>
       <c r="G24" s="5" t="s">
         <v>93</v>
       </c>
       <c r="H24" s="12"/>
-      <c r="I24" s="111"/>
+      <c r="I24" s="141"/>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7245,11 +7398,11 @@
       <c r="B25" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="107" t="s">
-        <v>435</v>
+      <c r="C25" s="134" t="s">
+        <v>428</v>
       </c>
       <c r="D25" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E25" s="26">
         <v>2</v>
@@ -7259,61 +7412,77 @@
         <v>91</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="111"/>
+      <c r="I25" s="141"/>
       <c r="J25" s="12" t="s">
         <v>90</v>
       </c>
       <c r="K25" s="25"/>
     </row>
-    <row r="26" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="108"/>
-      <c r="D26" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="E26" s="24">
+      <c r="C26" s="135"/>
+      <c r="D26" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="E26" s="45">
         <v>3</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="15"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="111"/>
+      <c r="I26" s="141"/>
       <c r="J26" s="12"/>
       <c r="K26" s="25"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
+      <c r="A27" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>494</v>
+      </c>
+      <c r="C27" s="101" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="E27" s="45">
+        <v>1</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="5" t="s">
         <v>84</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="111"/>
+      <c r="I27" s="141"/>
       <c r="K27" s="23"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="45"/>
+      <c r="A28" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="B28" s="100"/>
+      <c r="C28" s="109"/>
+      <c r="D28" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="E28" s="45">
+        <v>3</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="5" t="s">
         <v>83</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="111"/>
+      <c r="I28" s="141"/>
       <c r="J28" s="7" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="K28" s="7"/>
     </row>
@@ -7323,7 +7492,7 @@
       <c r="G29" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I29" s="111"/>
+      <c r="I29" s="141"/>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -7332,7 +7501,7 @@
       <c r="G30" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I30" s="114"/>
+      <c r="I30" s="146"/>
       <c r="J30" s="7" t="s">
         <v>209</v>
       </c>
@@ -7341,13 +7510,13 @@
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="95" t="s">
+      <c r="G31" s="114" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="95"/>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="95"/>
+      <c r="H31" s="114"/>
+      <c r="I31" s="114"/>
+      <c r="J31" s="114"/>
+      <c r="K31" s="114"/>
     </row>
     <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
@@ -7355,10 +7524,10 @@
       <c r="G32" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H32" s="12" t="s">
+      <c r="H32" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="I32" s="113"/>
+      <c r="I32" s="132"/>
       <c r="J32" s="7" t="s">
         <v>77</v>
       </c>
@@ -7372,10 +7541,10 @@
       <c r="G33" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="H33" s="98" t="s">
         <v>75</v>
       </c>
-      <c r="I33" s="115"/>
+      <c r="I33" s="133"/>
       <c r="J33" s="7" t="s">
         <v>74</v>
       </c>
@@ -7389,11 +7558,14 @@
       <c r="G34" s="5" t="s">
         <v>73</v>
       </c>
+      <c r="H34" s="98" t="s">
+        <v>494</v>
+      </c>
       <c r="I34" s="70" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="K34" s="4"/>
     </row>
@@ -7403,14 +7575,14 @@
       <c r="G35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="H35" s="98" t="s">
         <v>71</v>
       </c>
       <c r="I35" s="70" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="K35" s="4"/>
     </row>
@@ -7420,14 +7592,14 @@
       <c r="G36" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H36" s="44" t="s">
+      <c r="H36" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="I36" s="74" t="s">
-        <v>364</v>
+      <c r="I36" s="73" t="s">
+        <v>358</v>
       </c>
       <c r="J36" s="44" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="K36" s="42"/>
     </row>
@@ -7435,16 +7607,16 @@
       <c r="D37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="13" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="H37" s="72" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I37" s="56">
         <v>0</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="K37" s="24">
         <v>5</v>
@@ -7565,6 +7737,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="I17:I30"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="G31:K31"/>
     <mergeCell ref="I32:I33"/>
     <mergeCell ref="A2:E2"/>
@@ -7581,16 +7762,8 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="I3:I10"/>
     <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="I17:I30"/>
-    <mergeCell ref="A24:E24"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7601,7 +7774,7 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7658,12 +7831,12 @@
       <c r="A2" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="124" t="s">
+      <c r="B2" s="164"/>
+      <c r="C2" s="148" t="s">
         <v>198</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="E2" s="40" t="s">
         <v>197</v>
@@ -7672,6 +7845,7 @@
       <c r="G2" s="48" t="s">
         <v>199</v>
       </c>
+      <c r="H2" s="167"/>
       <c r="I2" s="21" t="s">
         <v>134</v>
       </c>
@@ -7682,10 +7856,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="109"/>
+        <v>415</v>
+      </c>
+      <c r="B3" s="165"/>
+      <c r="C3" s="139"/>
       <c r="D3" s="7"/>
       <c r="E3" s="40" t="s">
         <v>197</v>
@@ -7694,6 +7868,7 @@
       <c r="G3" s="10" t="s">
         <v>196</v>
       </c>
+      <c r="H3" s="168"/>
       <c r="I3" s="21">
         <v>0</v>
       </c>
@@ -7705,8 +7880,8 @@
       <c r="A4" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="109" t="s">
+      <c r="B4" s="165"/>
+      <c r="C4" s="139" t="s">
         <v>194</v>
       </c>
       <c r="D4" s="7"/>
@@ -7715,14 +7890,14 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="H4" s="17"/>
+        <v>275</v>
+      </c>
+      <c r="H4" s="169"/>
       <c r="I4" s="38" t="s">
         <v>193</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="K4" s="41" t="s">
         <v>179</v>
@@ -7732,8 +7907,8 @@
       <c r="A5" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="109"/>
+      <c r="B5" s="165"/>
+      <c r="C5" s="139"/>
       <c r="D5" s="7"/>
       <c r="E5" s="40" t="s">
         <v>182</v>
@@ -7745,7 +7920,7 @@
       <c r="A6" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="165"/>
       <c r="C6" s="22">
         <v>0</v>
       </c>
@@ -7760,7 +7935,8 @@
       <c r="A7" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="109" t="s">
+      <c r="B7" s="165"/>
+      <c r="C7" s="139" t="s">
         <v>194</v>
       </c>
       <c r="D7" s="7"/>
@@ -7775,7 +7951,8 @@
       <c r="A8" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C8" s="109"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="139"/>
       <c r="D8" s="7"/>
       <c r="E8" s="39" t="s">
         <v>182</v>
@@ -7791,6 +7968,7 @@
       <c r="A9" s="5" t="s">
         <v>188</v>
       </c>
+      <c r="B9" s="165"/>
       <c r="C9" s="22" t="s">
         <v>187</v>
       </c>
@@ -7807,6 +7985,7 @@
       <c r="A10" s="5" t="s">
         <v>186</v>
       </c>
+      <c r="B10" s="165"/>
       <c r="C10" s="22" t="s">
         <v>185</v>
       </c>
@@ -7823,12 +8002,12 @@
       <c r="A11" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="165"/>
       <c r="C11" s="21" t="s">
         <v>183</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E11" s="39" t="s">
         <v>182</v>
@@ -7842,7 +8021,7 @@
       <c r="A12" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="166"/>
       <c r="C12" s="38" t="s">
         <v>180</v>
       </c>
@@ -8147,10 +8326,12 @@
       <c r="D58" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="H2:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8161,8 +8342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD902308-2995-4981-9D8D-2D9FAE7EB6D0}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8170,19 +8351,19 @@
     <col min="1" max="1" width="28" style="4" customWidth="1"/>
     <col min="2" max="2" width="20" style="21" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="75" customWidth="1"/>
-    <col min="5" max="5" width="4" style="80" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="74" customWidth="1"/>
+    <col min="5" max="5" width="4" style="94" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="28" style="4" customWidth="1"/>
     <col min="8" max="8" width="20" style="4" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" style="75" customWidth="1"/>
-    <col min="11" max="11" width="4" style="80" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" style="74" customWidth="1"/>
+    <col min="11" max="11" width="4" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -8193,7 +8374,7 @@
       <c r="D1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="1" t="s">
         <v>174</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -8208,100 +8389,100 @@
       <c r="J1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="153" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
-        <v>471</v>
-      </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="G2" s="100" t="s">
-        <v>493</v>
-      </c>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
+      <c r="A2" s="126" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="G2" s="126" t="s">
+        <v>482</v>
+      </c>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="B3" s="140" t="s">
-        <v>477</v>
-      </c>
-      <c r="C3" s="107" t="s">
+        <v>462</v>
+      </c>
+      <c r="B3" s="149" t="s">
+        <v>467</v>
+      </c>
+      <c r="C3" s="134" t="s">
         <v>194</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="142">
+      <c r="E3" s="111">
         <v>2</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="75"/>
+      <c r="H3" s="74"/>
       <c r="I3" s="36"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="40"/>
+      <c r="K3" s="154"/>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>473</v>
-      </c>
-      <c r="B4" s="141"/>
-      <c r="C4" s="116"/>
+        <v>463</v>
+      </c>
+      <c r="B4" s="150"/>
+      <c r="C4" s="135"/>
       <c r="D4" s="44" t="s">
-        <v>478</v>
-      </c>
-      <c r="E4" s="143">
+        <v>468</v>
+      </c>
+      <c r="E4" s="112">
         <v>1</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="42"/>
       <c r="H4" s="46"/>
-      <c r="I4" s="138"/>
+      <c r="I4" s="109"/>
       <c r="J4" s="44"/>
-      <c r="K4" s="134"/>
+      <c r="K4" s="155"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="B5" s="141"/>
-      <c r="C5" s="77" t="s">
+        <v>465</v>
+      </c>
+      <c r="B5" s="150"/>
+      <c r="C5" s="76" t="s">
         <v>134</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="144">
+      <c r="E5" s="113">
         <v>4</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="42"/>
       <c r="H5" s="46"/>
-      <c r="I5" s="138"/>
+      <c r="I5" s="109"/>
       <c r="J5" s="44"/>
-      <c r="K5" s="135"/>
+      <c r="K5" s="156"/>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="B6" s="87" t="s">
-        <v>491</v>
-      </c>
-      <c r="C6" s="77" t="s">
-        <v>483</v>
+        <v>474</v>
+      </c>
+      <c r="B6" s="86" t="s">
+        <v>480</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>473</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E6" s="64">
         <v>3</v>
@@ -8309,211 +8490,219 @@
       <c r="F6" s="51"/>
       <c r="G6" s="42"/>
       <c r="H6" s="46"/>
-      <c r="I6" s="77"/>
+      <c r="I6" s="76"/>
       <c r="J6" s="44"/>
-      <c r="K6" s="136"/>
+      <c r="K6" s="44"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="100" t="s">
-        <v>492</v>
-      </c>
-      <c r="B7" s="100"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
+      <c r="A7" s="126" t="s">
+        <v>481</v>
+      </c>
+      <c r="B7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
       <c r="F7" s="51"/>
       <c r="G7" s="42"/>
       <c r="H7" s="42"/>
-      <c r="I7" s="138"/>
+      <c r="I7" s="109"/>
       <c r="J7" s="44"/>
-      <c r="K7" s="134"/>
+      <c r="K7" s="155"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>476</v>
-      </c>
-      <c r="C8" s="77" t="s">
+        <v>466</v>
+      </c>
+      <c r="C8" s="76" t="s">
         <v>134</v>
       </c>
       <c r="D8" s="44"/>
-      <c r="E8" s="134"/>
+      <c r="E8" s="112">
+        <v>2</v>
+      </c>
       <c r="F8" s="51"/>
       <c r="G8" s="42"/>
       <c r="H8" s="42"/>
-      <c r="I8" s="138"/>
+      <c r="I8" s="109"/>
       <c r="J8" s="44"/>
-      <c r="K8" s="134"/>
+      <c r="K8" s="155"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>476</v>
-      </c>
-      <c r="C9" s="77" t="s">
+        <v>466</v>
+      </c>
+      <c r="C9" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="134"/>
+      <c r="D9" s="44" t="s">
+        <v>487</v>
+      </c>
+      <c r="E9" s="112">
+        <v>3</v>
+      </c>
       <c r="F9" s="51"/>
       <c r="G9" s="42"/>
       <c r="H9" s="42"/>
-      <c r="I9" s="77"/>
+      <c r="I9" s="76"/>
       <c r="J9" s="44"/>
-      <c r="K9" s="134"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="B10" s="47" t="s">
-        <v>497</v>
-      </c>
-      <c r="C10" s="77" t="s">
-        <v>483</v>
-      </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="134"/>
+      <c r="K9" s="155"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="C10" s="97" t="s">
+        <v>473</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="161">
+        <v>1</v>
+      </c>
       <c r="F10" s="51"/>
       <c r="G10" s="42"/>
       <c r="H10" s="42"/>
-      <c r="I10" s="77"/>
+      <c r="I10" s="76"/>
       <c r="J10" s="44"/>
-      <c r="K10" s="134"/>
+      <c r="K10" s="155"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
       <c r="D11" s="44"/>
-      <c r="E11" s="134"/>
+      <c r="E11" s="112"/>
       <c r="F11" s="51"/>
       <c r="G11" s="42"/>
       <c r="H11" s="46"/>
       <c r="I11" s="47"/>
       <c r="J11" s="44"/>
-      <c r="K11" s="134"/>
+      <c r="K11" s="155"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
-      <c r="B12" s="87"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="47"/>
       <c r="D12" s="44"/>
-      <c r="E12" s="134"/>
+      <c r="E12" s="112"/>
       <c r="F12" s="51"/>
       <c r="G12" s="42"/>
       <c r="H12" s="44"/>
       <c r="I12" s="47"/>
       <c r="J12" s="44"/>
-      <c r="K12" s="134"/>
+      <c r="K12" s="155"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="42"/>
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
       <c r="D13" s="44"/>
-      <c r="E13" s="136"/>
+      <c r="E13" s="64"/>
       <c r="F13" s="51"/>
       <c r="G13" s="42"/>
       <c r="H13" s="46"/>
       <c r="I13" s="47"/>
       <c r="J13" s="44"/>
-      <c r="K13" s="136"/>
+      <c r="K13" s="44"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="137"/>
-      <c r="B14" s="139"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="E14" s="137"/>
+      <c r="A14" s="108"/>
+      <c r="B14" s="110"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="151"/>
       <c r="F14" s="51"/>
-      <c r="G14" s="137"/>
-      <c r="H14" s="137"/>
-      <c r="I14" s="137"/>
-      <c r="J14" s="137"/>
-      <c r="K14" s="137"/>
+      <c r="G14" s="108"/>
+      <c r="H14" s="108"/>
+      <c r="I14" s="108"/>
+      <c r="J14" s="108"/>
+      <c r="K14" s="157"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="42"/>
       <c r="B15" s="47"/>
-      <c r="C15" s="138"/>
+      <c r="C15" s="109"/>
       <c r="D15" s="44"/>
-      <c r="E15" s="45"/>
+      <c r="E15" s="102"/>
       <c r="F15" s="51"/>
       <c r="G15" s="42"/>
       <c r="H15" s="46"/>
-      <c r="I15" s="138"/>
+      <c r="I15" s="109"/>
       <c r="J15" s="44"/>
-      <c r="K15" s="45"/>
+      <c r="K15" s="42"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="46"/>
       <c r="B16" s="47"/>
-      <c r="C16" s="138"/>
+      <c r="C16" s="109"/>
       <c r="D16" s="64"/>
-      <c r="E16" s="45"/>
+      <c r="E16" s="102"/>
       <c r="F16" s="51"/>
       <c r="G16" s="46"/>
       <c r="H16" s="46"/>
-      <c r="I16" s="138"/>
+      <c r="I16" s="109"/>
       <c r="J16" s="64"/>
-      <c r="K16" s="45"/>
+      <c r="K16" s="42"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="42"/>
       <c r="B17" s="47"/>
-      <c r="C17" s="138"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="44"/>
-      <c r="E17" s="45"/>
+      <c r="E17" s="102"/>
       <c r="F17" s="51"/>
       <c r="G17" s="42"/>
       <c r="H17" s="46"/>
-      <c r="I17" s="138"/>
+      <c r="I17" s="109"/>
       <c r="J17" s="44"/>
-      <c r="K17" s="45"/>
+      <c r="K17" s="42"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="42"/>
       <c r="B18" s="47"/>
-      <c r="C18" s="138"/>
+      <c r="C18" s="109"/>
       <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
+      <c r="E18" s="102"/>
       <c r="F18" s="51"/>
       <c r="G18" s="42"/>
       <c r="H18" s="46"/>
-      <c r="I18" s="138"/>
+      <c r="I18" s="109"/>
       <c r="J18" s="44"/>
-      <c r="K18" s="45"/>
+      <c r="K18" s="42"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C19" s="36"/>
       <c r="D19" s="7"/>
-      <c r="H19" s="75"/>
+      <c r="H19" s="74"/>
       <c r="I19" s="36"/>
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C20" s="36"/>
       <c r="D20" s="7"/>
-      <c r="H20" s="75"/>
+      <c r="H20" s="74"/>
       <c r="I20" s="36"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C21" s="36"/>
       <c r="D21" s="7"/>
-      <c r="H21" s="75"/>
+      <c r="H21" s="74"/>
       <c r="I21" s="36"/>
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="36"/>
       <c r="D22" s="7"/>
-      <c r="H22" s="75"/>
+      <c r="H22" s="74"/>
       <c r="I22" s="36"/>
       <c r="J22" s="7"/>
     </row>
@@ -8522,33 +8711,33 @@
       <c r="B23" s="23"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="E23" s="152"/>
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
+      <c r="K23" s="158"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" s="36"/>
       <c r="D24" s="4"/>
-      <c r="H24" s="75"/>
+      <c r="H24" s="74"/>
       <c r="I24" s="36"/>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="79"/>
+      <c r="B25" s="78"/>
       <c r="C25" s="36"/>
       <c r="D25" s="7"/>
-      <c r="H25" s="76"/>
+      <c r="H25" s="75"/>
       <c r="I25" s="36"/>
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="75"/>
+      <c r="C26" s="74"/>
       <c r="D26" s="4"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="75"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -8558,7 +8747,7 @@
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C28" s="21"/>
       <c r="D28" s="7"/>
-      <c r="H28" s="75"/>
+      <c r="H28" s="74"/>
       <c r="I28" s="21"/>
       <c r="J28" s="7"/>
     </row>
@@ -8700,7 +8889,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8795,20 +8984,20 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>244</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>245</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G9" s="31" t="s">
         <v>246</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -8818,10 +9007,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614F32F9-8D4F-4B7C-ACE2-D0F7B904B029}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8837,7 +9026,7 @@
     <col min="9" max="9" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>220</v>
       </c>
@@ -8863,60 +9052,64 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="162" t="s">
         <v>221</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="162" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="159" t="s">
+        <v>247</v>
+      </c>
+      <c r="F3" s="159" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="159" t="s">
         <v>248</v>
       </c>
-      <c r="F3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F4" s="163" t="s">
+        <v>217</v>
+      </c>
+      <c r="G4" s="160"/>
+      <c r="H4" s="160" t="s">
+        <v>218</v>
+      </c>
+      <c r="I4" s="160"/>
+      <c r="J4" s="160"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="159" t="s">
         <v>249</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51" t="s">
-        <v>218</v>
-      </c>
-      <c r="I4" s="51"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>250</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
       <c r="H5" s="51"/>
       <c r="I5" s="51"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="163" t="s">
         <v>226</v>
       </c>
+      <c r="B6" s="160"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="160"/>
       <c r="F6" s="51"/>
       <c r="G6" s="51"/>
       <c r="H6" s="51"/>
       <c r="I6" s="51"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
       <c r="H7" s="51"/>
       <c r="I7" s="51"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>214</v>
       </c>
@@ -8934,24 +9127,27 @@
       <c r="H8" s="52"/>
       <c r="I8" s="53"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>251</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="162" t="s">
+        <v>250</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
       <c r="I9" s="51"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="159" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="163" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>253</v>
-      </c>
+      <c r="B11" s="160"/>
+      <c r="C11" s="160"/>
+      <c r="D11" s="160"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated the costs of basic woods and leathers.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CK.DESKTOP-BR5NVLN\Documents\Git Repositories\Creative\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0492A019-F26D-46B7-AA08-B252930648AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE016D19-7C21-40AC-A5B5-95BE3F376A74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="1" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -4660,117 +4660,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4798,6 +4687,111 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -4815,6 +4809,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5132,8 +5132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
   <dimension ref="A1:AC70"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5240,54 +5240,54 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="F2" s="125" t="s">
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="F2" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="K2" s="125" t="s">
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="K2" s="130" t="s">
         <v>448</v>
       </c>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="P2" s="116" t="s">
+      <c r="L2" s="130"/>
+      <c r="M2" s="130"/>
+      <c r="N2" s="130"/>
+      <c r="P2" s="140" t="s">
         <v>215</v>
       </c>
-      <c r="Q2" s="123" t="s">
+      <c r="Q2" s="141" t="s">
         <v>258</v>
       </c>
-      <c r="R2" s="120" t="s">
+      <c r="R2" s="135" t="s">
         <v>228</v>
       </c>
-      <c r="S2" s="120" t="s">
+      <c r="S2" s="135" t="s">
         <v>62</v>
       </c>
-      <c r="U2" s="116" t="s">
+      <c r="U2" s="140" t="s">
         <v>233</v>
       </c>
-      <c r="V2" s="118" t="s">
+      <c r="V2" s="143" t="s">
         <v>270</v>
       </c>
-      <c r="W2" s="120" t="s">
+      <c r="W2" s="135" t="s">
         <v>228</v>
       </c>
-      <c r="X2" s="120" t="s">
+      <c r="X2" s="135" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" s="115" t="s">
+      <c r="Z2" s="142" t="s">
         <v>284</v>
       </c>
-      <c r="AA2" s="115"/>
-      <c r="AB2" s="115"/>
-      <c r="AC2" s="115"/>
+      <c r="AA2" s="142"/>
+      <c r="AB2" s="142"/>
+      <c r="AC2" s="142"/>
     </row>
     <row r="3" spans="1:29" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -5324,14 +5324,14 @@
         <v>0.06</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="P3" s="117"/>
-      <c r="Q3" s="122"/>
-      <c r="R3" s="122"/>
-      <c r="S3" s="122"/>
-      <c r="U3" s="117"/>
-      <c r="V3" s="119"/>
-      <c r="W3" s="121"/>
-      <c r="X3" s="121"/>
+      <c r="P3" s="136"/>
+      <c r="Q3" s="132"/>
+      <c r="R3" s="132"/>
+      <c r="S3" s="132"/>
+      <c r="U3" s="136"/>
+      <c r="V3" s="133"/>
+      <c r="W3" s="144"/>
+      <c r="X3" s="144"/>
       <c r="Z3" s="10" t="s">
         <v>285</v>
       </c>
@@ -5474,66 +5474,66 @@
       <c r="AC5" s="77"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="131" t="s">
         <v>333</v>
       </c>
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="127" t="s">
         <v>407</v>
       </c>
-      <c r="C6" s="122" t="s">
+      <c r="C6" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="122" t="s">
+      <c r="D6" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="114" t="s">
+      <c r="F6" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="114"/>
-      <c r="H6" s="114"/>
-      <c r="I6" s="114"/>
-      <c r="K6" s="114" t="s">
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="K6" s="134" t="s">
         <v>450</v>
       </c>
-      <c r="L6" s="114"/>
-      <c r="M6" s="114"/>
-      <c r="N6" s="114"/>
-      <c r="P6" s="117" t="s">
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="P6" s="136" t="s">
         <v>225</v>
       </c>
-      <c r="Q6" s="124" t="s">
+      <c r="Q6" s="127" t="s">
         <v>261</v>
       </c>
-      <c r="R6" s="122" t="s">
+      <c r="R6" s="132" t="s">
         <v>229</v>
       </c>
-      <c r="S6" s="122" t="s">
+      <c r="S6" s="132" t="s">
         <v>43</v>
       </c>
-      <c r="U6" s="117" t="s">
+      <c r="U6" s="136" t="s">
         <v>236</v>
       </c>
-      <c r="V6" s="119" t="s">
+      <c r="V6" s="133" t="s">
         <v>265</v>
       </c>
-      <c r="W6" s="122" t="s">
+      <c r="W6" s="132" t="s">
         <v>229</v>
       </c>
-      <c r="X6" s="122" t="s">
+      <c r="X6" s="132" t="s">
         <v>43</v>
       </c>
-      <c r="Z6" s="114" t="s">
+      <c r="Z6" s="134" t="s">
         <v>294</v>
       </c>
-      <c r="AA6" s="114"/>
-      <c r="AB6" s="114"/>
-      <c r="AC6" s="114"/>
+      <c r="AA6" s="134"/>
+      <c r="AB6" s="134"/>
+      <c r="AC6" s="134"/>
     </row>
     <row r="7" spans="1:29" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="128"/>
-      <c r="B7" s="124"/>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
+      <c r="A7" s="131"/>
+      <c r="B7" s="127"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
       <c r="F7" s="9" t="s">
         <v>319</v>
       </c>
@@ -5556,14 +5556,14 @@
         <v>0.08</v>
       </c>
       <c r="N7" s="103"/>
-      <c r="P7" s="117"/>
-      <c r="Q7" s="122"/>
-      <c r="R7" s="122"/>
-      <c r="S7" s="122"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="119"/>
-      <c r="W7" s="122"/>
-      <c r="X7" s="122"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="132"/>
+      <c r="R7" s="132"/>
+      <c r="S7" s="132"/>
+      <c r="U7" s="136"/>
+      <c r="V7" s="133"/>
+      <c r="W7" s="132"/>
+      <c r="X7" s="132"/>
       <c r="Z7" s="10" t="s">
         <v>295</v>
       </c>
@@ -5725,52 +5725,52 @@
       </c>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="128" t="s">
+      <c r="A11" s="131" t="s">
         <v>338</v>
       </c>
-      <c r="B11" s="119" t="s">
+      <c r="B11" s="133" t="s">
         <v>404</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="122" t="s">
+      <c r="D11" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="128" t="s">
+      <c r="F11" s="131" t="s">
         <v>316</v>
       </c>
-      <c r="G11" s="119" t="s">
+      <c r="G11" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="124" t="s">
+      <c r="H11" s="127" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="124" t="s">
+      <c r="I11" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="114" t="s">
+      <c r="K11" s="134" t="s">
         <v>447</v>
       </c>
-      <c r="L11" s="114"/>
-      <c r="M11" s="114"/>
-      <c r="N11" s="114"/>
-      <c r="Z11" s="114" t="s">
+      <c r="L11" s="134"/>
+      <c r="M11" s="134"/>
+      <c r="N11" s="134"/>
+      <c r="Z11" s="134" t="s">
         <v>288</v>
       </c>
-      <c r="AA11" s="114"/>
-      <c r="AB11" s="114"/>
-      <c r="AC11" s="114"/>
+      <c r="AA11" s="134"/>
+      <c r="AB11" s="134"/>
+      <c r="AC11" s="134"/>
     </row>
     <row r="12" spans="1:29" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="128"/>
-      <c r="B12" s="119"/>
-      <c r="C12" s="122"/>
-      <c r="D12" s="122"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="124"/>
+      <c r="A12" s="131"/>
+      <c r="B12" s="133"/>
+      <c r="C12" s="132"/>
+      <c r="D12" s="132"/>
+      <c r="F12" s="131"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="127"/>
+      <c r="I12" s="127"/>
       <c r="K12" s="9" t="s">
         <v>488</v>
       </c>
@@ -5825,40 +5825,40 @@
       <c r="AC13" s="44"/>
     </row>
     <row r="14" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="128" t="s">
+      <c r="A14" s="131" t="s">
         <v>340</v>
       </c>
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="133" t="s">
         <v>402</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="122" t="s">
+      <c r="D14" s="132" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="114" t="s">
+      <c r="F14" s="134" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="114"/>
-      <c r="H14" s="114"/>
-      <c r="I14" s="114"/>
-      <c r="K14" s="129" t="s">
+      <c r="G14" s="134"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="134"/>
+      <c r="K14" s="137" t="s">
         <v>499</v>
       </c>
-      <c r="L14" s="130"/>
-      <c r="M14" s="131"/>
-      <c r="N14" s="130"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="139"/>
+      <c r="N14" s="138"/>
       <c r="Z14" s="44"/>
       <c r="AA14" s="92"/>
       <c r="AB14" s="44"/>
       <c r="AC14" s="44"/>
     </row>
     <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="128"/>
-      <c r="B15" s="119"/>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
+      <c r="A15" s="131"/>
+      <c r="B15" s="133"/>
+      <c r="C15" s="132"/>
+      <c r="D15" s="132"/>
       <c r="F15" s="9" t="s">
         <v>314</v>
       </c>
@@ -5871,10 +5871,10 @@
       <c r="I15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="129"/>
-      <c r="L15" s="130"/>
-      <c r="M15" s="131"/>
-      <c r="N15" s="130"/>
+      <c r="K15" s="137"/>
+      <c r="L15" s="138"/>
+      <c r="M15" s="139"/>
+      <c r="N15" s="138"/>
       <c r="Z15" s="44"/>
       <c r="AA15" s="64"/>
       <c r="AB15" s="64"/>
@@ -5961,21 +5961,21 @@
       <c r="I18" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="K18" s="159"/>
+      <c r="K18" s="122"/>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="126" t="s">
+      <c r="A19" s="128" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="126"/>
-      <c r="C19" s="126"/>
-      <c r="D19" s="126"/>
-      <c r="F19" s="114" t="s">
+      <c r="B19" s="128"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="128"/>
+      <c r="F19" s="134" t="s">
         <v>310</v>
       </c>
-      <c r="G19" s="114"/>
-      <c r="H19" s="114"/>
-      <c r="I19" s="114"/>
+      <c r="G19" s="134"/>
+      <c r="H19" s="134"/>
+      <c r="I19" s="134"/>
     </row>
     <row r="20" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
@@ -6252,12 +6252,12 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="126" t="s">
+      <c r="A36" s="128" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="126"/>
-      <c r="C36" s="126"/>
-      <c r="D36" s="126"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="128"/>
     </row>
     <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
@@ -6372,12 +6372,12 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="126" t="s">
+      <c r="A45" s="128" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="126"/>
-      <c r="C45" s="126"/>
-      <c r="D45" s="126"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="128"/>
+      <c r="D45" s="128"/>
     </row>
     <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="84" t="s">
@@ -6393,7 +6393,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>371</v>
       </c>
@@ -6422,12 +6422,12 @@
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A49" s="126" t="s">
+      <c r="A49" s="128" t="s">
         <v>253</v>
       </c>
-      <c r="B49" s="126"/>
-      <c r="C49" s="126"/>
-      <c r="D49" s="126"/>
+      <c r="B49" s="128"/>
+      <c r="C49" s="128"/>
+      <c r="D49" s="128"/>
     </row>
     <row r="50" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="80" t="s">
@@ -6484,12 +6484,12 @@
       </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A54" s="126" t="s">
+      <c r="A54" s="128" t="s">
         <v>254</v>
       </c>
-      <c r="B54" s="126"/>
-      <c r="C54" s="126"/>
-      <c r="D54" s="126"/>
+      <c r="B54" s="128"/>
+      <c r="C54" s="128"/>
+      <c r="D54" s="128"/>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" s="80" t="s">
@@ -6558,12 +6558,12 @@
       </c>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A60" s="126" t="s">
+      <c r="A60" s="128" t="s">
         <v>255</v>
       </c>
-      <c r="B60" s="126"/>
-      <c r="C60" s="126"/>
-      <c r="D60" s="126"/>
+      <c r="B60" s="128"/>
+      <c r="C60" s="128"/>
+      <c r="D60" s="128"/>
     </row>
     <row r="61" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="80" t="s">
@@ -6709,27 +6709,20 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="Z11:AC11"/>
+    <mergeCell ref="Z6:AC6"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="X6:X7"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="P6:P7"/>
     <mergeCell ref="Q6:Q7"/>
@@ -6746,22 +6739,29 @@
     <mergeCell ref="N14:N15"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:I6"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="Z11:AC11"/>
-    <mergeCell ref="Z6:AC6"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="X6:X7"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6772,7 +6772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E7B11-1527-417B-9532-F0F2C5A89902}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -6827,31 +6827,31 @@
       <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="129" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
       <c r="F2" s="18"/>
-      <c r="G2" s="125" t="s">
+      <c r="G2" s="130" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="130"/>
       <c r="L2" s="32"/>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="144" t="s">
+      <c r="B3" s="159" t="s">
         <v>203</v>
       </c>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="149" t="s">
         <v>131</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -6867,7 +6867,7 @@
       <c r="H3" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I3" s="132"/>
+      <c r="I3" s="150"/>
       <c r="J3" s="7" t="s">
         <v>168</v>
       </c>
@@ -6879,8 +6879,8 @@
       <c r="A4" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="145"/>
-      <c r="C4" s="135"/>
+      <c r="B4" s="160"/>
+      <c r="C4" s="153"/>
       <c r="D4" s="7" t="s">
         <v>305</v>
       </c>
@@ -6894,7 +6894,7 @@
       <c r="H4" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="I4" s="141"/>
+      <c r="I4" s="147"/>
       <c r="J4" s="7" t="s">
         <v>150</v>
       </c>
@@ -6906,8 +6906,8 @@
       <c r="A5" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="145"/>
-      <c r="C5" s="135"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="153"/>
       <c r="D5" s="7" t="s">
         <v>307</v>
       </c>
@@ -6921,7 +6921,7 @@
       <c r="H5" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="I5" s="141"/>
+      <c r="I5" s="147"/>
       <c r="J5" s="7" t="s">
         <v>161</v>
       </c>
@@ -6933,8 +6933,8 @@
       <c r="A6" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B6" s="145"/>
-      <c r="C6" s="135"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="153"/>
       <c r="D6" s="7" t="s">
         <v>308</v>
       </c>
@@ -6948,7 +6948,7 @@
       <c r="H6" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="I6" s="141"/>
+      <c r="I6" s="147"/>
       <c r="J6" s="7" t="s">
         <v>157</v>
       </c>
@@ -6960,8 +6960,8 @@
       <c r="A7" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="145"/>
-      <c r="C7" s="135"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="153"/>
       <c r="D7" s="7" t="s">
         <v>309</v>
       </c>
@@ -6975,7 +6975,7 @@
       <c r="H7" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="I7" s="141"/>
+      <c r="I7" s="147"/>
       <c r="J7" s="29" t="s">
         <v>144</v>
       </c>
@@ -6987,8 +6987,8 @@
       <c r="A8" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B8" s="145"/>
-      <c r="C8" s="139" t="s">
+      <c r="B8" s="160"/>
+      <c r="C8" s="145" t="s">
         <v>87</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -7004,7 +7004,7 @@
       <c r="H8" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I8" s="141"/>
+      <c r="I8" s="147"/>
       <c r="J8" s="7" t="s">
         <v>150</v>
       </c>
@@ -7019,7 +7019,7 @@
       <c r="B9" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="139"/>
+      <c r="C9" s="145"/>
       <c r="D9" s="7" t="s">
         <v>152</v>
       </c>
@@ -7033,7 +7033,7 @@
       <c r="H9" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="I9" s="141"/>
+      <c r="I9" s="147"/>
       <c r="J9" s="29" t="s">
         <v>209</v>
       </c>
@@ -7064,7 +7064,7 @@
       <c r="H10" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I10" s="146"/>
+      <c r="I10" s="151"/>
       <c r="J10" s="29" t="s">
         <v>144</v>
       </c>
@@ -7073,36 +7073,36 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="117" t="s">
+      <c r="A11" s="136" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="141" t="s">
+      <c r="B11" s="147" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="139" t="s">
+      <c r="C11" s="145" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="124" t="s">
+      <c r="D11" s="127" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="137">
+      <c r="E11" s="155">
         <v>3</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="114" t="s">
+      <c r="G11" s="134" t="s">
         <v>140</v>
       </c>
-      <c r="H11" s="114"/>
-      <c r="I11" s="114"/>
-      <c r="J11" s="114"/>
-      <c r="K11" s="114"/>
+      <c r="H11" s="134"/>
+      <c r="I11" s="134"/>
+      <c r="J11" s="134"/>
+      <c r="K11" s="134"/>
     </row>
     <row r="12" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="143"/>
-      <c r="B12" s="142"/>
-      <c r="C12" s="140"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="138"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="157"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="154"/>
+      <c r="E12" s="156"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
         <v>139</v>
@@ -7119,13 +7119,13 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="126" t="s">
+      <c r="A13" s="128" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="126"/>
-      <c r="C13" s="126"/>
-      <c r="D13" s="126"/>
-      <c r="E13" s="126"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="128"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
         <v>135</v>
@@ -7148,7 +7148,7 @@
       <c r="B14" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="134" t="s">
+      <c r="C14" s="149" t="s">
         <v>87</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -7179,7 +7179,7 @@
       <c r="B15" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="139"/>
+      <c r="C15" s="145"/>
       <c r="D15" s="11" t="s">
         <v>125</v>
       </c>
@@ -7202,40 +7202,40 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="117" t="s">
+      <c r="A16" s="136" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="147" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="139"/>
-      <c r="D16" s="124" t="s">
+      <c r="C16" s="145"/>
+      <c r="D16" s="127" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="147">
+      <c r="E16" s="148">
         <v>1</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="114" t="s">
+      <c r="G16" s="134" t="s">
         <v>118</v>
       </c>
-      <c r="H16" s="114"/>
-      <c r="I16" s="114"/>
-      <c r="J16" s="114"/>
-      <c r="K16" s="114"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="134"/>
+      <c r="J16" s="134"/>
+      <c r="K16" s="134"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="117"/>
-      <c r="B17" s="141"/>
-      <c r="C17" s="139"/>
-      <c r="D17" s="124"/>
-      <c r="E17" s="147"/>
+      <c r="A17" s="136"/>
+      <c r="B17" s="147"/>
+      <c r="C17" s="145"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="148"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
         <v>117</v>
       </c>
       <c r="H17" s="12"/>
-      <c r="I17" s="132"/>
+      <c r="I17" s="150"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7245,7 +7245,7 @@
       <c r="B18" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="139"/>
+      <c r="C18" s="145"/>
       <c r="D18" s="7" t="s">
         <v>114</v>
       </c>
@@ -7257,7 +7257,7 @@
         <v>113</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="141"/>
+      <c r="I18" s="147"/>
       <c r="K18"/>
     </row>
     <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7267,7 +7267,7 @@
       <c r="B19" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="139" t="s">
+      <c r="C19" s="145" t="s">
         <v>131</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -7281,7 +7281,7 @@
         <v>109</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="I19" s="141"/>
+      <c r="I19" s="147"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7291,7 +7291,7 @@
       <c r="B20" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="139"/>
+      <c r="C20" s="145"/>
       <c r="D20" s="7" t="s">
         <v>106</v>
       </c>
@@ -7303,7 +7303,7 @@
         <v>105</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="141"/>
+      <c r="I20" s="147"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -7313,7 +7313,7 @@
       <c r="B21" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="139"/>
+      <c r="C21" s="145"/>
       <c r="D21" s="7" t="s">
         <v>102</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>101</v>
       </c>
       <c r="H21" s="12"/>
-      <c r="I21" s="141"/>
+      <c r="I21" s="147"/>
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7335,7 +7335,7 @@
       <c r="B22" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="139"/>
+      <c r="C22" s="145"/>
       <c r="D22" s="7" t="s">
         <v>98</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>97</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="I22" s="141"/>
+      <c r="I22" s="147"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7357,7 +7357,7 @@
       <c r="B23" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="140"/>
+      <c r="C23" s="146"/>
       <c r="D23" s="7" t="s">
         <v>94</v>
       </c>
@@ -7369,26 +7369,26 @@
         <v>204</v>
       </c>
       <c r="H23" s="12"/>
-      <c r="I23" s="141"/>
+      <c r="I23" s="147"/>
       <c r="J23" s="7" t="s">
         <v>209</v>
       </c>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="126" t="s">
+      <c r="A24" s="128" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="126"/>
-      <c r="C24" s="126"/>
-      <c r="D24" s="126"/>
-      <c r="E24" s="126"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="4"/>
       <c r="G24" s="5" t="s">
         <v>93</v>
       </c>
       <c r="H24" s="12"/>
-      <c r="I24" s="141"/>
+      <c r="I24" s="147"/>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7398,7 +7398,7 @@
       <c r="B25" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="134" t="s">
+      <c r="C25" s="149" t="s">
         <v>428</v>
       </c>
       <c r="D25" s="63" t="s">
@@ -7412,7 +7412,7 @@
         <v>91</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="141"/>
+      <c r="I25" s="147"/>
       <c r="J25" s="12" t="s">
         <v>90</v>
       </c>
@@ -7425,7 +7425,7 @@
       <c r="B26" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="135"/>
+      <c r="C26" s="153"/>
       <c r="D26" s="44" t="s">
         <v>279</v>
       </c>
@@ -7435,7 +7435,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="15"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="141"/>
+      <c r="I26" s="147"/>
       <c r="J26" s="12"/>
       <c r="K26" s="25"/>
     </row>
@@ -7460,7 +7460,7 @@
         <v>84</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="141"/>
+      <c r="I27" s="147"/>
       <c r="K27" s="23"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -7480,7 +7480,7 @@
         <v>83</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="141"/>
+      <c r="I28" s="147"/>
       <c r="J28" s="7" t="s">
         <v>276</v>
       </c>
@@ -7492,7 +7492,7 @@
       <c r="G29" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I29" s="141"/>
+      <c r="I29" s="147"/>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -7501,7 +7501,7 @@
       <c r="G30" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I30" s="146"/>
+      <c r="I30" s="151"/>
       <c r="J30" s="7" t="s">
         <v>209</v>
       </c>
@@ -7510,13 +7510,13 @@
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="114" t="s">
+      <c r="G31" s="134" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="114"/>
-      <c r="I31" s="114"/>
-      <c r="J31" s="114"/>
-      <c r="K31" s="114"/>
+      <c r="H31" s="134"/>
+      <c r="I31" s="134"/>
+      <c r="J31" s="134"/>
+      <c r="K31" s="134"/>
     </row>
     <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
@@ -7527,7 +7527,7 @@
       <c r="H32" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="I32" s="132"/>
+      <c r="I32" s="150"/>
       <c r="J32" s="7" t="s">
         <v>77</v>
       </c>
@@ -7544,7 +7544,7 @@
       <c r="H33" s="98" t="s">
         <v>75</v>
       </c>
-      <c r="I33" s="133"/>
+      <c r="I33" s="152"/>
       <c r="J33" s="7" t="s">
         <v>74</v>
       </c>
@@ -7737,15 +7737,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="I17:I30"/>
-    <mergeCell ref="A24:E24"/>
     <mergeCell ref="G31:K31"/>
     <mergeCell ref="I32:I33"/>
     <mergeCell ref="A2:E2"/>
@@ -7762,6 +7753,15 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="I3:I10"/>
     <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="I17:I30"/>
+    <mergeCell ref="A24:E24"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7831,8 +7831,8 @@
       <c r="A2" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="148" t="s">
+      <c r="B2" s="162"/>
+      <c r="C2" s="161" t="s">
         <v>198</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -7845,7 +7845,7 @@
       <c r="G2" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="H2" s="167"/>
+      <c r="H2" s="165"/>
       <c r="I2" s="21" t="s">
         <v>134</v>
       </c>
@@ -7858,8 +7858,8 @@
       <c r="A3" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="B3" s="165"/>
-      <c r="C3" s="139"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="145"/>
       <c r="D3" s="7"/>
       <c r="E3" s="40" t="s">
         <v>197</v>
@@ -7868,7 +7868,7 @@
       <c r="G3" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="H3" s="168"/>
+      <c r="H3" s="166"/>
       <c r="I3" s="21">
         <v>0</v>
       </c>
@@ -7880,8 +7880,8 @@
       <c r="A4" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="165"/>
-      <c r="C4" s="139" t="s">
+      <c r="B4" s="163"/>
+      <c r="C4" s="145" t="s">
         <v>194</v>
       </c>
       <c r="D4" s="7"/>
@@ -7892,7 +7892,7 @@
       <c r="G4" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="H4" s="169"/>
+      <c r="H4" s="167"/>
       <c r="I4" s="38" t="s">
         <v>193</v>
       </c>
@@ -7907,8 +7907,8 @@
       <c r="A5" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B5" s="165"/>
-      <c r="C5" s="139"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="145"/>
       <c r="D5" s="7"/>
       <c r="E5" s="40" t="s">
         <v>182</v>
@@ -7920,7 +7920,7 @@
       <c r="A6" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B6" s="165"/>
+      <c r="B6" s="163"/>
       <c r="C6" s="22">
         <v>0</v>
       </c>
@@ -7935,8 +7935,8 @@
       <c r="A7" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="165"/>
-      <c r="C7" s="139" t="s">
+      <c r="B7" s="163"/>
+      <c r="C7" s="145" t="s">
         <v>194</v>
       </c>
       <c r="D7" s="7"/>
@@ -7951,8 +7951,8 @@
       <c r="A8" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B8" s="165"/>
-      <c r="C8" s="139"/>
+      <c r="B8" s="163"/>
+      <c r="C8" s="145"/>
       <c r="D8" s="7"/>
       <c r="E8" s="39" t="s">
         <v>182</v>
@@ -7968,7 +7968,7 @@
       <c r="A9" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B9" s="165"/>
+      <c r="B9" s="163"/>
       <c r="C9" s="22" t="s">
         <v>187</v>
       </c>
@@ -7985,7 +7985,7 @@
       <c r="A10" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B10" s="165"/>
+      <c r="B10" s="163"/>
       <c r="C10" s="22" t="s">
         <v>185</v>
       </c>
@@ -8002,7 +8002,7 @@
       <c r="A11" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="165"/>
+      <c r="B11" s="163"/>
       <c r="C11" s="21" t="s">
         <v>183</v>
       </c>
@@ -8021,7 +8021,7 @@
       <c r="A12" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="B12" s="166"/>
+      <c r="B12" s="164"/>
       <c r="C12" s="38" t="s">
         <v>180</v>
       </c>
@@ -8389,34 +8389,34 @@
       <c r="J1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="153" t="s">
+      <c r="K1" s="116" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="128" t="s">
         <v>461</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="G2" s="126" t="s">
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="G2" s="128" t="s">
         <v>482</v>
       </c>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="168" t="s">
         <v>467</v>
       </c>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="149" t="s">
         <v>194</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -8429,14 +8429,14 @@
       <c r="H3" s="74"/>
       <c r="I3" s="36"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="154"/>
+      <c r="K3" s="117"/>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="B4" s="150"/>
-      <c r="C4" s="135"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="153"/>
       <c r="D4" s="44" t="s">
         <v>468</v>
       </c>
@@ -8448,13 +8448,13 @@
       <c r="H4" s="46"/>
       <c r="I4" s="109"/>
       <c r="J4" s="44"/>
-      <c r="K4" s="155"/>
+      <c r="K4" s="118"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="B5" s="150"/>
+      <c r="B5" s="169"/>
       <c r="C5" s="76" t="s">
         <v>134</v>
       </c>
@@ -8469,7 +8469,7 @@
       <c r="H5" s="46"/>
       <c r="I5" s="109"/>
       <c r="J5" s="44"/>
-      <c r="K5" s="156"/>
+      <c r="K5" s="119"/>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -8495,19 +8495,19 @@
       <c r="K6" s="44"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="126" t="s">
+      <c r="A7" s="128" t="s">
         <v>481</v>
       </c>
-      <c r="B7" s="126"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
       <c r="F7" s="51"/>
       <c r="G7" s="42"/>
       <c r="H7" s="42"/>
       <c r="I7" s="109"/>
       <c r="J7" s="44"/>
-      <c r="K7" s="155"/>
+      <c r="K7" s="118"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -8528,7 +8528,7 @@
       <c r="H8" s="42"/>
       <c r="I8" s="109"/>
       <c r="J8" s="44"/>
-      <c r="K8" s="155"/>
+      <c r="K8" s="118"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -8551,7 +8551,7 @@
       <c r="H9" s="42"/>
       <c r="I9" s="76"/>
       <c r="J9" s="44"/>
-      <c r="K9" s="155"/>
+      <c r="K9" s="118"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
@@ -8564,7 +8564,7 @@
         <v>473</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="E10" s="161">
+      <c r="E10" s="124">
         <v>1</v>
       </c>
       <c r="F10" s="51"/>
@@ -8572,7 +8572,7 @@
       <c r="H10" s="42"/>
       <c r="I10" s="76"/>
       <c r="J10" s="44"/>
-      <c r="K10" s="155"/>
+      <c r="K10" s="118"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
@@ -8585,7 +8585,7 @@
       <c r="H11" s="46"/>
       <c r="I11" s="47"/>
       <c r="J11" s="44"/>
-      <c r="K11" s="155"/>
+      <c r="K11" s="118"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
@@ -8598,7 +8598,7 @@
       <c r="H12" s="44"/>
       <c r="I12" s="47"/>
       <c r="J12" s="44"/>
-      <c r="K12" s="155"/>
+      <c r="K12" s="118"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="42"/>
@@ -8618,13 +8618,13 @@
       <c r="B14" s="110"/>
       <c r="C14" s="108"/>
       <c r="D14" s="108"/>
-      <c r="E14" s="151"/>
+      <c r="E14" s="114"/>
       <c r="F14" s="51"/>
       <c r="G14" s="108"/>
       <c r="H14" s="108"/>
       <c r="I14" s="108"/>
       <c r="J14" s="108"/>
-      <c r="K14" s="157"/>
+      <c r="K14" s="120"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="42"/>
@@ -8711,12 +8711,12 @@
       <c r="B23" s="23"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="152"/>
+      <c r="E23" s="115"/>
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
-      <c r="K23" s="158"/>
+      <c r="K23" s="121"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" s="36"/>
@@ -9053,37 +9053,37 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="162" t="s">
+      <c r="A2" s="125" t="s">
         <v>221</v>
       </c>
-      <c r="F2" s="162" t="s">
+      <c r="F2" s="125" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="122" t="s">
         <v>247</v>
       </c>
-      <c r="F3" s="159" t="s">
+      <c r="F3" s="122" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="159" t="s">
+      <c r="A4" s="122" t="s">
         <v>248</v>
       </c>
-      <c r="F4" s="163" t="s">
+      <c r="F4" s="126" t="s">
         <v>217</v>
       </c>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160" t="s">
+      <c r="G4" s="123"/>
+      <c r="H4" s="123" t="s">
         <v>218</v>
       </c>
-      <c r="I4" s="160"/>
-      <c r="J4" s="160"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="159" t="s">
+      <c r="A5" s="122" t="s">
         <v>249</v>
       </c>
       <c r="F5" s="51"/>
@@ -9092,12 +9092,12 @@
       <c r="I5" s="51"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="163" t="s">
+      <c r="A6" s="126" t="s">
         <v>226</v>
       </c>
-      <c r="B6" s="160"/>
-      <c r="C6" s="160"/>
-      <c r="D6" s="160"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
       <c r="F6" s="51"/>
       <c r="G6" s="51"/>
       <c r="H6" s="51"/>
@@ -9128,7 +9128,7 @@
       <c r="I8" s="53"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="162" t="s">
+      <c r="A9" s="125" t="s">
         <v>250</v>
       </c>
       <c r="F9" s="51"/>
@@ -9137,17 +9137,17 @@
       <c r="I9" s="51"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="159" t="s">
+      <c r="A10" s="122" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="163" t="s">
+      <c r="A11" s="126" t="s">
         <v>252</v>
       </c>
-      <c r="B11" s="160"/>
-      <c r="C11" s="160"/>
-      <c r="D11" s="160"/>
+      <c r="B11" s="123"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="123"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
started to codify component sizes.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CK.DESKTOP-BR5NVLN\Documents\Git Repositories\Creative\materials_and_crafting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Git Repositories\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE016D19-7C21-40AC-A5B5-95BE3F376A74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93653994-D13D-4FF2-9EDA-3B52A7344779}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
@@ -25,14 +25,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -2041,9 +2033,6 @@
     <t>Handaxe (1d6 S)</t>
   </si>
   <si>
-    <t>1 haft (1.5 lbs)</t>
-  </si>
-  <si>
     <t>Handstaff (1d6 B)</t>
   </si>
   <si>
@@ -2944,79 +2933,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>10 needle blades (0.1 lb each)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 folding fan (1 lb)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 crescent blade (0.5 lb)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 haft (1 lb)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1 straight blade
-(1.33 lbs)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 one-handed hilt (0.66 lb)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>1 crescent blade (1.33 lbs)</t>
     </r>
     <r>
@@ -3029,195 +2945,6 @@
       </rPr>
       <t xml:space="preserve">
 1 one-handed hilt (0.66 lb)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 hammer head (0.5 lb)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 haft (1 lb)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 curved blade (0.5 lb)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 haft (1 lb)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 axe head (0.5 lb)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 haft (1.25 lb)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 straight or curved blade (0.5 lb)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 one-handed hilt (0.5 lb)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 thick shaft (1.25 lbs)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3 weights (0.25 lbs. each)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1 sickle (1.5 lbs) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">OR </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>kama (1.5 lbs)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 rope (0.5 lb)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 straight blade (0.5 lb)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 carved handle (0.5 lb)</t>
     </r>
   </si>
   <si>
@@ -3387,30 +3114,6 @@
   <si>
     <t>1 wooden plate (4 lbs) OR 1 metal plate (4 lbs)
 1 metal strip (2 lbs)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 dagger (1 lbs)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 rope (0.5 lb)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -4095,12 +3798,301 @@
     <t>1 length of metal wire
 1 sheathe of soft insulative metal</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 straight blade (0.5 lb, 10")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1 carved handle (0.5 lb, 5")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 dagger (1 lbs)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1 rope (0.5 lb, 5')</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1 sickle (1.5 lbs) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">OR </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">kama (1.5 lbs) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1 rope (0.5 lb, 5')</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 thick shaft (1.25 lbs, 15")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3 weights (0.25 lbs. each)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 straight or curved blade (0.5 lb, 10")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1 one-handed hilt (0.5 lb, 5")</t>
+    </r>
+  </si>
+  <si>
+    <t>1 haft (1.5 lbs, 20")</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 curved blade (0.5 lb, 5")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1 haft (1 lb, 10")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 axe head (0.5 lb, ?")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1 haft (1.25 lb, ?")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 hammer head (0.5 lb, 2")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1 haft (1 lb, 10")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1 straight blade
+(1.33 lbs, 15")
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 one-handed hilt (0.66 lb, 5")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 crescent blade (0.5 lb, 15")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1 haft (1 lb, 5")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10 needle blades (0.1 lb each, 5")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1 folding fan (1 lb)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4687,59 +4679,80 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4750,44 +4763,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5132,11 +5124,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
   <dimension ref="A1:AC70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="7" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="4" customWidth="1"/>
@@ -5164,7 +5156,7 @@
     <col min="28" max="29" width="10" style="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5191,7 +5183,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>1</v>
@@ -5239,62 +5231,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+    <row r="2" spans="1:29" ht="15" customHeight="1">
+      <c r="A2" s="143" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="F2" s="130" t="s">
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="F2" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="K2" s="130" t="s">
-        <v>448</v>
-      </c>
-      <c r="L2" s="130"/>
-      <c r="M2" s="130"/>
-      <c r="N2" s="130"/>
-      <c r="P2" s="140" t="s">
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="K2" s="138" t="s">
+        <v>436</v>
+      </c>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
+      <c r="P2" s="127" t="s">
         <v>215</v>
       </c>
-      <c r="Q2" s="141" t="s">
+      <c r="Q2" s="129" t="s">
         <v>258</v>
       </c>
-      <c r="R2" s="135" t="s">
+      <c r="R2" s="131" t="s">
         <v>228</v>
       </c>
-      <c r="S2" s="135" t="s">
+      <c r="S2" s="131" t="s">
         <v>62</v>
       </c>
-      <c r="U2" s="140" t="s">
+      <c r="U2" s="127" t="s">
         <v>233</v>
       </c>
-      <c r="V2" s="143" t="s">
+      <c r="V2" s="134" t="s">
         <v>270</v>
       </c>
-      <c r="W2" s="135" t="s">
+      <c r="W2" s="131" t="s">
         <v>228</v>
       </c>
-      <c r="X2" s="135" t="s">
+      <c r="X2" s="131" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" s="142" t="s">
+      <c r="Z2" s="133" t="s">
         <v>284</v>
       </c>
-      <c r="AA2" s="142"/>
-      <c r="AB2" s="142"/>
-      <c r="AC2" s="142"/>
-    </row>
-    <row r="3" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+      <c r="AA2" s="133"/>
+      <c r="AB2" s="133"/>
+      <c r="AC2" s="133"/>
+    </row>
+    <row r="3" spans="1:29" ht="75">
       <c r="A3" s="9" t="s">
         <v>330</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>409</v>
+        <v>494</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>7</v>
@@ -5315,23 +5307,23 @@
         <v>8</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="L3" s="64" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="M3" s="79">
         <v>0.06</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="P3" s="136"/>
-      <c r="Q3" s="132"/>
-      <c r="R3" s="132"/>
-      <c r="S3" s="132"/>
-      <c r="U3" s="136"/>
-      <c r="V3" s="133"/>
-      <c r="W3" s="144"/>
-      <c r="X3" s="144"/>
+      <c r="P3" s="128"/>
+      <c r="Q3" s="130"/>
+      <c r="R3" s="130"/>
+      <c r="S3" s="130"/>
+      <c r="U3" s="128"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="136"/>
+      <c r="X3" s="136"/>
       <c r="Z3" s="10" t="s">
         <v>285</v>
       </c>
@@ -5339,12 +5331,12 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="75">
       <c r="A4" s="10" t="s">
         <v>331</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>427</v>
+        <v>495</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>31</v>
@@ -5365,10 +5357,10 @@
         <v>14</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="L4" s="64" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="M4" s="79">
         <v>0.05</v>
@@ -5405,12 +5397,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="75" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>332</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>408</v>
+        <v>496</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>17</v>
@@ -5431,10 +5423,10 @@
         <v>16</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="L5" s="64" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="M5" s="45">
         <v>0.06</v>
@@ -5473,67 +5465,67 @@
       <c r="AB5" s="77"/>
       <c r="AC5" s="77"/>
     </row>
-    <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="131" t="s">
+    <row r="6" spans="1:29" ht="15" customHeight="1">
+      <c r="A6" s="144" t="s">
         <v>333</v>
       </c>
-      <c r="B6" s="127" t="s">
-        <v>407</v>
-      </c>
-      <c r="C6" s="132" t="s">
+      <c r="B6" s="137" t="s">
+        <v>497</v>
+      </c>
+      <c r="C6" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="132" t="s">
+      <c r="D6" s="130" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="134" t="s">
+      <c r="F6" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="134"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="K6" s="134" t="s">
-        <v>450</v>
-      </c>
-      <c r="L6" s="134"/>
-      <c r="M6" s="134"/>
-      <c r="N6" s="134"/>
-      <c r="P6" s="136" t="s">
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="K6" s="132" t="s">
+        <v>438</v>
+      </c>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="P6" s="128" t="s">
         <v>225</v>
       </c>
-      <c r="Q6" s="127" t="s">
+      <c r="Q6" s="137" t="s">
         <v>261</v>
       </c>
-      <c r="R6" s="132" t="s">
+      <c r="R6" s="130" t="s">
         <v>229</v>
       </c>
-      <c r="S6" s="132" t="s">
+      <c r="S6" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="U6" s="136" t="s">
+      <c r="U6" s="128" t="s">
         <v>236</v>
       </c>
-      <c r="V6" s="133" t="s">
+      <c r="V6" s="135" t="s">
         <v>265</v>
       </c>
-      <c r="W6" s="132" t="s">
+      <c r="W6" s="130" t="s">
         <v>229</v>
       </c>
-      <c r="X6" s="132" t="s">
+      <c r="X6" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="Z6" s="134" t="s">
+      <c r="Z6" s="132" t="s">
         <v>294</v>
       </c>
-      <c r="AA6" s="134"/>
-      <c r="AB6" s="134"/>
-      <c r="AC6" s="134"/>
-    </row>
-    <row r="7" spans="1:29" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="131"/>
-      <c r="B7" s="127"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
+      <c r="AA6" s="132"/>
+      <c r="AB6" s="132"/>
+      <c r="AC6" s="132"/>
+    </row>
+    <row r="7" spans="1:29" ht="120" customHeight="1">
+      <c r="A7" s="144"/>
+      <c r="B7" s="137"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
       <c r="F7" s="9" t="s">
         <v>319</v>
       </c>
@@ -5547,23 +5539,23 @@
         <v>21</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="L7" s="64" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="M7" s="45">
         <v>0.08</v>
       </c>
       <c r="N7" s="103"/>
-      <c r="P7" s="136"/>
-      <c r="Q7" s="132"/>
-      <c r="R7" s="132"/>
-      <c r="S7" s="132"/>
-      <c r="U7" s="136"/>
-      <c r="V7" s="133"/>
-      <c r="W7" s="132"/>
-      <c r="X7" s="132"/>
+      <c r="P7" s="128"/>
+      <c r="Q7" s="130"/>
+      <c r="R7" s="130"/>
+      <c r="S7" s="130"/>
+      <c r="U7" s="128"/>
+      <c r="V7" s="135"/>
+      <c r="W7" s="130"/>
+      <c r="X7" s="130"/>
       <c r="Z7" s="10" t="s">
         <v>295</v>
       </c>
@@ -5573,12 +5565,12 @@
       <c r="AB7" s="44"/>
       <c r="AC7" s="44"/>
     </row>
-    <row r="8" spans="1:29" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="75" customHeight="1" thickBot="1">
       <c r="A8" s="10" t="s">
         <v>334</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>406</v>
+        <v>498</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>7</v>
@@ -5599,10 +5591,10 @@
         <v>23</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="L8" s="64" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
       <c r="M8" s="45">
         <v>0.08</v>
@@ -5639,12 +5631,12 @@
       <c r="AB8" s="64"/>
       <c r="AC8" s="64"/>
     </row>
-    <row r="9" spans="1:29" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="195" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>335</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>405</v>
+        <v>501</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>17</v>
@@ -5665,10 +5657,10 @@
         <v>26</v>
       </c>
       <c r="K9" s="104" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="L9" s="64" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="M9" s="45">
         <v>0.08</v>
@@ -5683,12 +5675,12 @@
       <c r="AB9" s="64"/>
       <c r="AC9" s="64"/>
     </row>
-    <row r="10" spans="1:29" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="90">
       <c r="A10" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B10" s="88" t="s">
-        <v>336</v>
+        <v>499</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>31</v>
@@ -5709,10 +5701,10 @@
         <v>8</v>
       </c>
       <c r="K10" s="104" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="L10" s="64" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="M10" s="79">
         <v>0.08</v>
@@ -5724,58 +5716,58 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="131" t="s">
-        <v>338</v>
-      </c>
-      <c r="B11" s="133" t="s">
-        <v>404</v>
-      </c>
-      <c r="C11" s="132" t="s">
+    <row r="11" spans="1:29" ht="15" customHeight="1">
+      <c r="A11" s="144" t="s">
+        <v>337</v>
+      </c>
+      <c r="B11" s="135" t="s">
+        <v>500</v>
+      </c>
+      <c r="C11" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="132" t="s">
+      <c r="D11" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="131" t="s">
+      <c r="F11" s="144" t="s">
         <v>316</v>
       </c>
-      <c r="G11" s="133" t="s">
+      <c r="G11" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="127" t="s">
+      <c r="H11" s="137" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="127" t="s">
+      <c r="I11" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="134" t="s">
-        <v>447</v>
-      </c>
-      <c r="L11" s="134"/>
-      <c r="M11" s="134"/>
-      <c r="N11" s="134"/>
-      <c r="Z11" s="134" t="s">
+      <c r="K11" s="132" t="s">
+        <v>435</v>
+      </c>
+      <c r="L11" s="132"/>
+      <c r="M11" s="132"/>
+      <c r="N11" s="132"/>
+      <c r="Z11" s="132" t="s">
         <v>288</v>
       </c>
-      <c r="AA11" s="134"/>
-      <c r="AB11" s="134"/>
-      <c r="AC11" s="134"/>
-    </row>
-    <row r="12" spans="1:29" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="131"/>
-      <c r="B12" s="133"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="127"/>
-      <c r="I12" s="127"/>
+      <c r="AA11" s="132"/>
+      <c r="AB11" s="132"/>
+      <c r="AC11" s="132"/>
+    </row>
+    <row r="12" spans="1:29" ht="75" customHeight="1">
+      <c r="A12" s="144"/>
+      <c r="B12" s="135"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="F12" s="144"/>
+      <c r="G12" s="135"/>
+      <c r="H12" s="137"/>
+      <c r="I12" s="137"/>
       <c r="K12" s="9" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="N12" s="4"/>
       <c r="Z12" s="10" t="s">
@@ -5787,12 +5779,12 @@
       <c r="AB12" s="44"/>
       <c r="AC12" s="44"/>
     </row>
-    <row r="13" spans="1:29" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="210" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>403</v>
+        <v>502</v>
       </c>
       <c r="C13" s="69" t="s">
         <v>31</v>
@@ -5813,10 +5805,10 @@
         <v>33</v>
       </c>
       <c r="K13" s="106" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="Z13" s="10" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="AA13" s="66" t="s">
         <v>290</v>
@@ -5824,41 +5816,41 @@
       <c r="AB13" s="44"/>
       <c r="AC13" s="44"/>
     </row>
-    <row r="14" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="131" t="s">
-        <v>340</v>
-      </c>
-      <c r="B14" s="133" t="s">
-        <v>402</v>
-      </c>
-      <c r="C14" s="132" t="s">
+    <row r="14" spans="1:29" ht="15" customHeight="1">
+      <c r="A14" s="144" t="s">
+        <v>339</v>
+      </c>
+      <c r="B14" s="135" t="s">
+        <v>398</v>
+      </c>
+      <c r="C14" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="132" t="s">
+      <c r="D14" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="134" t="s">
+      <c r="F14" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="134"/>
-      <c r="H14" s="134"/>
-      <c r="I14" s="134"/>
-      <c r="K14" s="137" t="s">
-        <v>499</v>
-      </c>
-      <c r="L14" s="138"/>
-      <c r="M14" s="139"/>
-      <c r="N14" s="138"/>
+      <c r="G14" s="132"/>
+      <c r="H14" s="132"/>
+      <c r="I14" s="132"/>
+      <c r="K14" s="140" t="s">
+        <v>487</v>
+      </c>
+      <c r="L14" s="141"/>
+      <c r="M14" s="142"/>
+      <c r="N14" s="141"/>
       <c r="Z14" s="44"/>
       <c r="AA14" s="92"/>
       <c r="AB14" s="44"/>
       <c r="AC14" s="44"/>
     </row>
-    <row r="15" spans="1:29" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="131"/>
-      <c r="B15" s="133"/>
-      <c r="C15" s="132"/>
-      <c r="D15" s="132"/>
+    <row r="15" spans="1:29" ht="90">
+      <c r="A15" s="144"/>
+      <c r="B15" s="135"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="130"/>
       <c r="F15" s="9" t="s">
         <v>314</v>
       </c>
@@ -5871,21 +5863,21 @@
       <c r="I15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="137"/>
-      <c r="L15" s="138"/>
-      <c r="M15" s="139"/>
-      <c r="N15" s="138"/>
+      <c r="K15" s="140"/>
+      <c r="L15" s="141"/>
+      <c r="M15" s="142"/>
+      <c r="N15" s="141"/>
       <c r="Z15" s="44"/>
       <c r="AA15" s="64"/>
       <c r="AB15" s="64"/>
       <c r="AC15" s="64"/>
     </row>
-    <row r="16" spans="1:29" ht="285" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="285">
       <c r="A16" s="85" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B16" s="71" t="s">
-        <v>401</v>
+        <v>503</v>
       </c>
       <c r="C16" s="69" t="s">
         <v>17</v>
@@ -5906,15 +5898,15 @@
         <v>39</v>
       </c>
       <c r="K16" s="106" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="165" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>400</v>
+        <v>504</v>
       </c>
       <c r="C17" s="69" t="s">
         <v>28</v>
@@ -5936,12 +5928,12 @@
       </c>
       <c r="K17" s="106"/>
     </row>
-    <row r="18" spans="1:16" ht="195" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="195">
       <c r="A18" s="65" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>399</v>
+        <v>505</v>
       </c>
       <c r="C18" s="69" t="s">
         <v>17</v>
@@ -5963,26 +5955,26 @@
       </c>
       <c r="K18" s="122"/>
     </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="128" t="s">
+    <row r="19" spans="1:16" ht="15" customHeight="1">
+      <c r="A19" s="139" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="128"/>
-      <c r="C19" s="128"/>
-      <c r="D19" s="128"/>
-      <c r="F19" s="134" t="s">
+      <c r="B19" s="139"/>
+      <c r="C19" s="139"/>
+      <c r="D19" s="139"/>
+      <c r="F19" s="132" t="s">
         <v>310</v>
       </c>
-      <c r="G19" s="134"/>
-      <c r="H19" s="134"/>
-      <c r="I19" s="134"/>
-    </row>
-    <row r="20" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="G19" s="132"/>
+      <c r="H19" s="132"/>
+      <c r="I19" s="132"/>
+    </row>
+    <row r="20" spans="1:16" ht="75">
       <c r="A20" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C20" s="69" t="s">
         <v>49</v>
@@ -5991,24 +5983,24 @@
         <v>8</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="G20" s="89" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
       <c r="C21" s="69" t="s">
         <v>49</v>
@@ -6017,10 +6009,10 @@
         <v>43</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="G21" s="90" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>61</v>
@@ -6031,12 +6023,12 @@
       <c r="K21" s="93"/>
       <c r="P21" s="93"/>
     </row>
-    <row r="22" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="75">
       <c r="A22" s="10" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C22" s="69" t="s">
         <v>50</v>
@@ -6045,10 +6037,10 @@
         <v>8</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="G22" s="90" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>65</v>
@@ -6057,12 +6049,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="60.75" thickBot="1">
       <c r="A23" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C23" s="69" t="s">
         <v>51</v>
@@ -6071,10 +6063,10 @@
         <v>52</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
       <c r="G23" s="91" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="H23" s="17" t="s">
         <v>27</v>
@@ -6083,12 +6075,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="60">
       <c r="A24" s="10" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C24" s="69" t="s">
         <v>53</v>
@@ -6097,12 +6089,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="60">
       <c r="A25" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C25" s="69" t="s">
         <v>50</v>
@@ -6111,12 +6103,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="60">
       <c r="A26" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C26" s="69" t="s">
         <v>54</v>
@@ -6125,12 +6117,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="30">
       <c r="A27" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C27" s="69" t="s">
         <v>50</v>
@@ -6139,12 +6131,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="30">
       <c r="A28" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C28" s="69" t="s">
         <v>51</v>
@@ -6153,9 +6145,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="30">
       <c r="A29" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B29" s="88" t="s">
         <v>56</v>
@@ -6167,12 +6159,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="60">
       <c r="A30" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C30" s="69" t="s">
         <v>50</v>
@@ -6181,12 +6173,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="30">
       <c r="A31" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C31" s="69" t="s">
         <v>58</v>
@@ -6195,12 +6187,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="30" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C32" s="69" t="s">
         <v>59</v>
@@ -6209,12 +6201,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="45.75" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B33" s="87" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C33" s="69" t="s">
         <v>51</v>
@@ -6223,26 +6215,26 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="45">
       <c r="A34" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="B34" s="87" t="s">
+        <v>397</v>
+      </c>
+      <c r="C34" s="69" t="s">
         <v>354</v>
-      </c>
-      <c r="B34" s="87" t="s">
-        <v>398</v>
-      </c>
-      <c r="C34" s="69" t="s">
-        <v>355</v>
       </c>
       <c r="D34" s="69" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="45">
       <c r="A35" s="65" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C35" s="69" t="s">
         <v>51</v>
@@ -6251,20 +6243,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="128" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="139" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="128"/>
-      <c r="C36" s="128"/>
-      <c r="D36" s="128"/>
-    </row>
-    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B36" s="139"/>
+      <c r="C36" s="139"/>
+      <c r="D36" s="139"/>
+    </row>
+    <row r="37" spans="1:4" ht="45">
       <c r="A37" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C37" s="69" t="s">
         <v>61</v>
@@ -6273,12 +6265,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="45">
       <c r="A38" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C38" s="69" t="s">
         <v>63</v>
@@ -6287,12 +6279,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="45" customHeight="1">
       <c r="A39" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C39" s="69" t="s">
         <v>63</v>
@@ -6301,12 +6293,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="45">
       <c r="A40" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C40" s="71" t="s">
         <v>304</v>
@@ -6315,12 +6307,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="45" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C41" s="71" t="s">
         <v>303</v>
@@ -6329,12 +6321,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="45">
       <c r="A42" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C42" s="69" t="s">
         <v>61</v>
@@ -6343,12 +6335,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="45">
       <c r="A43" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C43" s="69" t="s">
         <v>65</v>
@@ -6357,12 +6349,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="30">
       <c r="A44" s="65" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C44" s="69" t="s">
         <v>10</v>
@@ -6371,20 +6363,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="128" t="s">
+    <row r="45" spans="1:4">
+      <c r="A45" s="139" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="128"/>
-      <c r="C45" s="128"/>
-      <c r="D45" s="128"/>
-    </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B45" s="139"/>
+      <c r="C45" s="139"/>
+      <c r="D45" s="139"/>
+    </row>
+    <row r="46" spans="1:4" ht="45">
       <c r="A46" s="84" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B46" s="71" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C46" s="71" t="s">
         <v>282</v>
@@ -6393,26 +6385,26 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="90" customHeight="1">
       <c r="A47" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C47" s="71" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D47" s="69" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="60" customHeight="1">
       <c r="A48" s="65" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C48" s="71" t="s">
         <v>281</v>
@@ -6421,17 +6413,17 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A49" s="128" t="s">
+    <row r="49" spans="1:29">
+      <c r="A49" s="139" t="s">
         <v>253</v>
       </c>
-      <c r="B49" s="128"/>
-      <c r="C49" s="128"/>
-      <c r="D49" s="128"/>
-    </row>
-    <row r="50" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="139"/>
+      <c r="C49" s="139"/>
+      <c r="D49" s="139"/>
+    </row>
+    <row r="50" spans="1:29" ht="30">
       <c r="A50" s="80" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="B50" s="58"/>
       <c r="C50" s="58" t="s">
@@ -6441,26 +6433,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" ht="30">
       <c r="A51" s="81" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="B51" s="67" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="D51" s="58" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29" ht="60">
       <c r="A52" s="81" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="B52" s="60" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="C52" s="58" t="s">
         <v>51</v>
@@ -6469,12 +6461,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29" ht="30" customHeight="1">
       <c r="A53" s="83" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="B53" s="60" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
       <c r="C53" s="58" t="s">
         <v>28</v>
@@ -6483,20 +6475,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A54" s="128" t="s">
+    <row r="54" spans="1:29">
+      <c r="A54" s="139" t="s">
         <v>254</v>
       </c>
-      <c r="B54" s="128"/>
-      <c r="C54" s="128"/>
-      <c r="D54" s="128"/>
-    </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B54" s="139"/>
+      <c r="C54" s="139"/>
+      <c r="D54" s="139"/>
+    </row>
+    <row r="55" spans="1:29">
       <c r="A55" s="80" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="B55" s="58" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="C55" s="58" t="s">
         <v>7</v>
@@ -6505,9 +6497,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29" ht="30">
       <c r="A56" s="81" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="B56" s="58"/>
       <c r="C56" s="58" t="s">
@@ -6517,9 +6509,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29" ht="45">
       <c r="A57" s="81" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="B57" s="58"/>
       <c r="C57" s="58" t="s">
@@ -6529,12 +6521,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29" ht="60">
       <c r="A58" s="81" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="B58" s="60" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="C58" s="58" t="s">
         <v>61</v>
@@ -6543,59 +6535,59 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29" ht="60">
       <c r="A59" s="81" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="B59" s="60" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="C59" s="58" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="D59" s="58" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A60" s="128" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29">
+      <c r="A60" s="139" t="s">
         <v>255</v>
       </c>
-      <c r="B60" s="128"/>
-      <c r="C60" s="128"/>
-      <c r="D60" s="128"/>
-    </row>
-    <row r="61" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+      <c r="B60" s="139"/>
+      <c r="C60" s="139"/>
+      <c r="D60" s="139"/>
+    </row>
+    <row r="61" spans="1:29" ht="45">
       <c r="A61" s="80" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
       <c r="B61" s="60" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="C61" s="58" t="s">
         <v>51</v>
       </c>
       <c r="D61" s="58"/>
     </row>
-    <row r="62" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29" ht="45">
       <c r="A62" s="107" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="B62" s="105"/>
       <c r="C62" s="58" t="s">
         <v>10</v>
       </c>
       <c r="D62" s="58" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
       <c r="M62" s="99"/>
       <c r="AA62" s="95"/>
       <c r="AB62" s="95"/>
       <c r="AC62" s="95"/>
     </row>
-    <row r="63" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29" ht="45">
       <c r="A63" s="107" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="B63" s="105"/>
       <c r="C63" s="58" t="s">
@@ -6607,9 +6599,9 @@
       <c r="AB63" s="95"/>
       <c r="AC63" s="95"/>
     </row>
-    <row r="64" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29" ht="45">
       <c r="A64" s="107" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
       <c r="B64" s="105"/>
       <c r="C64" s="58" t="s">
@@ -6621,13 +6613,13 @@
       <c r="AB64" s="95"/>
       <c r="AC64" s="95"/>
     </row>
-    <row r="65" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" ht="60">
       <c r="A65" s="107" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="B65" s="105"/>
       <c r="C65" s="58" t="s">
-        <v>496</v>
+        <v>484</v>
       </c>
       <c r="D65" s="58"/>
       <c r="M65" s="99"/>
@@ -6635,7 +6627,7 @@
       <c r="AB65" s="95"/>
       <c r="AC65" s="95"/>
     </row>
-    <row r="66" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" ht="15" customHeight="1">
       <c r="A66" s="96" t="s">
         <v>256</v>
       </c>
@@ -6647,7 +6639,7 @@
       <c r="AB66" s="95"/>
       <c r="AC66" s="95"/>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29">
       <c r="A67" s="107" t="s">
         <v>266</v>
       </c>
@@ -6661,7 +6653,7 @@
       <c r="AB67" s="95"/>
       <c r="AC67" s="95"/>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29">
       <c r="A68" s="107" t="s">
         <v>257</v>
       </c>
@@ -6675,32 +6667,32 @@
       <c r="AB68" s="95"/>
       <c r="AC68" s="95"/>
     </row>
-    <row r="69" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" ht="15" customHeight="1">
       <c r="A69" s="107" t="s">
         <v>267</v>
       </c>
       <c r="B69" s="105"/>
       <c r="C69" s="58"/>
       <c r="D69" s="58" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="M69" s="99"/>
       <c r="AA69" s="95"/>
       <c r="AB69" s="95"/>
       <c r="AC69" s="95"/>
     </row>
-    <row r="70" spans="1:29" ht="225" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:29" ht="225" customHeight="1" thickBot="1">
       <c r="A70" s="82" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="B70" s="61" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="C70" s="59" t="s">
         <v>10</v>
       </c>
       <c r="D70" s="59" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="M70" s="99"/>
       <c r="AA70" s="95"/>
@@ -6709,6 +6701,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A14:A15"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
@@ -6725,43 +6754,6 @@
     <mergeCell ref="X6:X7"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6776,7 +6768,7 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28" style="4" customWidth="1"/>
     <col min="2" max="2" width="20" style="4" customWidth="1"/>
@@ -6792,7 +6784,7 @@
     <col min="12" max="12" width="10" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>178</v>
       </c>
@@ -6826,32 +6818,32 @@
       </c>
       <c r="L1" s="33"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="143" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
       <c r="F2" s="18"/>
-      <c r="G2" s="130" t="s">
+      <c r="G2" s="138" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130"/>
-      <c r="K2" s="130"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
       <c r="L2" s="32"/>
     </row>
-    <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="45" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="159" t="s">
+      <c r="B3" s="157" t="s">
         <v>203</v>
       </c>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="147" t="s">
         <v>131</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -6867,7 +6859,7 @@
       <c r="H3" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I3" s="150"/>
+      <c r="I3" s="145"/>
       <c r="J3" s="7" t="s">
         <v>168</v>
       </c>
@@ -6875,12 +6867,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="60">
       <c r="A4" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="160"/>
-      <c r="C4" s="153"/>
+      <c r="B4" s="158"/>
+      <c r="C4" s="148"/>
       <c r="D4" s="7" t="s">
         <v>305</v>
       </c>
@@ -6894,7 +6886,7 @@
       <c r="H4" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="I4" s="147"/>
+      <c r="I4" s="154"/>
       <c r="J4" s="7" t="s">
         <v>150</v>
       </c>
@@ -6902,12 +6894,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="45">
       <c r="A5" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="160"/>
-      <c r="C5" s="153"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="148"/>
       <c r="D5" s="7" t="s">
         <v>307</v>
       </c>
@@ -6921,7 +6913,7 @@
       <c r="H5" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="I5" s="147"/>
+      <c r="I5" s="154"/>
       <c r="J5" s="7" t="s">
         <v>161</v>
       </c>
@@ -6929,12 +6921,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="60" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B6" s="160"/>
-      <c r="C6" s="153"/>
+      <c r="B6" s="158"/>
+      <c r="C6" s="148"/>
       <c r="D6" s="7" t="s">
         <v>308</v>
       </c>
@@ -6948,7 +6940,7 @@
       <c r="H6" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="I6" s="147"/>
+      <c r="I6" s="154"/>
       <c r="J6" s="7" t="s">
         <v>157</v>
       </c>
@@ -6956,12 +6948,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="160"/>
-      <c r="C7" s="153"/>
+      <c r="B7" s="158"/>
+      <c r="C7" s="148"/>
       <c r="D7" s="7" t="s">
         <v>309</v>
       </c>
@@ -6975,7 +6967,7 @@
       <c r="H7" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="I7" s="147"/>
+      <c r="I7" s="154"/>
       <c r="J7" s="29" t="s">
         <v>144</v>
       </c>
@@ -6983,12 +6975,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="75" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B8" s="160"/>
-      <c r="C8" s="145" t="s">
+      <c r="B8" s="158"/>
+      <c r="C8" s="152" t="s">
         <v>87</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -7004,7 +6996,7 @@
       <c r="H8" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I8" s="147"/>
+      <c r="I8" s="154"/>
       <c r="J8" s="7" t="s">
         <v>150</v>
       </c>
@@ -7012,14 +7004,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="45" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>154</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="145"/>
+      <c r="C9" s="152"/>
       <c r="D9" s="7" t="s">
         <v>152</v>
       </c>
@@ -7033,7 +7025,7 @@
       <c r="H9" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="I9" s="147"/>
+      <c r="I9" s="154"/>
       <c r="J9" s="29" t="s">
         <v>209</v>
       </c>
@@ -7041,7 +7033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>149</v>
       </c>
@@ -7064,7 +7056,7 @@
       <c r="H10" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I10" s="151"/>
+      <c r="I10" s="159"/>
       <c r="J10" s="29" t="s">
         <v>144</v>
       </c>
@@ -7072,37 +7064,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="136" t="s">
+    <row r="11" spans="1:12" ht="15" customHeight="1">
+      <c r="A11" s="128" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="147" t="s">
+      <c r="B11" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="145" t="s">
+      <c r="C11" s="152" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="127" t="s">
+      <c r="D11" s="137" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="155">
+      <c r="E11" s="150">
         <v>3</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="134" t="s">
+      <c r="G11" s="132" t="s">
         <v>140</v>
       </c>
-      <c r="H11" s="134"/>
-      <c r="I11" s="134"/>
-      <c r="J11" s="134"/>
-      <c r="K11" s="134"/>
-    </row>
-    <row r="12" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="158"/>
-      <c r="B12" s="157"/>
-      <c r="C12" s="146"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="156"/>
+      <c r="H11" s="132"/>
+      <c r="I11" s="132"/>
+      <c r="J11" s="132"/>
+      <c r="K11" s="132"/>
+    </row>
+    <row r="12" spans="1:12" ht="45" customHeight="1">
+      <c r="A12" s="156"/>
+      <c r="B12" s="155"/>
+      <c r="C12" s="153"/>
+      <c r="D12" s="149"/>
+      <c r="E12" s="151"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
         <v>139</v>
@@ -7118,14 +7110,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="128" t="s">
+    <row r="13" spans="1:12" ht="15" customHeight="1">
+      <c r="A13" s="139" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="128"/>
-      <c r="C13" s="128"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="128"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="139"/>
+      <c r="E13" s="139"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
         <v>135</v>
@@ -7141,14 +7133,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>133</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="149" t="s">
+      <c r="C14" s="147" t="s">
         <v>87</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -7172,14 +7164,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="15" t="s">
         <v>127</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="145"/>
+      <c r="C15" s="152"/>
       <c r="D15" s="11" t="s">
         <v>125</v>
       </c>
@@ -7201,51 +7193,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="136" t="s">
+    <row r="16" spans="1:12" ht="15" customHeight="1">
+      <c r="A16" s="128" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="147" t="s">
+      <c r="B16" s="154" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="145"/>
-      <c r="D16" s="127" t="s">
+      <c r="C16" s="152"/>
+      <c r="D16" s="137" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="148">
+      <c r="E16" s="160">
         <v>1</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="134" t="s">
+      <c r="G16" s="132" t="s">
         <v>118</v>
       </c>
-      <c r="H16" s="134"/>
-      <c r="I16" s="134"/>
-      <c r="J16" s="134"/>
-      <c r="K16" s="134"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="136"/>
-      <c r="B17" s="147"/>
-      <c r="C17" s="145"/>
-      <c r="D17" s="127"/>
-      <c r="E17" s="148"/>
+      <c r="H16" s="132"/>
+      <c r="I16" s="132"/>
+      <c r="J16" s="132"/>
+      <c r="K16" s="132"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1">
+      <c r="A17" s="128"/>
+      <c r="B17" s="154"/>
+      <c r="C17" s="152"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="160"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
         <v>117</v>
       </c>
       <c r="H17" s="12"/>
-      <c r="I17" s="150"/>
+      <c r="I17" s="145"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>116</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="145"/>
+      <c r="C18" s="152"/>
       <c r="D18" s="7" t="s">
         <v>114</v>
       </c>
@@ -7257,17 +7249,17 @@
         <v>113</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="147"/>
+      <c r="I18" s="154"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>112</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="145" t="s">
+      <c r="C19" s="152" t="s">
         <v>131</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -7281,17 +7273,17 @@
         <v>109</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="I19" s="147"/>
+      <c r="I19" s="154"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="30">
       <c r="A20" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="145"/>
+      <c r="C20" s="152"/>
       <c r="D20" s="7" t="s">
         <v>106</v>
       </c>
@@ -7303,17 +7295,17 @@
         <v>105</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="147"/>
+      <c r="I20" s="154"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="45">
       <c r="A21" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="145"/>
+      <c r="C21" s="152"/>
       <c r="D21" s="7" t="s">
         <v>102</v>
       </c>
@@ -7325,17 +7317,17 @@
         <v>101</v>
       </c>
       <c r="H21" s="12"/>
-      <c r="I21" s="147"/>
+      <c r="I21" s="154"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="30">
       <c r="A22" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="145"/>
+      <c r="C22" s="152"/>
       <c r="D22" s="7" t="s">
         <v>98</v>
       </c>
@@ -7347,17 +7339,17 @@
         <v>97</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="I22" s="147"/>
+      <c r="I22" s="154"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="30">
       <c r="A23" s="16" t="s">
         <v>96</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="146"/>
+      <c r="C23" s="153"/>
       <c r="D23" s="7" t="s">
         <v>94</v>
       </c>
@@ -7369,37 +7361,37 @@
         <v>204</v>
       </c>
       <c r="H23" s="12"/>
-      <c r="I23" s="147"/>
+      <c r="I23" s="154"/>
       <c r="J23" s="7" t="s">
         <v>209</v>
       </c>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="128" t="s">
+    <row r="24" spans="1:11" ht="15" customHeight="1">
+      <c r="A24" s="139" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="128"/>
-      <c r="C24" s="128"/>
-      <c r="D24" s="128"/>
-      <c r="E24" s="128"/>
+      <c r="B24" s="139"/>
+      <c r="C24" s="139"/>
+      <c r="D24" s="139"/>
+      <c r="E24" s="139"/>
       <c r="F24" s="4"/>
       <c r="G24" s="5" t="s">
         <v>93</v>
       </c>
       <c r="H24" s="12"/>
-      <c r="I24" s="147"/>
+      <c r="I24" s="154"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="30" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="149" t="s">
-        <v>428</v>
+      <c r="C25" s="147" t="s">
+        <v>416</v>
       </c>
       <c r="D25" s="63" t="s">
         <v>278</v>
@@ -7412,20 +7404,20 @@
         <v>91</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="147"/>
+      <c r="I25" s="154"/>
       <c r="J25" s="12" t="s">
         <v>90</v>
       </c>
       <c r="K25" s="25"/>
     </row>
-    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="45">
       <c r="A26" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B26" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="153"/>
+      <c r="C26" s="148"/>
       <c r="D26" s="44" t="s">
         <v>279</v>
       </c>
@@ -7435,22 +7427,22 @@
       <c r="F26" s="4"/>
       <c r="G26" s="15"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="147"/>
+      <c r="I26" s="154"/>
       <c r="J26" s="12"/>
       <c r="K26" s="25"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="5" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="B27" s="47" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="C27" s="101" t="s">
         <v>194</v>
       </c>
       <c r="D27" s="44" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="E27" s="45">
         <v>1</v>
@@ -7460,17 +7452,17 @@
         <v>84</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="147"/>
+      <c r="I27" s="154"/>
       <c r="K27" s="23"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="5" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="B28" s="100"/>
       <c r="C28" s="109"/>
       <c r="D28" s="44" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="E28" s="45">
         <v>3</v>
@@ -7480,45 +7472,45 @@
         <v>83</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="147"/>
+      <c r="I28" s="154"/>
       <c r="J28" s="7" t="s">
         <v>276</v>
       </c>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="30" customHeight="1">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I29" s="147"/>
+      <c r="I29" s="154"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I30" s="151"/>
+      <c r="I30" s="159"/>
       <c r="J30" s="7" t="s">
         <v>209</v>
       </c>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="134" t="s">
+      <c r="G31" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="134"/>
-      <c r="I31" s="134"/>
-      <c r="J31" s="134"/>
-      <c r="K31" s="134"/>
-    </row>
-    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="H31" s="132"/>
+      <c r="I31" s="132"/>
+      <c r="J31" s="132"/>
+      <c r="K31" s="132"/>
+    </row>
+    <row r="32" spans="1:11" ht="30">
       <c r="D32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="6" t="s">
@@ -7527,7 +7519,7 @@
       <c r="H32" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="I32" s="150"/>
+      <c r="I32" s="145"/>
       <c r="J32" s="7" t="s">
         <v>77</v>
       </c>
@@ -7535,7 +7527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:11" ht="45">
       <c r="D33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="5" t="s">
@@ -7544,7 +7536,7 @@
       <c r="H33" s="98" t="s">
         <v>75</v>
       </c>
-      <c r="I33" s="152"/>
+      <c r="I33" s="146"/>
       <c r="J33" s="7" t="s">
         <v>74</v>
       </c>
@@ -7552,24 +7544,24 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="4:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:11" ht="90">
       <c r="D34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="5" t="s">
         <v>73</v>
       </c>
       <c r="H34" s="98" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="I34" s="70" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="4:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:11" ht="105">
       <c r="D35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="5" t="s">
@@ -7579,14 +7571,14 @@
         <v>71</v>
       </c>
       <c r="I35" s="70" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="4:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:11" ht="105">
       <c r="D36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="5" t="s">
@@ -7596,14 +7588,14 @@
         <v>69</v>
       </c>
       <c r="I36" s="73" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J36" s="44" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="K36" s="42"/>
     </row>
-    <row r="37" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" ht="30.75" thickBot="1">
       <c r="D37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="13" t="s">
@@ -7622,7 +7614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:11">
       <c r="D38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="42"/>
@@ -7631,7 +7623,7 @@
       <c r="J38" s="44"/>
       <c r="K38" s="42"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:11">
       <c r="D39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="42"/>
@@ -7640,103 +7632,112 @@
       <c r="J39" s="44"/>
       <c r="K39" s="42"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:11">
       <c r="D40" s="4"/>
       <c r="F40" s="4"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:11">
       <c r="D41" s="4"/>
       <c r="F41" s="4"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:11">
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:11">
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:11">
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
       <c r="K44" s="4"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:11">
       <c r="D45" s="4"/>
       <c r="F45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:11">
       <c r="D46" s="4"/>
       <c r="F46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:11">
       <c r="D47" s="4"/>
       <c r="F47" s="4"/>
       <c r="K47" s="4"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:11">
       <c r="D48" s="4"/>
       <c r="F48" s="4"/>
       <c r="K48" s="4"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:11">
       <c r="D49" s="4"/>
       <c r="F49" s="4"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:11">
       <c r="D50" s="4"/>
       <c r="F50" s="4"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:11">
       <c r="D51" s="4"/>
       <c r="F51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:11">
       <c r="D52" s="4"/>
       <c r="F52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:11">
       <c r="D53" s="4"/>
       <c r="F53" s="4"/>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:11">
       <c r="D54" s="4"/>
       <c r="F54" s="4"/>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:11">
       <c r="D55" s="4"/>
       <c r="F55" s="4"/>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:11">
       <c r="D56" s="4"/>
       <c r="F56" s="4"/>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:11">
       <c r="D57" s="4"/>
       <c r="F57" s="4"/>
       <c r="K57" s="4"/>
     </row>
-    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:11">
       <c r="D58" s="4"/>
       <c r="F58" s="4"/>
       <c r="K58" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="I17:I30"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="G31:K31"/>
     <mergeCell ref="I32:I33"/>
     <mergeCell ref="A2:E2"/>
@@ -7753,15 +7754,6 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="I3:I10"/>
     <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="I17:I30"/>
-    <mergeCell ref="A24:E24"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7777,7 +7769,7 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28" style="4" customWidth="1"/>
     <col min="2" max="2" width="20" style="4" customWidth="1"/>
@@ -7793,7 +7785,7 @@
     <col min="12" max="12" width="10" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>201</v>
       </c>
@@ -7827,7 +7819,7 @@
       </c>
       <c r="L1" s="33"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="49" t="s">
         <v>200</v>
       </c>
@@ -7854,12 +7846,12 @@
       </c>
       <c r="L2" s="32"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="5" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="B3" s="163"/>
-      <c r="C3" s="145"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="7"/>
       <c r="E3" s="40" t="s">
         <v>197</v>
@@ -7876,12 +7868,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>195</v>
       </c>
       <c r="B4" s="163"/>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="152" t="s">
         <v>194</v>
       </c>
       <c r="D4" s="7"/>
@@ -7903,12 +7895,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="5" t="s">
         <v>192</v>
       </c>
       <c r="B5" s="163"/>
-      <c r="C5" s="145"/>
+      <c r="C5" s="152"/>
       <c r="D5" s="7"/>
       <c r="E5" s="40" t="s">
         <v>182</v>
@@ -7916,7 +7908,7 @@
       <c r="F5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>191</v>
       </c>
@@ -7931,12 +7923,12 @@
       <c r="F6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>190</v>
       </c>
       <c r="B7" s="163"/>
-      <c r="C7" s="145" t="s">
+      <c r="C7" s="152" t="s">
         <v>194</v>
       </c>
       <c r="D7" s="7"/>
@@ -7947,12 +7939,12 @@
       <c r="J7" s="29"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>189</v>
       </c>
       <c r="B8" s="163"/>
-      <c r="C8" s="145"/>
+      <c r="C8" s="152"/>
       <c r="D8" s="7"/>
       <c r="E8" s="39" t="s">
         <v>182</v>
@@ -7964,7 +7956,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>188</v>
       </c>
@@ -7981,7 +7973,7 @@
       <c r="I9" s="11"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
         <v>186</v>
       </c>
@@ -7998,7 +7990,7 @@
       <c r="I10" s="11"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
         <v>184</v>
       </c>
@@ -8017,7 +8009,7 @@
       <c r="I11" s="11"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A12" s="13" t="s">
         <v>181</v>
       </c>
@@ -8035,7 +8027,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="B13" s="8"/>
       <c r="C13" s="21"/>
       <c r="D13" s="7"/>
@@ -8047,7 +8039,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15" customHeight="1">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -8058,7 +8050,7 @@
       <c r="I14" s="11"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="B15" s="8"/>
       <c r="C15" s="36"/>
       <c r="D15" s="7"/>
@@ -8067,7 +8059,7 @@
       <c r="I15" s="11"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="36"/>
@@ -8077,7 +8069,7 @@
       <c r="I16" s="11"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="B17" s="8"/>
       <c r="C17" s="36"/>
       <c r="D17" s="7"/>
@@ -8086,7 +8078,7 @@
       <c r="I17" s="11"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="B18" s="8"/>
       <c r="C18" s="36"/>
       <c r="D18" s="7"/>
@@ -8095,7 +8087,7 @@
       <c r="I18" s="11"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="B19" s="8"/>
       <c r="C19" s="36"/>
       <c r="D19" s="7"/>
@@ -8104,7 +8096,7 @@
       <c r="I19" s="11"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="B20" s="8"/>
       <c r="C20" s="36"/>
       <c r="D20" s="7"/>
@@ -8113,21 +8105,21 @@
       <c r="I20" s="11"/>
       <c r="K20" s="23"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="B21" s="8"/>
       <c r="C21" s="36"/>
       <c r="D21" s="7"/>
       <c r="F21" s="4"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="B22" s="8"/>
       <c r="C22" s="36"/>
       <c r="D22" s="7"/>
       <c r="F22" s="4"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -8136,28 +8128,28 @@
       <c r="F23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="B24" s="8"/>
       <c r="C24" s="36"/>
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="B25" s="11"/>
       <c r="C25" s="36"/>
       <c r="D25" s="7"/>
       <c r="F25" s="4"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="D27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="35"/>
@@ -8166,7 +8158,7 @@
       <c r="J27" s="35"/>
       <c r="K27" s="35"/>
     </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="30" customHeight="1">
       <c r="B28" s="8"/>
       <c r="C28" s="21"/>
       <c r="D28" s="7"/>
@@ -8175,154 +8167,154 @@
       <c r="I28" s="11"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="D32" s="4"/>
       <c r="F32" s="4"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:11">
       <c r="D33" s="4"/>
       <c r="F33" s="4"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:11">
       <c r="D34" s="4"/>
       <c r="F34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:11">
       <c r="D35" s="4"/>
       <c r="F35" s="4"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:11">
       <c r="D36" s="4"/>
       <c r="F36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:11">
       <c r="D37" s="4"/>
       <c r="F37" s="4"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:11">
       <c r="D38" s="4"/>
       <c r="F38" s="4"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:11">
       <c r="D39" s="4"/>
       <c r="F39" s="4"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:11">
       <c r="D40" s="4"/>
       <c r="F40" s="4"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:11">
       <c r="D41" s="4"/>
       <c r="F41" s="4"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:11">
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:11">
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:11">
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
       <c r="K44" s="4"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:11">
       <c r="D45" s="4"/>
       <c r="F45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:11">
       <c r="D46" s="4"/>
       <c r="F46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:11">
       <c r="D47" s="4"/>
       <c r="F47" s="4"/>
       <c r="K47" s="4"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:11">
       <c r="D48" s="4"/>
       <c r="F48" s="4"/>
       <c r="K48" s="4"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:11">
       <c r="D49" s="4"/>
       <c r="F49" s="4"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:11">
       <c r="D50" s="4"/>
       <c r="F50" s="4"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:11">
       <c r="D51" s="4"/>
       <c r="F51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:11">
       <c r="D52" s="4"/>
       <c r="F52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:11">
       <c r="D53" s="4"/>
       <c r="F53" s="4"/>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:11">
       <c r="D54" s="4"/>
       <c r="F54" s="4"/>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:11">
       <c r="D55" s="4"/>
       <c r="F55" s="4"/>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:11">
       <c r="D56" s="4"/>
       <c r="F56" s="4"/>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:11">
       <c r="D57" s="4"/>
       <c r="F57" s="4"/>
       <c r="K57" s="4"/>
     </row>
-    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:11">
       <c r="D58" s="4"/>
     </row>
   </sheetData>
@@ -8346,7 +8338,7 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28" style="4" customWidth="1"/>
     <col min="2" max="2" width="20" style="21" customWidth="1"/>
@@ -8361,9 +8353,9 @@
     <col min="11" max="11" width="4" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -8393,30 +8385,30 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="s">
-        <v>461</v>
-      </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="G2" s="128" t="s">
-        <v>482</v>
-      </c>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
+      <c r="A2" s="139" t="s">
+        <v>449</v>
+      </c>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="G2" s="139" t="s">
+        <v>470</v>
+      </c>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="139"/>
+      <c r="K2" s="139"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="B3" s="168" t="s">
-        <v>467</v>
-      </c>
-      <c r="C3" s="149" t="s">
+        <v>455</v>
+      </c>
+      <c r="C3" s="147" t="s">
         <v>194</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -8431,14 +8423,14 @@
       <c r="J3" s="7"/>
       <c r="K3" s="117"/>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="5" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="B4" s="169"/>
-      <c r="C4" s="153"/>
+      <c r="C4" s="148"/>
       <c r="D4" s="44" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="E4" s="112">
         <v>1</v>
@@ -8450,9 +8442,9 @@
       <c r="J4" s="44"/>
       <c r="K4" s="118"/>
     </row>
-    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="B5" s="169"/>
       <c r="C5" s="76" t="s">
@@ -8471,18 +8463,18 @@
       <c r="J5" s="44"/>
       <c r="K5" s="119"/>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="45">
       <c r="A6" s="5" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="B6" s="86" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="C6" s="76" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="E6" s="64">
         <v>3</v>
@@ -8494,14 +8486,14 @@
       <c r="J6" s="44"/>
       <c r="K6" s="44"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="128" t="s">
-        <v>481</v>
-      </c>
-      <c r="B7" s="128"/>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
+    <row r="7" spans="1:11">
+      <c r="A7" s="139" t="s">
+        <v>469</v>
+      </c>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
       <c r="F7" s="51"/>
       <c r="G7" s="42"/>
       <c r="H7" s="42"/>
@@ -8509,12 +8501,12 @@
       <c r="J7" s="44"/>
       <c r="K7" s="118"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="6" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="C8" s="76" t="s">
         <v>134</v>
@@ -8530,18 +8522,18 @@
       <c r="J8" s="44"/>
       <c r="K8" s="118"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="5" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="C9" s="76" t="s">
         <v>134</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="E9" s="112">
         <v>3</v>
@@ -8553,15 +8545,15 @@
       <c r="J9" s="44"/>
       <c r="K9" s="118"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1">
       <c r="A10" s="13" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
       <c r="C10" s="97" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="124">
@@ -8574,7 +8566,7 @@
       <c r="J10" s="44"/>
       <c r="K10" s="118"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="42"/>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
@@ -8587,7 +8579,7 @@
       <c r="J11" s="44"/>
       <c r="K11" s="118"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="42"/>
       <c r="B12" s="86"/>
       <c r="C12" s="47"/>
@@ -8600,7 +8592,7 @@
       <c r="J12" s="44"/>
       <c r="K12" s="118"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="42"/>
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
@@ -8613,7 +8605,7 @@
       <c r="J13" s="44"/>
       <c r="K13" s="44"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="108"/>
       <c r="B14" s="110"/>
       <c r="C14" s="108"/>
@@ -8626,7 +8618,7 @@
       <c r="J14" s="108"/>
       <c r="K14" s="120"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="42"/>
       <c r="B15" s="47"/>
       <c r="C15" s="109"/>
@@ -8639,7 +8631,7 @@
       <c r="J15" s="44"/>
       <c r="K15" s="42"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="46"/>
       <c r="B16" s="47"/>
       <c r="C16" s="109"/>
@@ -8652,7 +8644,7 @@
       <c r="J16" s="64"/>
       <c r="K16" s="42"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="42"/>
       <c r="B17" s="47"/>
       <c r="C17" s="109"/>
@@ -8665,7 +8657,7 @@
       <c r="J17" s="44"/>
       <c r="K17" s="42"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="42"/>
       <c r="B18" s="47"/>
       <c r="C18" s="109"/>
@@ -8678,35 +8670,35 @@
       <c r="J18" s="44"/>
       <c r="K18" s="42"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="C19" s="36"/>
       <c r="D19" s="7"/>
       <c r="H19" s="74"/>
       <c r="I19" s="36"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="C20" s="36"/>
       <c r="D20" s="7"/>
       <c r="H20" s="74"/>
       <c r="I20" s="36"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="C21" s="36"/>
       <c r="D21" s="7"/>
       <c r="H21" s="74"/>
       <c r="I21" s="36"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="C22" s="36"/>
       <c r="D22" s="7"/>
       <c r="H22" s="74"/>
       <c r="I22" s="36"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="18"/>
       <c r="B23" s="23"/>
       <c r="C23" s="18"/>
@@ -8718,14 +8710,14 @@
       <c r="J23" s="18"/>
       <c r="K23" s="121"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="C24" s="36"/>
       <c r="D24" s="4"/>
       <c r="H24" s="74"/>
       <c r="I24" s="36"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="B25" s="78"/>
       <c r="C25" s="36"/>
       <c r="D25" s="7"/>
@@ -8733,141 +8725,141 @@
       <c r="I25" s="36"/>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="C26" s="74"/>
       <c r="D26" s="4"/>
       <c r="H26" s="74"/>
       <c r="I26" s="74"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="D27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="C28" s="21"/>
       <c r="D28" s="7"/>
       <c r="H28" s="74"/>
       <c r="I28" s="21"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="D29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="D30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="D31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="D32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:10">
       <c r="D33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:10">
       <c r="D34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:10">
       <c r="D35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:10">
       <c r="D36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:10">
       <c r="D37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:10">
       <c r="D38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:10">
       <c r="D39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:10">
       <c r="D40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:10">
       <c r="D41" s="4"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:10">
       <c r="D42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:10">
       <c r="D43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:10">
       <c r="D44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:10">
       <c r="D45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:10">
       <c r="D46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:10">
       <c r="D47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:10">
       <c r="D48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:10">
       <c r="D49" s="4"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:10">
       <c r="D50" s="4"/>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:10">
       <c r="D51" s="4"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:10">
       <c r="D52" s="4"/>
       <c r="J52" s="4"/>
     </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:10">
       <c r="D53" s="4"/>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:10">
       <c r="D54" s="4"/>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:10">
       <c r="D55" s="4"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:10">
       <c r="D56" s="4"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:10">
       <c r="D57" s="4"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:10">
       <c r="D58" s="4"/>
       <c r="J58" s="4"/>
     </row>
@@ -8892,7 +8884,7 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -8905,7 +8897,7 @@
     <col min="9" max="9" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>210</v>
       </c>
@@ -8931,7 +8923,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="4" t="s">
         <v>238</v>
       </c>
@@ -8939,7 +8931,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
         <v>239</v>
       </c>
@@ -8947,10 +8939,10 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>213</v>
       </c>
@@ -8976,7 +8968,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="F7" t="s">
         <v>242</v>
       </c>
@@ -8984,15 +8976,15 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="60">
       <c r="F8" t="s">
         <v>244</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60">
       <c r="F9" t="s">
         <v>245</v>
       </c>
@@ -9013,7 +9005,7 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -9026,7 +9018,7 @@
     <col min="9" max="9" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>220</v>
       </c>
@@ -9052,7 +9044,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="125" t="s">
         <v>221</v>
       </c>
@@ -9060,7 +9052,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="122" t="s">
         <v>247</v>
       </c>
@@ -9068,7 +9060,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="122" t="s">
         <v>248</v>
       </c>
@@ -9082,7 +9074,7 @@
       <c r="I4" s="123"/>
       <c r="J4" s="123"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="122" t="s">
         <v>249</v>
       </c>
@@ -9091,7 +9083,7 @@
       <c r="H5" s="51"/>
       <c r="I5" s="51"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="126" t="s">
         <v>226</v>
       </c>
@@ -9103,13 +9095,13 @@
       <c r="H6" s="51"/>
       <c r="I6" s="51"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
       <c r="H7" s="51"/>
       <c r="I7" s="51"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="1" t="s">
         <v>214</v>
       </c>
@@ -9127,7 +9119,7 @@
       <c r="H8" s="52"/>
       <c r="I8" s="53"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="125" t="s">
         <v>250</v>
       </c>
@@ -9136,12 +9128,12 @@
       <c r="H9" s="51"/>
       <c r="I9" s="51"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="122" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="126" t="s">
         <v>252</v>
       </c>

</xml_diff>

<commit_message>
fixed a few issues with balancing.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Git Repositories\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93653994-D13D-4FF2-9EDA-3B52A7344779}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4AEAB2-6BBC-4AC1-B2A0-802B66E839C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
@@ -105,27 +105,6 @@
     <t>50 gp</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1 metal plate (8 lbs, cuirass)
-4 metal plates (1.25 lbs each, arm plating)
-4 quilts of leather padding (1 lbs each, joint protection)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1 quilt of leather padding (5 lbs, hidden, padding)
-1 chain shirt (20 lbs, hidden, padding)
-</t>
-    </r>
-  </si>
-  <si>
     <t>42 lbs.</t>
   </si>
   <si>
@@ -159,36 +138,6 @@
   </si>
   <si>
     <t>1.5 lbs.</t>
-  </si>
-  <si>
-    <r>
-      <t>1 quilt of leather padding (8 lbs, coat)
-4 quilts of leather padding (2.5 lbs each, limb protection)
-20 metal spikes (1 lb each, welded to the plates and protruding through the leather)
-7</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> metal plates (1 lb each, hidden, sewn in)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
   </si>
   <si>
     <t>75 gp</t>
@@ -4085,6 +4034,57 @@
       </rPr>
       <t xml:space="preserve">
 1 folding fan (1 lb)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1 quilt of leather padding (5 lbs, coat)
+4 quilts of leather padding (2 lbs each, limb protection)
+20 metal spikes (1 lb each, welded to the plates and protruding through the leather)
+7</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> metal plates (1 lb each, hidden, sewn in)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 metal plate (8 lbs, cuirass)
+4 metal plates (1.5 lbs each, arm plating)
+4 quilts of leather padding (0.75 lbs each, joint protection)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1 quilt of leather padding (5 lbs, hidden, padding)
+1 chain shirt (20 lbs, hidden, padding)
+</t>
     </r>
   </si>
 </sst>
@@ -4679,6 +4679,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -4688,60 +4721,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4754,15 +4769,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -4774,12 +4780,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5124,8 +5124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
   <dimension ref="A1:AC70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5183,7 +5183,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>1</v>
@@ -5195,7 +5195,7 @@
         <v>3</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>1</v>
@@ -5207,7 +5207,7 @@
         <v>3</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>1</v>
@@ -5219,7 +5219,7 @@
         <v>3</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>1</v>
@@ -5232,61 +5232,61 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="15" customHeight="1">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="F2" s="138" t="s">
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="F2" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="K2" s="138" t="s">
-        <v>436</v>
-      </c>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="P2" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q2" s="129" t="s">
-        <v>258</v>
-      </c>
-      <c r="R2" s="131" t="s">
-        <v>228</v>
-      </c>
-      <c r="S2" s="131" t="s">
-        <v>62</v>
-      </c>
-      <c r="U2" s="127" t="s">
-        <v>233</v>
-      </c>
-      <c r="V2" s="134" t="s">
-        <v>270</v>
-      </c>
-      <c r="W2" s="131" t="s">
-        <v>228</v>
-      </c>
-      <c r="X2" s="131" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z2" s="133" t="s">
-        <v>284</v>
-      </c>
-      <c r="AA2" s="133"/>
-      <c r="AB2" s="133"/>
-      <c r="AC2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="K2" s="134" t="s">
+        <v>434</v>
+      </c>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="P2" s="138" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q2" s="140" t="s">
+        <v>256</v>
+      </c>
+      <c r="R2" s="141" t="s">
+        <v>226</v>
+      </c>
+      <c r="S2" s="141" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" s="138" t="s">
+        <v>231</v>
+      </c>
+      <c r="V2" s="143" t="s">
+        <v>268</v>
+      </c>
+      <c r="W2" s="141" t="s">
+        <v>226</v>
+      </c>
+      <c r="X2" s="141" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z2" s="142" t="s">
+        <v>282</v>
+      </c>
+      <c r="AA2" s="142"/>
+      <c r="AB2" s="142"/>
+      <c r="AC2" s="142"/>
     </row>
     <row r="3" spans="1:29" ht="75">
       <c r="A3" s="9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>7</v>
@@ -5295,7 +5295,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>9</v>
@@ -5307,45 +5307,45 @@
         <v>8</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="L3" s="64" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="M3" s="79">
         <v>0.06</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="P3" s="128"/>
-      <c r="Q3" s="130"/>
-      <c r="R3" s="130"/>
-      <c r="S3" s="130"/>
-      <c r="U3" s="128"/>
-      <c r="V3" s="135"/>
-      <c r="W3" s="136"/>
-      <c r="X3" s="136"/>
+      <c r="P3" s="139"/>
+      <c r="Q3" s="128"/>
+      <c r="R3" s="128"/>
+      <c r="S3" s="128"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="127"/>
+      <c r="W3" s="144"/>
+      <c r="X3" s="144"/>
       <c r="Z3" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AA3" s="75" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="75">
       <c r="A4" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>12</v>
@@ -5357,52 +5357,52 @@
         <v>14</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="L4" s="64" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="M4" s="79">
         <v>0.05</v>
       </c>
       <c r="N4" s="50"/>
       <c r="P4" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="Q4" s="75" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="R4" s="74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="S4" s="74" t="s">
         <v>23</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="V4" s="75" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="W4" s="74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="X4" s="74" t="s">
         <v>23</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="AA4" s="75" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="75" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>17</v>
@@ -5411,126 +5411,126 @@
         <v>8</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="L5" s="64" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="M5" s="45">
         <v>0.06</v>
       </c>
       <c r="N5" s="46"/>
       <c r="P5" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q5" s="75" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="R5" s="74" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="S5" s="74" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="V5" s="75" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W5" s="74" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="X5" s="74" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Z5" s="65" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="AA5" s="77" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AB5" s="77"/>
       <c r="AC5" s="77"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1">
-      <c r="A6" s="144" t="s">
-        <v>333</v>
-      </c>
-      <c r="B6" s="137" t="s">
-        <v>497</v>
-      </c>
-      <c r="C6" s="130" t="s">
+      <c r="A6" s="130" t="s">
+        <v>331</v>
+      </c>
+      <c r="B6" s="133" t="s">
+        <v>495</v>
+      </c>
+      <c r="C6" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="130" t="s">
+      <c r="D6" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="132" t="s">
+      <c r="F6" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="132"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="132"/>
-      <c r="K6" s="132" t="s">
-        <v>438</v>
-      </c>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="132"/>
-      <c r="P6" s="128" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q6" s="137" t="s">
-        <v>261</v>
-      </c>
-      <c r="R6" s="130" t="s">
-        <v>229</v>
-      </c>
-      <c r="S6" s="130" t="s">
-        <v>43</v>
-      </c>
-      <c r="U6" s="128" t="s">
-        <v>236</v>
-      </c>
-      <c r="V6" s="135" t="s">
-        <v>265</v>
-      </c>
-      <c r="W6" s="130" t="s">
-        <v>229</v>
-      </c>
-      <c r="X6" s="130" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z6" s="132" t="s">
-        <v>294</v>
-      </c>
-      <c r="AA6" s="132"/>
-      <c r="AB6" s="132"/>
-      <c r="AC6" s="132"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="K6" s="129" t="s">
+        <v>436</v>
+      </c>
+      <c r="L6" s="129"/>
+      <c r="M6" s="129"/>
+      <c r="N6" s="129"/>
+      <c r="P6" s="139" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q6" s="133" t="s">
+        <v>259</v>
+      </c>
+      <c r="R6" s="128" t="s">
+        <v>227</v>
+      </c>
+      <c r="S6" s="128" t="s">
+        <v>41</v>
+      </c>
+      <c r="U6" s="139" t="s">
+        <v>234</v>
+      </c>
+      <c r="V6" s="127" t="s">
+        <v>263</v>
+      </c>
+      <c r="W6" s="128" t="s">
+        <v>227</v>
+      </c>
+      <c r="X6" s="128" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z6" s="129" t="s">
+        <v>292</v>
+      </c>
+      <c r="AA6" s="129"/>
+      <c r="AB6" s="129"/>
+      <c r="AC6" s="129"/>
     </row>
     <row r="7" spans="1:29" ht="120" customHeight="1">
-      <c r="A7" s="144"/>
-      <c r="B7" s="137"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
+      <c r="A7" s="130"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
       <c r="F7" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>20</v>
@@ -5539,38 +5539,38 @@
         <v>21</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="L7" s="64" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M7" s="45">
         <v>0.08</v>
       </c>
       <c r="N7" s="103"/>
-      <c r="P7" s="128"/>
-      <c r="Q7" s="130"/>
-      <c r="R7" s="130"/>
-      <c r="S7" s="130"/>
-      <c r="U7" s="128"/>
-      <c r="V7" s="135"/>
-      <c r="W7" s="130"/>
-      <c r="X7" s="130"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="128"/>
+      <c r="R7" s="128"/>
+      <c r="S7" s="128"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="127"/>
+      <c r="W7" s="128"/>
+      <c r="X7" s="128"/>
       <c r="Z7" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="AA7" s="66" t="s">
         <v>295</v>
-      </c>
-      <c r="AA7" s="66" t="s">
-        <v>297</v>
       </c>
       <c r="AB7" s="44"/>
       <c r="AC7" s="44"/>
     </row>
     <row r="8" spans="1:29" ht="75" customHeight="1" thickBot="1">
       <c r="A8" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>7</v>
@@ -5579,64 +5579,64 @@
         <v>22</v>
       </c>
       <c r="F8" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>322</v>
-      </c>
       <c r="H8" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="L8" s="64" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="M8" s="45">
         <v>0.08</v>
       </c>
       <c r="N8" s="42"/>
       <c r="P8" s="13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="Q8" s="17" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="R8" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="S8" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="S8" s="14" t="s">
-        <v>231</v>
-      </c>
       <c r="U8" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="V8" s="17" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="W8" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="X8" s="14"/>
       <c r="Z8" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA8" s="67" t="s">
         <v>296</v>
-      </c>
-      <c r="AA8" s="67" t="s">
-        <v>298</v>
       </c>
       <c r="AB8" s="64"/>
       <c r="AC8" s="64"/>
     </row>
-    <row r="9" spans="1:29" ht="195" customHeight="1">
+    <row r="9" spans="1:29" ht="210" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>17</v>
@@ -5645,228 +5645,228 @@
         <v>14</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G9" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="K9" s="104" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="L9" s="64" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="M9" s="45">
         <v>0.08</v>
       </c>
       <c r="N9" s="51"/>
       <c r="Z9" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="AA9" s="67" t="s">
         <v>299</v>
-      </c>
-      <c r="AA9" s="67" t="s">
-        <v>301</v>
       </c>
       <c r="AB9" s="64"/>
       <c r="AC9" s="64"/>
     </row>
     <row r="10" spans="1:29" ht="90">
       <c r="A10" s="10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B10" s="88" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="K10" s="104" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="L10" s="64" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="M10" s="79">
         <v>0.08</v>
       </c>
       <c r="Z10" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA10" s="68" t="s">
         <v>300</v>
       </c>
-      <c r="AA10" s="68" t="s">
-        <v>302</v>
-      </c>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1">
-      <c r="A11" s="144" t="s">
-        <v>337</v>
-      </c>
-      <c r="B11" s="135" t="s">
-        <v>500</v>
-      </c>
-      <c r="C11" s="130" t="s">
+      <c r="A11" s="130" t="s">
+        <v>335</v>
+      </c>
+      <c r="B11" s="127" t="s">
+        <v>498</v>
+      </c>
+      <c r="C11" s="128" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="128" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="130" t="s">
+        <v>314</v>
+      </c>
+      <c r="G11" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="130" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="144" t="s">
-        <v>316</v>
-      </c>
-      <c r="G11" s="135" t="s">
+      <c r="H11" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="137" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="137" t="s">
+      <c r="I11" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="132" t="s">
-        <v>435</v>
-      </c>
-      <c r="L11" s="132"/>
-      <c r="M11" s="132"/>
-      <c r="N11" s="132"/>
-      <c r="Z11" s="132" t="s">
-        <v>288</v>
-      </c>
-      <c r="AA11" s="132"/>
-      <c r="AB11" s="132"/>
-      <c r="AC11" s="132"/>
+      <c r="K11" s="129" t="s">
+        <v>433</v>
+      </c>
+      <c r="L11" s="129"/>
+      <c r="M11" s="129"/>
+      <c r="N11" s="129"/>
+      <c r="Z11" s="129" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA11" s="129"/>
+      <c r="AB11" s="129"/>
+      <c r="AC11" s="129"/>
     </row>
     <row r="12" spans="1:29" ht="75" customHeight="1">
-      <c r="A12" s="144"/>
-      <c r="B12" s="135"/>
-      <c r="C12" s="130"/>
-      <c r="D12" s="130"/>
-      <c r="F12" s="144"/>
-      <c r="G12" s="135"/>
-      <c r="H12" s="137"/>
-      <c r="I12" s="137"/>
+      <c r="A12" s="130"/>
+      <c r="B12" s="127"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="127"/>
+      <c r="H12" s="133"/>
+      <c r="I12" s="133"/>
       <c r="K12" s="9" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="N12" s="4"/>
       <c r="Z12" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AA12" s="66" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AB12" s="44"/>
       <c r="AC12" s="44"/>
     </row>
     <row r="13" spans="1:29" ht="210" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C13" s="69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="69" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>32</v>
+        <v>504</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K13" s="106" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="Z13" s="10" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AA13" s="66" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AB13" s="44"/>
       <c r="AC13" s="44"/>
     </row>
     <row r="14" spans="1:29" ht="15" customHeight="1">
-      <c r="A14" s="144" t="s">
-        <v>339</v>
-      </c>
-      <c r="B14" s="135" t="s">
-        <v>398</v>
-      </c>
-      <c r="C14" s="130" t="s">
+      <c r="A14" s="130" t="s">
+        <v>337</v>
+      </c>
+      <c r="B14" s="127" t="s">
+        <v>396</v>
+      </c>
+      <c r="C14" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="130" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="132" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="132"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="132"/>
-      <c r="K14" s="140" t="s">
-        <v>487</v>
-      </c>
-      <c r="L14" s="141"/>
-      <c r="M14" s="142"/>
-      <c r="N14" s="141"/>
+      <c r="D14" s="128" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="129" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="129"/>
+      <c r="H14" s="129"/>
+      <c r="I14" s="129"/>
+      <c r="K14" s="135" t="s">
+        <v>485</v>
+      </c>
+      <c r="L14" s="132"/>
+      <c r="M14" s="136"/>
+      <c r="N14" s="132"/>
       <c r="Z14" s="44"/>
       <c r="AA14" s="92"/>
       <c r="AB14" s="44"/>
       <c r="AC14" s="44"/>
     </row>
     <row r="15" spans="1:29" ht="90">
-      <c r="A15" s="144"/>
-      <c r="B15" s="135"/>
-      <c r="C15" s="130"/>
-      <c r="D15" s="130"/>
+      <c r="A15" s="130"/>
+      <c r="B15" s="127"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="128"/>
       <c r="F15" s="9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K15" s="140"/>
-      <c r="L15" s="141"/>
-      <c r="M15" s="142"/>
-      <c r="N15" s="141"/>
+        <v>31</v>
+      </c>
+      <c r="K15" s="135"/>
+      <c r="L15" s="132"/>
+      <c r="M15" s="136"/>
+      <c r="N15" s="132"/>
       <c r="Z15" s="44"/>
       <c r="AA15" s="64"/>
       <c r="AB15" s="64"/>
@@ -5874,10 +5874,10 @@
     </row>
     <row r="16" spans="1:29" ht="285">
       <c r="A16" s="85" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B16" s="71" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C16" s="69" t="s">
         <v>17</v>
@@ -5886,136 +5886,136 @@
         <v>8</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K16" s="106" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="165" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C17" s="69" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="I17" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="K17" s="106"/>
     </row>
     <row r="18" spans="1:16" ht="195">
       <c r="A18" s="65" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C18" s="69" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="G18" s="44" t="s">
+      <c r="I18" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="44" t="s">
+      <c r="K18" s="122"/>
+    </row>
+    <row r="19" spans="1:16" ht="15" customHeight="1">
+      <c r="A19" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="K18" s="122"/>
-    </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1">
-      <c r="A19" s="139" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="139"/>
-      <c r="C19" s="139"/>
-      <c r="D19" s="139"/>
-      <c r="F19" s="132" t="s">
-        <v>310</v>
-      </c>
-      <c r="G19" s="132"/>
-      <c r="H19" s="132"/>
-      <c r="I19" s="132"/>
+      <c r="B19" s="131"/>
+      <c r="C19" s="131"/>
+      <c r="D19" s="131"/>
+      <c r="F19" s="129" t="s">
+        <v>308</v>
+      </c>
+      <c r="G19" s="129"/>
+      <c r="H19" s="129"/>
+      <c r="I19" s="129"/>
     </row>
     <row r="20" spans="1:16" ht="75">
       <c r="A20" s="9" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C20" s="69" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="69" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G20" s="89" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C21" s="69" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D21" s="69" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G21" s="90" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>8</v>
@@ -6025,107 +6025,107 @@
     </row>
     <row r="22" spans="1:16" ht="75">
       <c r="A22" s="10" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C22" s="69" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D22" s="69" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G22" s="90" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="60.75" thickBot="1">
       <c r="A23" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C23" s="69" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D23" s="69" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G23" s="91" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="60">
       <c r="A24" s="10" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C24" s="69" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D24" s="69" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="60">
       <c r="A25" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C25" s="69" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D25" s="69" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="60">
       <c r="A26" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C26" s="69" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D26" s="69" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="30">
       <c r="A27" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C27" s="69" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D27" s="69" t="s">
         <v>14</v>
@@ -6133,69 +6133,69 @@
     </row>
     <row r="28" spans="1:16" ht="30">
       <c r="A28" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C28" s="69" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D28" s="69" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="30">
       <c r="A29" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B29" s="88" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C29" s="69" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D29" s="69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="60">
       <c r="A30" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C30" s="69" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D30" s="69" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="30">
       <c r="A31" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C31" s="69" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D31" s="69" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="30" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C32" s="69" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="69" t="s">
         <v>14</v>
@@ -6203,13 +6203,13 @@
     </row>
     <row r="33" spans="1:4" ht="45.75" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B33" s="87" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C33" s="69" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D33" s="69" t="s">
         <v>14</v>
@@ -6217,105 +6217,105 @@
     </row>
     <row r="34" spans="1:4" ht="45">
       <c r="A34" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B34" s="87" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C34" s="69" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D34" s="69" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="45">
       <c r="A35" s="65" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C35" s="69" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D35" s="69" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="139" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="139"/>
-      <c r="C36" s="139"/>
-      <c r="D36" s="139"/>
+      <c r="A36" s="131" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="131"/>
+      <c r="C36" s="131"/>
+      <c r="D36" s="131"/>
     </row>
     <row r="37" spans="1:4" ht="45">
       <c r="A37" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C37" s="69" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D37" s="69" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45">
       <c r="A38" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C38" s="69" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D38" s="69" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="45" customHeight="1">
       <c r="A39" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C39" s="69" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D39" s="69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="45">
       <c r="A40" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C40" s="71" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D40" s="69" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="45" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C41" s="71" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D41" s="69" t="s">
         <v>23</v>
@@ -6323,27 +6323,27 @@
     </row>
     <row r="42" spans="1:4" ht="45">
       <c r="A42" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C42" s="69" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D42" s="69" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="45">
       <c r="A43" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C43" s="69" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D43" s="69" t="s">
         <v>8</v>
@@ -6351,10 +6351,10 @@
     </row>
     <row r="44" spans="1:4" ht="30">
       <c r="A44" s="65" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C44" s="69" t="s">
         <v>10</v>
@@ -6364,84 +6364,84 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="139" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" s="139"/>
-      <c r="C45" s="139"/>
-      <c r="D45" s="139"/>
+      <c r="A45" s="131" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="131"/>
+      <c r="C45" s="131"/>
+      <c r="D45" s="131"/>
     </row>
     <row r="46" spans="1:4" ht="45">
       <c r="A46" s="84" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B46" s="71" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C46" s="71" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D46" s="69" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="90" customHeight="1">
       <c r="A47" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C47" s="71" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D47" s="69" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="60" customHeight="1">
       <c r="A48" s="65" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C48" s="71" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D48" s="69" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:29">
-      <c r="A49" s="139" t="s">
-        <v>253</v>
-      </c>
-      <c r="B49" s="139"/>
-      <c r="C49" s="139"/>
-      <c r="D49" s="139"/>
+      <c r="A49" s="131" t="s">
+        <v>251</v>
+      </c>
+      <c r="B49" s="131"/>
+      <c r="C49" s="131"/>
+      <c r="D49" s="131"/>
     </row>
     <row r="50" spans="1:29" ht="30">
       <c r="A50" s="80" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B50" s="58"/>
       <c r="C50" s="58" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D50" s="58" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="30">
       <c r="A51" s="81" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B51" s="67" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D51" s="58" t="s">
         <v>14</v>
@@ -6449,46 +6449,46 @@
     </row>
     <row r="52" spans="1:29" ht="60">
       <c r="A52" s="81" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B52" s="60" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C52" s="58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D52" s="58" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:29" ht="30" customHeight="1">
       <c r="A53" s="83" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B53" s="60" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C53" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D53" s="58" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:29">
-      <c r="A54" s="139" t="s">
-        <v>254</v>
-      </c>
-      <c r="B54" s="139"/>
-      <c r="C54" s="139"/>
-      <c r="D54" s="139"/>
+      <c r="A54" s="131" t="s">
+        <v>252</v>
+      </c>
+      <c r="B54" s="131"/>
+      <c r="C54" s="131"/>
+      <c r="D54" s="131"/>
     </row>
     <row r="55" spans="1:29">
       <c r="A55" s="80" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B55" s="58" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C55" s="58" t="s">
         <v>7</v>
@@ -6499,23 +6499,23 @@
     </row>
     <row r="56" spans="1:29" ht="30">
       <c r="A56" s="81" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B56" s="58"/>
       <c r="C56" s="58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D56" s="58" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:29" ht="45">
       <c r="A57" s="81" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B57" s="58"/>
       <c r="C57" s="58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D57" s="58" t="s">
         <v>23</v>
@@ -6523,13 +6523,13 @@
     </row>
     <row r="58" spans="1:29" ht="60">
       <c r="A58" s="81" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B58" s="60" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C58" s="58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D58" s="58" t="s">
         <v>23</v>
@@ -6537,48 +6537,48 @@
     </row>
     <row r="59" spans="1:29" ht="60">
       <c r="A59" s="81" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B59" s="60" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C59" s="58" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D59" s="58" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="60" spans="1:29">
-      <c r="A60" s="139" t="s">
-        <v>255</v>
-      </c>
-      <c r="B60" s="139"/>
-      <c r="C60" s="139"/>
-      <c r="D60" s="139"/>
+      <c r="A60" s="131" t="s">
+        <v>253</v>
+      </c>
+      <c r="B60" s="131"/>
+      <c r="C60" s="131"/>
+      <c r="D60" s="131"/>
     </row>
     <row r="61" spans="1:29" ht="45">
       <c r="A61" s="80" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B61" s="60" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C61" s="58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D61" s="58"/>
     </row>
     <row r="62" spans="1:29" ht="45">
       <c r="A62" s="107" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B62" s="105"/>
       <c r="C62" s="58" t="s">
         <v>10</v>
       </c>
       <c r="D62" s="58" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="M62" s="99"/>
       <c r="AA62" s="95"/>
@@ -6587,11 +6587,11 @@
     </row>
     <row r="63" spans="1:29" ht="45">
       <c r="A63" s="107" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B63" s="105"/>
       <c r="C63" s="58" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D63" s="58"/>
       <c r="M63" s="99"/>
@@ -6601,11 +6601,11 @@
     </row>
     <row r="64" spans="1:29" ht="45">
       <c r="A64" s="107" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B64" s="105"/>
       <c r="C64" s="58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D64" s="58"/>
       <c r="M64" s="99"/>
@@ -6615,11 +6615,11 @@
     </row>
     <row r="65" spans="1:29" ht="60">
       <c r="A65" s="107" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B65" s="105"/>
       <c r="C65" s="58" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D65" s="58"/>
       <c r="M65" s="99"/>
@@ -6629,7 +6629,7 @@
     </row>
     <row r="66" spans="1:29" ht="15" customHeight="1">
       <c r="A66" s="96" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B66" s="96"/>
       <c r="C66" s="96"/>
@@ -6641,12 +6641,12 @@
     </row>
     <row r="67" spans="1:29">
       <c r="A67" s="107" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B67" s="105"/>
       <c r="C67" s="58"/>
       <c r="D67" s="58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M67" s="99"/>
       <c r="AA67" s="95"/>
@@ -6655,12 +6655,12 @@
     </row>
     <row r="68" spans="1:29">
       <c r="A68" s="107" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B68" s="105"/>
       <c r="C68" s="58"/>
       <c r="D68" s="58" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M68" s="99"/>
       <c r="AA68" s="95"/>
@@ -6669,12 +6669,12 @@
     </row>
     <row r="69" spans="1:29" ht="15" customHeight="1">
       <c r="A69" s="107" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B69" s="105"/>
       <c r="C69" s="58"/>
       <c r="D69" s="58" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="M69" s="99"/>
       <c r="AA69" s="95"/>
@@ -6683,16 +6683,16 @@
     </row>
     <row r="70" spans="1:29" ht="225" customHeight="1" thickBot="1">
       <c r="A70" s="82" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B70" s="61" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C70" s="59" t="s">
         <v>10</v>
       </c>
       <c r="D70" s="59" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="M70" s="99"/>
       <c r="AA70" s="95"/>
@@ -6701,43 +6701,6 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A14:A15"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
@@ -6754,6 +6717,43 @@
     <mergeCell ref="X6:X7"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="P6:P7"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6764,7 +6764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E7B11-1527-417B-9532-F0F2C5A89902}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -6786,82 +6786,82 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="143" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
+      <c r="A2" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
       <c r="F2" s="18"/>
-      <c r="G2" s="138" t="s">
-        <v>172</v>
-      </c>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
+      <c r="G2" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
       <c r="L2" s="32"/>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="157" t="s">
-        <v>203</v>
-      </c>
-      <c r="C3" s="147" t="s">
-        <v>131</v>
+        <v>169</v>
+      </c>
+      <c r="B3" s="159" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="149" t="s">
+        <v>129</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E3" s="20">
         <v>3</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="I3" s="145"/>
+        <v>167</v>
+      </c>
+      <c r="I3" s="150"/>
       <c r="J3" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K3" s="4">
         <v>2</v>
@@ -6869,26 +6869,26 @@
     </row>
     <row r="4" spans="1:12" ht="60">
       <c r="A4" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" s="158"/>
-      <c r="C4" s="148"/>
+        <v>165</v>
+      </c>
+      <c r="B4" s="160"/>
+      <c r="C4" s="153"/>
       <c r="D4" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E4" s="30">
         <v>2</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="I4" s="154"/>
+        <v>163</v>
+      </c>
+      <c r="I4" s="147"/>
       <c r="J4" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K4" s="7">
         <v>2</v>
@@ -6896,26 +6896,26 @@
     </row>
     <row r="5" spans="1:12" ht="45">
       <c r="A5" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B5" s="158"/>
-      <c r="C5" s="148"/>
+        <v>162</v>
+      </c>
+      <c r="B5" s="160"/>
+      <c r="C5" s="153"/>
       <c r="D5" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E5" s="20">
         <v>3</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="I5" s="154"/>
+        <v>160</v>
+      </c>
+      <c r="I5" s="147"/>
       <c r="J5" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K5" s="4">
         <v>3</v>
@@ -6923,26 +6923,26 @@
     </row>
     <row r="6" spans="1:12" ht="60" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B6" s="158"/>
-      <c r="C6" s="148"/>
+        <v>158</v>
+      </c>
+      <c r="B6" s="160"/>
+      <c r="C6" s="153"/>
       <c r="D6" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E6" s="30">
         <v>1</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="I6" s="154"/>
+        <v>156</v>
+      </c>
+      <c r="I6" s="147"/>
       <c r="J6" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K6" s="4">
         <v>2</v>
@@ -6950,26 +6950,26 @@
     </row>
     <row r="7" spans="1:12" ht="75" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B7" s="158"/>
-      <c r="C7" s="148"/>
+        <v>154</v>
+      </c>
+      <c r="B7" s="160"/>
+      <c r="C7" s="153"/>
       <c r="D7" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E7" s="7">
         <v>2</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="I7" s="154"/>
+        <v>153</v>
+      </c>
+      <c r="I7" s="147"/>
       <c r="J7" s="29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K7" s="4">
         <v>2</v>
@@ -6977,28 +6977,28 @@
     </row>
     <row r="8" spans="1:12" ht="75" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B8" s="158"/>
-      <c r="C8" s="152" t="s">
-        <v>87</v>
+        <v>200</v>
+      </c>
+      <c r="B8" s="160"/>
+      <c r="C8" s="145" t="s">
+        <v>85</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E8" s="7">
         <v>5</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="I8" s="154"/>
+        <v>149</v>
+      </c>
+      <c r="I8" s="147"/>
       <c r="J8" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K8" s="7">
         <v>2</v>
@@ -7006,28 +7006,28 @@
     </row>
     <row r="9" spans="1:12" ht="45" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="C9" s="152"/>
+        <v>151</v>
+      </c>
+      <c r="C9" s="145"/>
       <c r="D9" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E9" s="30">
         <v>2</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I9" s="147"/>
+      <c r="J9" s="29" t="s">
         <v>207</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="I9" s="154"/>
-      <c r="J9" s="29" t="s">
-        <v>209</v>
       </c>
       <c r="K9" s="4">
         <v>3</v>
@@ -7035,99 +7035,99 @@
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E10" s="30">
         <v>2</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="I10" s="159"/>
+        <v>143</v>
+      </c>
+      <c r="I10" s="151"/>
       <c r="J10" s="29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K10" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1">
-      <c r="A11" s="128" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11" s="154" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11" s="152" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="137" t="s">
+      <c r="A11" s="139" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="150">
+      <c r="B11" s="147" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="145" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="155">
         <v>3</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="132" t="s">
-        <v>140</v>
-      </c>
-      <c r="H11" s="132"/>
-      <c r="I11" s="132"/>
-      <c r="J11" s="132"/>
-      <c r="K11" s="132"/>
+      <c r="G11" s="129" t="s">
+        <v>138</v>
+      </c>
+      <c r="H11" s="129"/>
+      <c r="I11" s="129"/>
+      <c r="J11" s="129"/>
+      <c r="K11" s="129"/>
     </row>
     <row r="12" spans="1:12" ht="45" customHeight="1">
-      <c r="A12" s="156"/>
-      <c r="B12" s="155"/>
-      <c r="C12" s="153"/>
-      <c r="D12" s="149"/>
-      <c r="E12" s="151"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="157"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="154"/>
+      <c r="E12" s="156"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="62" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K12" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1">
-      <c r="A13" s="139" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="139"/>
-      <c r="C13" s="139"/>
-      <c r="D13" s="139"/>
-      <c r="E13" s="139"/>
+      <c r="A13" s="131" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="131"/>
+      <c r="C13" s="131"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="131"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="54" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K13" s="7">
         <v>1</v>
@@ -7135,30 +7135,30 @@
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="147" t="s">
-        <v>87</v>
+        <v>130</v>
+      </c>
+      <c r="C14" s="149" t="s">
+        <v>85</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E14" s="20">
         <v>1</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="54">
         <v>0</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K14" s="7">
         <v>1</v>
@@ -7166,260 +7166,260 @@
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="152"/>
+        <v>124</v>
+      </c>
+      <c r="C15" s="145"/>
       <c r="D15" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E15" s="20">
         <v>1</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H15" s="28"/>
       <c r="I15" s="62" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K15" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="128" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" s="154" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="152"/>
-      <c r="D16" s="137" t="s">
+      <c r="A16" s="139" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="160">
+      <c r="B16" s="147" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="145"/>
+      <c r="D16" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="148">
         <v>1</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="132" t="s">
-        <v>118</v>
-      </c>
-      <c r="H16" s="132"/>
-      <c r="I16" s="132"/>
-      <c r="J16" s="132"/>
-      <c r="K16" s="132"/>
+      <c r="G16" s="129" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="129"/>
+      <c r="I16" s="129"/>
+      <c r="J16" s="129"/>
+      <c r="K16" s="129"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
-      <c r="A17" s="128"/>
-      <c r="B17" s="154"/>
-      <c r="C17" s="152"/>
-      <c r="D17" s="137"/>
-      <c r="E17" s="160"/>
+      <c r="A17" s="139"/>
+      <c r="B17" s="147"/>
+      <c r="C17" s="145"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="148"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H17" s="12"/>
-      <c r="I17" s="145"/>
+      <c r="I17" s="150"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="152"/>
+        <v>113</v>
+      </c>
+      <c r="C18" s="145"/>
       <c r="D18" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E18" s="20">
         <v>1</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="154"/>
+      <c r="I18" s="147"/>
       <c r="K18"/>
     </row>
     <row r="19" spans="1:11" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" s="152" t="s">
-        <v>131</v>
+        <v>109</v>
+      </c>
+      <c r="C19" s="145" t="s">
+        <v>129</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E19" s="20">
         <v>2</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="I19" s="154"/>
+      <c r="I19" s="147"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="30">
       <c r="A20" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="152"/>
+        <v>105</v>
+      </c>
+      <c r="C20" s="145"/>
       <c r="D20" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E20" s="20">
         <v>3</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="154"/>
+      <c r="I20" s="147"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="45">
       <c r="A21" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="152"/>
+        <v>101</v>
+      </c>
+      <c r="C21" s="145"/>
       <c r="D21" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E21" s="20">
         <v>4</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H21" s="12"/>
-      <c r="I21" s="154"/>
+      <c r="I21" s="147"/>
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="152"/>
+        <v>97</v>
+      </c>
+      <c r="C22" s="145"/>
       <c r="D22" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E22" s="20">
         <v>3</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="I22" s="154"/>
+      <c r="I22" s="147"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C23" s="153"/>
+        <v>93</v>
+      </c>
+      <c r="C23" s="146"/>
       <c r="D23" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E23" s="20">
         <v>2</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H23" s="12"/>
-      <c r="I23" s="154"/>
+      <c r="I23" s="147"/>
       <c r="J23" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1">
-      <c r="A24" s="139" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="139"/>
-      <c r="C24" s="139"/>
-      <c r="D24" s="139"/>
-      <c r="E24" s="139"/>
+      <c r="A24" s="131" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="131"/>
+      <c r="C24" s="131"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="131"/>
       <c r="F24" s="4"/>
       <c r="G24" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H24" s="12"/>
-      <c r="I24" s="154"/>
+      <c r="I24" s="147"/>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="147" t="s">
-        <v>416</v>
+        <v>86</v>
+      </c>
+      <c r="C25" s="149" t="s">
+        <v>414</v>
       </c>
       <c r="D25" s="63" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E25" s="26">
         <v>2</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="154"/>
+      <c r="I25" s="147"/>
       <c r="J25" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K25" s="25"/>
     </row>
     <row r="26" spans="1:11" ht="45">
       <c r="A26" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B26" s="100" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="148"/>
+        <v>83</v>
+      </c>
+      <c r="C26" s="153"/>
       <c r="D26" s="44" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E26" s="45">
         <v>3</v>
@@ -7427,54 +7427,54 @@
       <c r="F26" s="4"/>
       <c r="G26" s="15"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="154"/>
+      <c r="I26" s="147"/>
       <c r="J26" s="12"/>
       <c r="K26" s="25"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>480</v>
+      </c>
+      <c r="C27" s="101" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="44" t="s">
         <v>479</v>
-      </c>
-      <c r="B27" s="47" t="s">
-        <v>482</v>
-      </c>
-      <c r="C27" s="101" t="s">
-        <v>194</v>
-      </c>
-      <c r="D27" s="44" t="s">
-        <v>481</v>
       </c>
       <c r="E27" s="45">
         <v>1</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="154"/>
+      <c r="I27" s="147"/>
       <c r="K27" s="23"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B28" s="100"/>
       <c r="C28" s="109"/>
       <c r="D28" s="44" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E28" s="45">
         <v>3</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="154"/>
+      <c r="I28" s="147"/>
       <c r="J28" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K28" s="7"/>
     </row>
@@ -7482,46 +7482,46 @@
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I29" s="154"/>
+        <v>80</v>
+      </c>
+      <c r="I29" s="147"/>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11">
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I30" s="159"/>
+        <v>79</v>
+      </c>
+      <c r="I30" s="151"/>
       <c r="J30" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K30" s="4"/>
     </row>
     <row r="31" spans="1:11">
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="132" t="s">
-        <v>80</v>
-      </c>
-      <c r="H31" s="132"/>
-      <c r="I31" s="132"/>
-      <c r="J31" s="132"/>
-      <c r="K31" s="132"/>
+      <c r="G31" s="129" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" s="129"/>
+      <c r="I31" s="129"/>
+      <c r="J31" s="129"/>
+      <c r="K31" s="129"/>
     </row>
     <row r="32" spans="1:11" ht="30">
       <c r="D32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H32" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="I32" s="145"/>
+        <v>76</v>
+      </c>
+      <c r="I32" s="150"/>
       <c r="J32" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K32" s="7">
         <v>1</v>
@@ -7531,14 +7531,14 @@
       <c r="D33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H33" s="98" t="s">
-        <v>75</v>
-      </c>
-      <c r="I33" s="146"/>
+        <v>73</v>
+      </c>
+      <c r="I33" s="152"/>
       <c r="J33" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K33" s="7">
         <v>-1</v>
@@ -7548,16 +7548,16 @@
       <c r="D34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H34" s="98" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I34" s="70" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K34" s="4"/>
     </row>
@@ -7565,16 +7565,16 @@
       <c r="D35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H35" s="98" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I35" s="70" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K35" s="4"/>
     </row>
@@ -7582,16 +7582,16 @@
       <c r="D36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H36" s="100" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I36" s="73" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J36" s="44" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="K36" s="42"/>
     </row>
@@ -7599,16 +7599,16 @@
       <c r="D37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H37" s="72" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I37" s="56">
         <v>0</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K37" s="24">
         <v>5</v>
@@ -7729,15 +7729,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="I17:I30"/>
-    <mergeCell ref="A24:E24"/>
     <mergeCell ref="G31:K31"/>
     <mergeCell ref="I32:I33"/>
     <mergeCell ref="A2:E2"/>
@@ -7754,6 +7745,15 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="I3:I10"/>
     <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="I17:I30"/>
+    <mergeCell ref="A24:E24"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7766,7 +7766,7 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7787,130 +7787,130 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="49" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B2" s="162"/>
       <c r="C2" s="161" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="48" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H2" s="165"/>
       <c r="I2" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K2" s="40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L2" s="32"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B3" s="163"/>
-      <c r="C3" s="152"/>
+      <c r="C3" s="145"/>
       <c r="D3" s="7"/>
       <c r="E3" s="40" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H3" s="166"/>
       <c r="I3" s="21">
         <v>0</v>
       </c>
       <c r="K3" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1">
       <c r="A4" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4" s="163"/>
-      <c r="C4" s="152" t="s">
-        <v>194</v>
+      <c r="C4" s="145" t="s">
+        <v>192</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H4" s="167"/>
       <c r="I4" s="38" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K4" s="41" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B5" s="163"/>
-      <c r="C5" s="152"/>
+      <c r="C5" s="145"/>
       <c r="D5" s="7"/>
       <c r="E5" s="40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B6" s="163"/>
       <c r="C6" s="22">
@@ -7925,15 +7925,15 @@
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B7" s="163"/>
-      <c r="C7" s="152" t="s">
-        <v>194</v>
+      <c r="C7" s="145" t="s">
+        <v>192</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F7" s="4"/>
       <c r="J7" s="29"/>
@@ -7941,13 +7941,13 @@
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B8" s="163"/>
-      <c r="C8" s="152"/>
+      <c r="C8" s="145"/>
       <c r="D8" s="7"/>
       <c r="E8" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="32"/>
@@ -7958,15 +7958,15 @@
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B9" s="163"/>
       <c r="C9" s="22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="39" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F9" s="4"/>
       <c r="H9" s="11"/>
@@ -7975,15 +7975,15 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B10" s="163"/>
       <c r="C10" s="22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="39" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F10" s="4"/>
       <c r="H10" s="11"/>
@@ -7992,17 +7992,17 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B11" s="163"/>
       <c r="C11" s="21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F11" s="4"/>
       <c r="H11" s="11"/>
@@ -8011,15 +8011,15 @@
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A12" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B12" s="164"/>
       <c r="C12" s="38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="37" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F12" s="4"/>
       <c r="H12" s="28"/>
@@ -8355,64 +8355,64 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K1" s="116" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="139" t="s">
-        <v>449</v>
-      </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="G2" s="139" t="s">
-        <v>470</v>
-      </c>
-      <c r="H2" s="139"/>
-      <c r="I2" s="139"/>
-      <c r="J2" s="139"/>
-      <c r="K2" s="139"/>
+      <c r="A2" s="131" t="s">
+        <v>447</v>
+      </c>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="G2" s="131" t="s">
+        <v>468</v>
+      </c>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B3" s="168" t="s">
-        <v>455</v>
-      </c>
-      <c r="C3" s="147" t="s">
-        <v>194</v>
+        <v>453</v>
+      </c>
+      <c r="C3" s="149" t="s">
+        <v>192</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E3" s="111">
         <v>2</v>
@@ -8425,12 +8425,12 @@
     </row>
     <row r="4" spans="1:11" ht="30">
       <c r="A4" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B4" s="169"/>
-      <c r="C4" s="148"/>
+      <c r="C4" s="153"/>
       <c r="D4" s="44" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E4" s="112">
         <v>1</v>
@@ -8444,14 +8444,14 @@
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B5" s="169"/>
       <c r="C5" s="76" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E5" s="113">
         <v>4</v>
@@ -8465,16 +8465,16 @@
     </row>
     <row r="6" spans="1:11" ht="45">
       <c r="A6" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B6" s="86" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C6" s="76" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E6" s="64">
         <v>3</v>
@@ -8487,13 +8487,13 @@
       <c r="K6" s="44"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="139" t="s">
-        <v>469</v>
-      </c>
-      <c r="B7" s="139"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="139"/>
+      <c r="A7" s="131" t="s">
+        <v>467</v>
+      </c>
+      <c r="B7" s="131"/>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
       <c r="F7" s="51"/>
       <c r="G7" s="42"/>
       <c r="H7" s="42"/>
@@ -8503,13 +8503,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C8" s="76" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="112">
@@ -8524,16 +8524,16 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C9" s="76" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E9" s="112">
         <v>3</v>
@@ -8547,13 +8547,13 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1">
       <c r="A10" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C10" s="97" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="124">
@@ -8899,44 +8899,44 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30">
       <c r="A2" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -8944,52 +8944,52 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1">
       <c r="A6" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="F7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60">
       <c r="F8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60">
       <c r="F9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -9020,63 +9020,63 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="125" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F2" s="125" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="122" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F3" s="122" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="122" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F4" s="126" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G4" s="123"/>
       <c r="H4" s="123" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I4" s="123"/>
       <c r="J4" s="123"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="122" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
@@ -9085,7 +9085,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="126" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B6" s="123"/>
       <c r="C6" s="123"/>
@@ -9103,16 +9103,16 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F8" s="52"/>
       <c r="G8" s="52"/>
@@ -9121,7 +9121,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="125" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
@@ -9130,12 +9130,12 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="122" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="126" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B11" s="123"/>
       <c r="C11" s="123"/>

</xml_diff>

<commit_message>
tweaked a few things.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Git Repositories\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB9AFBD-7A2F-4D89-9A99-8D6E5DE335D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B936B3-E450-4E6C-8154-CBD333DEF9E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="394" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
@@ -7031,59 +7031,83 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -7091,6 +7115,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7103,41 +7133,26 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7145,18 +7160,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -7171,33 +7198,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7524,8 +7524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
   <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7632,54 +7632,54 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="15" customHeight="1">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="148" t="s">
         <v>342</v>
       </c>
-      <c r="B2" s="157"/>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
-      <c r="F2" s="152" t="s">
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="F2" s="149" t="s">
         <v>570</v>
       </c>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="K2" s="152" t="s">
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="K2" s="149" t="s">
         <v>413</v>
       </c>
-      <c r="L2" s="152"/>
-      <c r="M2" s="152"/>
-      <c r="N2" s="152"/>
-      <c r="P2" s="146" t="s">
+      <c r="L2" s="149"/>
+      <c r="M2" s="149"/>
+      <c r="N2" s="149"/>
+      <c r="P2" s="154" t="s">
         <v>168</v>
       </c>
-      <c r="Q2" s="148" t="s">
+      <c r="Q2" s="156" t="s">
         <v>205</v>
       </c>
-      <c r="R2" s="149" t="s">
+      <c r="R2" s="157" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="149" t="s">
+      <c r="S2" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="U2" s="146" t="s">
+      <c r="U2" s="154" t="s">
         <v>186</v>
       </c>
-      <c r="V2" s="148" t="s">
+      <c r="V2" s="156" t="s">
         <v>360</v>
       </c>
-      <c r="W2" s="149" t="s">
+      <c r="W2" s="157" t="s">
         <v>181</v>
       </c>
-      <c r="X2" s="149" t="s">
+      <c r="X2" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="Z2" s="152" t="s">
+      <c r="Z2" s="149" t="s">
         <v>226</v>
       </c>
-      <c r="AA2" s="152"/>
-      <c r="AB2" s="152"/>
-      <c r="AC2" s="152"/>
+      <c r="AA2" s="149"/>
+      <c r="AB2" s="149"/>
+      <c r="AC2" s="149"/>
     </row>
     <row r="3" spans="1:29" ht="105">
       <c r="A3" s="10" t="s">
@@ -7716,14 +7716,14 @@
         <v>423</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="P3" s="147"/>
-      <c r="Q3" s="144"/>
-      <c r="R3" s="150"/>
-      <c r="S3" s="150"/>
-      <c r="U3" s="147"/>
-      <c r="V3" s="144"/>
-      <c r="W3" s="150"/>
-      <c r="X3" s="150"/>
+      <c r="P3" s="155"/>
+      <c r="Q3" s="143"/>
+      <c r="R3" s="158"/>
+      <c r="S3" s="158"/>
+      <c r="U3" s="155"/>
+      <c r="V3" s="143"/>
+      <c r="W3" s="158"/>
+      <c r="X3" s="158"/>
       <c r="Z3" s="10" t="s">
         <v>591</v>
       </c>
@@ -7882,66 +7882,66 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1">
-      <c r="A6" s="143" t="s">
+      <c r="A6" s="146" t="s">
         <v>259</v>
       </c>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="143" t="s">
         <v>328</v>
       </c>
-      <c r="C6" s="145" t="s">
+      <c r="C6" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="145" t="s">
+      <c r="D6" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="151" t="s">
+      <c r="F6" s="144" t="s">
         <v>569</v>
       </c>
-      <c r="G6" s="151"/>
-      <c r="H6" s="151"/>
-      <c r="I6" s="151"/>
-      <c r="K6" s="151" t="s">
+      <c r="G6" s="144"/>
+      <c r="H6" s="144"/>
+      <c r="I6" s="144"/>
+      <c r="K6" s="144" t="s">
         <v>301</v>
       </c>
-      <c r="L6" s="151"/>
-      <c r="M6" s="151"/>
-      <c r="N6" s="151"/>
-      <c r="P6" s="147" t="s">
+      <c r="L6" s="144"/>
+      <c r="M6" s="144"/>
+      <c r="N6" s="144"/>
+      <c r="P6" s="155" t="s">
         <v>178</v>
       </c>
-      <c r="Q6" s="144" t="s">
+      <c r="Q6" s="143" t="s">
         <v>208</v>
       </c>
-      <c r="R6" s="145" t="s">
+      <c r="R6" s="142" t="s">
         <v>182</v>
       </c>
-      <c r="S6" s="145" t="s">
+      <c r="S6" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="U6" s="147" t="s">
+      <c r="U6" s="155" t="s">
         <v>189</v>
       </c>
-      <c r="V6" s="144" t="s">
+      <c r="V6" s="143" t="s">
         <v>212</v>
       </c>
-      <c r="W6" s="145" t="s">
+      <c r="W6" s="142" t="s">
         <v>182</v>
       </c>
-      <c r="X6" s="145" t="s">
+      <c r="X6" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="Z6" s="151" t="s">
+      <c r="Z6" s="144" t="s">
         <v>230</v>
       </c>
-      <c r="AA6" s="151"/>
-      <c r="AB6" s="151"/>
-      <c r="AC6" s="151"/>
+      <c r="AA6" s="144"/>
+      <c r="AB6" s="144"/>
+      <c r="AC6" s="144"/>
     </row>
     <row r="7" spans="1:29" ht="120" customHeight="1">
-      <c r="A7" s="143"/>
-      <c r="B7" s="144"/>
-      <c r="C7" s="145"/>
-      <c r="D7" s="145"/>
+      <c r="A7" s="146"/>
+      <c r="B7" s="143"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="142"/>
       <c r="F7" s="9" t="s">
         <v>248</v>
       </c>
@@ -7964,14 +7964,14 @@
         <v>424</v>
       </c>
       <c r="N7" s="84"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="144"/>
-      <c r="R7" s="145"/>
-      <c r="S7" s="145"/>
-      <c r="U7" s="147"/>
-      <c r="V7" s="144"/>
-      <c r="W7" s="145"/>
-      <c r="X7" s="145"/>
+      <c r="P7" s="155"/>
+      <c r="Q7" s="143"/>
+      <c r="R7" s="142"/>
+      <c r="S7" s="142"/>
+      <c r="U7" s="155"/>
+      <c r="V7" s="143"/>
+      <c r="W7" s="142"/>
+      <c r="X7" s="142"/>
       <c r="Z7" s="10" t="s">
         <v>231</v>
       </c>
@@ -8135,52 +8135,52 @@
       </c>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1">
-      <c r="A11" s="143" t="s">
+      <c r="A11" s="146" t="s">
         <v>394</v>
       </c>
-      <c r="B11" s="144" t="s">
+      <c r="B11" s="143" t="s">
         <v>331</v>
       </c>
-      <c r="C11" s="145" t="s">
+      <c r="C11" s="142" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="145" t="s">
+      <c r="D11" s="142" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="143" t="s">
+      <c r="F11" s="146" t="s">
         <v>245</v>
       </c>
-      <c r="G11" s="144" t="s">
+      <c r="G11" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="159" t="s">
+      <c r="H11" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="159" t="s">
+      <c r="I11" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="151" t="s">
+      <c r="K11" s="144" t="s">
         <v>338</v>
       </c>
-      <c r="L11" s="151"/>
-      <c r="M11" s="151"/>
-      <c r="N11" s="151"/>
-      <c r="Z11" s="151" t="s">
+      <c r="L11" s="144"/>
+      <c r="M11" s="144"/>
+      <c r="N11" s="144"/>
+      <c r="Z11" s="144" t="s">
         <v>227</v>
       </c>
-      <c r="AA11" s="151"/>
-      <c r="AB11" s="151"/>
-      <c r="AC11" s="151"/>
+      <c r="AA11" s="144"/>
+      <c r="AB11" s="144"/>
+      <c r="AC11" s="144"/>
     </row>
     <row r="12" spans="1:29" ht="75" customHeight="1">
-      <c r="A12" s="143"/>
-      <c r="B12" s="144"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="145"/>
-      <c r="F12" s="143"/>
-      <c r="G12" s="144"/>
-      <c r="H12" s="159"/>
-      <c r="I12" s="159"/>
+      <c r="A12" s="146"/>
+      <c r="B12" s="143"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="142"/>
+      <c r="F12" s="146"/>
+      <c r="G12" s="143"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="147"/>
       <c r="K12" s="9" t="s">
         <v>321</v>
       </c>
@@ -8235,40 +8235,40 @@
       <c r="AC13" s="40"/>
     </row>
     <row r="14" spans="1:29" ht="15" customHeight="1">
-      <c r="A14" s="143" t="s">
+      <c r="A14" s="146" t="s">
         <v>398</v>
       </c>
-      <c r="B14" s="144" t="s">
+      <c r="B14" s="143" t="s">
         <v>333</v>
       </c>
-      <c r="C14" s="145" t="s">
+      <c r="C14" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="145" t="s">
+      <c r="D14" s="142" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="151" t="s">
+      <c r="F14" s="144" t="s">
         <v>571</v>
       </c>
-      <c r="G14" s="151"/>
-      <c r="H14" s="151"/>
-      <c r="I14" s="151"/>
-      <c r="K14" s="153" t="s">
+      <c r="G14" s="144"/>
+      <c r="H14" s="144"/>
+      <c r="I14" s="144"/>
+      <c r="K14" s="150" t="s">
         <v>326</v>
       </c>
-      <c r="L14" s="154"/>
-      <c r="M14" s="155"/>
-      <c r="N14" s="156"/>
+      <c r="L14" s="151"/>
+      <c r="M14" s="152"/>
+      <c r="N14" s="153"/>
       <c r="Z14" s="40"/>
       <c r="AA14" s="79"/>
       <c r="AB14" s="40"/>
       <c r="AC14" s="40"/>
     </row>
     <row r="15" spans="1:29" ht="75" customHeight="1">
-      <c r="A15" s="143"/>
-      <c r="B15" s="144"/>
-      <c r="C15" s="145"/>
-      <c r="D15" s="145"/>
+      <c r="A15" s="146"/>
+      <c r="B15" s="143"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="142"/>
       <c r="F15" s="9" t="s">
         <v>243</v>
       </c>
@@ -8281,10 +8281,10 @@
       <c r="I15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="153"/>
-      <c r="L15" s="154"/>
-      <c r="M15" s="155"/>
-      <c r="N15" s="156"/>
+      <c r="K15" s="150"/>
+      <c r="L15" s="151"/>
+      <c r="M15" s="152"/>
+      <c r="N15" s="153"/>
       <c r="Z15" s="40"/>
       <c r="AA15" s="122"/>
       <c r="AB15" s="122"/>
@@ -8350,22 +8350,22 @@
       <c r="K17" s="127"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1">
-      <c r="A18" s="142" t="s">
+      <c r="A18" s="159" t="s">
         <v>343</v>
       </c>
-      <c r="B18" s="142"/>
-      <c r="C18" s="142"/>
-      <c r="D18" s="142"/>
-      <c r="F18" s="143" t="s">
+      <c r="B18" s="159"/>
+      <c r="C18" s="159"/>
+      <c r="D18" s="159"/>
+      <c r="F18" s="146" t="s">
         <v>240</v>
       </c>
-      <c r="G18" s="144" t="s">
+      <c r="G18" s="143" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="158" t="s">
+      <c r="H18" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="158" t="s">
+      <c r="I18" s="145" t="s">
         <v>39</v>
       </c>
       <c r="K18" s="46"/>
@@ -8384,37 +8384,37 @@
       <c r="D19" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="143"/>
-      <c r="G19" s="144"/>
-      <c r="H19" s="158"/>
-      <c r="I19" s="158"/>
+      <c r="F19" s="146"/>
+      <c r="G19" s="143"/>
+      <c r="H19" s="145"/>
+      <c r="I19" s="145"/>
       <c r="K19" s="46"/>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1">
-      <c r="A20" s="143" t="s">
+      <c r="A20" s="146" t="s">
         <v>264</v>
       </c>
-      <c r="B20" s="144" t="s">
+      <c r="B20" s="143" t="s">
         <v>425</v>
       </c>
-      <c r="C20" s="145" t="s">
+      <c r="C20" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="145" t="s">
+      <c r="D20" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="151" t="s">
+      <c r="F20" s="144" t="s">
         <v>339</v>
       </c>
-      <c r="G20" s="151"/>
-      <c r="H20" s="151"/>
-      <c r="I20" s="151"/>
+      <c r="G20" s="144"/>
+      <c r="H20" s="144"/>
+      <c r="I20" s="144"/>
     </row>
     <row r="21" spans="1:16" ht="105" customHeight="1">
-      <c r="A21" s="143"/>
-      <c r="B21" s="144"/>
-      <c r="C21" s="145"/>
-      <c r="D21" s="145"/>
+      <c r="A21" s="146"/>
+      <c r="B21" s="143"/>
+      <c r="C21" s="142"/>
+      <c r="D21" s="142"/>
       <c r="F21" s="7" t="s">
         <v>286</v>
       </c>
@@ -8677,12 +8677,12 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="142" t="s">
+      <c r="A37" s="159" t="s">
         <v>344</v>
       </c>
-      <c r="B37" s="142"/>
-      <c r="C37" s="142"/>
-      <c r="D37" s="142"/>
+      <c r="B37" s="159"/>
+      <c r="C37" s="159"/>
+      <c r="D37" s="159"/>
     </row>
     <row r="38" spans="1:4" ht="60">
       <c r="A38" s="10" t="s">
@@ -8797,12 +8797,12 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="142" t="s">
+      <c r="A46" s="159" t="s">
         <v>345</v>
       </c>
-      <c r="B46" s="142"/>
-      <c r="C46" s="142"/>
-      <c r="D46" s="142"/>
+      <c r="B46" s="159"/>
+      <c r="C46" s="159"/>
+      <c r="D46" s="159"/>
     </row>
     <row r="47" spans="1:4" ht="60" customHeight="1">
       <c r="A47" s="72" t="s">
@@ -8847,12 +8847,12 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1">
-      <c r="A50" s="142" t="s">
+      <c r="A50" s="159" t="s">
         <v>346</v>
       </c>
-      <c r="B50" s="142"/>
-      <c r="C50" s="142"/>
-      <c r="D50" s="142"/>
+      <c r="B50" s="159"/>
+      <c r="C50" s="159"/>
+      <c r="D50" s="159"/>
     </row>
     <row r="51" spans="1:4" ht="75" customHeight="1">
       <c r="A51" s="107" t="s">
@@ -8911,12 +8911,12 @@
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="142" t="s">
+      <c r="A55" s="159" t="s">
         <v>348</v>
       </c>
-      <c r="B55" s="142"/>
-      <c r="C55" s="142"/>
-      <c r="D55" s="142"/>
+      <c r="B55" s="159"/>
+      <c r="C55" s="159"/>
+      <c r="D55" s="159"/>
     </row>
     <row r="56" spans="1:4" ht="30">
       <c r="A56" s="69" t="s">
@@ -8989,12 +8989,12 @@
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="142" t="s">
+      <c r="A61" s="159" t="s">
         <v>204</v>
       </c>
-      <c r="B61" s="142"/>
-      <c r="C61" s="142"/>
-      <c r="D61" s="142"/>
+      <c r="B61" s="159"/>
+      <c r="C61" s="159"/>
+      <c r="D61" s="159"/>
     </row>
     <row r="62" spans="1:4" ht="105">
       <c r="A62" s="69" t="s">
@@ -9067,12 +9067,12 @@
       </c>
     </row>
     <row r="67" spans="1:29">
-      <c r="A67" s="142" t="s">
+      <c r="A67" s="159" t="s">
         <v>347</v>
       </c>
-      <c r="B67" s="142"/>
-      <c r="C67" s="142"/>
-      <c r="D67" s="142"/>
+      <c r="B67" s="159"/>
+      <c r="C67" s="159"/>
+      <c r="D67" s="159"/>
     </row>
     <row r="68" spans="1:29" ht="90">
       <c r="A68" s="107" t="s">
@@ -9146,41 +9146,17 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A55:D55"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
@@ -9197,17 +9173,41 @@
     <mergeCell ref="X6:X7"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="P6:P7"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9273,31 +9273,31 @@
       <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="148" t="s">
         <v>412</v>
       </c>
-      <c r="B2" s="157"/>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
       <c r="F2" s="18"/>
-      <c r="G2" s="160" t="s">
+      <c r="G2" s="168" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
-      <c r="J2" s="160"/>
-      <c r="K2" s="160"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="168"/>
+      <c r="J2" s="168"/>
+      <c r="K2" s="168"/>
       <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:12" ht="60" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="174" t="s">
+      <c r="B3" s="162" t="s">
         <v>470</v>
       </c>
-      <c r="C3" s="161" t="s">
+      <c r="C3" s="169" t="s">
         <v>104</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -9313,7 +9313,7 @@
       <c r="H3" s="116" t="s">
         <v>138</v>
       </c>
-      <c r="I3" s="169"/>
+      <c r="I3" s="160"/>
       <c r="J3" s="7" t="s">
         <v>137</v>
       </c>
@@ -9325,8 +9325,8 @@
       <c r="A4" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B4" s="175"/>
-      <c r="C4" s="162"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="172"/>
       <c r="D4" s="7" t="s">
         <v>369</v>
       </c>
@@ -9340,7 +9340,7 @@
       <c r="H4" s="116" t="s">
         <v>134</v>
       </c>
-      <c r="I4" s="170"/>
+      <c r="I4" s="177"/>
       <c r="J4" s="7" t="s">
         <v>120</v>
       </c>
@@ -9352,8 +9352,8 @@
       <c r="A5" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="175"/>
-      <c r="C5" s="162"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="172"/>
       <c r="D5" s="7" t="s">
         <v>372</v>
       </c>
@@ -9367,7 +9367,7 @@
       <c r="H5" s="116" t="s">
         <v>131</v>
       </c>
-      <c r="I5" s="170"/>
+      <c r="I5" s="177"/>
       <c r="J5" s="7" t="s">
         <v>130</v>
       </c>
@@ -9379,8 +9379,8 @@
       <c r="A6" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="175"/>
-      <c r="C6" s="162"/>
+      <c r="B6" s="163"/>
+      <c r="C6" s="172"/>
       <c r="D6" s="7" t="s">
         <v>371</v>
       </c>
@@ -9394,7 +9394,7 @@
       <c r="H6" s="116" t="s">
         <v>127</v>
       </c>
-      <c r="I6" s="170"/>
+      <c r="I6" s="177"/>
       <c r="J6" s="7" t="s">
         <v>126</v>
       </c>
@@ -9406,8 +9406,8 @@
       <c r="A7" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="175"/>
-      <c r="C7" s="162"/>
+      <c r="B7" s="163"/>
+      <c r="C7" s="172"/>
       <c r="D7" s="7" t="s">
         <v>370</v>
       </c>
@@ -9421,7 +9421,7 @@
       <c r="H7" s="116" t="s">
         <v>124</v>
       </c>
-      <c r="I7" s="170"/>
+      <c r="I7" s="177"/>
       <c r="J7" s="25" t="s">
         <v>115</v>
       </c>
@@ -9433,7 +9433,7 @@
       <c r="A8" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="175"/>
+      <c r="B8" s="163"/>
       <c r="C8" s="166" t="s">
         <v>70</v>
       </c>
@@ -9450,7 +9450,7 @@
       <c r="H8" s="116" t="s">
         <v>121</v>
       </c>
-      <c r="I8" s="170"/>
+      <c r="I8" s="177"/>
       <c r="J8" s="7" t="s">
         <v>120</v>
       </c>
@@ -9462,7 +9462,7 @@
       <c r="A9" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="175"/>
+      <c r="B9" s="163"/>
       <c r="C9" s="166"/>
       <c r="D9" s="7" t="s">
         <v>122</v>
@@ -9477,7 +9477,7 @@
       <c r="H9" s="116" t="s">
         <v>586</v>
       </c>
-      <c r="I9" s="170"/>
+      <c r="I9" s="177"/>
       <c r="J9" s="25" t="s">
         <v>164</v>
       </c>
@@ -9489,7 +9489,7 @@
       <c r="A10" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="175"/>
+      <c r="B10" s="163"/>
       <c r="C10" s="50" t="s">
         <v>104</v>
       </c>
@@ -9506,7 +9506,7 @@
       <c r="H10" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="I10" s="171"/>
+      <c r="I10" s="165"/>
       <c r="J10" s="25" t="s">
         <v>115</v>
       </c>
@@ -9515,39 +9515,39 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1">
-      <c r="A11" s="147" t="s">
+      <c r="A11" s="155" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="175"/>
+      <c r="B11" s="163"/>
       <c r="C11" s="166" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="159" t="s">
+      <c r="D11" s="147" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="164" t="s">
+      <c r="E11" s="174" t="s">
         <v>156</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="151" t="s">
+      <c r="G11" s="144" t="s">
         <v>112</v>
       </c>
-      <c r="H11" s="151"/>
-      <c r="I11" s="151"/>
-      <c r="J11" s="151"/>
-      <c r="K11" s="151"/>
+      <c r="H11" s="144"/>
+      <c r="I11" s="144"/>
+      <c r="J11" s="144"/>
+      <c r="K11" s="144"/>
     </row>
     <row r="12" spans="1:12" ht="45" customHeight="1">
-      <c r="A12" s="168"/>
-      <c r="B12" s="176"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="164"/>
       <c r="C12" s="167"/>
-      <c r="D12" s="163"/>
-      <c r="E12" s="165"/>
+      <c r="D12" s="173"/>
+      <c r="E12" s="175"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="174" t="s">
+      <c r="H12" s="162" t="s">
         <v>471</v>
       </c>
       <c r="I12" s="55" t="s">
@@ -9561,18 +9561,18 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1">
-      <c r="A13" s="142" t="s">
+      <c r="A13" s="159" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="142"/>
-      <c r="C13" s="142"/>
-      <c r="D13" s="142"/>
-      <c r="E13" s="142"/>
+      <c r="B13" s="159"/>
+      <c r="C13" s="159"/>
+      <c r="D13" s="159"/>
+      <c r="E13" s="159"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H13" s="175"/>
+      <c r="H13" s="163"/>
       <c r="I13" s="49" t="s">
         <v>106</v>
       </c>
@@ -9587,10 +9587,10 @@
       <c r="A14" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="174" t="s">
+      <c r="B14" s="162" t="s">
         <v>470</v>
       </c>
-      <c r="C14" s="161" t="s">
+      <c r="C14" s="169" t="s">
         <v>70</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -9603,7 +9603,7 @@
       <c r="G14" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H14" s="175"/>
+      <c r="H14" s="163"/>
       <c r="I14" s="49">
         <v>0</v>
       </c>
@@ -9618,7 +9618,7 @@
       <c r="A15" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="175"/>
+      <c r="B15" s="163"/>
       <c r="C15" s="166"/>
       <c r="D15" s="11" t="s">
         <v>99</v>
@@ -9630,7 +9630,7 @@
       <c r="G15" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="H15" s="176"/>
+      <c r="H15" s="164"/>
       <c r="I15" s="55" t="s">
         <v>97</v>
       </c>
@@ -9642,40 +9642,40 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="147" t="s">
+      <c r="A16" s="155" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="175"/>
+      <c r="B16" s="163"/>
       <c r="C16" s="166"/>
-      <c r="D16" s="159" t="s">
+      <c r="D16" s="147" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="172" t="s">
+      <c r="E16" s="171" t="s">
         <v>148</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="151" t="s">
+      <c r="G16" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="151"/>
-      <c r="I16" s="151"/>
-      <c r="J16" s="151"/>
-      <c r="K16" s="151"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
-      <c r="A17" s="147"/>
-      <c r="B17" s="175"/>
+      <c r="A17" s="155"/>
+      <c r="B17" s="163"/>
       <c r="C17" s="166"/>
-      <c r="D17" s="159"/>
-      <c r="E17" s="172"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="171"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H17" s="174" t="s">
+      <c r="H17" s="162" t="s">
         <v>470</v>
       </c>
-      <c r="I17" s="169"/>
+      <c r="I17" s="160"/>
       <c r="J17" s="7" t="s">
         <v>137</v>
       </c>
@@ -9687,7 +9687,7 @@
       <c r="A18" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="175"/>
+      <c r="B18" s="163"/>
       <c r="C18" s="166"/>
       <c r="D18" s="7" t="s">
         <v>90</v>
@@ -9699,8 +9699,8 @@
       <c r="G18" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H18" s="175"/>
-      <c r="I18" s="173"/>
+      <c r="H18" s="163"/>
+      <c r="I18" s="161"/>
       <c r="J18" s="7" t="s">
         <v>120</v>
       </c>
@@ -9712,7 +9712,7 @@
       <c r="A19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="175"/>
+      <c r="B19" s="163"/>
       <c r="C19" s="166" t="s">
         <v>104</v>
       </c>
@@ -9726,8 +9726,8 @@
       <c r="G19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="175"/>
-      <c r="I19" s="173"/>
+      <c r="H19" s="163"/>
+      <c r="I19" s="161"/>
       <c r="J19" s="7" t="s">
         <v>130</v>
       </c>
@@ -9739,7 +9739,7 @@
       <c r="A20" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="175"/>
+      <c r="B20" s="163"/>
       <c r="C20" s="166"/>
       <c r="D20" s="7" t="s">
         <v>84</v>
@@ -9751,8 +9751,8 @@
       <c r="G20" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="175"/>
-      <c r="I20" s="173"/>
+      <c r="H20" s="163"/>
+      <c r="I20" s="161"/>
       <c r="J20" s="7" t="s">
         <v>126</v>
       </c>
@@ -9764,7 +9764,7 @@
       <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="175"/>
+      <c r="B21" s="163"/>
       <c r="C21" s="166"/>
       <c r="D21" s="7" t="s">
         <v>461</v>
@@ -9776,8 +9776,8 @@
       <c r="G21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H21" s="175"/>
-      <c r="I21" s="173"/>
+      <c r="H21" s="163"/>
+      <c r="I21" s="161"/>
       <c r="J21" s="25" t="s">
         <v>115</v>
       </c>
@@ -9789,7 +9789,7 @@
       <c r="A22" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="175"/>
+      <c r="B22" s="163"/>
       <c r="C22" s="166"/>
       <c r="D22" s="7" t="s">
         <v>79</v>
@@ -9801,8 +9801,8 @@
       <c r="G22" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="H22" s="175"/>
-      <c r="I22" s="173"/>
+      <c r="H22" s="163"/>
+      <c r="I22" s="161"/>
       <c r="J22" s="7" t="s">
         <v>120</v>
       </c>
@@ -9814,7 +9814,7 @@
       <c r="A23" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="176"/>
+      <c r="B23" s="164"/>
       <c r="C23" s="167"/>
       <c r="D23" s="7" t="s">
         <v>76</v>
@@ -9826,8 +9826,8 @@
       <c r="G23" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="H23" s="175"/>
-      <c r="I23" s="173"/>
+      <c r="H23" s="163"/>
+      <c r="I23" s="161"/>
       <c r="J23" s="7" t="s">
         <v>164</v>
       </c>
@@ -9836,21 +9836,21 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1">
-      <c r="A24" s="142" t="s">
+      <c r="A24" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="142"/>
-      <c r="C24" s="142"/>
-      <c r="D24" s="142"/>
-      <c r="E24" s="142"/>
+      <c r="B24" s="159"/>
+      <c r="C24" s="159"/>
+      <c r="D24" s="159"/>
+      <c r="E24" s="159"/>
       <c r="F24" s="4"/>
       <c r="G24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="H24" s="175" t="s">
+      <c r="H24" s="163" t="s">
         <v>585</v>
       </c>
-      <c r="I24" s="173"/>
+      <c r="I24" s="161"/>
       <c r="K24" s="139" t="s">
         <v>148</v>
       </c>
@@ -9862,7 +9862,7 @@
       <c r="B25" s="118" t="s">
         <v>485</v>
       </c>
-      <c r="C25" s="161" t="s">
+      <c r="C25" s="169" t="s">
         <v>294</v>
       </c>
       <c r="D25" s="56" t="s">
@@ -9875,8 +9875,8 @@
       <c r="G25" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="H25" s="175"/>
-      <c r="I25" s="173"/>
+      <c r="H25" s="163"/>
+      <c r="I25" s="161"/>
       <c r="J25" s="12" t="s">
         <v>72</v>
       </c>
@@ -9891,7 +9891,7 @@
       <c r="B26" s="64" t="s">
         <v>469</v>
       </c>
-      <c r="C26" s="177"/>
+      <c r="C26" s="170"/>
       <c r="D26" s="17" t="s">
         <v>221</v>
       </c>
@@ -9902,10 +9902,10 @@
       <c r="G26" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H26" s="175" t="s">
+      <c r="H26" s="163" t="s">
         <v>470</v>
       </c>
-      <c r="I26" s="173"/>
+      <c r="I26" s="161"/>
       <c r="J26" s="12"/>
       <c r="K26" s="139" t="s">
         <v>148</v>
@@ -9917,8 +9917,8 @@
       <c r="G27" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H27" s="175"/>
-      <c r="I27" s="173"/>
+      <c r="H27" s="163"/>
+      <c r="I27" s="161"/>
       <c r="J27" s="7" t="s">
         <v>218</v>
       </c>
@@ -9932,8 +9932,8 @@
       <c r="G28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H28" s="175"/>
-      <c r="I28" s="173"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="161"/>
       <c r="K28" s="139" t="s">
         <v>148</v>
       </c>
@@ -9944,8 +9944,8 @@
       <c r="G29" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="H29" s="176"/>
-      <c r="I29" s="171"/>
+      <c r="H29" s="164"/>
+      <c r="I29" s="165"/>
       <c r="J29" s="7" t="s">
         <v>164</v>
       </c>
@@ -9956,13 +9956,13 @@
     <row r="30" spans="1:11">
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="151" t="s">
+      <c r="G30" s="144" t="s">
         <v>65</v>
       </c>
-      <c r="H30" s="151"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="151"/>
-      <c r="K30" s="160"/>
+      <c r="H30" s="144"/>
+      <c r="I30" s="144"/>
+      <c r="J30" s="144"/>
+      <c r="K30" s="168"/>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="D31" s="4"/>
@@ -9973,7 +9973,7 @@
       <c r="H31" s="116" t="s">
         <v>481</v>
       </c>
-      <c r="I31" s="169"/>
+      <c r="I31" s="160"/>
       <c r="J31" s="7" t="s">
         <v>63</v>
       </c>
@@ -9990,7 +9990,7 @@
       <c r="H32" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="I32" s="173"/>
+      <c r="I32" s="161"/>
       <c r="J32" s="7" t="s">
         <v>60</v>
       </c>
@@ -10168,6 +10168,22 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="I3:I10"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="I31:I32"/>
     <mergeCell ref="B3:B12"/>
     <mergeCell ref="B14:B23"/>
@@ -10180,22 +10196,6 @@
     <mergeCell ref="H17:H23"/>
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="I3:I10"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10260,21 +10260,21 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="148" t="s">
         <v>453</v>
       </c>
-      <c r="B2" s="157"/>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
       <c r="F2" s="18"/>
-      <c r="G2" s="152" t="s">
+      <c r="G2" s="149" t="s">
         <v>454</v>
       </c>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="149"/>
     </row>
     <row r="3" spans="1:11" ht="30">
       <c r="A3" s="5" t="s">
@@ -10283,7 +10283,7 @@
       <c r="B3" s="119" t="s">
         <v>481</v>
       </c>
-      <c r="C3" s="178" t="s">
+      <c r="C3" s="183" t="s">
         <v>366</v>
       </c>
       <c r="D3" s="40" t="s">
@@ -10299,7 +10299,7 @@
       <c r="H3" s="116" t="s">
         <v>482</v>
       </c>
-      <c r="I3" s="186"/>
+      <c r="I3" s="195"/>
       <c r="J3" s="40" t="s">
         <v>466</v>
       </c>
@@ -10314,7 +10314,7 @@
       <c r="B4" s="126" t="s">
         <v>483</v>
       </c>
-      <c r="C4" s="183"/>
+      <c r="C4" s="185"/>
       <c r="D4" s="40" t="s">
         <v>323</v>
       </c>
@@ -10328,32 +10328,32 @@
       <c r="H4" s="116" t="s">
         <v>482</v>
       </c>
-      <c r="I4" s="187"/>
+      <c r="I4" s="196"/>
       <c r="J4" s="40"/>
       <c r="K4" s="131" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
-      <c r="A5" s="142" t="s">
+      <c r="A5" s="159" t="s">
         <v>455</v>
       </c>
-      <c r="B5" s="142"/>
-      <c r="C5" s="142"/>
-      <c r="D5" s="142"/>
-      <c r="E5" s="142"/>
+      <c r="B5" s="159"/>
+      <c r="C5" s="159"/>
+      <c r="D5" s="159"/>
+      <c r="E5" s="159"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="150" t="s">
+      <c r="G5" s="158" t="s">
         <v>458</v>
       </c>
-      <c r="H5" s="170" t="s">
+      <c r="H5" s="177" t="s">
         <v>482</v>
       </c>
-      <c r="I5" s="187"/>
-      <c r="J5" s="158" t="s">
+      <c r="I5" s="196"/>
+      <c r="J5" s="145" t="s">
         <v>462</v>
       </c>
-      <c r="K5" s="197" t="s">
+      <c r="K5" s="190" t="s">
         <v>146</v>
       </c>
     </row>
@@ -10361,7 +10361,7 @@
       <c r="A6" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="B6" s="174" t="s">
+      <c r="B6" s="162" t="s">
         <v>468</v>
       </c>
       <c r="C6" s="120" t="s">
@@ -10374,17 +10374,17 @@
         <v>148</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="150"/>
-      <c r="H6" s="170"/>
-      <c r="I6" s="187"/>
-      <c r="J6" s="158"/>
-      <c r="K6" s="197"/>
+      <c r="G6" s="158"/>
+      <c r="H6" s="177"/>
+      <c r="I6" s="196"/>
+      <c r="J6" s="145"/>
+      <c r="K6" s="190"/>
     </row>
     <row r="7" spans="1:11" ht="75" customHeight="1" thickBot="1">
       <c r="A7" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="B7" s="189"/>
+      <c r="B7" s="178"/>
       <c r="C7" s="64" t="s">
         <v>367</v>
       </c>
@@ -10395,28 +10395,28 @@
         <v>156</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="150" t="s">
+      <c r="G7" s="158" t="s">
         <v>457</v>
       </c>
-      <c r="H7" s="170" t="s">
+      <c r="H7" s="177" t="s">
         <v>522</v>
       </c>
-      <c r="I7" s="187"/>
-      <c r="J7" s="159" t="s">
+      <c r="I7" s="196"/>
+      <c r="J7" s="147" t="s">
         <v>460</v>
       </c>
-      <c r="K7" s="172" t="s">
+      <c r="K7" s="171" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="D8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="184"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="188"/>
-      <c r="J8" s="163"/>
-      <c r="K8" s="185"/>
+      <c r="G8" s="193"/>
+      <c r="H8" s="165"/>
+      <c r="I8" s="197"/>
+      <c r="J8" s="173"/>
+      <c r="K8" s="194"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" thickBot="1">
       <c r="A9" s="1" t="s">
@@ -10435,34 +10435,34 @@
         <v>142</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="142" t="s">
+      <c r="G9" s="159" t="s">
         <v>465</v>
       </c>
-      <c r="H9" s="142"/>
-      <c r="I9" s="142"/>
-      <c r="J9" s="142"/>
-      <c r="K9" s="142"/>
+      <c r="H9" s="159"/>
+      <c r="I9" s="159"/>
+      <c r="J9" s="159"/>
+      <c r="K9" s="159"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="193" t="s">
+      <c r="A10" s="186" t="s">
         <v>535</v>
       </c>
-      <c r="B10" s="193"/>
-      <c r="C10" s="193"/>
-      <c r="D10" s="193"/>
-      <c r="E10" s="193"/>
+      <c r="B10" s="186"/>
+      <c r="C10" s="186"/>
+      <c r="D10" s="186"/>
+      <c r="E10" s="186"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="194" t="s">
+      <c r="G10" s="187" t="s">
         <v>495</v>
       </c>
-      <c r="H10" s="169" t="s">
+      <c r="H10" s="160" t="s">
         <v>555</v>
       </c>
-      <c r="I10" s="178"/>
-      <c r="J10" s="195" t="s">
+      <c r="I10" s="183"/>
+      <c r="J10" s="188" t="s">
         <v>501</v>
       </c>
-      <c r="K10" s="196" t="s">
+      <c r="K10" s="189" t="s">
         <v>148</v>
       </c>
     </row>
@@ -10470,10 +10470,10 @@
       <c r="A11" s="138" t="s">
         <v>543</v>
       </c>
-      <c r="B11" s="181" t="s">
+      <c r="B11" s="192" t="s">
         <v>468</v>
       </c>
-      <c r="C11" s="190"/>
+      <c r="C11" s="179"/>
       <c r="D11" s="114" t="s">
         <v>544</v>
       </c>
@@ -10481,18 +10481,18 @@
         <v>146</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="150"/>
-      <c r="H11" s="173"/>
-      <c r="I11" s="179"/>
-      <c r="J11" s="158"/>
-      <c r="K11" s="197"/>
+      <c r="G11" s="158"/>
+      <c r="H11" s="161"/>
+      <c r="I11" s="184"/>
+      <c r="J11" s="145"/>
+      <c r="K11" s="190"/>
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="138" t="s">
         <v>542</v>
       </c>
       <c r="B12" s="182"/>
-      <c r="C12" s="191"/>
+      <c r="C12" s="180"/>
       <c r="D12" s="114" t="s">
         <v>545</v>
       </c>
@@ -10500,11 +10500,11 @@
         <v>156</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="150"/>
-      <c r="H12" s="173"/>
-      <c r="I12" s="179"/>
-      <c r="J12" s="158"/>
-      <c r="K12" s="197"/>
+      <c r="G12" s="158"/>
+      <c r="H12" s="161"/>
+      <c r="I12" s="184"/>
+      <c r="J12" s="145"/>
+      <c r="K12" s="190"/>
     </row>
     <row r="13" spans="1:11" ht="45" customHeight="1">
       <c r="A13" s="138" t="s">
@@ -10513,7 +10513,7 @@
       <c r="B13" s="124" t="s">
         <v>549</v>
       </c>
-      <c r="C13" s="191"/>
+      <c r="C13" s="180"/>
       <c r="D13" s="114" t="s">
         <v>541</v>
       </c>
@@ -10521,11 +10521,11 @@
         <v>148</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="150"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="179"/>
-      <c r="J13" s="158"/>
-      <c r="K13" s="197"/>
+      <c r="G13" s="158"/>
+      <c r="H13" s="161"/>
+      <c r="I13" s="184"/>
+      <c r="J13" s="145"/>
+      <c r="K13" s="190"/>
     </row>
     <row r="14" spans="1:11" ht="105" customHeight="1">
       <c r="A14" s="10" t="s">
@@ -10534,7 +10534,7 @@
       <c r="B14" s="182" t="s">
         <v>547</v>
       </c>
-      <c r="C14" s="191"/>
+      <c r="C14" s="180"/>
       <c r="D14" s="40" t="s">
         <v>534</v>
       </c>
@@ -10548,7 +10548,7 @@
       <c r="H14" s="116" t="s">
         <v>555</v>
       </c>
-      <c r="I14" s="179"/>
+      <c r="I14" s="184"/>
       <c r="J14" s="7" t="s">
         <v>500</v>
       </c>
@@ -10561,7 +10561,7 @@
         <v>532</v>
       </c>
       <c r="B15" s="182"/>
-      <c r="C15" s="191"/>
+      <c r="C15" s="180"/>
       <c r="D15" s="40" t="s">
         <v>498</v>
       </c>
@@ -10575,7 +10575,7 @@
       <c r="H15" s="119" t="s">
         <v>536</v>
       </c>
-      <c r="I15" s="179"/>
+      <c r="I15" s="184"/>
       <c r="J15" s="7" t="s">
         <v>498</v>
       </c>
@@ -10590,7 +10590,7 @@
       <c r="B16" s="119" t="s">
         <v>548</v>
       </c>
-      <c r="C16" s="192"/>
+      <c r="C16" s="181"/>
       <c r="D16" s="40" t="s">
         <v>515</v>
       </c>
@@ -10598,34 +10598,34 @@
         <v>146</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="145" t="s">
+      <c r="G16" s="142" t="s">
         <v>502</v>
       </c>
-      <c r="H16" s="173" t="s">
+      <c r="H16" s="161" t="s">
         <v>537</v>
       </c>
-      <c r="I16" s="179"/>
-      <c r="J16" s="159" t="s">
+      <c r="I16" s="184"/>
+      <c r="J16" s="147" t="s">
         <v>515</v>
       </c>
-      <c r="K16" s="172" t="s">
+      <c r="K16" s="171" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
-      <c r="A17" s="142" t="s">
+      <c r="A17" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="142"/>
-      <c r="C17" s="142"/>
-      <c r="D17" s="142"/>
-      <c r="E17" s="142"/>
+      <c r="B17" s="159"/>
+      <c r="C17" s="159"/>
+      <c r="D17" s="159"/>
+      <c r="E17" s="159"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="145"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="179"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="172"/>
+      <c r="G17" s="142"/>
+      <c r="H17" s="161"/>
+      <c r="I17" s="184"/>
+      <c r="J17" s="147"/>
+      <c r="K17" s="171"/>
     </row>
     <row r="18" spans="1:11" ht="105" customHeight="1" thickBot="1">
       <c r="A18" s="136" t="s">
@@ -10648,7 +10648,7 @@
       <c r="H18" s="119" t="s">
         <v>538</v>
       </c>
-      <c r="I18" s="183"/>
+      <c r="I18" s="185"/>
       <c r="J18" s="40" t="s">
         <v>499</v>
       </c>
@@ -10659,13 +10659,13 @@
     <row r="19" spans="1:11">
       <c r="D19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="142" t="s">
+      <c r="G19" s="159" t="s">
         <v>504</v>
       </c>
-      <c r="H19" s="142"/>
-      <c r="I19" s="142"/>
-      <c r="J19" s="142"/>
-      <c r="K19" s="142"/>
+      <c r="H19" s="159"/>
+      <c r="I19" s="159"/>
+      <c r="J19" s="159"/>
+      <c r="K19" s="159"/>
     </row>
     <row r="20" spans="1:11" ht="60">
       <c r="D20" s="4"/>
@@ -10676,7 +10676,7 @@
       <c r="H20" s="118" t="s">
         <v>517</v>
       </c>
-      <c r="I20" s="178"/>
+      <c r="I20" s="183"/>
       <c r="J20" s="56" t="s">
         <v>513</v>
       </c>
@@ -10693,7 +10693,7 @@
       <c r="H21" s="119" t="s">
         <v>518</v>
       </c>
-      <c r="I21" s="179"/>
+      <c r="I21" s="184"/>
       <c r="J21" s="40" t="s">
         <v>514</v>
       </c>
@@ -10710,7 +10710,7 @@
       <c r="H22" s="119" t="s">
         <v>520</v>
       </c>
-      <c r="I22" s="179"/>
+      <c r="I22" s="184"/>
       <c r="J22" s="40" t="s">
         <v>512</v>
       </c>
@@ -10727,7 +10727,7 @@
       <c r="H23" s="119" t="s">
         <v>527</v>
       </c>
-      <c r="I23" s="179"/>
+      <c r="I23" s="184"/>
       <c r="J23" s="40" t="s">
         <v>529</v>
       </c>
@@ -10744,7 +10744,7 @@
       <c r="H24" s="64" t="s">
         <v>509</v>
       </c>
-      <c r="I24" s="180"/>
+      <c r="I24" s="191"/>
       <c r="J24" s="17" t="s">
         <v>164</v>
       </c>
@@ -10878,21 +10878,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="I10:I18"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="J10:J13"/>
-    <mergeCell ref="K10:K13"/>
-    <mergeCell ref="K5:K6"/>
     <mergeCell ref="G19:K19"/>
     <mergeCell ref="I20:I24"/>
     <mergeCell ref="B11:B12"/>
@@ -10909,6 +10894,21 @@
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="I10:I18"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="K10:K13"/>
+    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11083,7 +11083,7 @@
       <c r="A6" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="B6" s="175" t="s">
+      <c r="B6" s="163" t="s">
         <v>478</v>
       </c>
       <c r="C6" s="22">
@@ -11133,7 +11133,7 @@
       <c r="A9" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="B9" s="175" t="s">
+      <c r="B9" s="163" t="s">
         <v>467</v>
       </c>
       <c r="C9" s="22" t="s">
@@ -11561,29 +11561,29 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="159" t="s">
         <v>310</v>
       </c>
-      <c r="B2" s="142"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="G2" s="142" t="s">
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="G2" s="159" t="s">
         <v>319</v>
       </c>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="142"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="159"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="B3" s="174" t="s">
+      <c r="B3" s="162" t="s">
         <v>486</v>
       </c>
-      <c r="C3" s="161" t="s">
+      <c r="C3" s="169" t="s">
         <v>154</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -11602,8 +11602,8 @@
       <c r="A4" s="5" t="s">
         <v>559</v>
       </c>
-      <c r="B4" s="175"/>
-      <c r="C4" s="162"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="172"/>
       <c r="D4" s="40" t="s">
         <v>312</v>
       </c>
@@ -11621,7 +11621,7 @@
       <c r="A5" s="5" t="s">
         <v>560</v>
       </c>
-      <c r="B5" s="175"/>
+      <c r="B5" s="163"/>
       <c r="C5" s="67" t="s">
         <v>106</v>
       </c>
@@ -11662,13 +11662,13 @@
       <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="142" t="s">
+      <c r="A7" s="159" t="s">
         <v>318</v>
       </c>
-      <c r="B7" s="142"/>
-      <c r="C7" s="142"/>
-      <c r="D7" s="142"/>
-      <c r="E7" s="142"/>
+      <c r="B7" s="159"/>
+      <c r="C7" s="159"/>
+      <c r="D7" s="159"/>
+      <c r="E7" s="159"/>
       <c r="F7" s="46"/>
       <c r="G7" s="38"/>
       <c r="H7" s="38"/>
@@ -11680,7 +11680,7 @@
       <c r="A8" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="B8" s="174" t="s">
+      <c r="B8" s="162" t="s">
         <v>489</v>
       </c>
       <c r="C8" s="67" t="s">
@@ -11701,7 +11701,7 @@
       <c r="A9" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="B9" s="175"/>
+      <c r="B9" s="163"/>
       <c r="C9" s="67" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
added the spiked pavisse, and added armour strengths and weaknesses to certain damage types.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Git Repositories\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12739D72-8445-4099-8C73-837FE6AFB084}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290B0B38-A02E-4B24-BB02-E73AD94D0A38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="394" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="595">
   <si>
     <t>WEIGHT</t>
   </si>
@@ -1297,43 +1297,16 @@
     <t>Ring Mail (14 AC)</t>
   </si>
   <si>
-    <t>Plate Armour (18 AC)</t>
-  </si>
-  <si>
-    <t>Chain Mail (16 AC)</t>
-  </si>
-  <si>
-    <t>Spiked Armour (14 AC)</t>
-  </si>
-  <si>
     <t>Scale Mail (14 AC)</t>
   </si>
   <si>
-    <t>Hide Armour (13 AC)</t>
-  </si>
-  <si>
-    <t>Half Plate (15 AC)</t>
-  </si>
-  <si>
     <t>Breastplate (14 AC)</t>
   </si>
   <si>
-    <t>Chain Shirt (13 AC)</t>
-  </si>
-  <si>
     <t>11 lbs.</t>
   </si>
   <si>
     <t>14 lbs.</t>
-  </si>
-  <si>
-    <t>Studded Leather Armour (12 AC)</t>
-  </si>
-  <si>
-    <t>Leather Armour (11 AC)</t>
-  </si>
-  <si>
-    <t>Padded Armour (10 AC)</t>
   </si>
   <si>
     <t>Club (1d6 B)</t>
@@ -4582,53 +4555,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Halberd (1d10 S; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10 ft.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>reach</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Glaive (1d10 S, P; </t>
     </r>
     <r>
@@ -5806,18 +5732,6 @@
     </r>
   </si>
   <si>
-    <t>1 wooden plate (4 lbs, 13" radius)
-OR
-metal plate (4 lbs, 13" radius)
-1 metal strip (2 lbs)</t>
-  </si>
-  <si>
-    <t>1 wooden plate (1.5 lbs, 8" radius)
-OR
-metal plate (1.5 lbs, 8" radius)
-1 metal strip (0.5 lbs)</t>
-  </si>
-  <si>
     <t>1 wooden plate (6.5 lbs, 15" radius)
 OR
 metal plate (6.5 lbs, 15" radius)
@@ -6394,6 +6308,103 @@
       <t xml:space="preserve">
 1 haft (5 lbs, 50")</t>
     </r>
+  </si>
+  <si>
+    <t>Chain Shirt (13 AC; DR 2 against projectiles)</t>
+  </si>
+  <si>
+    <t>Padded Armour (10 AC; -1 on saves against extreme heat)</t>
+  </si>
+  <si>
+    <t>Studded Leather Armour (12 AC; DR 1 against bludgeoning; DV 1 against piercing)</t>
+  </si>
+  <si>
+    <t>Hide Armour (13 AC; +3 on saves against extreme cold)</t>
+  </si>
+  <si>
+    <t>Spiked Armour (14 AC; spiked 1)</t>
+  </si>
+  <si>
+    <t>Chain Mail (16 AC; 3 DR against projectiles)</t>
+  </si>
+  <si>
+    <t>1 wooden plate (2 lbs, 8" radius)
+OR
+metal plate (2 lbs, 8" radius)
+1 metal strip</t>
+  </si>
+  <si>
+    <t>1 wooden plate (4 lbs, 13" radius)
+OR
+metal plate (4 lbs, 13" radius)
+1 metal strip (1 lbs)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Halberd (1d10 S;
+1d6 P; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10 ft.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reach</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>1 wooden plate (2 lbs, 12x20")
+OR
+metal plate (2 lbs, 12x20")
+1 speartip (0.5 lbs, 5")</t>
+  </si>
+  <si>
+    <t>Spiked Pavisse (1d6 P; +1 AC, medium)</t>
+  </si>
+  <si>
+    <t>Leather Armour (11 AC; DR 1 against bludgeoning; DV 1 against piercing)</t>
+  </si>
+  <si>
+    <t>Plate Armour (18 AC; 4 DR against slashing, piercing; DV 4 against bludgeoning; -4 on saves against extreme heat)</t>
+  </si>
+  <si>
+    <t>Half Plate (15 AC; DR 2 against slashing, piercing, projectiles;
+-2 on saves against extreme heat)</t>
   </si>
 </sst>
 </file>
@@ -7543,8 +7554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
   <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7577,10 +7588,10 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -7593,7 +7604,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>0</v>
@@ -7602,10 +7613,10 @@
         <v>1</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="M1" s="95" t="s">
         <v>0</v>
@@ -7617,7 +7628,7 @@
         <v>171</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>0</v>
@@ -7629,7 +7640,7 @@
         <v>181</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>0</v>
@@ -7641,7 +7652,7 @@
         <v>220</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="AB1" s="3" t="s">
         <v>0</v>
@@ -7652,19 +7663,19 @@
     </row>
     <row r="2" spans="1:29" ht="15" customHeight="1">
       <c r="A2" s="148" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B2" s="148"/>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
       <c r="F2" s="149" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="G2" s="149"/>
       <c r="H2" s="149"/>
       <c r="I2" s="149"/>
       <c r="K2" s="149" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="L2" s="149"/>
       <c r="M2" s="149"/>
@@ -7685,7 +7696,7 @@
         <v>182</v>
       </c>
       <c r="V2" s="156" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="W2" s="157" t="s">
         <v>177</v>
@@ -7702,10 +7713,10 @@
     </row>
     <row r="3" spans="1:29" ht="180" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>3</v>
@@ -7714,10 +7725,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>248</v>
+        <v>592</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>5</v>
@@ -7726,13 +7737,13 @@
         <v>4</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="L3" s="57" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="N3" s="4"/>
       <c r="P3" s="155"/>
@@ -7744,13 +7755,13 @@
       <c r="W3" s="158"/>
       <c r="X3" s="158"/>
       <c r="Z3" s="10" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
       <c r="AA3" s="115" t="s">
-        <v>571</v>
+        <v>559</v>
       </c>
       <c r="AB3" s="115" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="AC3" s="115" t="s">
         <v>42</v>
@@ -7758,10 +7769,10 @@
     </row>
     <row r="4" spans="1:29" ht="180" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>21</v>
@@ -7770,10 +7781,10 @@
         <v>6</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>249</v>
+        <v>582</v>
       </c>
       <c r="G4" s="115" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>7</v>
@@ -7782,10 +7793,10 @@
         <v>8</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="L4" s="57" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>177</v>
@@ -7816,24 +7827,24 @@
         <v>15</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>573</v>
+        <v>561</v>
       </c>
       <c r="AA4" s="61" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="AB4" s="115" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="AC4" s="115" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="75" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>566</v>
+        <v>554</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>10</v>
@@ -7842,25 +7853,25 @@
         <v>4</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>247</v>
+        <v>583</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>576</v>
+        <v>564</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="L5" s="57" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="M5" s="38" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="N5" s="41"/>
       <c r="P5" s="5" t="s">
@@ -7888,24 +7899,24 @@
         <v>31</v>
       </c>
       <c r="Z5" s="10" t="s">
-        <v>572</v>
+        <v>560</v>
       </c>
       <c r="AA5" s="61" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="AB5" s="115" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="AC5" s="115" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1">
       <c r="A6" s="146" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="B6" s="143" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="C6" s="142" t="s">
         <v>10</v>
@@ -7914,13 +7925,13 @@
         <v>11</v>
       </c>
       <c r="F6" s="144" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="G6" s="144"/>
       <c r="H6" s="144"/>
       <c r="I6" s="144"/>
       <c r="K6" s="144" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="L6" s="144"/>
       <c r="M6" s="144"/>
@@ -7962,10 +7973,10 @@
       <c r="C7" s="142"/>
       <c r="D7" s="142"/>
       <c r="F7" s="9" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>12</v>
@@ -7974,13 +7985,13 @@
         <v>13</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="L7" s="57" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="M7" s="38" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="N7" s="84"/>
       <c r="P7" s="155"/>
@@ -8002,10 +8013,10 @@
     </row>
     <row r="8" spans="1:29" ht="90" customHeight="1" thickBot="1">
       <c r="A8" s="10" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>3</v>
@@ -8014,25 +8025,25 @@
         <v>14</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>244</v>
+        <v>581</v>
       </c>
       <c r="G8" s="115" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="L8" s="57" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="M8" s="38" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="N8" s="38"/>
       <c r="P8" s="13" t="s">
@@ -8051,10 +8062,10 @@
         <v>186</v>
       </c>
       <c r="V8" s="17" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="W8" s="14" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="X8" s="14" t="s">
         <v>8</v>
@@ -8063,17 +8074,17 @@
         <v>227</v>
       </c>
       <c r="AA8" s="60" t="s">
-        <v>575</v>
+        <v>563</v>
       </c>
       <c r="AB8" s="122"/>
       <c r="AC8" s="122"/>
     </row>
     <row r="9" spans="1:29" ht="165" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>10</v>
@@ -8082,10 +8093,10 @@
         <v>8</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>242</v>
+        <v>594</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>584</v>
+        <v>572</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>16</v>
@@ -8094,13 +8105,13 @@
         <v>17</v>
       </c>
       <c r="K9" s="85" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="L9" s="57" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="M9" s="38" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="N9" s="46"/>
       <c r="Z9" s="10" t="s">
@@ -8114,10 +8125,10 @@
     </row>
     <row r="10" spans="1:29" ht="90">
       <c r="A10" s="10" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B10" s="75" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>21</v>
@@ -8126,25 +8137,25 @@
         <v>11</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>241</v>
+        <v>584</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>4</v>
       </c>
       <c r="K10" s="85" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="L10" s="57" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="Z10" s="10" t="s">
         <v>230</v>
@@ -8155,10 +8166,10 @@
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1">
       <c r="A11" s="146" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="B11" s="143" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="C11" s="142" t="s">
         <v>19</v>
@@ -8167,10 +8178,10 @@
         <v>14</v>
       </c>
       <c r="F11" s="146" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G11" s="143" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="H11" s="147" t="s">
         <v>20</v>
@@ -8179,7 +8190,7 @@
         <v>15</v>
       </c>
       <c r="K11" s="144" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="L11" s="144"/>
       <c r="M11" s="144"/>
@@ -8201,10 +8212,10 @@
       <c r="H12" s="147"/>
       <c r="I12" s="147"/>
       <c r="K12" s="9" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="N12" s="4"/>
       <c r="Z12" s="10" t="s">
@@ -8218,10 +8229,10 @@
     </row>
     <row r="13" spans="1:29" ht="195" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C13" s="62" t="s">
         <v>21</v>
@@ -8230,10 +8241,10 @@
         <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>239</v>
+        <v>585</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>30</v>
@@ -8242,23 +8253,23 @@
         <v>22</v>
       </c>
       <c r="K13" s="86" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="Z13" s="10" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="AA13" s="59" t="s">
-        <v>570</v>
+        <v>558</v>
       </c>
       <c r="AB13" s="40"/>
       <c r="AC13" s="40"/>
     </row>
     <row r="14" spans="1:29" ht="15" customHeight="1">
       <c r="A14" s="146" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="B14" s="143" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="C14" s="142" t="s">
         <v>10</v>
@@ -8267,13 +8278,13 @@
         <v>4</v>
       </c>
       <c r="F14" s="144" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="G14" s="144"/>
       <c r="H14" s="144"/>
       <c r="I14" s="144"/>
       <c r="K14" s="150" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="L14" s="151"/>
       <c r="M14" s="152"/>
@@ -8289,7 +8300,7 @@
       <c r="C15" s="142"/>
       <c r="D15" s="142"/>
       <c r="F15" s="9" t="s">
-        <v>238</v>
+        <v>586</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>24</v>
@@ -8311,10 +8322,10 @@
     </row>
     <row r="16" spans="1:29" ht="285.75" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>585</v>
+        <v>573</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>19</v>
@@ -8323,7 +8334,7 @@
         <v>28</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>237</v>
+        <v>593</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>215</v>
@@ -8335,7 +8346,7 @@
         <v>27</v>
       </c>
       <c r="K16" s="128" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="L16" s="102"/>
       <c r="M16" s="14"/>
@@ -8343,10 +8354,10 @@
     </row>
     <row r="17" spans="1:16" ht="75" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C17" s="106" t="s">
         <v>10</v>
@@ -8370,7 +8381,7 @@
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1">
       <c r="A18" s="159" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B18" s="159"/>
       <c r="C18" s="159"/>
@@ -8392,10 +8403,10 @@
     </row>
     <row r="19" spans="1:16" ht="150" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="C19" s="106" t="s">
         <v>36</v>
@@ -8411,10 +8422,10 @@
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1">
       <c r="A20" s="146" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B20" s="143" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="C20" s="142" t="s">
         <v>36</v>
@@ -8423,7 +8434,7 @@
         <v>31</v>
       </c>
       <c r="F20" s="144" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="G20" s="144"/>
       <c r="H20" s="144"/>
@@ -8435,26 +8446,26 @@
       <c r="C21" s="142"/>
       <c r="D21" s="142"/>
       <c r="F21" s="7" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="G21" s="76" t="s">
-        <v>561</v>
+        <v>587</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="K21" s="80"/>
       <c r="P21" s="80"/>
     </row>
     <row r="22" spans="1:16" ht="105">
       <c r="A22" s="10" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
       <c r="C22" s="106" t="s">
         <v>37</v>
@@ -8463,13 +8474,13 @@
         <v>4</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="G22" s="77" t="s">
-        <v>560</v>
+        <v>588</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>4</v>
@@ -8477,10 +8488,10 @@
     </row>
     <row r="23" spans="1:16" ht="105">
       <c r="A23" s="10" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="C23" s="106" t="s">
         <v>38</v>
@@ -8489,10 +8500,10 @@
         <v>39</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="G23" s="77" t="s">
-        <v>562</v>
+        <v>550</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>50</v>
@@ -8501,12 +8512,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="90.75" thickBot="1">
+    <row r="24" spans="1:16" ht="90">
       <c r="A24" s="10" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C24" s="106" t="s">
         <v>40</v>
@@ -8514,25 +8525,25 @@
       <c r="D24" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="G24" s="78" t="s">
-        <v>563</v>
-      </c>
-      <c r="H24" s="17" t="s">
+      <c r="F24" s="40" t="s">
+        <v>265</v>
+      </c>
+      <c r="G24" s="77" t="s">
+        <v>551</v>
+      </c>
+      <c r="H24" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="40" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="60">
+    <row r="25" spans="1:16" ht="105.75" thickBot="1">
       <c r="A25" s="10" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="C25" s="106" t="s">
         <v>37</v>
@@ -8540,13 +8551,25 @@
       <c r="D25" s="106" t="s">
         <v>23</v>
       </c>
+      <c r="F25" s="17" t="s">
+        <v>591</v>
+      </c>
+      <c r="G25" s="78" t="s">
+        <v>590</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="26" spans="1:16" ht="60">
       <c r="A26" s="10" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="C26" s="106" t="s">
         <v>41</v>
@@ -8557,10 +8580,10 @@
     </row>
     <row r="27" spans="1:16" ht="45">
       <c r="A27" s="10" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="C27" s="106" t="s">
         <v>37</v>
@@ -8571,10 +8594,10 @@
     </row>
     <row r="28" spans="1:16" ht="45">
       <c r="A28" s="10" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C28" s="106" t="s">
         <v>38</v>
@@ -8585,10 +8608,10 @@
     </row>
     <row r="29" spans="1:16" ht="30">
       <c r="A29" s="10" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="C29" s="106" t="s">
         <v>40</v>
@@ -8599,10 +8622,10 @@
     </row>
     <row r="30" spans="1:16" ht="60">
       <c r="A30" s="10" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C30" s="106" t="s">
         <v>37</v>
@@ -8613,10 +8636,10 @@
     </row>
     <row r="31" spans="1:16" ht="60" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="B31" s="77" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>37</v>
@@ -8627,10 +8650,10 @@
     </row>
     <row r="32" spans="1:16" ht="30" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="C32" s="106" t="s">
         <v>44</v>
@@ -8641,10 +8664,10 @@
     </row>
     <row r="33" spans="1:4" ht="45.75" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="C33" s="106" t="s">
         <v>45</v>
@@ -8655,10 +8678,10 @@
     </row>
     <row r="34" spans="1:4" ht="45">
       <c r="A34" s="10" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B34" s="74" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="C34" s="106" t="s">
         <v>38</v>
@@ -8669,13 +8692,13 @@
     </row>
     <row r="35" spans="1:4" ht="45">
       <c r="A35" s="10" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B35" s="74" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="C35" s="106" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="D35" s="106" t="s">
         <v>42</v>
@@ -8683,10 +8706,10 @@
     </row>
     <row r="36" spans="1:4" ht="60">
       <c r="A36" s="58" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B36" s="111" t="s">
-        <v>564</v>
+        <v>552</v>
       </c>
       <c r="C36" s="112" t="s">
         <v>38</v>
@@ -8697,7 +8720,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="159" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B37" s="159"/>
       <c r="C37" s="159"/>
@@ -8705,10 +8728,10 @@
     </row>
     <row r="38" spans="1:4" ht="60">
       <c r="A38" s="10" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="C38" s="106" t="s">
         <v>46</v>
@@ -8719,10 +8742,10 @@
     </row>
     <row r="39" spans="1:4" ht="60" customHeight="1">
       <c r="A39" s="10" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
       <c r="C39" s="106" t="s">
         <v>48</v>
@@ -8733,10 +8756,10 @@
     </row>
     <row r="40" spans="1:4" ht="60">
       <c r="A40" s="10" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
       <c r="C40" s="106" t="s">
         <v>48</v>
@@ -8747,10 +8770,10 @@
     </row>
     <row r="41" spans="1:4" ht="45" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="C41" s="109" t="s">
         <v>234</v>
@@ -8761,10 +8784,10 @@
     </row>
     <row r="42" spans="1:4" ht="60">
       <c r="A42" s="10" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="C42" s="109" t="s">
         <v>233</v>
@@ -8775,10 +8798,10 @@
     </row>
     <row r="43" spans="1:4" ht="90">
       <c r="A43" s="10" t="s">
-        <v>431</v>
+        <v>589</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="C43" s="106" t="s">
         <v>46</v>
@@ -8789,10 +8812,10 @@
     </row>
     <row r="44" spans="1:4" ht="45">
       <c r="A44" s="10" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="C44" s="106" t="s">
         <v>50</v>
@@ -8803,10 +8826,10 @@
     </row>
     <row r="45" spans="1:4" ht="60">
       <c r="A45" s="58" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="C45" s="106" t="s">
         <v>5</v>
@@ -8817,7 +8840,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="159" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B46" s="159"/>
       <c r="C46" s="159"/>
@@ -8825,13 +8848,13 @@
     </row>
     <row r="47" spans="1:4" ht="60" customHeight="1">
       <c r="A47" s="72" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="B47" s="109" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
       <c r="C47" s="109" t="s">
-        <v>586</v>
+        <v>574</v>
       </c>
       <c r="D47" s="106" t="s">
         <v>51</v>
@@ -8839,13 +8862,13 @@
     </row>
     <row r="48" spans="1:4" ht="135" customHeight="1">
       <c r="A48" s="10" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>565</v>
+        <v>553</v>
       </c>
       <c r="C48" s="109" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="D48" s="106" t="s">
         <v>32</v>
@@ -8853,10 +8876,10 @@
     </row>
     <row r="49" spans="1:4" ht="75" customHeight="1">
       <c r="A49" s="58" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="C49" s="109" t="s">
         <v>219</v>
@@ -8867,7 +8890,7 @@
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1">
       <c r="A50" s="159" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="B50" s="159"/>
       <c r="C50" s="159"/>
@@ -8875,10 +8898,10 @@
     </row>
     <row r="51" spans="1:4" ht="75" customHeight="1">
       <c r="A51" s="107" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="B51" s="108" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="C51" s="52" t="s">
         <v>40</v>
@@ -8889,13 +8912,13 @@
     </row>
     <row r="52" spans="1:4" ht="30">
       <c r="A52" s="107" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B52" s="60" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C52" s="52" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D52" s="52" t="s">
         <v>8</v>
@@ -8903,10 +8926,10 @@
     </row>
     <row r="53" spans="1:4" ht="75" customHeight="1">
       <c r="A53" s="107" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="B53" s="108" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C53" s="52" t="s">
         <v>10</v>
@@ -8917,10 +8940,10 @@
     </row>
     <row r="54" spans="1:4" ht="30" customHeight="1">
       <c r="A54" s="71" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B54" s="108" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C54" s="52" t="s">
         <v>19</v>
@@ -8931,7 +8954,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="159" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B55" s="159"/>
       <c r="C55" s="159"/>
@@ -8939,10 +8962,10 @@
     </row>
     <row r="56" spans="1:4" ht="30">
       <c r="A56" s="69" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="B56" s="108" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C56" s="52" t="s">
         <v>3</v>
@@ -8953,10 +8976,10 @@
     </row>
     <row r="57" spans="1:4" ht="60">
       <c r="A57" s="107" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="B57" s="108" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
       <c r="C57" s="52" t="s">
         <v>10</v>
@@ -8967,10 +8990,10 @@
     </row>
     <row r="58" spans="1:4" ht="60">
       <c r="A58" s="107" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="B58" s="108" t="s">
-        <v>587</v>
+        <v>575</v>
       </c>
       <c r="C58" s="52" t="s">
         <v>46</v>
@@ -8981,10 +9004,10 @@
     </row>
     <row r="59" spans="1:4" ht="60" customHeight="1">
       <c r="A59" s="107" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B59" s="108" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C59" s="52" t="s">
         <v>46</v>
@@ -8995,16 +9018,16 @@
     </row>
     <row r="60" spans="1:4" ht="75" customHeight="1">
       <c r="A60" s="107" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="B60" s="108" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
       <c r="C60" s="52" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D60" s="52" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -9017,13 +9040,13 @@
     </row>
     <row r="62" spans="1:4" ht="105">
       <c r="A62" s="69" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="B62" s="108" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C62" s="52" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="D62" s="52" t="s">
         <v>51</v>
@@ -9031,63 +9054,63 @@
     </row>
     <row r="63" spans="1:4" ht="105">
       <c r="A63" s="107" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B63" s="108" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="C63" s="52" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="D63" s="52" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="105">
       <c r="A64" s="107" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="B64" s="108" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="C64" s="52" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="D64" s="52" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="65" spans="1:29" ht="105">
       <c r="A65" s="107" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="B65" s="108" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="C65" s="52" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="D65" s="52" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="66" spans="1:29" ht="150" customHeight="1">
       <c r="A66" s="107" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="B66" s="114" t="s">
-        <v>567</v>
+        <v>555</v>
       </c>
       <c r="C66" s="52" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="D66" s="52" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="67" spans="1:29">
       <c r="A67" s="159" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B67" s="159"/>
       <c r="C67" s="159"/>
@@ -9095,10 +9118,10 @@
     </row>
     <row r="68" spans="1:29" ht="90">
       <c r="A68" s="107" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="B68" s="114" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="C68" s="52" t="s">
         <v>44</v>
@@ -9109,13 +9132,13 @@
     </row>
     <row r="69" spans="1:29" ht="90" customHeight="1">
       <c r="A69" s="107" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="B69" s="114" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="C69" s="52" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="D69" s="52" t="s">
         <v>27</v>
@@ -9123,16 +9146,16 @@
     </row>
     <row r="70" spans="1:29" s="27" customFormat="1" ht="90" customHeight="1">
       <c r="A70" s="107" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="B70" s="108" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="C70" s="108" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="D70" s="108" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
@@ -9151,16 +9174,16 @@
     </row>
     <row r="71" spans="1:29" ht="225" customHeight="1" thickBot="1">
       <c r="A71" s="70" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="B71" s="54" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="C71" s="53" t="s">
         <v>5</v>
       </c>
       <c r="D71" s="53" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -9237,7 +9260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E7B11-1527-417B-9532-F0F2C5A89902}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -9262,7 +9285,7 @@
         <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>140</v>
@@ -9275,10 +9298,10 @@
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>140</v>
@@ -9293,7 +9316,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="148" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="B2" s="148"/>
       <c r="C2" s="148"/>
@@ -9314,13 +9337,13 @@
         <v>136</v>
       </c>
       <c r="B3" s="162" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="C3" s="169" t="s">
         <v>100</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="E3" s="133" t="s">
         <v>152</v>
@@ -9347,7 +9370,7 @@
       <c r="B4" s="163"/>
       <c r="C4" s="172"/>
       <c r="D4" s="7" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="E4" s="135" t="s">
         <v>142</v>
@@ -9374,7 +9397,7 @@
       <c r="B5" s="163"/>
       <c r="C5" s="172"/>
       <c r="D5" s="7" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="E5" s="133" t="s">
         <v>152</v>
@@ -9401,7 +9424,7 @@
       <c r="B6" s="163"/>
       <c r="C6" s="172"/>
       <c r="D6" s="7" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="E6" s="135" t="s">
         <v>144</v>
@@ -9428,7 +9451,7 @@
       <c r="B7" s="163"/>
       <c r="C7" s="172"/>
       <c r="D7" s="7" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="E7" s="135" t="s">
         <v>142</v>
@@ -9460,7 +9483,7 @@
         <v>218</v>
       </c>
       <c r="E8" s="135" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="10" t="s">
@@ -9494,7 +9517,7 @@
         <v>159</v>
       </c>
       <c r="H9" s="116" t="s">
-        <v>569</v>
+        <v>557</v>
       </c>
       <c r="I9" s="177"/>
       <c r="J9" s="25" t="s">
@@ -9567,7 +9590,7 @@
         <v>107</v>
       </c>
       <c r="H12" s="162" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="I12" s="55" t="s">
         <v>106</v>
@@ -9607,7 +9630,7 @@
         <v>101</v>
       </c>
       <c r="B14" s="162" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="C14" s="169" t="s">
         <v>66</v>
@@ -9692,7 +9715,7 @@
         <v>88</v>
       </c>
       <c r="H17" s="162" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="I17" s="160"/>
       <c r="J17" s="7" t="s">
@@ -9786,10 +9809,10 @@
       <c r="B21" s="163"/>
       <c r="C21" s="166"/>
       <c r="D21" s="7" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="E21" s="133" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="5" t="s">
@@ -9867,7 +9890,7 @@
         <v>71</v>
       </c>
       <c r="H24" s="163" t="s">
-        <v>568</v>
+        <v>556</v>
       </c>
       <c r="I24" s="161"/>
       <c r="K24" s="139" t="s">
@@ -9879,10 +9902,10 @@
         <v>67</v>
       </c>
       <c r="B25" s="118" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="C25" s="169" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D25" s="56" t="s">
         <v>216</v>
@@ -9908,7 +9931,7 @@
         <v>65</v>
       </c>
       <c r="B26" s="64" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="C26" s="170"/>
       <c r="D26" s="17" t="s">
@@ -9922,7 +9945,7 @@
         <v>64</v>
       </c>
       <c r="H26" s="163" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="I26" s="161"/>
       <c r="J26" s="12"/>
@@ -9961,7 +9984,7 @@
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="5" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
       <c r="H29" s="164"/>
       <c r="I29" s="165"/>
@@ -9990,7 +10013,7 @@
         <v>60</v>
       </c>
       <c r="H31" s="116" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="I31" s="160"/>
       <c r="J31" s="7" t="s">
@@ -10024,13 +10047,13 @@
         <v>55</v>
       </c>
       <c r="H33" s="116" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="I33" s="63" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="K33" s="133" t="s">
         <v>144</v>
@@ -10043,13 +10066,13 @@
         <v>54</v>
       </c>
       <c r="H34" s="116" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="I34" s="63" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="K34" s="133" t="s">
         <v>142</v>
@@ -10062,13 +10085,13 @@
         <v>53</v>
       </c>
       <c r="H35" s="64" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="I35" s="129" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="K35" s="132" t="s">
         <v>142</v>
@@ -10250,7 +10273,7 @@
         <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>140</v>
@@ -10263,10 +10286,10 @@
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>140</v>
@@ -10280,7 +10303,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="148" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="B2" s="148"/>
       <c r="C2" s="148"/>
@@ -10288,7 +10311,7 @@
       <c r="E2" s="148"/>
       <c r="F2" s="18"/>
       <c r="G2" s="149" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="H2" s="149"/>
       <c r="I2" s="149"/>
@@ -10297,30 +10320,30 @@
     </row>
     <row r="3" spans="1:11" ht="30">
       <c r="A3" s="5" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="B3" s="119" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="C3" s="183" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E3" s="131" t="s">
         <v>144</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="38" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="H3" s="116" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="I3" s="195"/>
       <c r="J3" s="40" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="K3" s="131" t="s">
         <v>144</v>
@@ -10328,24 +10351,24 @@
     </row>
     <row r="4" spans="1:11" ht="30">
       <c r="A4" s="125" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="B4" s="126" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="C4" s="185"/>
       <c r="D4" s="40" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E4" s="131" t="s">
         <v>152</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="38" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="H4" s="116" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="I4" s="196"/>
       <c r="J4" s="40"/>
@@ -10355,7 +10378,7 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="159" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="B5" s="159"/>
       <c r="C5" s="159"/>
@@ -10363,14 +10386,14 @@
       <c r="E5" s="159"/>
       <c r="F5" s="4"/>
       <c r="G5" s="158" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="H5" s="177" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="I5" s="196"/>
       <c r="J5" s="145" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="K5" s="190" t="s">
         <v>142</v>
@@ -10378,16 +10401,16 @@
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="B6" s="162" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="C6" s="120" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="E6" s="131" t="s">
         <v>144</v>
@@ -10401,31 +10424,31 @@
     </row>
     <row r="7" spans="1:11" ht="75" customHeight="1" thickBot="1">
       <c r="A7" s="13" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="B7" s="178"/>
       <c r="C7" s="64" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E7" s="132" t="s">
         <v>152</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="158" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="H7" s="177" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="I7" s="196"/>
       <c r="J7" s="147" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="K7" s="171" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
@@ -10439,10 +10462,10 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" thickBot="1">
       <c r="A9" s="1" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>140</v>
@@ -10455,7 +10478,7 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="159" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="H9" s="159"/>
       <c r="I9" s="159"/>
@@ -10464,7 +10487,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
       <c r="A10" s="186" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="B10" s="186"/>
       <c r="C10" s="186"/>
@@ -10472,14 +10495,14 @@
       <c r="E10" s="186"/>
       <c r="F10" s="4"/>
       <c r="G10" s="187" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="H10" s="160" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="I10" s="183"/>
       <c r="J10" s="188" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="K10" s="189" t="s">
         <v>144</v>
@@ -10487,14 +10510,14 @@
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1">
       <c r="A11" s="138" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="B11" s="192" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="C11" s="179"/>
       <c r="D11" s="114" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="E11" s="137" t="s">
         <v>142</v>
@@ -10508,12 +10531,12 @@
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="138" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
       <c r="B12" s="182"/>
       <c r="C12" s="180"/>
       <c r="D12" s="114" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="E12" s="137" t="s">
         <v>152</v>
@@ -10527,14 +10550,14 @@
     </row>
     <row r="13" spans="1:11" ht="45" customHeight="1">
       <c r="A13" s="138" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="B13" s="124" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="C13" s="180"/>
       <c r="D13" s="114" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="E13" s="137" t="s">
         <v>144</v>
@@ -10548,28 +10571,28 @@
     </row>
     <row r="14" spans="1:11" ht="105" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="B14" s="182" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="C14" s="180"/>
       <c r="D14" s="40" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="E14" s="131" t="s">
         <v>144</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="7" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="H14" s="116" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="I14" s="184"/>
       <c r="J14" s="7" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="K14" s="133" t="s">
         <v>144</v>
@@ -10577,26 +10600,26 @@
     </row>
     <row r="15" spans="1:11" ht="105" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="B15" s="182"/>
       <c r="C15" s="180"/>
       <c r="D15" s="40" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="E15" s="131" t="s">
         <v>152</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="H15" s="119" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="I15" s="184"/>
       <c r="J15" s="7" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="K15" s="133" t="s">
         <v>152</v>
@@ -10604,28 +10627,28 @@
     </row>
     <row r="16" spans="1:11" ht="90" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="B16" s="119" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="C16" s="181"/>
       <c r="D16" s="40" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="E16" s="131" t="s">
         <v>142</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="142" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="H16" s="161" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="I16" s="184"/>
       <c r="J16" s="147" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="K16" s="171" t="s">
         <v>142</v>
@@ -10658,28 +10681,28 @@
         <v>211</v>
       </c>
       <c r="E18" s="132" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="38" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="H18" s="119" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="I18" s="185"/>
       <c r="J18" s="40" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="K18" s="131" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="D19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="159" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="H19" s="159"/>
       <c r="I19" s="159"/>
@@ -10690,14 +10713,14 @@
       <c r="D20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="130" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="H20" s="118" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="I20" s="183"/>
       <c r="J20" s="56" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="K20" s="134" t="s">
         <v>144</v>
@@ -10707,14 +10730,14 @@
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="38" t="s">
-        <v>502</v>
+        <v>492</v>
       </c>
       <c r="H21" s="119" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="I21" s="184"/>
       <c r="J21" s="40" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="K21" s="131" t="s">
         <v>142</v>
@@ -10724,14 +10747,14 @@
       <c r="D22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="38" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="H22" s="119" t="s">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="I22" s="184"/>
       <c r="J22" s="40" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="K22" s="131" t="s">
         <v>152</v>
@@ -10741,14 +10764,14 @@
       <c r="D23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="38" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="H23" s="119" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="I23" s="184"/>
       <c r="J23" s="40" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="K23" s="131" t="s">
         <v>152</v>
@@ -10758,10 +10781,10 @@
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="14" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="H24" s="64" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
       <c r="I24" s="191"/>
       <c r="J24" s="17" t="s">
@@ -10939,7 +10962,7 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10960,10 +10983,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>140</v>
@@ -10979,7 +11002,7 @@
         <v>61</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>140</v>
@@ -10997,7 +11020,7 @@
         <v>154</v>
       </c>
       <c r="B2" s="123" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="C2" s="198" t="s">
         <v>153</v>
@@ -11010,10 +11033,10 @@
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="43" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="H2" s="123" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="I2" s="21" t="s">
         <v>102</v>
@@ -11028,10 +11051,10 @@
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" s="5" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="B3" s="121" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="C3" s="166"/>
       <c r="D3" s="7"/>
@@ -11040,16 +11063,16 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="10" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="H3" s="121" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="I3" s="42">
         <v>0</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="K3" s="35" t="s">
         <v>144</v>
@@ -11060,7 +11083,7 @@
         <v>151</v>
       </c>
       <c r="B4" s="121" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="C4" s="166" t="s">
         <v>150</v>
@@ -11074,7 +11097,7 @@
         <v>213</v>
       </c>
       <c r="H4" s="110" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="I4" s="34" t="s">
         <v>149</v>
@@ -11091,7 +11114,7 @@
         <v>148</v>
       </c>
       <c r="B5" s="121" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="C5" s="166"/>
       <c r="D5" s="7"/>
@@ -11103,10 +11126,10 @@
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="B6" s="163" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="C6" s="22">
         <v>0</v>
@@ -11120,7 +11143,7 @@
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="B7" s="199"/>
       <c r="C7" s="166" t="s">
@@ -11136,7 +11159,7 @@
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="B8" s="199"/>
       <c r="C8" s="166"/>
@@ -11153,10 +11176,10 @@
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="B9" s="163" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>147</v>
@@ -11172,7 +11195,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="B10" s="199"/>
       <c r="C10" s="22" t="s">
@@ -11189,7 +11212,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="B11" s="199"/>
       <c r="C11" s="21" t="s">
@@ -11208,7 +11231,7 @@
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A12" s="13" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="B12" s="200"/>
       <c r="C12" s="34" t="s">
@@ -11552,10 +11575,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>140</v>
@@ -11570,7 +11593,7 @@
         <v>70</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>140</v>
@@ -11584,14 +11607,14 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="159" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B2" s="159"/>
       <c r="C2" s="159"/>
       <c r="D2" s="159"/>
       <c r="E2" s="159"/>
       <c r="G2" s="159" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="H2" s="159"/>
       <c r="I2" s="159"/>
@@ -11600,10 +11623,10 @@
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="B3" s="162" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="C3" s="169" t="s">
         <v>150</v>
@@ -11622,12 +11645,12 @@
     </row>
     <row r="4" spans="1:11" ht="30">
       <c r="A4" s="5" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="B4" s="163"/>
       <c r="C4" s="172"/>
       <c r="D4" s="40" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="E4" s="91">
         <v>1</v>
@@ -11641,7 +11664,7 @@
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="B5" s="163"/>
       <c r="C5" s="67" t="s">
@@ -11662,16 +11685,16 @@
     </row>
     <row r="6" spans="1:11" ht="105">
       <c r="A6" s="5" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="C6" s="67" t="s">
+        <v>293</v>
+      </c>
+      <c r="D6" s="40" t="s">
         <v>302</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>311</v>
       </c>
       <c r="E6" s="57">
         <v>3</v>
@@ -11685,7 +11708,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="159" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="B7" s="159"/>
       <c r="C7" s="159"/>
@@ -11700,10 +11723,10 @@
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="B8" s="162" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="C8" s="67" t="s">
         <v>102</v>
@@ -11721,14 +11744,14 @@
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="B9" s="163"/>
       <c r="C9" s="67" t="s">
         <v>102</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="E9" s="91">
         <v>3</v>
@@ -11742,13 +11765,13 @@
     </row>
     <row r="10" spans="1:11" ht="30.75" thickBot="1">
       <c r="A10" s="13" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="B10" s="64" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="C10" s="82" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="103">
@@ -12098,7 +12121,7 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>139</v>
@@ -12110,7 +12133,7 @@
         <v>176</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>139</v>
@@ -12181,7 +12204,7 @@
         <v>163</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>139</v>
@@ -12247,7 +12270,7 @@
         <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>139</v>
@@ -12259,7 +12282,7 @@
         <v>162</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>139</v>
@@ -12289,10 +12312,10 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1">
       <c r="F6" s="1" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>139</v>
@@ -12306,7 +12329,7 @@
         <v>191</v>
       </c>
       <c r="G7" s="116" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="133" t="s">
@@ -12318,11 +12341,11 @@
         <v>193</v>
       </c>
       <c r="G8" s="116" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="133" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75.75" thickBot="1">
@@ -12330,7 +12353,7 @@
         <v>192</v>
       </c>
       <c r="G9" s="64" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="132" t="s">

</xml_diff>

<commit_message>
added arctanite glass, and made a few calculations for emission radius.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Git Repositories\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290B0B38-A02E-4B24-BB02-E73AD94D0A38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34074A7B-E682-4A5F-BF33-7E5F1893D6E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="394" xr2:uid="{D75E2DFF-C49B-4F74-BBE9-A61BEFE726AF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="594">
   <si>
     <t>WEIGHT</t>
   </si>
@@ -4761,10 +4761,6 @@
   </si>
   <si>
     <t>1 bar of metal
-(100%)</t>
-  </si>
-  <si>
-    <t>1 bar of metal
 (100% lbs.)</t>
   </si>
   <si>
@@ -4782,32 +4778,8 @@
 (100% lbs.)</t>
   </si>
   <si>
-    <t>chain links
-(0.05 lbs each)</t>
-  </si>
-  <si>
-    <t>chain links 
-(0.1 lbs each)</t>
-  </si>
-  <si>
     <t>1 fur pelt
 (100% lbs.)</t>
-  </si>
-  <si>
-    <t>1 block of wood
-(100%)</t>
-  </si>
-  <si>
-    <t>2 silk weaves
-(100%)</t>
-  </si>
-  <si>
-    <t>2 cuts of leather
-(100%)</t>
-  </si>
-  <si>
-    <t>1 leather quilt
-(100%)</t>
   </si>
   <si>
     <t>Endless Loop Bowstring</t>
@@ -4967,10 +4939,6 @@
   <si>
     <t>1 bar of soft metal
 (100% lbs.)</t>
-  </si>
-  <si>
-    <t>1 bar of hard metal
-(100%)</t>
   </si>
   <si>
     <t>Internal Gun Hammer</t>
@@ -5552,22 +5520,6 @@
 (1/7th of lbs.)</t>
   </si>
   <si>
-    <t>1 length of metal wire
-(50% of lbs.)
-gemstone grains
-(50% of lbs.)</t>
-  </si>
-  <si>
-    <t>2 lengths of conductive metal silk
-(100% of lbs.)</t>
-  </si>
-  <si>
-    <t>1 length of wire
-(50% of lbs.)
-1 sheathe of soft insulative metal
-(50% of lbs.)</t>
-  </si>
-  <si>
     <t>Blunthead x 5</t>
   </si>
   <si>
@@ -6394,9 +6346,6 @@
 1 speartip (0.5 lbs, 5")</t>
   </si>
   <si>
-    <t>Spiked Pavisse (1d6 P; +1 AC, medium)</t>
-  </si>
-  <si>
     <t>Leather Armour (11 AC; DR 1 against bludgeoning; DV 1 against piercing)</t>
   </si>
   <si>
@@ -6405,6 +6354,53 @@
   <si>
     <t>Half Plate (15 AC; DR 2 against slashing, piercing, projectiles;
 -2 on saves against extreme heat)</t>
+  </si>
+  <si>
+    <t>Spiked Pavisse (1d6 P; +1 AC, light)</t>
+  </si>
+  <si>
+    <t>1 block of wood
+(100% lbs.)</t>
+  </si>
+  <si>
+    <t>2 silk weaves
+(100% lbs.)</t>
+  </si>
+  <si>
+    <t>2 cuts of leather
+(100% lbs.)</t>
+  </si>
+  <si>
+    <t>1 leather quilt
+(100% lbs.)</t>
+  </si>
+  <si>
+    <t>1 bar of hard metal
+(100% lbs.)</t>
+  </si>
+  <si>
+    <t>2 lengths of conductive metal silk
+(100% lbs.)</t>
+  </si>
+  <si>
+    <t>1 length of metal wire
+(50% lbs.)
+gemstone grains
+(50% lbs.)</t>
+  </si>
+  <si>
+    <t>1 length of wire
+(50% lbs.)
+1 sheathe of soft insulative metal
+(50% lbs.)</t>
+  </si>
+  <si>
+    <t>chain links
+(0.05 lbs. each, 0.25" each)</t>
+  </si>
+  <si>
+    <t>chain links 
+(0.1 lbs. each, 0.25" each)</t>
   </si>
 </sst>
 </file>
@@ -7061,6 +7057,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -7233,9 +7232,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7552,10 +7548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D4C9D-49C2-4D87-80F1-54C5ABE27D48}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AC71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7662,54 +7659,54 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="15" customHeight="1">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="149" t="s">
         <v>320</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="F2" s="149" t="s">
-        <v>543</v>
-      </c>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="K2" s="149" t="s">
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="F2" s="150" t="s">
+        <v>532</v>
+      </c>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
+      <c r="K2" s="150" t="s">
         <v>390</v>
       </c>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="P2" s="154" t="s">
+      <c r="L2" s="150"/>
+      <c r="M2" s="150"/>
+      <c r="N2" s="150"/>
+      <c r="P2" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="Q2" s="156" t="s">
+      <c r="Q2" s="157" t="s">
         <v>201</v>
       </c>
-      <c r="R2" s="157" t="s">
+      <c r="R2" s="158" t="s">
         <v>177</v>
       </c>
-      <c r="S2" s="157" t="s">
+      <c r="S2" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="U2" s="154" t="s">
+      <c r="U2" s="155" t="s">
         <v>182</v>
       </c>
-      <c r="V2" s="156" t="s">
+      <c r="V2" s="157" t="s">
         <v>337</v>
       </c>
-      <c r="W2" s="157" t="s">
+      <c r="W2" s="158" t="s">
         <v>177</v>
       </c>
-      <c r="X2" s="157" t="s">
+      <c r="X2" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" s="149" t="s">
+      <c r="Z2" s="150" t="s">
         <v>221</v>
       </c>
-      <c r="AA2" s="149"/>
-      <c r="AB2" s="149"/>
-      <c r="AC2" s="149"/>
+      <c r="AA2" s="150"/>
+      <c r="AB2" s="150"/>
+      <c r="AC2" s="150"/>
     </row>
     <row r="3" spans="1:29" ht="180" customHeight="1">
       <c r="A3" s="10" t="s">
@@ -7725,10 +7722,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>5</v>
@@ -7746,19 +7743,19 @@
         <v>400</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="P3" s="155"/>
-      <c r="Q3" s="143"/>
-      <c r="R3" s="158"/>
-      <c r="S3" s="158"/>
-      <c r="U3" s="155"/>
-      <c r="V3" s="143"/>
-      <c r="W3" s="158"/>
-      <c r="X3" s="158"/>
+      <c r="P3" s="156"/>
+      <c r="Q3" s="144"/>
+      <c r="R3" s="159"/>
+      <c r="S3" s="159"/>
+      <c r="U3" s="156"/>
+      <c r="V3" s="144"/>
+      <c r="W3" s="159"/>
+      <c r="X3" s="159"/>
       <c r="Z3" s="10" t="s">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="AA3" s="115" t="s">
-        <v>559</v>
+        <v>548</v>
       </c>
       <c r="AB3" s="115" t="s">
         <v>319</v>
@@ -7772,7 +7769,7 @@
         <v>367</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>545</v>
+        <v>534</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>21</v>
@@ -7781,10 +7778,10 @@
         <v>6</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="G4" s="115" t="s">
-        <v>566</v>
+        <v>555</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>7</v>
@@ -7827,7 +7824,7 @@
         <v>15</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>561</v>
+        <v>550</v>
       </c>
       <c r="AA4" s="61" t="s">
         <v>338</v>
@@ -7844,7 +7841,7 @@
         <v>366</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>10</v>
@@ -7853,10 +7850,10 @@
         <v>4</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>564</v>
+        <v>553</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>239</v>
@@ -7899,7 +7896,7 @@
         <v>31</v>
       </c>
       <c r="Z5" s="10" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="AA5" s="61" t="s">
         <v>327</v>
@@ -7912,71 +7909,71 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1">
-      <c r="A6" s="146" t="s">
+      <c r="A6" s="147" t="s">
         <v>241</v>
       </c>
-      <c r="B6" s="143" t="s">
+      <c r="B6" s="144" t="s">
         <v>308</v>
       </c>
-      <c r="C6" s="142" t="s">
+      <c r="C6" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="142" t="s">
+      <c r="D6" s="143" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="144" t="s">
-        <v>542</v>
-      </c>
-      <c r="G6" s="144"/>
-      <c r="H6" s="144"/>
-      <c r="I6" s="144"/>
-      <c r="K6" s="144" t="s">
+      <c r="F6" s="145" t="s">
+        <v>531</v>
+      </c>
+      <c r="G6" s="145"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="K6" s="145" t="s">
         <v>281</v>
       </c>
-      <c r="L6" s="144"/>
-      <c r="M6" s="144"/>
-      <c r="N6" s="144"/>
-      <c r="P6" s="155" t="s">
+      <c r="L6" s="145"/>
+      <c r="M6" s="145"/>
+      <c r="N6" s="145"/>
+      <c r="P6" s="156" t="s">
         <v>174</v>
       </c>
-      <c r="Q6" s="143" t="s">
+      <c r="Q6" s="144" t="s">
         <v>204</v>
       </c>
-      <c r="R6" s="142" t="s">
+      <c r="R6" s="143" t="s">
         <v>178</v>
       </c>
-      <c r="S6" s="142" t="s">
+      <c r="S6" s="143" t="s">
         <v>31</v>
       </c>
-      <c r="U6" s="155" t="s">
+      <c r="U6" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="V6" s="143" t="s">
+      <c r="V6" s="144" t="s">
         <v>208</v>
       </c>
-      <c r="W6" s="142" t="s">
+      <c r="W6" s="143" t="s">
         <v>178</v>
       </c>
-      <c r="X6" s="142" t="s">
+      <c r="X6" s="143" t="s">
         <v>31</v>
       </c>
-      <c r="Z6" s="144" t="s">
+      <c r="Z6" s="145" t="s">
         <v>225</v>
       </c>
-      <c r="AA6" s="144"/>
-      <c r="AB6" s="144"/>
-      <c r="AC6" s="144"/>
+      <c r="AA6" s="145"/>
+      <c r="AB6" s="145"/>
+      <c r="AC6" s="145"/>
     </row>
     <row r="7" spans="1:29" ht="135" customHeight="1">
-      <c r="A7" s="146"/>
-      <c r="B7" s="143"/>
-      <c r="C7" s="142"/>
-      <c r="D7" s="142"/>
+      <c r="A7" s="147"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="143"/>
+      <c r="D7" s="143"/>
       <c r="F7" s="9" t="s">
         <v>238</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>12</v>
@@ -7994,14 +7991,14 @@
         <v>401</v>
       </c>
       <c r="N7" s="84"/>
-      <c r="P7" s="155"/>
-      <c r="Q7" s="143"/>
-      <c r="R7" s="142"/>
-      <c r="S7" s="142"/>
-      <c r="U7" s="155"/>
-      <c r="V7" s="143"/>
-      <c r="W7" s="142"/>
-      <c r="X7" s="142"/>
+      <c r="P7" s="156"/>
+      <c r="Q7" s="144"/>
+      <c r="R7" s="143"/>
+      <c r="S7" s="143"/>
+      <c r="U7" s="156"/>
+      <c r="V7" s="144"/>
+      <c r="W7" s="143"/>
+      <c r="X7" s="143"/>
       <c r="Z7" s="10" t="s">
         <v>226</v>
       </c>
@@ -8025,13 +8022,13 @@
         <v>14</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="G8" s="115" t="s">
-        <v>570</v>
+        <v>559</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>15</v>
@@ -8074,7 +8071,7 @@
         <v>227</v>
       </c>
       <c r="AA8" s="60" t="s">
-        <v>563</v>
+        <v>552</v>
       </c>
       <c r="AB8" s="122"/>
       <c r="AC8" s="122"/>
@@ -8093,10 +8090,10 @@
         <v>8</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>594</v>
+        <v>582</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>16</v>
@@ -8137,10 +8134,10 @@
         <v>11</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>240</v>
@@ -8165,52 +8162,52 @@
       </c>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1">
-      <c r="A11" s="146" t="s">
+      <c r="A11" s="147" t="s">
         <v>371</v>
       </c>
-      <c r="B11" s="143" t="s">
+      <c r="B11" s="144" t="s">
         <v>311</v>
       </c>
-      <c r="C11" s="142" t="s">
+      <c r="C11" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="142" t="s">
+      <c r="D11" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="146" t="s">
+      <c r="F11" s="147" t="s">
         <v>237</v>
       </c>
-      <c r="G11" s="143" t="s">
-        <v>569</v>
-      </c>
-      <c r="H11" s="147" t="s">
+      <c r="G11" s="144" t="s">
+        <v>558</v>
+      </c>
+      <c r="H11" s="148" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="147" t="s">
+      <c r="I11" s="148" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="144" t="s">
+      <c r="K11" s="145" t="s">
         <v>316</v>
       </c>
-      <c r="L11" s="144"/>
-      <c r="M11" s="144"/>
-      <c r="N11" s="144"/>
-      <c r="Z11" s="144" t="s">
+      <c r="L11" s="145"/>
+      <c r="M11" s="145"/>
+      <c r="N11" s="145"/>
+      <c r="Z11" s="145" t="s">
         <v>222</v>
       </c>
-      <c r="AA11" s="144"/>
-      <c r="AB11" s="144"/>
-      <c r="AC11" s="144"/>
+      <c r="AA11" s="145"/>
+      <c r="AB11" s="145"/>
+      <c r="AC11" s="145"/>
     </row>
     <row r="12" spans="1:29" ht="75" customHeight="1">
-      <c r="A12" s="146"/>
-      <c r="B12" s="143"/>
-      <c r="C12" s="142"/>
-      <c r="D12" s="142"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="143"/>
-      <c r="H12" s="147"/>
-      <c r="I12" s="147"/>
+      <c r="A12" s="147"/>
+      <c r="B12" s="144"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="143"/>
+      <c r="F12" s="147"/>
+      <c r="G12" s="144"/>
+      <c r="H12" s="148"/>
+      <c r="I12" s="148"/>
       <c r="K12" s="9" t="s">
         <v>301</v>
       </c>
@@ -8241,7 +8238,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>315</v>
@@ -8259,48 +8256,48 @@
         <v>279</v>
       </c>
       <c r="AA13" s="59" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="AB13" s="40"/>
       <c r="AC13" s="40"/>
     </row>
     <row r="14" spans="1:29" ht="15" customHeight="1">
-      <c r="A14" s="146" t="s">
+      <c r="A14" s="147" t="s">
         <v>375</v>
       </c>
-      <c r="B14" s="143" t="s">
+      <c r="B14" s="144" t="s">
         <v>313</v>
       </c>
-      <c r="C14" s="142" t="s">
+      <c r="C14" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="142" t="s">
+      <c r="D14" s="143" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="144" t="s">
-        <v>544</v>
-      </c>
-      <c r="G14" s="144"/>
-      <c r="H14" s="144"/>
-      <c r="I14" s="144"/>
-      <c r="K14" s="150" t="s">
+      <c r="F14" s="145" t="s">
+        <v>533</v>
+      </c>
+      <c r="G14" s="145"/>
+      <c r="H14" s="145"/>
+      <c r="I14" s="145"/>
+      <c r="K14" s="151" t="s">
         <v>306</v>
       </c>
-      <c r="L14" s="151"/>
-      <c r="M14" s="152"/>
-      <c r="N14" s="153"/>
+      <c r="L14" s="152"/>
+      <c r="M14" s="153"/>
+      <c r="N14" s="154"/>
       <c r="Z14" s="40"/>
       <c r="AA14" s="79"/>
       <c r="AB14" s="40"/>
       <c r="AC14" s="40"/>
     </row>
     <row r="15" spans="1:29" ht="75" customHeight="1">
-      <c r="A15" s="146"/>
-      <c r="B15" s="143"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="142"/>
+      <c r="A15" s="147"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="143"/>
+      <c r="D15" s="143"/>
       <c r="F15" s="9" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>24</v>
@@ -8311,10 +8308,10 @@
       <c r="I15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="150"/>
-      <c r="L15" s="151"/>
-      <c r="M15" s="152"/>
-      <c r="N15" s="153"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="152"/>
+      <c r="M15" s="153"/>
+      <c r="N15" s="154"/>
       <c r="Z15" s="40"/>
       <c r="AA15" s="122"/>
       <c r="AB15" s="122"/>
@@ -8325,7 +8322,7 @@
         <v>373</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>19</v>
@@ -8334,7 +8331,7 @@
         <v>28</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>215</v>
@@ -8380,22 +8377,22 @@
       <c r="K17" s="127"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1">
-      <c r="A18" s="159" t="s">
+      <c r="A18" s="160" t="s">
         <v>321</v>
       </c>
-      <c r="B18" s="159"/>
-      <c r="C18" s="159"/>
-      <c r="D18" s="159"/>
-      <c r="F18" s="146" t="s">
+      <c r="B18" s="160"/>
+      <c r="C18" s="160"/>
+      <c r="D18" s="160"/>
+      <c r="F18" s="147" t="s">
         <v>235</v>
       </c>
-      <c r="G18" s="143" t="s">
+      <c r="G18" s="144" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="145" t="s">
+      <c r="H18" s="146" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="145" t="s">
+      <c r="I18" s="146" t="s">
         <v>35</v>
       </c>
       <c r="K18" s="46"/>
@@ -8414,42 +8411,42 @@
       <c r="D19" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="146"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="145"/>
-      <c r="I19" s="145"/>
+      <c r="F19" s="147"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="146"/>
+      <c r="I19" s="146"/>
       <c r="K19" s="46"/>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1">
-      <c r="A20" s="146" t="s">
+      <c r="A20" s="147" t="s">
         <v>246</v>
       </c>
-      <c r="B20" s="143" t="s">
+      <c r="B20" s="144" t="s">
         <v>402</v>
       </c>
-      <c r="C20" s="142" t="s">
+      <c r="C20" s="143" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="142" t="s">
+      <c r="D20" s="143" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="144" t="s">
+      <c r="F20" s="145" t="s">
         <v>317</v>
       </c>
-      <c r="G20" s="144"/>
-      <c r="H20" s="144"/>
-      <c r="I20" s="144"/>
+      <c r="G20" s="145"/>
+      <c r="H20" s="145"/>
+      <c r="I20" s="145"/>
     </row>
     <row r="21" spans="1:16" ht="105" customHeight="1">
-      <c r="A21" s="146"/>
-      <c r="B21" s="143"/>
-      <c r="C21" s="142"/>
-      <c r="D21" s="142"/>
+      <c r="A21" s="147"/>
+      <c r="B21" s="144"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="143"/>
       <c r="F21" s="7" t="s">
         <v>266</v>
       </c>
       <c r="G21" s="76" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>10</v>
@@ -8465,7 +8462,7 @@
         <v>272</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>549</v>
+        <v>538</v>
       </c>
       <c r="C22" s="106" t="s">
         <v>37</v>
@@ -8477,7 +8474,7 @@
         <v>273</v>
       </c>
       <c r="G22" s="77" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>44</v>
@@ -8503,7 +8500,7 @@
         <v>267</v>
       </c>
       <c r="G23" s="77" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>50</v>
@@ -8529,7 +8526,7 @@
         <v>265</v>
       </c>
       <c r="G24" s="77" t="s">
-        <v>551</v>
+        <v>540</v>
       </c>
       <c r="H24" s="40" t="s">
         <v>18</v>
@@ -8552,16 +8549,16 @@
         <v>23</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="G25" s="78" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>37</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="60">
@@ -8709,7 +8706,7 @@
         <v>258</v>
       </c>
       <c r="B36" s="111" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="C36" s="112" t="s">
         <v>38</v>
@@ -8719,12 +8716,12 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="159" t="s">
+      <c r="A37" s="160" t="s">
         <v>322</v>
       </c>
-      <c r="B37" s="159"/>
-      <c r="C37" s="159"/>
-      <c r="D37" s="159"/>
+      <c r="B37" s="160"/>
+      <c r="C37" s="160"/>
+      <c r="D37" s="160"/>
     </row>
     <row r="38" spans="1:4" ht="60">
       <c r="A38" s="10" t="s">
@@ -8745,7 +8742,7 @@
         <v>259</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>580</v>
+        <v>569</v>
       </c>
       <c r="C39" s="106" t="s">
         <v>48</v>
@@ -8759,7 +8756,7 @@
         <v>260</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>579</v>
+        <v>568</v>
       </c>
       <c r="C40" s="106" t="s">
         <v>48</v>
@@ -8798,7 +8795,7 @@
     </row>
     <row r="43" spans="1:4" ht="90">
       <c r="A43" s="10" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>419</v>
@@ -8839,22 +8836,22 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="159" t="s">
+      <c r="A46" s="160" t="s">
         <v>323</v>
       </c>
-      <c r="B46" s="159"/>
-      <c r="C46" s="159"/>
-      <c r="D46" s="159"/>
+      <c r="B46" s="160"/>
+      <c r="C46" s="160"/>
+      <c r="D46" s="160"/>
     </row>
     <row r="47" spans="1:4" ht="60" customHeight="1">
       <c r="A47" s="72" t="s">
         <v>361</v>
       </c>
       <c r="B47" s="109" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
       <c r="C47" s="109" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
       <c r="D47" s="106" t="s">
         <v>51</v>
@@ -8865,7 +8862,7 @@
         <v>368</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="C48" s="109" t="s">
         <v>264</v>
@@ -8889,12 +8886,12 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1">
-      <c r="A50" s="159" t="s">
+      <c r="A50" s="160" t="s">
         <v>324</v>
       </c>
-      <c r="B50" s="159"/>
-      <c r="C50" s="159"/>
-      <c r="D50" s="159"/>
+      <c r="B50" s="160"/>
+      <c r="C50" s="160"/>
+      <c r="D50" s="160"/>
     </row>
     <row r="51" spans="1:4" ht="75" customHeight="1">
       <c r="A51" s="107" t="s">
@@ -8953,12 +8950,12 @@
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="159" t="s">
+      <c r="A55" s="160" t="s">
         <v>326</v>
       </c>
-      <c r="B55" s="159"/>
-      <c r="C55" s="159"/>
-      <c r="D55" s="159"/>
+      <c r="B55" s="160"/>
+      <c r="C55" s="160"/>
+      <c r="D55" s="160"/>
     </row>
     <row r="56" spans="1:4" ht="30">
       <c r="A56" s="69" t="s">
@@ -8979,7 +8976,7 @@
         <v>351</v>
       </c>
       <c r="B57" s="108" t="s">
-        <v>576</v>
+        <v>565</v>
       </c>
       <c r="C57" s="52" t="s">
         <v>10</v>
@@ -8993,7 +8990,7 @@
         <v>353</v>
       </c>
       <c r="B58" s="108" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
       <c r="C58" s="52" t="s">
         <v>46</v>
@@ -9021,7 +9018,7 @@
         <v>356</v>
       </c>
       <c r="B60" s="108" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="C60" s="52" t="s">
         <v>239</v>
@@ -9031,22 +9028,22 @@
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="159" t="s">
+      <c r="A61" s="160" t="s">
         <v>200</v>
       </c>
-      <c r="B61" s="159"/>
-      <c r="C61" s="159"/>
-      <c r="D61" s="159"/>
+      <c r="B61" s="160"/>
+      <c r="C61" s="160"/>
+      <c r="D61" s="160"/>
     </row>
     <row r="62" spans="1:4" ht="105">
       <c r="A62" s="69" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="B62" s="108" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="C62" s="52" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="D62" s="52" t="s">
         <v>51</v>
@@ -9057,10 +9054,10 @@
         <v>357</v>
       </c>
       <c r="B63" s="108" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="C63" s="52" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="D63" s="52" t="s">
         <v>304</v>
@@ -9071,10 +9068,10 @@
         <v>358</v>
       </c>
       <c r="B64" s="108" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="C64" s="52" t="s">
-        <v>539</v>
+        <v>528</v>
       </c>
       <c r="D64" s="52" t="s">
         <v>332</v>
@@ -9085,10 +9082,10 @@
         <v>359</v>
       </c>
       <c r="B65" s="108" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C65" s="52" t="s">
-        <v>540</v>
+        <v>529</v>
       </c>
       <c r="D65" s="52" t="s">
         <v>334</v>
@@ -9099,29 +9096,29 @@
         <v>360</v>
       </c>
       <c r="B66" s="114" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="C66" s="52" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="D66" s="52" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="67" spans="1:29">
-      <c r="A67" s="159" t="s">
+      <c r="A67" s="160" t="s">
         <v>325</v>
       </c>
-      <c r="B67" s="159"/>
-      <c r="C67" s="159"/>
-      <c r="D67" s="159"/>
+      <c r="B67" s="160"/>
+      <c r="C67" s="160"/>
+      <c r="D67" s="160"/>
     </row>
     <row r="68" spans="1:29" ht="90">
       <c r="A68" s="107" t="s">
-        <v>548</v>
+        <v>537</v>
       </c>
       <c r="B68" s="114" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="C68" s="52" t="s">
         <v>44</v>
@@ -9132,10 +9129,10 @@
     </row>
     <row r="69" spans="1:29" ht="90" customHeight="1">
       <c r="A69" s="107" t="s">
-        <v>547</v>
+        <v>536</v>
       </c>
       <c r="B69" s="114" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="C69" s="52" t="s">
         <v>328</v>
@@ -9146,13 +9143,13 @@
     </row>
     <row r="70" spans="1:29" s="27" customFormat="1" ht="90" customHeight="1">
       <c r="A70" s="107" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="B70" s="108" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="C70" s="108" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="D70" s="108" t="s">
         <v>270</v>
@@ -9174,10 +9171,10 @@
     </row>
     <row r="71" spans="1:29" ht="225" customHeight="1" thickBot="1">
       <c r="A71" s="70" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="B71" s="54" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C71" s="53" t="s">
         <v>5</v>
@@ -9258,10 +9255,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E7B11-1527-417B-9532-F0F2C5A89902}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9315,31 +9313,31 @@
       <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="149" t="s">
         <v>389</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
       <c r="F2" s="18"/>
-      <c r="G2" s="168" t="s">
+      <c r="G2" s="169" t="s">
         <v>137</v>
       </c>
-      <c r="H2" s="168"/>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="168"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
       <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:12" ht="60" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="162" t="s">
-        <v>444</v>
-      </c>
-      <c r="C3" s="169" t="s">
+      <c r="B3" s="163" t="s">
+        <v>443</v>
+      </c>
+      <c r="C3" s="170" t="s">
         <v>100</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -9355,7 +9353,7 @@
       <c r="H3" s="116" t="s">
         <v>134</v>
       </c>
-      <c r="I3" s="160"/>
+      <c r="I3" s="161"/>
       <c r="J3" s="7" t="s">
         <v>133</v>
       </c>
@@ -9367,8 +9365,8 @@
       <c r="A4" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="163"/>
-      <c r="C4" s="172"/>
+      <c r="B4" s="164"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="7" t="s">
         <v>346</v>
       </c>
@@ -9382,7 +9380,7 @@
       <c r="H4" s="116" t="s">
         <v>130</v>
       </c>
-      <c r="I4" s="177"/>
+      <c r="I4" s="178"/>
       <c r="J4" s="7" t="s">
         <v>116</v>
       </c>
@@ -9394,8 +9392,8 @@
       <c r="A5" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="163"/>
-      <c r="C5" s="172"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="7" t="s">
         <v>349</v>
       </c>
@@ -9409,7 +9407,7 @@
       <c r="H5" s="116" t="s">
         <v>127</v>
       </c>
-      <c r="I5" s="177"/>
+      <c r="I5" s="178"/>
       <c r="J5" s="7" t="s">
         <v>126</v>
       </c>
@@ -9421,8 +9419,8 @@
       <c r="A6" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="163"/>
-      <c r="C6" s="172"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="173"/>
       <c r="D6" s="7" t="s">
         <v>348</v>
       </c>
@@ -9436,7 +9434,7 @@
       <c r="H6" s="116" t="s">
         <v>123</v>
       </c>
-      <c r="I6" s="177"/>
+      <c r="I6" s="178"/>
       <c r="J6" s="7" t="s">
         <v>122</v>
       </c>
@@ -9448,8 +9446,8 @@
       <c r="A7" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="163"/>
-      <c r="C7" s="172"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="173"/>
       <c r="D7" s="7" t="s">
         <v>347</v>
       </c>
@@ -9463,7 +9461,7 @@
       <c r="H7" s="116" t="s">
         <v>120</v>
       </c>
-      <c r="I7" s="177"/>
+      <c r="I7" s="178"/>
       <c r="J7" s="25" t="s">
         <v>111</v>
       </c>
@@ -9475,15 +9473,15 @@
       <c r="A8" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="163"/>
-      <c r="C8" s="166" t="s">
+      <c r="B8" s="164"/>
+      <c r="C8" s="167" t="s">
         <v>66</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>218</v>
       </c>
       <c r="E8" s="135" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="10" t="s">
@@ -9492,7 +9490,7 @@
       <c r="H8" s="116" t="s">
         <v>117</v>
       </c>
-      <c r="I8" s="177"/>
+      <c r="I8" s="178"/>
       <c r="J8" s="7" t="s">
         <v>116</v>
       </c>
@@ -9504,8 +9502,8 @@
       <c r="A9" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="163"/>
-      <c r="C9" s="166"/>
+      <c r="B9" s="164"/>
+      <c r="C9" s="167"/>
       <c r="D9" s="7" t="s">
         <v>118</v>
       </c>
@@ -9517,9 +9515,9 @@
         <v>159</v>
       </c>
       <c r="H9" s="116" t="s">
-        <v>557</v>
-      </c>
-      <c r="I9" s="177"/>
+        <v>546</v>
+      </c>
+      <c r="I9" s="178"/>
       <c r="J9" s="25" t="s">
         <v>160</v>
       </c>
@@ -9531,7 +9529,7 @@
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="163"/>
+      <c r="B10" s="164"/>
       <c r="C10" s="50" t="s">
         <v>100</v>
       </c>
@@ -9548,7 +9546,7 @@
       <c r="H10" s="116" t="s">
         <v>112</v>
       </c>
-      <c r="I10" s="165"/>
+      <c r="I10" s="166"/>
       <c r="J10" s="25" t="s">
         <v>111</v>
       </c>
@@ -9557,40 +9555,40 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1">
-      <c r="A11" s="155" t="s">
+      <c r="A11" s="156" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="163"/>
-      <c r="C11" s="166" t="s">
+      <c r="B11" s="164"/>
+      <c r="C11" s="167" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="147" t="s">
+      <c r="D11" s="148" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="174" t="s">
+      <c r="E11" s="175" t="s">
         <v>152</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="144" t="s">
+      <c r="G11" s="145" t="s">
         <v>108</v>
       </c>
-      <c r="H11" s="144"/>
-      <c r="I11" s="144"/>
-      <c r="J11" s="144"/>
-      <c r="K11" s="144"/>
+      <c r="H11" s="145"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="145"/>
+      <c r="K11" s="145"/>
     </row>
     <row r="12" spans="1:12" ht="45" customHeight="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="164"/>
-      <c r="C12" s="167"/>
-      <c r="D12" s="173"/>
-      <c r="E12" s="175"/>
+      <c r="A12" s="177"/>
+      <c r="B12" s="165"/>
+      <c r="C12" s="168"/>
+      <c r="D12" s="174"/>
+      <c r="E12" s="176"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H12" s="162" t="s">
-        <v>445</v>
+      <c r="H12" s="163" t="s">
+        <v>444</v>
       </c>
       <c r="I12" s="55" t="s">
         <v>106</v>
@@ -9603,18 +9601,18 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1">
-      <c r="A13" s="159" t="s">
+      <c r="A13" s="160" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="159"/>
-      <c r="C13" s="159"/>
-      <c r="D13" s="159"/>
-      <c r="E13" s="159"/>
+      <c r="B13" s="160"/>
+      <c r="C13" s="160"/>
+      <c r="D13" s="160"/>
+      <c r="E13" s="160"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="163"/>
+      <c r="H13" s="164"/>
       <c r="I13" s="49" t="s">
         <v>102</v>
       </c>
@@ -9629,10 +9627,10 @@
       <c r="A14" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="162" t="s">
-        <v>444</v>
-      </c>
-      <c r="C14" s="169" t="s">
+      <c r="B14" s="163" t="s">
+        <v>443</v>
+      </c>
+      <c r="C14" s="170" t="s">
         <v>66</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -9645,7 +9643,7 @@
       <c r="G14" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H14" s="163"/>
+      <c r="H14" s="164"/>
       <c r="I14" s="49">
         <v>0</v>
       </c>
@@ -9660,8 +9658,8 @@
       <c r="A15" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="163"/>
-      <c r="C15" s="166"/>
+      <c r="B15" s="164"/>
+      <c r="C15" s="167"/>
       <c r="D15" s="11" t="s">
         <v>95</v>
       </c>
@@ -9672,7 +9670,7 @@
       <c r="G15" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="164"/>
+      <c r="H15" s="165"/>
       <c r="I15" s="55" t="s">
         <v>93</v>
       </c>
@@ -9684,40 +9682,40 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="155" t="s">
+      <c r="A16" s="156" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="163"/>
-      <c r="C16" s="166"/>
-      <c r="D16" s="147" t="s">
+      <c r="B16" s="164"/>
+      <c r="C16" s="167"/>
+      <c r="D16" s="148" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="171" t="s">
+      <c r="E16" s="172" t="s">
         <v>144</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="144" t="s">
+      <c r="G16" s="145" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
+      <c r="H16" s="145"/>
+      <c r="I16" s="145"/>
+      <c r="J16" s="145"/>
+      <c r="K16" s="145"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
-      <c r="A17" s="155"/>
-      <c r="B17" s="163"/>
-      <c r="C17" s="166"/>
-      <c r="D17" s="147"/>
-      <c r="E17" s="171"/>
+      <c r="A17" s="156"/>
+      <c r="B17" s="164"/>
+      <c r="C17" s="167"/>
+      <c r="D17" s="148"/>
+      <c r="E17" s="172"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="162" t="s">
-        <v>444</v>
-      </c>
-      <c r="I17" s="160"/>
+      <c r="H17" s="163" t="s">
+        <v>443</v>
+      </c>
+      <c r="I17" s="161"/>
       <c r="J17" s="7" t="s">
         <v>133</v>
       </c>
@@ -9729,8 +9727,8 @@
       <c r="A18" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="163"/>
-      <c r="C18" s="166"/>
+      <c r="B18" s="164"/>
+      <c r="C18" s="167"/>
       <c r="D18" s="7" t="s">
         <v>86</v>
       </c>
@@ -9741,8 +9739,8 @@
       <c r="G18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="163"/>
-      <c r="I18" s="161"/>
+      <c r="H18" s="164"/>
+      <c r="I18" s="162"/>
       <c r="J18" s="7" t="s">
         <v>116</v>
       </c>
@@ -9754,8 +9752,8 @@
       <c r="A19" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="163"/>
-      <c r="C19" s="166" t="s">
+      <c r="B19" s="164"/>
+      <c r="C19" s="167" t="s">
         <v>100</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -9768,8 +9766,8 @@
       <c r="G19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="163"/>
-      <c r="I19" s="161"/>
+      <c r="H19" s="164"/>
+      <c r="I19" s="162"/>
       <c r="J19" s="7" t="s">
         <v>126</v>
       </c>
@@ -9781,8 +9779,8 @@
       <c r="A20" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="163"/>
-      <c r="C20" s="166"/>
+      <c r="B20" s="164"/>
+      <c r="C20" s="167"/>
       <c r="D20" s="7" t="s">
         <v>80</v>
       </c>
@@ -9793,8 +9791,8 @@
       <c r="G20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H20" s="163"/>
-      <c r="I20" s="161"/>
+      <c r="H20" s="164"/>
+      <c r="I20" s="162"/>
       <c r="J20" s="7" t="s">
         <v>122</v>
       </c>
@@ -9806,20 +9804,20 @@
       <c r="A21" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="163"/>
-      <c r="C21" s="166"/>
+      <c r="B21" s="164"/>
+      <c r="C21" s="167"/>
       <c r="D21" s="7" t="s">
         <v>436</v>
       </c>
       <c r="E21" s="133" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="H21" s="163"/>
-      <c r="I21" s="161"/>
+      <c r="H21" s="164"/>
+      <c r="I21" s="162"/>
       <c r="J21" s="25" t="s">
         <v>111</v>
       </c>
@@ -9831,8 +9829,8 @@
       <c r="A22" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="163"/>
-      <c r="C22" s="166"/>
+      <c r="B22" s="164"/>
+      <c r="C22" s="167"/>
       <c r="D22" s="7" t="s">
         <v>75</v>
       </c>
@@ -9843,8 +9841,8 @@
       <c r="G22" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="163"/>
-      <c r="I22" s="161"/>
+      <c r="H22" s="164"/>
+      <c r="I22" s="162"/>
       <c r="J22" s="7" t="s">
         <v>116</v>
       </c>
@@ -9856,8 +9854,8 @@
       <c r="A23" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="164"/>
-      <c r="C23" s="167"/>
+      <c r="B23" s="165"/>
+      <c r="C23" s="168"/>
       <c r="D23" s="7" t="s">
         <v>72</v>
       </c>
@@ -9868,8 +9866,8 @@
       <c r="G23" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H23" s="163"/>
-      <c r="I23" s="161"/>
+      <c r="H23" s="164"/>
+      <c r="I23" s="162"/>
       <c r="J23" s="7" t="s">
         <v>160</v>
       </c>
@@ -9878,21 +9876,21 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1">
-      <c r="A24" s="159" t="s">
+      <c r="A24" s="160" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="159"/>
-      <c r="C24" s="159"/>
-      <c r="D24" s="159"/>
-      <c r="E24" s="159"/>
+      <c r="B24" s="160"/>
+      <c r="C24" s="160"/>
+      <c r="D24" s="160"/>
+      <c r="E24" s="160"/>
       <c r="F24" s="4"/>
       <c r="G24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H24" s="163" t="s">
-        <v>556</v>
-      </c>
-      <c r="I24" s="161"/>
+      <c r="H24" s="164" t="s">
+        <v>545</v>
+      </c>
+      <c r="I24" s="162"/>
       <c r="K24" s="139" t="s">
         <v>144</v>
       </c>
@@ -9902,9 +9900,9 @@
         <v>67</v>
       </c>
       <c r="B25" s="118" t="s">
-        <v>459</v>
-      </c>
-      <c r="C25" s="169" t="s">
+        <v>452</v>
+      </c>
+      <c r="C25" s="170" t="s">
         <v>274</v>
       </c>
       <c r="D25" s="56" t="s">
@@ -9917,8 +9915,8 @@
       <c r="G25" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="163"/>
-      <c r="I25" s="161"/>
+      <c r="H25" s="164"/>
+      <c r="I25" s="162"/>
       <c r="J25" s="12" t="s">
         <v>68</v>
       </c>
@@ -9931,9 +9929,9 @@
         <v>65</v>
       </c>
       <c r="B26" s="64" t="s">
-        <v>443</v>
-      </c>
-      <c r="C26" s="170"/>
+        <v>442</v>
+      </c>
+      <c r="C26" s="171"/>
       <c r="D26" s="17" t="s">
         <v>217</v>
       </c>
@@ -9944,10 +9942,10 @@
       <c r="G26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H26" s="163" t="s">
-        <v>444</v>
-      </c>
-      <c r="I26" s="161"/>
+      <c r="H26" s="164" t="s">
+        <v>443</v>
+      </c>
+      <c r="I26" s="162"/>
       <c r="J26" s="12"/>
       <c r="K26" s="139" t="s">
         <v>144</v>
@@ -9959,8 +9957,8 @@
       <c r="G27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H27" s="163"/>
-      <c r="I27" s="161"/>
+      <c r="H27" s="164"/>
+      <c r="I27" s="162"/>
       <c r="J27" s="7" t="s">
         <v>214</v>
       </c>
@@ -9974,8 +9972,8 @@
       <c r="G28" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H28" s="163"/>
-      <c r="I28" s="161"/>
+      <c r="H28" s="164"/>
+      <c r="I28" s="162"/>
       <c r="K28" s="139" t="s">
         <v>144</v>
       </c>
@@ -9984,10 +9982,10 @@
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="H29" s="164"/>
-      <c r="I29" s="165"/>
+        <v>473</v>
+      </c>
+      <c r="H29" s="165"/>
+      <c r="I29" s="166"/>
       <c r="J29" s="7" t="s">
         <v>160</v>
       </c>
@@ -9998,13 +9996,13 @@
     <row r="30" spans="1:11">
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="144" t="s">
+      <c r="G30" s="145" t="s">
         <v>61</v>
       </c>
-      <c r="H30" s="144"/>
-      <c r="I30" s="144"/>
-      <c r="J30" s="144"/>
-      <c r="K30" s="168"/>
+      <c r="H30" s="145"/>
+      <c r="I30" s="145"/>
+      <c r="J30" s="145"/>
+      <c r="K30" s="169"/>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="D31" s="4"/>
@@ -10013,9 +10011,9 @@
         <v>60</v>
       </c>
       <c r="H31" s="116" t="s">
-        <v>455</v>
-      </c>
-      <c r="I31" s="160"/>
+        <v>448</v>
+      </c>
+      <c r="I31" s="161"/>
       <c r="J31" s="7" t="s">
         <v>59</v>
       </c>
@@ -10032,7 +10030,7 @@
       <c r="H32" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="I32" s="161"/>
+      <c r="I32" s="162"/>
       <c r="J32" s="7" t="s">
         <v>56</v>
       </c>
@@ -10047,7 +10045,7 @@
         <v>55</v>
       </c>
       <c r="H33" s="116" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="I33" s="63" t="s">
         <v>256</v>
@@ -10066,7 +10064,7 @@
         <v>54</v>
       </c>
       <c r="H34" s="116" t="s">
-        <v>446</v>
+        <v>592</v>
       </c>
       <c r="I34" s="63" t="s">
         <v>255</v>
@@ -10085,7 +10083,7 @@
         <v>53</v>
       </c>
       <c r="H35" s="64" t="s">
-        <v>447</v>
+        <v>593</v>
       </c>
       <c r="I35" s="129" t="s">
         <v>257</v>
@@ -10247,6 +10245,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78528ED-BDD5-4579-AF2D-C3BAE2A38DA8}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -10302,30 +10301,30 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="149" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
       <c r="F2" s="18"/>
-      <c r="G2" s="149" t="s">
+      <c r="G2" s="150" t="s">
         <v>429</v>
       </c>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
+      <c r="J2" s="150"/>
+      <c r="K2" s="150"/>
     </row>
     <row r="3" spans="1:11" ht="30">
       <c r="A3" s="5" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B3" s="119" t="s">
-        <v>455</v>
-      </c>
-      <c r="C3" s="183" t="s">
+        <v>448</v>
+      </c>
+      <c r="C3" s="184" t="s">
         <v>343</v>
       </c>
       <c r="D3" s="40" t="s">
@@ -10339,9 +10338,9 @@
         <v>431</v>
       </c>
       <c r="H3" s="116" t="s">
-        <v>456</v>
-      </c>
-      <c r="I3" s="195"/>
+        <v>449</v>
+      </c>
+      <c r="I3" s="196"/>
       <c r="J3" s="40" t="s">
         <v>440</v>
       </c>
@@ -10351,12 +10350,12 @@
     </row>
     <row r="4" spans="1:11" ht="30">
       <c r="A4" s="125" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B4" s="126" t="s">
-        <v>457</v>
-      </c>
-      <c r="C4" s="185"/>
+        <v>450</v>
+      </c>
+      <c r="C4" s="186"/>
       <c r="D4" s="40" t="s">
         <v>303</v>
       </c>
@@ -10368,65 +10367,65 @@
         <v>434</v>
       </c>
       <c r="H4" s="116" t="s">
-        <v>456</v>
-      </c>
-      <c r="I4" s="196"/>
+        <v>449</v>
+      </c>
+      <c r="I4" s="197"/>
       <c r="J4" s="40"/>
       <c r="K4" s="131" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
-      <c r="A5" s="159" t="s">
+      <c r="A5" s="160" t="s">
         <v>430</v>
       </c>
-      <c r="B5" s="159"/>
-      <c r="C5" s="159"/>
-      <c r="D5" s="159"/>
-      <c r="E5" s="159"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="160"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="160"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="158" t="s">
+      <c r="G5" s="159" t="s">
         <v>433</v>
       </c>
-      <c r="H5" s="177" t="s">
-        <v>456</v>
-      </c>
-      <c r="I5" s="196"/>
-      <c r="J5" s="145" t="s">
+      <c r="H5" s="178" t="s">
+        <v>449</v>
+      </c>
+      <c r="I5" s="197"/>
+      <c r="J5" s="146" t="s">
         <v>437</v>
       </c>
-      <c r="K5" s="190" t="s">
+      <c r="K5" s="191" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="B6" s="162" t="s">
-        <v>442</v>
+        <v>457</v>
+      </c>
+      <c r="B6" s="163" t="s">
+        <v>441</v>
       </c>
       <c r="C6" s="120" t="s">
         <v>344</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="E6" s="131" t="s">
         <v>144</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="158"/>
-      <c r="H6" s="177"/>
-      <c r="I6" s="196"/>
-      <c r="J6" s="145"/>
-      <c r="K6" s="190"/>
+      <c r="G6" s="159"/>
+      <c r="H6" s="178"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="191"/>
     </row>
     <row r="7" spans="1:11" ht="75" customHeight="1" thickBot="1">
       <c r="A7" s="13" t="s">
-        <v>464</v>
-      </c>
-      <c r="B7" s="178"/>
+        <v>456</v>
+      </c>
+      <c r="B7" s="179"/>
       <c r="C7" s="64" t="s">
         <v>344</v>
       </c>
@@ -10437,32 +10436,32 @@
         <v>152</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="158" t="s">
+      <c r="G7" s="159" t="s">
         <v>432</v>
       </c>
-      <c r="H7" s="177" t="s">
-        <v>495</v>
-      </c>
-      <c r="I7" s="196"/>
-      <c r="J7" s="147" t="s">
+      <c r="H7" s="178" t="s">
+        <v>487</v>
+      </c>
+      <c r="I7" s="197"/>
+      <c r="J7" s="148" t="s">
         <v>435</v>
       </c>
-      <c r="K7" s="171" t="s">
-        <v>484</v>
+      <c r="K7" s="172" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="D8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="193"/>
-      <c r="H8" s="165"/>
-      <c r="I8" s="197"/>
-      <c r="J8" s="173"/>
-      <c r="K8" s="194"/>
+      <c r="G8" s="194"/>
+      <c r="H8" s="166"/>
+      <c r="I8" s="198"/>
+      <c r="J8" s="174"/>
+      <c r="K8" s="195"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" thickBot="1">
       <c r="A9" s="1" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>318</v>
@@ -10477,122 +10476,122 @@
         <v>138</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="159" t="s">
+      <c r="G9" s="160" t="s">
         <v>439</v>
       </c>
-      <c r="H9" s="159"/>
-      <c r="I9" s="159"/>
-      <c r="J9" s="159"/>
-      <c r="K9" s="159"/>
+      <c r="H9" s="160"/>
+      <c r="I9" s="160"/>
+      <c r="J9" s="160"/>
+      <c r="K9" s="160"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="186" t="s">
-        <v>508</v>
-      </c>
-      <c r="B10" s="186"/>
-      <c r="C10" s="186"/>
-      <c r="D10" s="186"/>
-      <c r="E10" s="186"/>
+      <c r="A10" s="187" t="s">
+        <v>500</v>
+      </c>
+      <c r="B10" s="187"/>
+      <c r="C10" s="187"/>
+      <c r="D10" s="187"/>
+      <c r="E10" s="187"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="187" t="s">
-        <v>469</v>
-      </c>
-      <c r="H10" s="160" t="s">
-        <v>528</v>
-      </c>
-      <c r="I10" s="183"/>
-      <c r="J10" s="188" t="s">
-        <v>474</v>
-      </c>
-      <c r="K10" s="189" t="s">
+      <c r="G10" s="188" t="s">
+        <v>461</v>
+      </c>
+      <c r="H10" s="161" t="s">
+        <v>520</v>
+      </c>
+      <c r="I10" s="184"/>
+      <c r="J10" s="189" t="s">
+        <v>466</v>
+      </c>
+      <c r="K10" s="190" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1">
       <c r="A11" s="138" t="s">
-        <v>516</v>
-      </c>
-      <c r="B11" s="192" t="s">
-        <v>442</v>
-      </c>
-      <c r="C11" s="179"/>
+        <v>508</v>
+      </c>
+      <c r="B11" s="193" t="s">
+        <v>441</v>
+      </c>
+      <c r="C11" s="180"/>
       <c r="D11" s="114" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="E11" s="137" t="s">
         <v>142</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="158"/>
-      <c r="H11" s="161"/>
-      <c r="I11" s="184"/>
-      <c r="J11" s="145"/>
-      <c r="K11" s="190"/>
+      <c r="G11" s="159"/>
+      <c r="H11" s="162"/>
+      <c r="I11" s="185"/>
+      <c r="J11" s="146"/>
+      <c r="K11" s="191"/>
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="138" t="s">
-        <v>515</v>
-      </c>
-      <c r="B12" s="182"/>
-      <c r="C12" s="180"/>
+        <v>507</v>
+      </c>
+      <c r="B12" s="183"/>
+      <c r="C12" s="181"/>
       <c r="D12" s="114" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="E12" s="137" t="s">
         <v>152</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="158"/>
-      <c r="H12" s="161"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="145"/>
-      <c r="K12" s="190"/>
+      <c r="G12" s="159"/>
+      <c r="H12" s="162"/>
+      <c r="I12" s="185"/>
+      <c r="J12" s="146"/>
+      <c r="K12" s="191"/>
     </row>
     <row r="13" spans="1:11" ht="45" customHeight="1">
       <c r="A13" s="138" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="B13" s="124" t="s">
-        <v>522</v>
-      </c>
-      <c r="C13" s="180"/>
+        <v>514</v>
+      </c>
+      <c r="C13" s="181"/>
       <c r="D13" s="114" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="E13" s="137" t="s">
         <v>144</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="158"/>
-      <c r="H13" s="161"/>
-      <c r="I13" s="184"/>
-      <c r="J13" s="145"/>
-      <c r="K13" s="190"/>
+      <c r="G13" s="159"/>
+      <c r="H13" s="162"/>
+      <c r="I13" s="185"/>
+      <c r="J13" s="146"/>
+      <c r="K13" s="191"/>
     </row>
     <row r="14" spans="1:11" ht="105" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="B14" s="182" t="s">
-        <v>520</v>
-      </c>
-      <c r="C14" s="180"/>
+        <v>511</v>
+      </c>
+      <c r="B14" s="183" t="s">
+        <v>512</v>
+      </c>
+      <c r="C14" s="181"/>
       <c r="D14" s="40" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="E14" s="131" t="s">
         <v>144</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="7" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="H14" s="116" t="s">
-        <v>528</v>
-      </c>
-      <c r="I14" s="184"/>
+        <v>520</v>
+      </c>
+      <c r="I14" s="185"/>
       <c r="J14" s="7" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="K14" s="133" t="s">
         <v>144</v>
@@ -10600,26 +10599,26 @@
     </row>
     <row r="15" spans="1:11" ht="105" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>505</v>
-      </c>
-      <c r="B15" s="182"/>
-      <c r="C15" s="180"/>
+        <v>497</v>
+      </c>
+      <c r="B15" s="183"/>
+      <c r="C15" s="181"/>
       <c r="D15" s="40" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="E15" s="131" t="s">
         <v>152</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="H15" s="119" t="s">
-        <v>509</v>
-      </c>
-      <c r="I15" s="184"/>
+        <v>501</v>
+      </c>
+      <c r="I15" s="185"/>
       <c r="J15" s="7" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="K15" s="133" t="s">
         <v>152</v>
@@ -10627,47 +10626,47 @@
     </row>
     <row r="16" spans="1:11" ht="90" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="B16" s="119" t="s">
-        <v>521</v>
-      </c>
-      <c r="C16" s="181"/>
+        <v>513</v>
+      </c>
+      <c r="C16" s="182"/>
       <c r="D16" s="40" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="E16" s="131" t="s">
         <v>142</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="142" t="s">
-        <v>475</v>
-      </c>
-      <c r="H16" s="161" t="s">
-        <v>510</v>
-      </c>
-      <c r="I16" s="184"/>
-      <c r="J16" s="147" t="s">
-        <v>488</v>
-      </c>
-      <c r="K16" s="171" t="s">
+      <c r="G16" s="143" t="s">
+        <v>467</v>
+      </c>
+      <c r="H16" s="162" t="s">
+        <v>502</v>
+      </c>
+      <c r="I16" s="185"/>
+      <c r="J16" s="148" t="s">
+        <v>480</v>
+      </c>
+      <c r="K16" s="172" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
-      <c r="A17" s="159" t="s">
+      <c r="A17" s="160" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="159"/>
-      <c r="C17" s="159"/>
-      <c r="D17" s="159"/>
-      <c r="E17" s="159"/>
+      <c r="B17" s="160"/>
+      <c r="C17" s="160"/>
+      <c r="D17" s="160"/>
+      <c r="E17" s="160"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="142"/>
-      <c r="H17" s="161"/>
-      <c r="I17" s="184"/>
-      <c r="J17" s="147"/>
-      <c r="K17" s="171"/>
+      <c r="G17" s="143"/>
+      <c r="H17" s="162"/>
+      <c r="I17" s="185"/>
+      <c r="J17" s="148"/>
+      <c r="K17" s="172"/>
     </row>
     <row r="18" spans="1:11" ht="105" customHeight="1" thickBot="1">
       <c r="A18" s="136" t="s">
@@ -10681,46 +10680,46 @@
         <v>211</v>
       </c>
       <c r="E18" s="132" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="38" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="H18" s="119" t="s">
-        <v>511</v>
-      </c>
-      <c r="I18" s="185"/>
+        <v>503</v>
+      </c>
+      <c r="I18" s="186"/>
       <c r="J18" s="40" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="K18" s="131" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="D19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="159" t="s">
-        <v>477</v>
-      </c>
-      <c r="H19" s="159"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
-      <c r="K19" s="159"/>
+      <c r="G19" s="160" t="s">
+        <v>469</v>
+      </c>
+      <c r="H19" s="160"/>
+      <c r="I19" s="160"/>
+      <c r="J19" s="160"/>
+      <c r="K19" s="160"/>
     </row>
     <row r="20" spans="1:11" ht="60">
       <c r="D20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="130" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="H20" s="118" t="s">
-        <v>490</v>
-      </c>
-      <c r="I20" s="183"/>
+        <v>482</v>
+      </c>
+      <c r="I20" s="184"/>
       <c r="J20" s="56" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="K20" s="134" t="s">
         <v>144</v>
@@ -10730,14 +10729,14 @@
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="38" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="H21" s="119" t="s">
-        <v>491</v>
-      </c>
-      <c r="I21" s="184"/>
+        <v>483</v>
+      </c>
+      <c r="I21" s="185"/>
       <c r="J21" s="40" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="K21" s="131" t="s">
         <v>142</v>
@@ -10747,14 +10746,14 @@
       <c r="D22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="38" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="H22" s="119" t="s">
-        <v>493</v>
-      </c>
-      <c r="I22" s="184"/>
+        <v>485</v>
+      </c>
+      <c r="I22" s="185"/>
       <c r="J22" s="40" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="K22" s="131" t="s">
         <v>152</v>
@@ -10764,14 +10763,14 @@
       <c r="D23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="38" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="H23" s="119" t="s">
-        <v>500</v>
-      </c>
-      <c r="I23" s="184"/>
+        <v>492</v>
+      </c>
+      <c r="I23" s="185"/>
       <c r="J23" s="40" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="K23" s="131" t="s">
         <v>152</v>
@@ -10781,12 +10780,12 @@
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="14" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="H24" s="64" t="s">
-        <v>482</v>
-      </c>
-      <c r="I24" s="191"/>
+        <v>474</v>
+      </c>
+      <c r="I24" s="192"/>
       <c r="J24" s="17" t="s">
         <v>160</v>
       </c>
@@ -10959,10 +10958,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6E6499-880E-4FF5-B745-8B197E0A76DF}">
-  <dimension ref="A1:L58"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11022,7 +11022,7 @@
       <c r="B2" s="123" t="s">
         <v>441</v>
       </c>
-      <c r="C2" s="198" t="s">
+      <c r="C2" s="199" t="s">
         <v>153</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -11054,9 +11054,9 @@
         <v>269</v>
       </c>
       <c r="B3" s="121" t="s">
-        <v>449</v>
-      </c>
-      <c r="C3" s="166"/>
+        <v>584</v>
+      </c>
+      <c r="C3" s="167"/>
       <c r="D3" s="7"/>
       <c r="E3" s="36" t="s">
         <v>152</v>
@@ -11066,13 +11066,13 @@
         <v>387</v>
       </c>
       <c r="H3" s="121" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="I3" s="42">
         <v>0</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="K3" s="35" t="s">
         <v>144</v>
@@ -11083,9 +11083,9 @@
         <v>151</v>
       </c>
       <c r="B4" s="121" t="s">
-        <v>450</v>
-      </c>
-      <c r="C4" s="166" t="s">
+        <v>585</v>
+      </c>
+      <c r="C4" s="167" t="s">
         <v>150</v>
       </c>
       <c r="D4" s="7"/>
@@ -11097,7 +11097,7 @@
         <v>213</v>
       </c>
       <c r="H4" s="110" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="I4" s="34" t="s">
         <v>149</v>
@@ -11114,9 +11114,9 @@
         <v>148</v>
       </c>
       <c r="B5" s="121" t="s">
-        <v>451</v>
-      </c>
-      <c r="C5" s="166"/>
+        <v>586</v>
+      </c>
+      <c r="C5" s="167"/>
       <c r="D5" s="7"/>
       <c r="E5" s="36" t="s">
         <v>144</v>
@@ -11128,8 +11128,8 @@
       <c r="A6" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="B6" s="163" t="s">
-        <v>452</v>
+      <c r="B6" s="164" t="s">
+        <v>587</v>
       </c>
       <c r="C6" s="22">
         <v>0</v>
@@ -11145,8 +11145,8 @@
       <c r="A7" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="B7" s="199"/>
-      <c r="C7" s="166" t="s">
+      <c r="B7" s="200"/>
+      <c r="C7" s="167" t="s">
         <v>150</v>
       </c>
       <c r="D7" s="7"/>
@@ -11161,8 +11161,8 @@
       <c r="A8" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="B8" s="199"/>
-      <c r="C8" s="166"/>
+      <c r="B8" s="200"/>
+      <c r="C8" s="167"/>
       <c r="D8" s="7"/>
       <c r="E8" s="35" t="s">
         <v>144</v>
@@ -11178,7 +11178,7 @@
       <c r="A9" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="B9" s="163" t="s">
+      <c r="B9" s="164" t="s">
         <v>441</v>
       </c>
       <c r="C9" s="22" t="s">
@@ -11195,15 +11195,17 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="B10" s="199"/>
-      <c r="C10" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="7"/>
+        <v>385</v>
+      </c>
+      <c r="B10" s="164"/>
+      <c r="C10" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>212</v>
+      </c>
       <c r="E10" s="35" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F10" s="4"/>
       <c r="H10" s="11"/>
@@ -11212,30 +11214,30 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B11" s="199"/>
+        <v>386</v>
+      </c>
+      <c r="B11" s="164"/>
       <c r="C11" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>212</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D11" s="7"/>
       <c r="E11" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F11" s="4"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1">
+    <row r="12" spans="1:12" ht="45" customHeight="1" thickBot="1">
       <c r="A12" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="B12" s="200"/>
-      <c r="C12" s="34" t="s">
-        <v>143</v>
+        <v>384</v>
+      </c>
+      <c r="B12" s="110" t="s">
+        <v>441</v>
+      </c>
+      <c r="C12" s="142" t="s">
+        <v>146</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="33" t="s">
@@ -11259,31 +11261,29 @@
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
     </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+    <row r="14" spans="1:12">
+      <c r="B14" s="8"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="7"/>
       <c r="F14" s="4"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="K14" s="4"/>
+      <c r="K14"/>
     </row>
     <row r="15" spans="1:12">
+      <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="32"/>
-      <c r="D15" s="7"/>
+      <c r="D15" s="11"/>
       <c r="F15" s="4"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
-      <c r="K15"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="32"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="7"/>
       <c r="F16" s="4"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -11314,16 +11314,14 @@
       <c r="F19" s="4"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
-      <c r="K19" s="4"/>
+      <c r="K19" s="23"/>
     </row>
     <row r="20" spans="1:11">
       <c r="B20" s="8"/>
       <c r="C20" s="32"/>
       <c r="D20" s="7"/>
       <c r="F20" s="4"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="K20" s="23"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11">
       <c r="B21" s="8"/>
@@ -11333,55 +11331,55 @@
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="B22" s="8"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="7"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
       <c r="F22" s="4"/>
-      <c r="K22" s="7"/>
+      <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="B24" s="8"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="32"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="7"/>
       <c r="F24" s="4"/>
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="B25" s="11"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="K25" s="7"/>
+      <c r="K25" s="4"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="D27" s="4"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+    </row>
+    <row r="27" spans="1:11" ht="30" customHeight="1">
+      <c r="B27" s="8"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="7"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-    </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1">
-      <c r="B28" s="8"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="7"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="D28" s="4"/>
       <c r="F28" s="4"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
@@ -11390,9 +11388,7 @@
     <row r="29" spans="1:11">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="K29" s="7"/>
+      <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11">
       <c r="D30" s="4"/>
@@ -11531,18 +11527,13 @@
     </row>
     <row r="57" spans="4:11">
       <c r="D57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="K57" s="4"/>
-    </row>
-    <row r="58" spans="4:11">
-      <c r="D58" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B9:B12"/>
     <mergeCell ref="B6:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11552,10 +11543,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD902308-2995-4981-9D8D-2D9FAE7EB6D0}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11606,29 +11598,29 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="160" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="159"/>
-      <c r="C2" s="159"/>
-      <c r="D2" s="159"/>
-      <c r="E2" s="159"/>
-      <c r="G2" s="159" t="s">
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="G2" s="160" t="s">
         <v>299</v>
       </c>
-      <c r="H2" s="159"/>
-      <c r="I2" s="159"/>
-      <c r="J2" s="159"/>
-      <c r="K2" s="159"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="B3" s="162" t="s">
-        <v>460</v>
-      </c>
-      <c r="C3" s="169" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3" s="163" t="s">
+        <v>453</v>
+      </c>
+      <c r="C3" s="170" t="s">
         <v>150</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -11645,10 +11637,10 @@
     </row>
     <row r="4" spans="1:11" ht="30">
       <c r="A4" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="B4" s="163"/>
-      <c r="C4" s="172"/>
+        <v>521</v>
+      </c>
+      <c r="B4" s="164"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="40" t="s">
         <v>292</v>
       </c>
@@ -11664,9 +11656,9 @@
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>533</v>
-      </c>
-      <c r="B5" s="163"/>
+        <v>522</v>
+      </c>
+      <c r="B5" s="164"/>
       <c r="C5" s="67" t="s">
         <v>102</v>
       </c>
@@ -11685,10 +11677,10 @@
     </row>
     <row r="6" spans="1:11" ht="105">
       <c r="A6" s="5" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="C6" s="67" t="s">
         <v>293</v>
@@ -11707,13 +11699,13 @@
       <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="159" t="s">
+      <c r="A7" s="160" t="s">
         <v>298</v>
       </c>
-      <c r="B7" s="159"/>
-      <c r="C7" s="159"/>
-      <c r="D7" s="159"/>
-      <c r="E7" s="159"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="160"/>
+      <c r="D7" s="160"/>
+      <c r="E7" s="160"/>
       <c r="F7" s="46"/>
       <c r="G7" s="38"/>
       <c r="H7" s="38"/>
@@ -11723,10 +11715,10 @@
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>535</v>
-      </c>
-      <c r="B8" s="162" t="s">
-        <v>463</v>
+        <v>524</v>
+      </c>
+      <c r="B8" s="163" t="s">
+        <v>588</v>
       </c>
       <c r="C8" s="67" t="s">
         <v>102</v>
@@ -11744,9 +11736,9 @@
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="B9" s="163"/>
+        <v>525</v>
+      </c>
+      <c r="B9" s="164"/>
       <c r="C9" s="67" t="s">
         <v>102</v>
       </c>
@@ -11765,10 +11757,10 @@
     </row>
     <row r="10" spans="1:11" ht="30.75" thickBot="1">
       <c r="A10" s="13" t="s">
-        <v>537</v>
+        <v>526</v>
       </c>
       <c r="B10" s="64" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="C10" s="82" t="s">
         <v>293</v>
@@ -12097,6 +12089,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614F32F9-8D4F-4B7C-ACE2-D0F7B904B029}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12246,10 +12239,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BDD3E4-CD4B-4172-8C8B-0D7A30DAAB4E}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:I4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12329,7 +12323,7 @@
         <v>191</v>
       </c>
       <c r="G7" s="116" t="s">
-        <v>530</v>
+        <v>589</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="133" t="s">
@@ -12341,11 +12335,11 @@
         <v>193</v>
       </c>
       <c r="G8" s="116" t="s">
-        <v>529</v>
+        <v>590</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="133" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75.75" thickBot="1">
@@ -12353,7 +12347,7 @@
         <v>192</v>
       </c>
       <c r="G9" s="64" t="s">
-        <v>531</v>
+        <v>591</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="132" t="s">

</xml_diff>

<commit_message>
worked on step dice and exotic weapon strikers.
</commit_message>
<xml_diff>
--- a/Items and Components.xlsx
+++ b/Items and Components.xlsx
@@ -2355,7 +2355,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1 trident head (1.5 lbs, 10")
+      <t xml:space="preserve">1 trident tip (1.5 lbs, 10")
 </t>
     </r>
     <r>
@@ -4679,16 +4679,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">slashing 2
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">forceful 1 </t>
+forceful 1 </t>
     </r>
     <r>
       <rPr>
@@ -4697,6 +4688,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">IF</t>
     </r>
@@ -4706,19 +4698,10 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> slashing
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">finesse
+finesse
 heavy </t>
     </r>
     <r>
@@ -5638,7 +5621,7 @@
     <t xml:space="preserve">Needletip</t>
   </si>
   <si>
-    <t xml:space="preserve">thrusting 1
+    <t xml:space="preserve">thrusting
 thrown</t>
   </si>
   <si>
@@ -5656,11 +5639,12 @@
     <t xml:space="preserve">Glyph Guard</t>
   </si>
   <si>
-    <t xml:space="preserve">Trident Head</t>
+    <t xml:space="preserve">Trident Tip</t>
   </si>
   <si>
     <t xml:space="preserve">thrusting
-multi-pronged</t>
+multi-pronged
+superior parry</t>
   </si>
   <si>
     <t xml:space="preserve">One-Handed Grip</t>
@@ -6982,7 +6966,7 @@
     <numFmt numFmtId="165" formatCode="dd\-mmm"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -7036,19 +7020,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -7233,7 +7204,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="141">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7498,62 +7469,66 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7562,10 +7537,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7631,10 +7602,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7821,11 +7788,11 @@
   </sheetPr>
   <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.85"/>
@@ -9533,11 +9500,11 @@
   </sheetPr>
   <dimension ref="A1:Y57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J36" activeCellId="0" sqref="J36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.99"/>
@@ -9634,10 +9601,10 @@
         <v>328</v>
       </c>
       <c r="J3" s="69"/>
-      <c r="K3" s="70" t="s">
+      <c r="K3" s="37" t="s">
         <v>329</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="70" t="s">
         <v>330</v>
       </c>
       <c r="Y3" s="67" t="s">
@@ -9661,8 +9628,8 @@
       <c r="H4" s="50"/>
       <c r="I4" s="68"/>
       <c r="J4" s="69"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="71"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="70"/>
     </row>
     <row r="5" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -9902,7 +9869,7 @@
       <c r="I13" s="64" t="s">
         <v>373</v>
       </c>
-      <c r="J13" s="66" t="s">
+      <c r="J13" s="80" t="s">
         <v>374</v>
       </c>
       <c r="K13" s="1" t="s">
@@ -9926,7 +9893,7 @@
         <v>377</v>
       </c>
       <c r="I14" s="64"/>
-      <c r="J14" s="66" t="s">
+      <c r="J14" s="80" t="s">
         <v>378</v>
       </c>
       <c r="K14" s="1" t="s">
@@ -9958,7 +9925,7 @@
         <v>382</v>
       </c>
       <c r="I15" s="64"/>
-      <c r="J15" s="66" t="n">
+      <c r="J15" s="80" t="n">
         <v>0</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -9982,11 +9949,11 @@
         <v>331</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="80" t="s">
+      <c r="H16" s="81" t="s">
         <v>386</v>
       </c>
       <c r="I16" s="64"/>
-      <c r="J16" s="66" t="s">
+      <c r="J16" s="80" t="s">
         <v>387</v>
       </c>
       <c r="K16" s="1" t="s">
@@ -10035,7 +10002,7 @@
       <c r="H18" s="79" t="s">
         <v>393</v>
       </c>
-      <c r="I18" s="81" t="s">
+      <c r="I18" s="82" t="s">
         <v>322</v>
       </c>
       <c r="J18" s="69"/>
@@ -10055,7 +10022,7 @@
       <c r="D19" s="37" t="s">
         <v>395</v>
       </c>
-      <c r="E19" s="82"/>
+      <c r="E19" s="66"/>
       <c r="F19" s="83" t="s">
         <v>331</v>
       </c>
@@ -10063,7 +10030,7 @@
       <c r="H19" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="I19" s="81"/>
+      <c r="I19" s="82"/>
       <c r="J19" s="69"/>
       <c r="K19" s="1" t="s">
         <v>339</v>
@@ -10089,7 +10056,7 @@
       <c r="H20" s="19" t="s">
         <v>399</v>
       </c>
-      <c r="I20" s="81"/>
+      <c r="I20" s="82"/>
       <c r="J20" s="69"/>
       <c r="K20" s="1" t="s">
         <v>344</v>
@@ -10115,7 +10082,7 @@
       <c r="H21" s="19" t="s">
         <v>402</v>
       </c>
-      <c r="I21" s="81"/>
+      <c r="I21" s="82"/>
       <c r="J21" s="69"/>
       <c r="K21" s="1" t="s">
         <v>349</v>
@@ -10143,7 +10110,7 @@
       <c r="H22" s="19" t="s">
         <v>405</v>
       </c>
-      <c r="I22" s="81"/>
+      <c r="I22" s="82"/>
       <c r="J22" s="69"/>
       <c r="K22" s="1" t="s">
         <v>354</v>
@@ -10169,7 +10136,7 @@
       <c r="H23" s="19" t="s">
         <v>408</v>
       </c>
-      <c r="I23" s="81"/>
+      <c r="I23" s="82"/>
       <c r="J23" s="69"/>
       <c r="K23" s="1" t="s">
         <v>339</v>
@@ -10195,7 +10162,7 @@
       <c r="H24" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="I24" s="81"/>
+      <c r="I24" s="82"/>
       <c r="J24" s="69"/>
       <c r="K24" s="1" t="s">
         <v>364</v>
@@ -10204,7 +10171,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
         <v>412</v>
       </c>
@@ -10230,7 +10197,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="80" t="s">
+      <c r="A26" s="81" t="s">
         <v>416</v>
       </c>
       <c r="B26" s="64"/>
@@ -10410,7 +10377,7 @@
       <c r="I34" s="57" t="s">
         <v>435</v>
       </c>
-      <c r="J34" s="66" t="s">
+      <c r="J34" s="80" t="s">
         <v>441</v>
       </c>
       <c r="K34" s="1" t="s">
@@ -10430,7 +10397,7 @@
       <c r="I35" s="57" t="s">
         <v>444</v>
       </c>
-      <c r="J35" s="66" t="s">
+      <c r="J35" s="80" t="s">
         <v>378</v>
       </c>
       <c r="K35" s="1" t="s">
@@ -10650,7 +10617,7 @@
       <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.99"/>
@@ -10785,7 +10752,7 @@
       <c r="G5" s="24" t="s">
         <v>463</v>
       </c>
-      <c r="H5" s="100" t="s">
+      <c r="H5" s="68" t="s">
         <v>457</v>
       </c>
       <c r="I5" s="97"/>
@@ -10800,10 +10767,10 @@
       <c r="A6" s="19" t="s">
         <v>465</v>
       </c>
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="100" t="s">
         <v>466</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="101" t="s">
         <v>467</v>
       </c>
       <c r="D6" s="31" t="s">
@@ -10814,7 +10781,7 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="24"/>
-      <c r="H6" s="100"/>
+      <c r="H6" s="68"/>
       <c r="I6" s="97"/>
       <c r="J6" s="37"/>
       <c r="K6" s="83"/>
@@ -10823,7 +10790,7 @@
       <c r="A7" s="32" t="s">
         <v>469</v>
       </c>
-      <c r="B7" s="101"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="90" t="s">
         <v>467</v>
       </c>
@@ -10837,7 +10804,7 @@
       <c r="G7" s="49" t="s">
         <v>470</v>
       </c>
-      <c r="H7" s="103" t="s">
+      <c r="H7" s="102" t="s">
         <v>471</v>
       </c>
       <c r="I7" s="97"/>
@@ -10852,7 +10819,7 @@
       <c r="D8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="49"/>
-      <c r="H8" s="103"/>
+      <c r="H8" s="102"/>
       <c r="I8" s="97"/>
       <c r="J8" s="76"/>
       <c r="K8" s="92"/>
@@ -10883,22 +10850,22 @@
       <c r="K9" s="42"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="103" t="s">
         <v>476</v>
       </c>
-      <c r="B10" s="104"/>
-      <c r="C10" s="104"/>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="105" t="s">
+      <c r="G10" s="104" t="s">
         <v>477</v>
       </c>
       <c r="H10" s="86" t="s">
         <v>478</v>
       </c>
-      <c r="I10" s="106"/>
-      <c r="J10" s="107" t="s">
+      <c r="I10" s="105"/>
+      <c r="J10" s="106" t="s">
         <v>479</v>
       </c>
       <c r="K10" s="89" t="s">
@@ -10909,10 +10876,10 @@
       <c r="A11" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="82" t="s">
         <v>466</v>
       </c>
-      <c r="C11" s="108"/>
+      <c r="C11" s="107"/>
       <c r="D11" s="37" t="s">
         <v>481</v>
       </c>
@@ -10920,18 +10887,18 @@
         <v>331</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="105"/>
+      <c r="G11" s="104"/>
       <c r="H11" s="86"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="107"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="106"/>
       <c r="K11" s="89"/>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="26" t="s">
         <v>482</v>
       </c>
-      <c r="B12" s="81"/>
-      <c r="C12" s="108"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="107"/>
       <c r="D12" s="37" t="s">
         <v>483</v>
       </c>
@@ -10939,20 +10906,20 @@
         <v>334</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="105"/>
+      <c r="G12" s="104"/>
       <c r="H12" s="86"/>
-      <c r="I12" s="106"/>
-      <c r="J12" s="107"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="106"/>
       <c r="K12" s="89"/>
     </row>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
         <v>484</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="108" t="s">
         <v>485</v>
       </c>
-      <c r="C13" s="108"/>
+      <c r="C13" s="107"/>
       <c r="D13" s="37" t="s">
         <v>486</v>
       </c>
@@ -10960,10 +10927,10 @@
         <v>330</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="105"/>
+      <c r="G13" s="104"/>
       <c r="H13" s="86"/>
-      <c r="I13" s="106"/>
-      <c r="J13" s="107"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="106"/>
       <c r="K13" s="89"/>
     </row>
     <row r="14" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10973,7 +10940,7 @@
       <c r="B14" s="84" t="s">
         <v>488</v>
       </c>
-      <c r="C14" s="108"/>
+      <c r="C14" s="107"/>
       <c r="D14" s="31" t="s">
         <v>489</v>
       </c>
@@ -10987,7 +10954,7 @@
       <c r="H14" s="57" t="s">
         <v>478</v>
       </c>
-      <c r="I14" s="106"/>
+      <c r="I14" s="105"/>
       <c r="J14" s="1" t="s">
         <v>491</v>
       </c>
@@ -11000,7 +10967,7 @@
         <v>492</v>
       </c>
       <c r="B15" s="84"/>
-      <c r="C15" s="108"/>
+      <c r="C15" s="107"/>
       <c r="D15" s="31" t="s">
         <v>493</v>
       </c>
@@ -11014,7 +10981,7 @@
       <c r="H15" s="95" t="s">
         <v>495</v>
       </c>
-      <c r="I15" s="106"/>
+      <c r="I15" s="105"/>
       <c r="J15" s="1" t="s">
         <v>493</v>
       </c>
@@ -11029,7 +10996,7 @@
       <c r="B16" s="95" t="s">
         <v>497</v>
       </c>
-      <c r="C16" s="108"/>
+      <c r="C16" s="107"/>
       <c r="D16" s="31" t="s">
         <v>498</v>
       </c>
@@ -11040,10 +11007,10 @@
       <c r="G16" s="24" t="s">
         <v>499</v>
       </c>
-      <c r="H16" s="100" t="s">
+      <c r="H16" s="68" t="s">
         <v>500</v>
       </c>
-      <c r="I16" s="106"/>
+      <c r="I16" s="105"/>
       <c r="J16" s="37" t="s">
         <v>498</v>
       </c>
@@ -11061,8 +11028,8 @@
       <c r="E17" s="42"/>
       <c r="F17" s="2"/>
       <c r="G17" s="24"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="106"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="105"/>
       <c r="J17" s="37"/>
       <c r="K17" s="83"/>
     </row>
@@ -11087,7 +11054,7 @@
       <c r="H18" s="95" t="s">
         <v>505</v>
       </c>
-      <c r="I18" s="106"/>
+      <c r="I18" s="105"/>
       <c r="J18" s="31" t="s">
         <v>506</v>
       </c>
@@ -11109,13 +11076,13 @@
     <row r="20" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="110" t="s">
+      <c r="G20" s="109" t="s">
         <v>508</v>
       </c>
       <c r="H20" s="86" t="s">
         <v>509</v>
       </c>
-      <c r="I20" s="111"/>
+      <c r="I20" s="110"/>
       <c r="J20" s="88" t="s">
         <v>510</v>
       </c>
@@ -11132,7 +11099,7 @@
       <c r="H21" s="95" t="s">
         <v>512</v>
       </c>
-      <c r="I21" s="111"/>
+      <c r="I21" s="110"/>
       <c r="J21" s="31" t="s">
         <v>513</v>
       </c>
@@ -11149,7 +11116,7 @@
       <c r="H22" s="95" t="s">
         <v>515</v>
       </c>
-      <c r="I22" s="111"/>
+      <c r="I22" s="110"/>
       <c r="J22" s="31" t="s">
         <v>516</v>
       </c>
@@ -11166,7 +11133,7 @@
       <c r="H23" s="95" t="s">
         <v>518</v>
       </c>
-      <c r="I23" s="111"/>
+      <c r="I23" s="110"/>
       <c r="J23" s="31" t="s">
         <v>519</v>
       </c>
@@ -11183,7 +11150,7 @@
       <c r="H24" s="90" t="s">
         <v>521</v>
       </c>
-      <c r="I24" s="111"/>
+      <c r="I24" s="110"/>
       <c r="J24" s="33" t="s">
         <v>364</v>
       </c>
@@ -11370,7 +11337,7 @@
       <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.99"/>
@@ -11421,13 +11388,13 @@
       <c r="L1" s="60"/>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="111" t="s">
         <v>523</v>
       </c>
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="112" t="s">
         <v>466</v>
       </c>
-      <c r="C2" s="114" t="s">
+      <c r="C2" s="113" t="s">
         <v>524</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -11437,13 +11404,13 @@
         <v>334</v>
       </c>
       <c r="F2" s="61"/>
-      <c r="G2" s="115" t="s">
+      <c r="G2" s="114" t="s">
         <v>525</v>
       </c>
-      <c r="H2" s="113" t="s">
+      <c r="H2" s="112" t="s">
         <v>466</v>
       </c>
-      <c r="I2" s="116" t="s">
+      <c r="I2" s="115" t="s">
         <v>378</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -11461,7 +11428,7 @@
       <c r="B3" s="84" t="s">
         <v>527</v>
       </c>
-      <c r="C3" s="114"/>
+      <c r="C3" s="113"/>
       <c r="D3" s="1"/>
       <c r="E3" s="56" t="s">
         <v>334</v>
@@ -11473,13 +11440,13 @@
       <c r="H3" s="84" t="s">
         <v>529</v>
       </c>
-      <c r="I3" s="117" t="n">
+      <c r="I3" s="116" t="n">
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="K3" s="118" t="s">
+      <c r="K3" s="117" t="s">
         <v>330</v>
       </c>
     </row>
@@ -11494,23 +11461,23 @@
         <v>448</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="118" t="s">
+      <c r="E4" s="117" t="s">
         <v>330</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="32" t="s">
         <v>533</v>
       </c>
-      <c r="H4" s="119" t="s">
+      <c r="H4" s="118" t="s">
         <v>534</v>
       </c>
-      <c r="I4" s="120" t="s">
+      <c r="I4" s="119" t="s">
         <v>535</v>
       </c>
       <c r="J4" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="K4" s="121" t="s">
+      <c r="K4" s="120" t="s">
         <v>331</v>
       </c>
     </row>
@@ -11540,7 +11507,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="118" t="n">
+      <c r="E6" s="117" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="2"/>
@@ -11555,7 +11522,7 @@
         <v>448</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="118" t="s">
+      <c r="E7" s="117" t="s">
         <v>330</v>
       </c>
       <c r="F7" s="2"/>
@@ -11568,7 +11535,7 @@
       <c r="B8" s="84"/>
       <c r="C8" s="72"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="118" t="s">
+      <c r="E8" s="117" t="s">
         <v>330</v>
       </c>
       <c r="F8" s="2"/>
@@ -11589,7 +11556,7 @@
         <v>543</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="118" t="s">
+      <c r="E9" s="117" t="s">
         <v>331</v>
       </c>
       <c r="F9" s="2"/>
@@ -11602,13 +11569,13 @@
         <v>544</v>
       </c>
       <c r="B10" s="84"/>
-      <c r="C10" s="116" t="s">
+      <c r="C10" s="115" t="s">
         <v>535</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="E10" s="118" t="s">
+      <c r="E10" s="117" t="s">
         <v>330</v>
       </c>
       <c r="F10" s="2"/>
@@ -11621,11 +11588,11 @@
         <v>546</v>
       </c>
       <c r="B11" s="84"/>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="115" t="s">
         <v>547</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="118" t="s">
+      <c r="E11" s="117" t="s">
         <v>331</v>
       </c>
       <c r="F11" s="2"/>
@@ -11637,27 +11604,27 @@
       <c r="A12" s="32" t="s">
         <v>548</v>
       </c>
-      <c r="B12" s="119" t="s">
+      <c r="B12" s="118" t="s">
         <v>466</v>
       </c>
-      <c r="C12" s="122" t="s">
+      <c r="C12" s="121" t="s">
         <v>549</v>
       </c>
       <c r="D12" s="33"/>
-      <c r="E12" s="123" t="s">
+      <c r="E12" s="122" t="s">
         <v>331</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="124"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
       <c r="J12" s="63"/>
       <c r="K12" s="63"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3"/>
-      <c r="C13" s="116"/>
+      <c r="C13" s="115"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="118"/>
+      <c r="E13" s="117"/>
       <c r="F13" s="2"/>
       <c r="G13" s="63"/>
       <c r="H13" s="63"/>
@@ -11667,7 +11634,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3"/>
-      <c r="C14" s="125"/>
+      <c r="C14" s="124"/>
       <c r="D14" s="1"/>
       <c r="F14" s="2"/>
       <c r="H14" s="4"/>
@@ -11676,7 +11643,7 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="125"/>
+      <c r="C15" s="124"/>
       <c r="D15" s="4"/>
       <c r="F15" s="2"/>
       <c r="H15" s="4"/>
@@ -11685,7 +11652,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3"/>
-      <c r="C16" s="125"/>
+      <c r="C16" s="124"/>
       <c r="D16" s="1"/>
       <c r="F16" s="2"/>
       <c r="H16" s="4"/>
@@ -11694,7 +11661,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3"/>
-      <c r="C17" s="125"/>
+      <c r="C17" s="124"/>
       <c r="D17" s="1"/>
       <c r="F17" s="2"/>
       <c r="H17" s="4"/>
@@ -11703,7 +11670,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3"/>
-      <c r="C18" s="125"/>
+      <c r="C18" s="124"/>
       <c r="D18" s="1"/>
       <c r="F18" s="2"/>
       <c r="H18" s="4"/>
@@ -11712,23 +11679,23 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3"/>
-      <c r="C19" s="125"/>
+      <c r="C19" s="124"/>
       <c r="D19" s="1"/>
       <c r="F19" s="2"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="K19" s="126"/>
+      <c r="K19" s="125"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3"/>
-      <c r="C20" s="125"/>
+      <c r="C20" s="124"/>
       <c r="D20" s="1"/>
       <c r="F20" s="2"/>
       <c r="K20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3"/>
-      <c r="C21" s="125"/>
+      <c r="C21" s="124"/>
       <c r="D21" s="1"/>
       <c r="F21" s="2"/>
       <c r="K21" s="1"/>
@@ -11744,14 +11711,14 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="3"/>
-      <c r="C23" s="125"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="2"/>
       <c r="F23" s="2"/>
       <c r="K23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="4"/>
-      <c r="C24" s="125"/>
+      <c r="C24" s="124"/>
       <c r="D24" s="1"/>
       <c r="F24" s="2"/>
       <c r="K24" s="1"/>
@@ -11766,15 +11733,15 @@
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="127"/>
-      <c r="H26" s="127"/>
-      <c r="I26" s="127"/>
-      <c r="J26" s="127"/>
-      <c r="K26" s="127"/>
+      <c r="G26" s="126"/>
+      <c r="H26" s="126"/>
+      <c r="I26" s="126"/>
+      <c r="J26" s="126"/>
+      <c r="K26" s="126"/>
     </row>
     <row r="27" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="3"/>
-      <c r="C27" s="116"/>
+      <c r="C27" s="115"/>
       <c r="D27" s="1"/>
       <c r="F27" s="2"/>
       <c r="H27" s="4"/>
@@ -11960,10 +11927,10 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="116" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="115" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="3.98"/>
@@ -12027,7 +11994,7 @@
       <c r="A3" s="19" t="s">
         <v>553</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="82" t="s">
         <v>554</v>
       </c>
       <c r="C3" s="65" t="s">
@@ -12041,14 +12008,14 @@
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="125"/>
+      <c r="I3" s="124"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="B4" s="81"/>
+      <c r="B4" s="82"/>
       <c r="C4" s="65"/>
       <c r="D4" s="31" t="s">
         <v>556</v>
@@ -12059,7 +12026,7 @@
       <c r="F4" s="35"/>
       <c r="G4" s="20"/>
       <c r="H4" s="21"/>
-      <c r="I4" s="128"/>
+      <c r="I4" s="127"/>
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
     </row>
@@ -12067,7 +12034,7 @@
       <c r="A5" s="19" t="s">
         <v>557</v>
       </c>
-      <c r="B5" s="81"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="72" t="s">
         <v>378</v>
       </c>
@@ -12080,7 +12047,7 @@
       <c r="F5" s="35"/>
       <c r="G5" s="20"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="128"/>
+      <c r="I5" s="127"/>
       <c r="J5" s="31"/>
       <c r="K5" s="20"/>
     </row>
@@ -12118,7 +12085,7 @@
       <c r="F7" s="35"/>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
-      <c r="I7" s="128"/>
+      <c r="I7" s="127"/>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
     </row>
@@ -12126,7 +12093,7 @@
       <c r="A8" s="79" t="s">
         <v>562</v>
       </c>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="82" t="s">
         <v>563</v>
       </c>
       <c r="C8" s="72" t="s">
@@ -12139,7 +12106,7 @@
       <c r="F8" s="35"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="128"/>
+      <c r="I8" s="127"/>
       <c r="J8" s="31"/>
       <c r="K8" s="31"/>
     </row>
@@ -12147,7 +12114,7 @@
       <c r="A9" s="19" t="s">
         <v>564</v>
       </c>
-      <c r="B9" s="81"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="72" t="s">
         <v>378</v>
       </c>
@@ -12171,11 +12138,11 @@
       <c r="B10" s="90" t="s">
         <v>567</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="121" t="s">
         <v>441</v>
       </c>
       <c r="D10" s="33"/>
-      <c r="E10" s="129" t="n">
+      <c r="E10" s="128" t="n">
         <v>1</v>
       </c>
       <c r="F10" s="35"/>
@@ -12187,161 +12154,161 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
-      <c r="B11" s="117"/>
-      <c r="C11" s="117"/>
+      <c r="B11" s="116"/>
+      <c r="C11" s="116"/>
       <c r="D11" s="31"/>
       <c r="E11" s="17"/>
       <c r="F11" s="35"/>
       <c r="G11" s="20"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="117"/>
+      <c r="I11" s="116"/>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20"/>
       <c r="B12" s="95"/>
-      <c r="C12" s="117"/>
+      <c r="C12" s="116"/>
       <c r="D12" s="31"/>
       <c r="E12" s="17"/>
       <c r="F12" s="35"/>
       <c r="G12" s="20"/>
       <c r="H12" s="31"/>
-      <c r="I12" s="117"/>
+      <c r="I12" s="116"/>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20"/>
-      <c r="B13" s="117"/>
-      <c r="C13" s="117"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="116"/>
       <c r="D13" s="31"/>
       <c r="E13" s="17"/>
       <c r="F13" s="35"/>
       <c r="G13" s="20"/>
       <c r="H13" s="21"/>
-      <c r="I13" s="117"/>
+      <c r="I13" s="116"/>
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="130"/>
-      <c r="B14" s="131"/>
-      <c r="C14" s="130"/>
-      <c r="D14" s="130"/>
-      <c r="E14" s="132"/>
+      <c r="A14" s="129"/>
+      <c r="B14" s="130"/>
+      <c r="C14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="131"/>
       <c r="F14" s="35"/>
-      <c r="G14" s="130"/>
-      <c r="H14" s="130"/>
-      <c r="I14" s="130"/>
-      <c r="J14" s="130"/>
-      <c r="K14" s="133"/>
+      <c r="G14" s="129"/>
+      <c r="H14" s="129"/>
+      <c r="I14" s="129"/>
+      <c r="J14" s="129"/>
+      <c r="K14" s="132"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20"/>
-      <c r="B15" s="117"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="127"/>
       <c r="D15" s="31"/>
       <c r="E15" s="21"/>
       <c r="F15" s="35"/>
       <c r="G15" s="20"/>
       <c r="H15" s="21"/>
-      <c r="I15" s="128"/>
+      <c r="I15" s="127"/>
       <c r="J15" s="31"/>
       <c r="K15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="21"/>
-      <c r="B16" s="117"/>
-      <c r="C16" s="128"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="127"/>
       <c r="D16" s="17"/>
       <c r="E16" s="21"/>
       <c r="F16" s="35"/>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
-      <c r="I16" s="128"/>
+      <c r="I16" s="127"/>
       <c r="J16" s="17"/>
       <c r="K16" s="20"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20"/>
-      <c r="B17" s="117"/>
-      <c r="C17" s="128"/>
+      <c r="B17" s="116"/>
+      <c r="C17" s="127"/>
       <c r="D17" s="31"/>
       <c r="E17" s="21"/>
       <c r="F17" s="35"/>
       <c r="G17" s="20"/>
       <c r="H17" s="21"/>
-      <c r="I17" s="128"/>
+      <c r="I17" s="127"/>
       <c r="J17" s="31"/>
       <c r="K17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20"/>
-      <c r="B18" s="117"/>
-      <c r="C18" s="128"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="127"/>
       <c r="D18" s="31"/>
       <c r="E18" s="21"/>
       <c r="F18" s="35"/>
       <c r="G18" s="20"/>
       <c r="H18" s="21"/>
-      <c r="I18" s="128"/>
+      <c r="I18" s="127"/>
       <c r="J18" s="31"/>
       <c r="K18" s="20"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="125"/>
+      <c r="C19" s="124"/>
       <c r="D19" s="1"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="125"/>
+      <c r="I19" s="124"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="125"/>
+      <c r="C20" s="124"/>
       <c r="D20" s="1"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="125"/>
+      <c r="I20" s="124"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="125"/>
+      <c r="C21" s="124"/>
       <c r="D21" s="1"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="125"/>
+      <c r="I21" s="124"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="125"/>
+      <c r="C22" s="124"/>
       <c r="D22" s="1"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="125"/>
+      <c r="I22" s="124"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="61"/>
-      <c r="B23" s="126"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="61"/>
       <c r="D23" s="61"/>
-      <c r="E23" s="134"/>
+      <c r="E23" s="133"/>
       <c r="G23" s="61"/>
       <c r="H23" s="61"/>
       <c r="I23" s="61"/>
       <c r="J23" s="61"/>
-      <c r="K23" s="135"/>
+      <c r="K23" s="134"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="125"/>
+      <c r="C24" s="124"/>
       <c r="D24" s="2"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="125"/>
+      <c r="I24" s="124"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="57"/>
-      <c r="C25" s="125"/>
+      <c r="C25" s="124"/>
       <c r="D25" s="1"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="125"/>
+      <c r="I25" s="124"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12356,10 +12323,10 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="116"/>
+      <c r="C28" s="115"/>
       <c r="D28" s="1"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="116"/>
+      <c r="I28" s="115"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12512,7 +12479,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -12552,26 +12519,26 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="135" t="s">
         <v>570</v>
       </c>
-      <c r="F2" s="136" t="s">
+      <c r="F2" s="135" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="136" t="s">
         <v>572</v>
       </c>
-      <c r="F3" s="137" t="s">
+      <c r="F3" s="136" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="137" t="s">
+      <c r="A4" s="136" t="s">
         <v>574</v>
       </c>
-      <c r="F4" s="138" t="s">
+      <c r="F4" s="137" t="s">
         <v>575</v>
       </c>
       <c r="G4" s="41"/>
@@ -12582,7 +12549,7 @@
       <c r="J4" s="41"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="136" t="s">
         <v>577</v>
       </c>
       <c r="F5" s="35"/>
@@ -12591,7 +12558,7 @@
       <c r="I5" s="35"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="138" t="s">
+      <c r="A6" s="137" t="s">
         <v>95</v>
       </c>
       <c r="B6" s="41"/>
@@ -12621,13 +12588,13 @@
       <c r="D8" s="59" t="s">
         <v>317</v>
       </c>
-      <c r="F8" s="139"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="140"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="139"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="136" t="s">
+      <c r="A9" s="135" t="s">
         <v>579</v>
       </c>
       <c r="F9" s="35"/>
@@ -12636,12 +12603,12 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="137" t="s">
+      <c r="A10" s="136" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="138" t="s">
+      <c r="A11" s="137" t="s">
         <v>581</v>
       </c>
       <c r="B11" s="41"/>
@@ -12670,7 +12637,7 @@
       <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -12710,10 +12677,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="111" t="s">
         <v>584</v>
       </c>
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="140" t="s">
         <v>585</v>
       </c>
     </row>
@@ -12721,7 +12688,7 @@
       <c r="A3" s="19" t="s">
         <v>586</v>
       </c>
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="140" t="s">
         <v>587</v>
       </c>
     </row>
@@ -12743,7 +12710,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F7" s="112" t="s">
+      <c r="F7" s="111" t="s">
         <v>589</v>
       </c>
       <c r="G7" s="57" t="s">

</xml_diff>